<commit_message>
Added new peroperty agents [Total:850]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J801"/>
+  <dimension ref="A1:J851"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -42072,6 +42072,2102 @@
         </is>
       </c>
     </row>
+    <row r="802">
+      <c r="A802" s="1" t="inlineStr">
+        <is>
+          <t>A52100017213</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Pritesh Amrutlal Bothara</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>A52100017213</t>
+        </is>
+      </c>
+      <c r="D802" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bC%2fNE%2b75M%2b4JWouUTqH%2bcwvcGKOmDwr2by98tbrA6WYastAPvEj8GwK6xM%2btm45flE2A9C0wBK%2bJL2M7K7nBfC3p1T0z5aktmSPEzXd%2bXR2wSJc%2fHdsZCVB2AGyHOlStymEIN65lHA1pvOcpb6mso6fx4M9kfEkDGZgTXDH1iw%2bW2oWDxdNmRw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E802" t="inlineStr">
+        <is>
+          <t>09579690690</t>
+        </is>
+      </c>
+      <c r="F802" t="inlineStr">
+        <is>
+          <t>Shirur</t>
+        </is>
+      </c>
+      <c r="G802" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H802" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I802" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J802" t="inlineStr">
+        <is>
+          <t>412210</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" s="1" t="inlineStr">
+        <is>
+          <t>A52100016981</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Pratapsinh Bhanudas Sitap</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>A52100016981</t>
+        </is>
+      </c>
+      <c r="D803" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=0QT91lR3h22NcdFPYXTxzv2ePXZgV4kjRiHhHbmiV78%2fbXTgj%2fpaymS9zBqedKs0NfeQcmw2xjSrNq9JgRZYaYwC1K%2fICVlOY8DVG6OeAYif5yI%2fjtkHGd3%2bq2rLjhbNJEu4bW6JC1KQl8B42v%2fX4AqO7puj9p3jXeBn1ECb3XZQ80W7%2fT9DHg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E803" t="inlineStr">
+        <is>
+          <t>08380040006</t>
+        </is>
+      </c>
+      <c r="F803" t="inlineStr">
+        <is>
+          <t>Gotandi</t>
+        </is>
+      </c>
+      <c r="G803" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H803" t="inlineStr">
+        <is>
+          <t>Indapur</t>
+        </is>
+      </c>
+      <c r="I803" t="inlineStr">
+        <is>
+          <t>Ghorpadwadi</t>
+        </is>
+      </c>
+      <c r="J803" t="inlineStr">
+        <is>
+          <t>413120</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" s="1" t="inlineStr">
+        <is>
+          <t>A52100017191</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Pruthviraj Vitthal Waghmare</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>A52100017191</t>
+        </is>
+      </c>
+      <c r="D804" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xaKWt6uIaAZBiy%2b6nQwmUOX7pfDkQOrxwraW6rtfZDn0sXoKK1xHa1zSD1%2ft9UrqB36af%2bvqFrx9C6G0MO7sQopDHI0atA8VHYTDAiV%2boZKIaC9ylyUs7KDDlyPV6p1oHjP8mXXpxvqMU7gd0PPZ1lHg1bTkVVaOsjFgKSQSfZcwzN%2fDGm7azg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E804" t="inlineStr">
+        <is>
+          <t>09881528944</t>
+        </is>
+      </c>
+      <c r="F804" t="inlineStr">
+        <is>
+          <t>Papadewasti</t>
+        </is>
+      </c>
+      <c r="G804" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H804" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I804" t="inlineStr">
+        <is>
+          <t>Fursungi</t>
+        </is>
+      </c>
+      <c r="J804" t="inlineStr">
+        <is>
+          <t>412308</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" s="1" t="inlineStr">
+        <is>
+          <t>A52100017306</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Yusuf Yakub Khan</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>A52100017306</t>
+        </is>
+      </c>
+      <c r="D805" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=JSSRLnQRhLppxU44ORX7iWBRYhiFtyiu%2fbeO8jbcE0XuaQ1ITXfwGFaiY%2fD7w0B76qJMn%2f946GlpV66M%2b7JJgz0%2fP2yE0D%2btvJnPahaGi0H8NXwtY%2f0bCX3gbLFTVu9ll4JX0ghwztPyhggdcYPED%2b%2bDqBwIwJ5m4xrUZdzZuEBQoNRwesXnnA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E805" t="inlineStr">
+        <is>
+          <t>02026860255</t>
+        </is>
+      </c>
+      <c r="F805" t="inlineStr">
+        <is>
+          <t>Kondhwa Bk</t>
+        </is>
+      </c>
+      <c r="G805" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H805" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I805" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J805" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" s="1" t="inlineStr">
+        <is>
+          <t>A52100017014</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Sachin Dipajirao Dhere</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>A52100017014</t>
+        </is>
+      </c>
+      <c r="D806" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6lZY7uyJt6E%2fDM93iidTSyCrFVlcsMIIi8cAVUlLeKZ%2fONzzaDG5u6cMgbiMvxyjN64NMe8J8ZVmCyQ1MbHJmVDHUg01l87nYQLj5giLBA1F%2bVnjiB43ZVQuX%2bogfB9j4ZwnEbu6vGbI2hNquLNc2VNIZe7UXXi%2fTRC%2bxWJeG3%2fXsDF5Au%2fj7g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E806" t="inlineStr">
+        <is>
+          <t>02226588545</t>
+        </is>
+      </c>
+      <c r="F806" t="inlineStr">
+        <is>
+          <t>Pimple Gurav</t>
+        </is>
+      </c>
+      <c r="G806" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H806" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I806" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J806" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" s="1" t="inlineStr">
+        <is>
+          <t>A52100017082</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Bharat Chandrakant Gaware</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>A52100017082</t>
+        </is>
+      </c>
+      <c r="D807" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wwbenbJLay330cXZG2xUr3ldvu9m1R9jvnm8bkrkuUETPkL%2fMWqZtydhKorbMG7THShLKaIxz3B%2brpSpXYyfVtsQb3OI5%2fTtzuNt6VTKPssazOHSWN%2bQ4cwAA0Rbw7Srd3Xfp%2fsKizWBcVpus9sreNABpKzxUw1kQCOqCZqRg%2bOITXEiR968Mw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E807" t="inlineStr">
+        <is>
+          <t>09270381852</t>
+        </is>
+      </c>
+      <c r="F807" t="inlineStr">
+        <is>
+          <t>Chandan Nagar</t>
+        </is>
+      </c>
+      <c r="G807" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H807" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I807" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J807" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" s="1" t="inlineStr">
+        <is>
+          <t>A52100017073</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Charushila Vishal Bhalerao</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>A52100017073</t>
+        </is>
+      </c>
+      <c r="D808" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=zQKsRc2LkRn%2fXV9LKRTNsl1sbrGci%2bhtFTho0V7sfuaTGJQU%2b5N5fFtotXJjgcVcYuYIgeU0Vw%2bbNvVf0lKrLCHIkuPTWYd0p78%2bbza8LmObh8b%2b4iTDxEpzTxVw%2bpS4E9Ffobh0aiPSa9kqtQNap8fb60tseH2WHTKZe2bNmx0sgnf9PyHnKw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E808" t="inlineStr">
+        <is>
+          <t>02041242041</t>
+        </is>
+      </c>
+      <c r="F808" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G808" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H808" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I808" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J808" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" s="1" t="inlineStr">
+        <is>
+          <t>A52100003166</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Popatlal Ratanchand Khater</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>A52100003166</t>
+        </is>
+      </c>
+      <c r="D809" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Luhe8tRgFJsZSkoTxM5e3Y7nTallsQKb5BWIi3YpjF1nW26Uwzua7mrGvfEJa%2bF0YGcVh1DgvA0m4QqRhegfUMs2s1nYk8ty4kB586QJypduwO1RQtCVK3xWwIiTrtBz28fVPS29tq85hRTDC2p%2bVtCgLvUKmPdT9fygyJC%2fCkt%2fXRumhZGtQA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E809" t="inlineStr">
+        <is>
+          <t>02027492761</t>
+        </is>
+      </c>
+      <c r="F809" t="inlineStr">
+        <is>
+          <t>Purnanagar</t>
+        </is>
+      </c>
+      <c r="G809" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H809" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I809" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J809" t="inlineStr">
+        <is>
+          <t>411019</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" s="1" t="inlineStr">
+        <is>
+          <t>A52100017085</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Manish Kumar  Gupta</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>A52100017085</t>
+        </is>
+      </c>
+      <c r="D810" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QcN2OS1bqHULudJ0Z%2bA1%2bszgwB35ugqGRcjLlOpddk0NRrE9RquIoAI8YINFH5MlLhuKDvXE7zEh%2bk%2fS45hzhDiUX%2f34W0ctPJ3EjAfTkQKRRRko6Y1b6pB6tNgYGdto1YQ3nSoBDJM0U3Gts3yShXpXWJ2nJd9feSib8nz%2fFZrqDFFdJ47NQA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E810" t="inlineStr">
+        <is>
+          <t>09810322190</t>
+        </is>
+      </c>
+      <c r="F810" t="inlineStr">
+        <is>
+          <t>Mangaldas Road</t>
+        </is>
+      </c>
+      <c r="G810" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H810" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I810" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J810" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" s="1" t="inlineStr">
+        <is>
+          <t>A52100017092</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Karan Anil Dhumal</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>A52100017092</t>
+        </is>
+      </c>
+      <c r="D811" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hvHv7XrB8ZXwGxbwQrGUlImPhGImMa7wLUEbiT77nOnWgzeGH1mHVuIiqVTTC%2bGS8f685P57Cd%2fc%2bBH9fuGF779dGwes5eQuSI2eIfx01Cxg%2fcVWMcnnne2U3ja38zgGMilmexhvd78Gk%2beDELEyzdF%2bGWtNrOOD35q4eR%2bLS%2fiGJTljtWehIQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E811" t="inlineStr">
+        <is>
+          <t>09890528535</t>
+        </is>
+      </c>
+      <c r="F811" t="inlineStr">
+        <is>
+          <t>Mit College Rambaug Colony</t>
+        </is>
+      </c>
+      <c r="G811" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H811" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I811" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J811" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" s="1" t="inlineStr">
+        <is>
+          <t>A52100017078</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Kamal Kerman Framna</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>A52100017078</t>
+        </is>
+      </c>
+      <c r="D812" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=gEVpU57tggtbT5054sk4Brc4GJ0tANG7TVJ0%2bOdc2fD4fWS6Io%2fbC0D%2bENAsgO9X7nrt%2bVPlKOUObzGRbvntXip%2fJ41L3p30SJu4vGtBvMeIYSA51joIh2ntGZzrG3MYfqDk23XGtadn0suZPsRSHRomgKTXzZYemgM8tYpfyzYKJDUpscV8NQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E812" t="inlineStr">
+        <is>
+          <t>02022222222</t>
+        </is>
+      </c>
+      <c r="F812" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G812" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H812" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I812" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J812" t="inlineStr">
+        <is>
+          <t>411013</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" s="1" t="inlineStr">
+        <is>
+          <t>A52100017394</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Nitin Baburao Ghuge</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>A52100017394</t>
+        </is>
+      </c>
+      <c r="D813" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ZxZNpt%2bbrx5QQ7IyqBzluFkiVggHAhBEZxn%2fcS4MEVvXqmzQ1OJDrz%2fJsbCFhMEAMETKJKE1IFP2MimqgFWLEeHeNeiMFBnlolkigjpjaauzTtmIqJoYiU0%2bFvaloLU7fuFBM4JX3wkrFVO1M9%2fXIAfFvvXLS82hfynpKQJ30UdouRwT3ZTWuQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E813" t="inlineStr">
+        <is>
+          <t>02040054364</t>
+        </is>
+      </c>
+      <c r="F813" t="inlineStr">
+        <is>
+          <t>Wanworie</t>
+        </is>
+      </c>
+      <c r="G813" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H813" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I813" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J813" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" s="1" t="inlineStr">
+        <is>
+          <t>A52100017156</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Itu  Dwivedi</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>A52100017156</t>
+        </is>
+      </c>
+      <c r="D814" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=mkdXj7KZpOR6QmWJdOUV6KKjwSfQJ3%2fXQTpbq3Qg%2btX21NDwVkS5z1NkkMUcTRhiA9KwiYReso2ddGQkCOtWuohyyXMEIqGKFK6HLjdP3UyPQMsfS6aZqnuobuhaHLfoqXtHleh0y74WJrbqgyI6JY%2bvNR%2b5qYmF2%2fvy5IzDkVOeT8dgEpnqaw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E814" t="inlineStr">
+        <is>
+          <t>02043431735</t>
+        </is>
+      </c>
+      <c r="F814" t="inlineStr">
+        <is>
+          <t>Lohegaon</t>
+        </is>
+      </c>
+      <c r="G814" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H814" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I814" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J814" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" s="1" t="inlineStr">
+        <is>
+          <t>A52100021568</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Bhushan Bhika Patil</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>A52100021568</t>
+        </is>
+      </c>
+      <c r="D815" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=mm6zn3Y1p7D%2fN4qebJ1nYq6Cbupu4m0j0ZMoKkfVH1%2bPTiPbmWAmPrRZDul2gxgd0wBfki797OqlUniWoqho%2bub704SjEZwV%2bJFw79kXbi6Mkjg6V%2fgp7D1YyfzAR25Jx2wkUy3atAPeErZOZAoL1n1x9mSFXELBWDUExonQofFS65ewu3K8xA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E815" t="inlineStr">
+        <is>
+          <t>08412852333</t>
+        </is>
+      </c>
+      <c r="F815" t="inlineStr">
+        <is>
+          <t>Moshi Pune</t>
+        </is>
+      </c>
+      <c r="G815" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H815" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I815" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J815" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" s="1" t="inlineStr">
+        <is>
+          <t>A52100017130</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Sunny  Thomas</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>A52100017130</t>
+        </is>
+      </c>
+      <c r="D816" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=8%2f8N6QyAtt0JX1xSo2WHCRETCeOhMdNxmHNzJYeralhJ0UGJsktSaNnMEXq35qOvO9ED7nZR4fW5pLaKWHHuSO7KvmD%2fejgSKP1rrBiZNZHbAhQ0Yqg6flGngTOztdX8XGettSVgP%2bXPN%2bCroqbJqy79RWaQkTd%2fIA5xr8ouFY1kKxxSY%2bChLg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E816" t="inlineStr">
+        <is>
+          <t>02026616262</t>
+        </is>
+      </c>
+      <c r="F816" t="inlineStr">
+        <is>
+          <t>Yerwada</t>
+        </is>
+      </c>
+      <c r="G816" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H816" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I816" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J816" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" s="1" t="inlineStr">
+        <is>
+          <t>A52100017406</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Noorealam Hussain Shamshad Hussain</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>A52100017406</t>
+        </is>
+      </c>
+      <c r="D817" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=sWJP4gQ5zBVBV%2bFQu%2bdyyQuyy07rnlhZAYYrJi9Jaz0O04%2bkve3j%2b4YNGl2%2bTB9PxxcYwbstIfbOyPPFWpnkmzBwU7Or8ajqyG3WU%2bsqEGXNcpVLk%2faV11w50JmMnUYGajvtlg9h37Yt8NXTYQBvZNfc0tHHmVsW0SYBa%2bTijVPxI%2brdLpqTEA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E817" t="inlineStr">
+        <is>
+          <t>02046302604</t>
+        </is>
+      </c>
+      <c r="F817" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G817" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H817" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I817" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J817" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" s="1" t="inlineStr">
+        <is>
+          <t>A52100017930</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Sharad Vamanrao Medhi</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>A52100017930</t>
+        </is>
+      </c>
+      <c r="D818" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5tPGVByDxJ4ZgHYM0LYdO11ELcBmSTrssPEUAeyoj0qOi1ljaSHkfmmwcXQzlf0HICfAUmXxyzoSFNcojHY5mzmeXiLDvqsHQPZwepEApX46h42AkFc6CLsmP6UA1lMsKxov%2bIJjObehlo5rS08zmc7JnHHAgnKQOZFinxfqNUF9GYGom%2b2L%2bQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E818" t="inlineStr">
+        <is>
+          <t>09011008575</t>
+        </is>
+      </c>
+      <c r="F818" t="inlineStr">
+        <is>
+          <t>Erandwane, Law College Road</t>
+        </is>
+      </c>
+      <c r="G818" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H818" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I818" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J818" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" s="1" t="inlineStr">
+        <is>
+          <t>A52100017077</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Sanjay Lalchand Asrani</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>A52100017077</t>
+        </is>
+      </c>
+      <c r="D819" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=tSRXH7bFS%2bkqWx82kpjg0YNEcRTTO8SQnB0sRd09cIQlSKh5v7f%2bC%2fQczfLLVZGLRZqT%2f7p1IktKqkaWdEaHehb5eOOeb8PIWZ3kvLf99fy8TYmO22elRijNw2EZD0sYBrl77NMLBm4XhWakPNdYhgqJn2xE7oU11wpssld71Nw0I0EDdO8PqQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E819" t="inlineStr">
+        <is>
+          <t>07722005152</t>
+        </is>
+      </c>
+      <c r="F819" t="inlineStr">
+        <is>
+          <t>Kharadi,</t>
+        </is>
+      </c>
+      <c r="G819" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H819" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I819" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J819" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" s="1" t="inlineStr">
+        <is>
+          <t>A52100017114</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Ajay Pandurang Temghare</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>A52100017114</t>
+        </is>
+      </c>
+      <c r="D820" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LlfEYdsrIk%2bOCN6YCA4zn6fzeqGzFZ9J2zYSL3kW%2fW83iinaZVI9kNN%2bnot4MAT8B5PETPtDkXNjbN6GyY2aAPlQ34eRcYVojZOxlpNHMAyV%2fE51EdiwVy50fDXKck6z1KEuU9rd0ngc0uRGtiqq6uW55t1Ib23s4MThEgHT3FjAtCFW2MqoZg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E820" t="inlineStr">
+        <is>
+          <t>02025870168</t>
+        </is>
+      </c>
+      <c r="F820" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G820" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H820" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I820" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J820" t="inlineStr">
+        <is>
+          <t>412101</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" s="1" t="inlineStr">
+        <is>
+          <t>A52100017128</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Rajesh Tukaram Kamthe</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>A52100017128</t>
+        </is>
+      </c>
+      <c r="D821" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=lU%2bwJV%2bXWkDu9ZI%2b4N%2bYBmwAbDZofgW%2bTfD34nayEoLnomxN%2f96Gxb6VUsfkaebchPBUmyiudCdUDpGQmrSstGj0PA3Ux0%2bLPu5mpSvEtzL8xiimjPKUrLll6Lhfh6AoxkduSZHa0IYKj3TOp2akJSwnOtC7OHHLZHZZQFavQFlOKYv7SE00KQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E821" t="inlineStr"/>
+      <c r="F821" t="inlineStr"/>
+      <c r="G821" t="inlineStr"/>
+      <c r="H821" t="inlineStr"/>
+      <c r="I821" t="inlineStr"/>
+      <c r="J821" t="inlineStr"/>
+    </row>
+    <row r="822">
+      <c r="A822" s="1" t="inlineStr">
+        <is>
+          <t>A52100017079</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Pratik Sunil Pathak</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>A52100017079</t>
+        </is>
+      </c>
+      <c r="D822" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Iapyp3BScB6oSs6ErXDsXVUErrQk9WvUgzdqCwp9sA3O17%2ftaPssLdQT%2fIM4LeXHfq%2fdYyEI32Xt6Cjw4C1YkZQDiUgg%2beqzsgLysA4QFK2thidrKhlfLTjBpPz5xbdLwDYnQUDeZJbiZhEdWQNP20bUpCLo8CJL0a3EjDIOc6DhKNtasonrxg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E822" t="inlineStr"/>
+      <c r="F822" t="inlineStr"/>
+      <c r="G822" t="inlineStr"/>
+      <c r="H822" t="inlineStr"/>
+      <c r="I822" t="inlineStr"/>
+      <c r="J822" t="inlineStr"/>
+    </row>
+    <row r="823">
+      <c r="A823" s="1" t="inlineStr">
+        <is>
+          <t>A52100017122</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Jitendra Lachhman Manglani</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>A52100017122</t>
+        </is>
+      </c>
+      <c r="D823" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=y6ghD7iQKYpa2o1e6jyVpfsyPwwdCEvSRTPR8LLiYPwS7O9HnlEk4GWqvvqtuIsHwudxFXdE2ZnBBoIRugOn5Qma%2faxyfrUXbMujf%2bJMXrpGmV0U5IA85PByIOb%2bBow1T8kGZRohNXDe7vRpXopBko%2bWD6N0rf1WhykFH2BM5ugdU%2baGSLaAOQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E823" t="inlineStr"/>
+      <c r="F823" t="inlineStr"/>
+      <c r="G823" t="inlineStr"/>
+      <c r="H823" t="inlineStr"/>
+      <c r="I823" t="inlineStr"/>
+      <c r="J823" t="inlineStr"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="1" t="inlineStr">
+        <is>
+          <t>A52100017113</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Vishakha Sachin Wakude</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>A52100017113</t>
+        </is>
+      </c>
+      <c r="D824" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wz260lcUTY48tvwz4ju4usUzTm2YiEZg5MPe7Lcwm6Twao%2fJB%2b7%2b%2b8V%2fZkvkLKnHzUm4EDvOIB945am%2by2O5PkhQGrogx7FZ44Kn1UkPjjHjNWgpHK%2bwy2%2buQHXS1MW0Ywubgaqswid0wWoKyp%2bUyvpVIMDCAP35KoQ2IpJQLL%2fSdHMCptethw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E824" t="inlineStr"/>
+      <c r="F824" t="inlineStr"/>
+      <c r="G824" t="inlineStr"/>
+      <c r="H824" t="inlineStr"/>
+      <c r="I824" t="inlineStr"/>
+      <c r="J824" t="inlineStr"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="1" t="inlineStr">
+        <is>
+          <t>A52100017089</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Pradnya Chaitanya Bangar</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>A52100017089</t>
+        </is>
+      </c>
+      <c r="D825" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=F0NPmJ3vt57RACz8kSXnpwnKAcd7R4qlxKD7ELdBGYwaoILE8soVn0u%2bh3i5iKBbWz5mVMBNoLULm5AZMTZxeCG0Zuc2r9M%2f1Mjvx9fsDzg%2bxR2hutS5UoLLQwYzOCYQTQwee20U0YR3PlH53IuDyBMIEMHz57cUE2%2b7h8JVQMZS9ZzGjtjzRw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E825" t="inlineStr"/>
+      <c r="F825" t="inlineStr"/>
+      <c r="G825" t="inlineStr"/>
+      <c r="H825" t="inlineStr"/>
+      <c r="I825" t="inlineStr"/>
+      <c r="J825" t="inlineStr"/>
+    </row>
+    <row r="826">
+      <c r="A826" s="1" t="inlineStr">
+        <is>
+          <t>A52100017143</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Sandeep Homlal Pandey</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>A52100017143</t>
+        </is>
+      </c>
+      <c r="D826" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2bWgJeXePsdnNtvt09faqY3gfOZQXakjA%2fCyxz0jI8ip4O0cV0eK0%2f%2f6PP71EjO8NuKaZbbjjrjO2aNkifSGCKLYgsnzwnVWIHjb0qUUwL5FHnq1%2bcL0wrIFWra6oBYv3Ue4SXSHe5Qb8iPj4BBKk%2bhxZU5mzx0UOn%2fdfljr5ipCEVSE5FTFavg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E826" t="inlineStr"/>
+      <c r="F826" t="inlineStr"/>
+      <c r="G826" t="inlineStr"/>
+      <c r="H826" t="inlineStr"/>
+      <c r="I826" t="inlineStr"/>
+      <c r="J826" t="inlineStr"/>
+    </row>
+    <row r="827">
+      <c r="A827" s="1" t="inlineStr">
+        <is>
+          <t>A52100017173</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Raj Bharatrao Suryawanshi</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>A52100017173</t>
+        </is>
+      </c>
+      <c r="D827" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CCNiDfDmul6jPmzVS3T6xf9pKX7yBJG5qc3zHLWWhojatPd%2b7P%2bWJot1kvTMp8MymdAAIhCIEa58xw5xL%2bH1k%2blJicXwQc8GoEkykiyqu8j9%2bxSvB9L6qpwov%2fufPvWkkuHjkrtS5jwC4fgvB6Lju8B7%2fj9JRkSBLqDAbtumLejUfoelF8J8Rw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E827" t="inlineStr"/>
+      <c r="F827" t="inlineStr"/>
+      <c r="G827" t="inlineStr"/>
+      <c r="H827" t="inlineStr"/>
+      <c r="I827" t="inlineStr"/>
+      <c r="J827" t="inlineStr"/>
+    </row>
+    <row r="828">
+      <c r="A828" s="1" t="inlineStr">
+        <is>
+          <t>A52100018439</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Santosh Ramrao Patil</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>A52100018439</t>
+        </is>
+      </c>
+      <c r="D828" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=iPgmaw0iG4ZpR6eB6LJFYuPI4pSOmNndfWIrJ%2fPM49tLWP5l6ota1v7wFI12MBzwsyuF8Z3brGjtdS1AZDQYobqAk5BYAbSgKNplF9jxZtf4Zg0HbWffsuiJIapEQyki550FhRViDo7qWfiw%2ffIrn5K0uIdsUAN7sLg3jR3Wf2ybLv%2bAtnd87w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E828" t="inlineStr"/>
+      <c r="F828" t="inlineStr"/>
+      <c r="G828" t="inlineStr"/>
+      <c r="H828" t="inlineStr"/>
+      <c r="I828" t="inlineStr"/>
+      <c r="J828" t="inlineStr"/>
+    </row>
+    <row r="829">
+      <c r="A829" s="1" t="inlineStr">
+        <is>
+          <t>A52100018508</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Dquor Spaces Llp</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>A52100018508</t>
+        </is>
+      </c>
+      <c r="D829" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=M7%2boMjlQX3MRqCyF3%2bpOi%2bTVvRx9%2fH0PR48I0gXgtnqnhlMpRQS%2fy1kig67iMZXxBeI3jdkybJ43jTsLHNhO9sDcn9M4AagvFL6p351fuq6q8oey%2boNCuS%2bJuhCacNnz1Nyx%2fZJ0%2bzuU8jTG7cIzZzPrvJyl0Og6DMEvdUY68GnOWgmv2nb%2b9Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E829" t="inlineStr"/>
+      <c r="F829" t="inlineStr"/>
+      <c r="G829" t="inlineStr"/>
+      <c r="H829" t="inlineStr"/>
+      <c r="I829" t="inlineStr"/>
+      <c r="J829" t="inlineStr"/>
+    </row>
+    <row r="830">
+      <c r="A830" s="1" t="inlineStr">
+        <is>
+          <t>A52100017351</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Amit Ramchandra Raut Proprietor Of The Four Walls Properties</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>A52100017351</t>
+        </is>
+      </c>
+      <c r="D830" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CvZr3MkUFPgM3jnOavIjroNyDjmc1I7TGdfdmhsXS7hQQEFc1kVWa1eksr26hG2sCpdVkHmUMxFam600i17lPG7ueGoOMXemmQhluBm6XPDcLvRULnOYa2Lr3r7%2fGehb94tc8p7MNe6vb8BvdKMp%2bfH0EieGgQADBgh34yLCJkR5oiXJBgSCng%3d%3d</t>
+        </is>
+      </c>
+      <c r="E830" t="inlineStr"/>
+      <c r="F830" t="inlineStr"/>
+      <c r="G830" t="inlineStr"/>
+      <c r="H830" t="inlineStr"/>
+      <c r="I830" t="inlineStr"/>
+      <c r="J830" t="inlineStr"/>
+    </row>
+    <row r="831">
+      <c r="A831" s="1" t="inlineStr">
+        <is>
+          <t>A52100017154</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Hrishikesh Vinod Shah</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>A52100017154</t>
+        </is>
+      </c>
+      <c r="D831" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Yp8ed3BOn%2fqmsiBHeZbm8ZQKaBJSeL0enS%2fzZoSlgarOttNQb6K%2farXGGUvLzGH%2fws4eeSoR3cbdUkWvB4VMDk%2fr4lkbfkW4ucI0Zx%2bAI8HBDiMv79sO2QGlBQIvNfa9JukL9L448HtvAcdjvHC8BSCT3yiwOFv36JSXqRzoa%2fiMLfleIEeZrA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E831" t="inlineStr"/>
+      <c r="F831" t="inlineStr"/>
+      <c r="G831" t="inlineStr"/>
+      <c r="H831" t="inlineStr"/>
+      <c r="I831" t="inlineStr"/>
+      <c r="J831" t="inlineStr"/>
+    </row>
+    <row r="832">
+      <c r="A832" s="1" t="inlineStr">
+        <is>
+          <t>A52100017195</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Poonam Ganpat Dixit</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>A52100017195</t>
+        </is>
+      </c>
+      <c r="D832" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=GHsc%2bx%2fHOmnPtoEhJe916FS9r%2byAC4w8SfIcdU0N5PI%2fqBy0CoxP%2fYDnwr7p%2bZogGf2r%2bJPDWGiygOOWkkA3lkhD%2bD%2fF7Almy0gGJJ5e8R%2f%2bm4NQHwtcyA1bMxYOFVs223XNkjOcGhiaTGAUm3%2fGKgsfRvUS2%2fmXNhF%2fyH5AYwXDNVVgYURkQQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E832" t="inlineStr"/>
+      <c r="F832" t="inlineStr"/>
+      <c r="G832" t="inlineStr"/>
+      <c r="H832" t="inlineStr"/>
+      <c r="I832" t="inlineStr"/>
+      <c r="J832" t="inlineStr"/>
+    </row>
+    <row r="833">
+      <c r="A833" s="1" t="inlineStr">
+        <is>
+          <t>A52100017163</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Vimal Kanhaiyalal Nimani</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>A52100017163</t>
+        </is>
+      </c>
+      <c r="D833" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=vxeRlkhyinS4ZotcFg1%2f%2fnpYYP%2br9oE18KEgAyuGeLx18fJAcBuDA4WKjLk%2b06sNaZuvm3eqmC6SOVg%2bSMU6Mj3ob7PD7aZIKAP2SalEt9aJBijQR5mM6QQ1Ma3fkGNw%2fDm%2bTqwk3%2fTEH80Eno3nNjUeITAdqHjKvQuclS4a3Njz1wxf4yMRvg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E833" t="inlineStr"/>
+      <c r="F833" t="inlineStr"/>
+      <c r="G833" t="inlineStr"/>
+      <c r="H833" t="inlineStr"/>
+      <c r="I833" t="inlineStr"/>
+      <c r="J833" t="inlineStr"/>
+    </row>
+    <row r="834">
+      <c r="A834" s="1" t="inlineStr">
+        <is>
+          <t>A52100017198</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Anima  Prasad</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>A52100017198</t>
+        </is>
+      </c>
+      <c r="D834" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=OWC78TCWRXYU3kmdIXTM2JG%2bw%2bCScLFfm%2fuH2N3g%2bnQBruOs4t7Wqusk7cmnaZB8WaBUqe2Dl6yhvJmt1l0CX8HAvHlt0q7OltxhMBpGLnMrv5D1tTOTZQ8WYss5nYR3nC5gVFF1%2fRFmz%2b4gUqpIzMixIbvZeZe4vITQNQKE4oWzYS7LU1LLoQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E834" t="inlineStr"/>
+      <c r="F834" t="inlineStr"/>
+      <c r="G834" t="inlineStr"/>
+      <c r="H834" t="inlineStr"/>
+      <c r="I834" t="inlineStr"/>
+      <c r="J834" t="inlineStr"/>
+    </row>
+    <row r="835">
+      <c r="A835" s="1" t="inlineStr">
+        <is>
+          <t>A52100017231</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Abhishek Pradeeprao Patil</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>A52100017231</t>
+        </is>
+      </c>
+      <c r="D835" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=TQIvWrfkBWXk8O0Hbc9ZbOm%2b3foPwmpRchqPuJtdQy%2fkghemrjtbFdw7n%2bI6mHTRWcF5V5cIPqSyNvjMept5PqBKWej3DMi3bsQ4hT6Weus9kSms7sNIPZq%2bVYeBCmBGssx2SuOg1o7Ox5nW1pflP3C80648m66ZR7InFHErtHsDhMKDuww6Jg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E835" t="inlineStr"/>
+      <c r="F835" t="inlineStr"/>
+      <c r="G835" t="inlineStr"/>
+      <c r="H835" t="inlineStr"/>
+      <c r="I835" t="inlineStr"/>
+      <c r="J835" t="inlineStr"/>
+    </row>
+    <row r="836">
+      <c r="A836" s="1" t="inlineStr">
+        <is>
+          <t>A52100017157</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Namita Bhaskar Shibad</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>A52100017157</t>
+        </is>
+      </c>
+      <c r="D836" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2bgTDX5JTFf9EQLFShr9tXRAbuxl%2b8U26WWk9Zoe3QQmUxnq79m2nrS9JACZ26748DHRGLPDCWollcxpa9P7hKB4LoqQJipLKVrEN%2fa3WNtJyICbPecgr%2b6O2Ly0KUw7vKPo2FfxjaqAljo007zBeM4PoSrLCkLs5fJpOWMobtREpgodgQ%2b%2fgMQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E836" t="inlineStr"/>
+      <c r="F836" t="inlineStr"/>
+      <c r="G836" t="inlineStr"/>
+      <c r="H836" t="inlineStr"/>
+      <c r="I836" t="inlineStr"/>
+      <c r="J836" t="inlineStr"/>
+    </row>
+    <row r="837">
+      <c r="A837" s="1" t="inlineStr">
+        <is>
+          <t>A52100017200</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Pratik Mahadu Kadlak</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>A52100017200</t>
+        </is>
+      </c>
+      <c r="D837" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bGrzmsWtLsARl1z980KlEbwYgW0ChbVXyzUgTwA9dZvn%2fLLTWrqa%2fKuNPk3hh3pL2hbmI5XbRexEg8iB0G3gpYGnxdGXGGFJfpzJ39xwzR2b7n900XGTeQ8ZL0JaOeggHJMKwvvxUoIWZN30XMvdG%2bhJFC8yF0n%2ffySA4Ic24ZXGTcc4FLCfNg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E837" t="inlineStr"/>
+      <c r="F837" t="inlineStr"/>
+      <c r="G837" t="inlineStr"/>
+      <c r="H837" t="inlineStr"/>
+      <c r="I837" t="inlineStr"/>
+      <c r="J837" t="inlineStr"/>
+    </row>
+    <row r="838">
+      <c r="A838" s="1" t="inlineStr">
+        <is>
+          <t>A52100017228</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Raviraj Sunil Pawar</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>A52100017228</t>
+        </is>
+      </c>
+      <c r="D838" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=EgEsh6nIifvQlp8zcWW8v1lZZTDNf5nqCGIwvr7smn9THvcbQdx4s4sUYqBGSAU1SbFV90LRoExNQu%2brtQ9NTTk3UR%2fqSlmu62hY23x41c%2fDc3yiIX2SMZALcuDCSv7gZ0WxAz0bZGO7PaJ%2fY9Dm1Np8z6bfpC0WZe5uZs5UP1MAW%2frh7U3Yrg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E838" t="inlineStr"/>
+      <c r="F838" t="inlineStr"/>
+      <c r="G838" t="inlineStr"/>
+      <c r="H838" t="inlineStr"/>
+      <c r="I838" t="inlineStr"/>
+      <c r="J838" t="inlineStr"/>
+    </row>
+    <row r="839">
+      <c r="A839" s="1" t="inlineStr">
+        <is>
+          <t>A52100017433</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Sandeep Shankarrao Kulkarni Proprietor Of Sandeep Construction</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>A52100017433</t>
+        </is>
+      </c>
+      <c r="D839" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=cwnbihaN4aZJfmiPROkrXRGMHmo5TbTH1aLhzYhv%2bxR8me5gMPiP3gHx0bQnRikdPPBskBhvQIV2MCuJhCxhVckTr2B65Kj5Go%2bF85QYQNrm1wVX1LMAFWkzVbZkLnP9U7D4o8XVrSwl4beWKr6YDhoik8sO3DopW%2ffRvIk4VQW0mJTqEyPL%2fw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E839" t="inlineStr"/>
+      <c r="F839" t="inlineStr"/>
+      <c r="G839" t="inlineStr"/>
+      <c r="H839" t="inlineStr"/>
+      <c r="I839" t="inlineStr"/>
+      <c r="J839" t="inlineStr"/>
+    </row>
+    <row r="840">
+      <c r="A840" s="1" t="inlineStr">
+        <is>
+          <t>A52100017159</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Shekhar  Khandelwal</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>A52100017159</t>
+        </is>
+      </c>
+      <c r="D840" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=qqfWT0CgmdMGno5thZ6ccB8jWDYneoRxZMj7cA%2bYi7elBP1ydrh37uD5LH59NSnxJOer6wr5pZNjzYZSBY7wcFyhwJSkQ68Zzacx5IyqiIMNpymOptpCR6c9g2ffRD71tx%2fNi1gvWKGTVZxXcU%2btNaJ1T3xrUPcSm5uu4P3oIhnGWSohxGHY4w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E840" t="inlineStr"/>
+      <c r="F840" t="inlineStr"/>
+      <c r="G840" t="inlineStr"/>
+      <c r="H840" t="inlineStr"/>
+      <c r="I840" t="inlineStr"/>
+      <c r="J840" t="inlineStr"/>
+    </row>
+    <row r="841">
+      <c r="A841" s="1" t="inlineStr">
+        <is>
+          <t>A52100017223</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Manish Atmaram Dhengle</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>A52100017223</t>
+        </is>
+      </c>
+      <c r="D841" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=OzHN4Kjcv3geBR7adLIJdvIfuuY8rwCLqTVKd1pOBz5Ss3Ka9PcNmL14zE48s9IGf70UJYYo5aMj3MlSTuAEL5x0alc3uV9i2Inq72I%2bU8e54PVAcRpRQGSFQXCr92wBhUqr68nPD2tP4zG0ru3Tgxh7vMZrT13MRIRZz%2bx3%2fZlf3ghBCLftcA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E841" t="inlineStr"/>
+      <c r="F841" t="inlineStr"/>
+      <c r="G841" t="inlineStr"/>
+      <c r="H841" t="inlineStr"/>
+      <c r="I841" t="inlineStr"/>
+      <c r="J841" t="inlineStr"/>
+    </row>
+    <row r="842">
+      <c r="A842" s="1" t="inlineStr">
+        <is>
+          <t>A52100022493</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Sanjoo  Melwani</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>A52100022493</t>
+        </is>
+      </c>
+      <c r="D842" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ycssSP8tzPlMkNHtte8m3pZYkhRdIWRSjYrTsj8v%2ffMATHZMn9n7OLzI9Z6PasHilcQVPEsHb5oECHG1S%2b%2bT4kqH98UsZY4uuxYSfcKgZiCGDNqxu40qZ1%2f%2fgWfHwS8WFqDyTW6MGCTyTuO20O0y5I04TrRVa4GEHcuKn38TKPZF%2feYgYnQjAw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E842" t="inlineStr">
+        <is>
+          <t>02026152891</t>
+        </is>
+      </c>
+      <c r="F842" t="inlineStr">
+        <is>
+          <t>Alandi</t>
+        </is>
+      </c>
+      <c r="G842" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H842" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I842" t="inlineStr">
+        <is>
+          <t>Charholi</t>
+        </is>
+      </c>
+      <c r="J842" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" s="1" t="inlineStr">
+        <is>
+          <t>A52100017185</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Harshal Hemant Lunkad</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>A52100017185</t>
+        </is>
+      </c>
+      <c r="D843" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5NiXfJSGu2tGEB6446mHUJ9LGjHsLo3z80CTgO8Kc3mdgZNImjHl3yD3up6yMObjHGyuKZLV8SunohkCFN4yETp6BzFS4CPDTtCBt%2bW3HdPhWIGMV%2bFUuvITcsd8ibUnmKT9B%2f2YyW3j6VA9usXREY%2bQqQ31xtxx1jg3AX66mLMseUPVn5nwQg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E843" t="inlineStr">
+        <is>
+          <t>08087461718</t>
+        </is>
+      </c>
+      <c r="F843" t="inlineStr">
+        <is>
+          <t>Dapodi</t>
+        </is>
+      </c>
+      <c r="G843" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H843" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I843" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J843" t="inlineStr">
+        <is>
+          <t>411012</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" s="1" t="inlineStr">
+        <is>
+          <t>A52100017317</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Nikhil Ramrao Deshmukh</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>A52100017317</t>
+        </is>
+      </c>
+      <c r="D844" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6hbAcS1VupCIT4i2T9n38M1fJwuw3Rjsh0CNxTEZJJ7VJrsaZi1aKIBTj5o96pYWH5LSr8cIsQIqflMAM4Lk2uJ6LRozwd8iyp8KhFsaka4%2bIPXiWf9%2bxTHug3PwTYITIueZvv84BR9ogtNz%2bKPLyq0pIn0cEWYtfZwHBgIHn5NwgvcrMTbRkQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E844" t="inlineStr">
+        <is>
+          <t>02024690489</t>
+        </is>
+      </c>
+      <c r="F844" t="inlineStr">
+        <is>
+          <t>Dhayari</t>
+        </is>
+      </c>
+      <c r="G844" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H844" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I844" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J844" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" s="1" t="inlineStr">
+        <is>
+          <t>A52100017193</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Anant Damodar Sawant</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>A52100017193</t>
+        </is>
+      </c>
+      <c r="D845" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=dD2CVUXLmrTB4YO9nl%2b5GCknJQeuz%2b7sYMJ5Lo8xKfrphdnAd%2b7qU95zK9wJCNrPHbGZTcZF9Mt2vJe%2fhiXidnr1nywn7F%2buppLZMWTSzFZTV0LsamkvPXKdNhXA0PpPCwAgS7aZgN6Akm0mk2ug3HsBhMlfBz%2fm7h49qpkWqemeJM7F7sTMnA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E845" t="inlineStr">
+        <is>
+          <t>02025449577</t>
+        </is>
+      </c>
+      <c r="F845" t="inlineStr">
+        <is>
+          <t>Bopkhel</t>
+        </is>
+      </c>
+      <c r="G845" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H845" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I845" t="inlineStr">
+        <is>
+          <t>Kirkee (Cb)</t>
+        </is>
+      </c>
+      <c r="J845" t="inlineStr">
+        <is>
+          <t>411031</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" s="1" t="inlineStr">
+        <is>
+          <t>A52100017251</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Sunil Tukaram Pawar</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>A52100017251</t>
+        </is>
+      </c>
+      <c r="D846" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=y%2bFDvxarYY4vDJyLqS%2flqdpUBthHh67M0smuKoqVK2niCVU4sjzNxVOdlsyjuegYoe4vxS0hE9SlxNrd2k%2b4pn1NGfrWYASw7gCpDFt57SNIjRrzgCz13SocSVCcP%2fw7CdKnjw4eT6OdOE%2fhLSRC3Ur4aa08t68h5E6MfUBu2zt5Itk2wsWzeA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E846" t="inlineStr">
+        <is>
+          <t>02025432611</t>
+        </is>
+      </c>
+      <c r="F846" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G846" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H846" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I846" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J846" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" s="1" t="inlineStr">
+        <is>
+          <t>A52100018230</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Housewalas</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>A52100018230</t>
+        </is>
+      </c>
+      <c r="D847" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=I6nsLpSRKO0my0uhsDKH4c69vpelzb06%2bVgy6kNK2GQEfpY5tea69y7Lidadrxp8HcMehd1KiQ6FXPVaQcAxXypEpFB39Dru5%2f2itEu7cdQWri%2bBlHq4zox70etGkDbzXWnNPEEtId1K6Rdu1QmVVsG%2bdPh92GIX%2fWHlPqTbrobNbdHEEVzk0Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E847" t="inlineStr">
+        <is>
+          <t>02024619613</t>
+        </is>
+      </c>
+      <c r="F847" t="inlineStr">
+        <is>
+          <t>Ambegaon Bk</t>
+        </is>
+      </c>
+      <c r="G847" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H847" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I847" t="inlineStr">
+        <is>
+          <t>Ambegaon Bk</t>
+        </is>
+      </c>
+      <c r="J847" t="inlineStr">
+        <is>
+          <t>411046</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" s="1" t="inlineStr">
+        <is>
+          <t>A52100017224</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Rameez Jilani Shaikh</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>A52100017224</t>
+        </is>
+      </c>
+      <c r="D848" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=DWUuqDckvvV2r0U0znIgmPQQKs223hjrpyTxIy4pHn9CascW%2bxX1J2m0t3GSy1L4Lq75PLnOwAKqc1LpG7Qwsio58WTwkcfZhnqd%2b0DKqVvWT%2bIJ%2fHTyb74lpAMXhWWSSh1L%2b9XAzPgSB3lvTLj8uu4DXufvQaBR7cocSHuVot2DoN5nVvzabw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E848" t="inlineStr">
+        <is>
+          <t>08087708530</t>
+        </is>
+      </c>
+      <c r="F848" t="inlineStr">
+        <is>
+          <t>Kausar Baug</t>
+        </is>
+      </c>
+      <c r="G848" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H848" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I848" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J848" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" s="1" t="inlineStr">
+        <is>
+          <t>A52100017219</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Priya Shashank Bafna</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>A52100017219</t>
+        </is>
+      </c>
+      <c r="D849" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=S7HrDazgQuZnAIpvy%2fbhXoETH5Ayfp3BKArE6rnGtsfrzDXPCqTNfS9rAixn65dsFJoffQIcFoUN32a0XecEN8EcqKygvlrOvqnQK%2boLdTpWKq7phMYcrRHE9a6ecgYhCCvvagllmdmirA3%2bMq1INqVhMrU7cMdBXyfrQi4Uu9zVw9R%2bJ%2f8DuA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E849" t="inlineStr">
+        <is>
+          <t>02024216050</t>
+        </is>
+      </c>
+      <c r="F849" t="inlineStr">
+        <is>
+          <t>Bibwewadi</t>
+        </is>
+      </c>
+      <c r="G849" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H849" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I849" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J849" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" s="1" t="inlineStr">
+        <is>
+          <t>A52100017383</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Shreekant Nilkanth Kelkar</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>A52100017383</t>
+        </is>
+      </c>
+      <c r="D850" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=aEQ8l8rWSAAQdpTDSz9RbsD4gStKWFtpUAH7VdHo9%2bFBeASkFYwLdRRasotawBekDqtpw2hDlip%2f9sZyuakZY7smb7oUTaLxkaT%2biBxG0uf5tp%2b%2fcTlA50n2EHZSjGMT%2fO%2fiLTZjrWz6HBecblXh6f8g4KqbG8d35VjrF%2b3RipRVay69EwRrww%3d%3d</t>
+        </is>
+      </c>
+      <c r="E850" t="inlineStr">
+        <is>
+          <t>02025460084</t>
+        </is>
+      </c>
+      <c r="F850" t="inlineStr">
+        <is>
+          <t>Maha Ganesh Colony</t>
+        </is>
+      </c>
+      <c r="G850" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H850" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I850" t="inlineStr">
+        <is>
+          <t>Karve Nagar</t>
+        </is>
+      </c>
+      <c r="J850" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" s="1" t="inlineStr">
+        <is>
+          <t>A52100017192</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Krupa Maruti Jadhav</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>A52100017192</t>
+        </is>
+      </c>
+      <c r="D851" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=zQeqzcUqv4emV7cEyGW8Rodx7hcHu3qRb5pc9WugC4YhpXi4B3d53oA4i4xVrBhGP6fi2ZNl2MCdZ2vZY1jXxpYY0kOuw6Epl562lsmmUCRBKWRWXEq5UVarJ%2b00qTwrbmB26cwllTIzXc6RHlXw%2fMDUdPNcdgqhLKpk%2bsspCSUV2wpNTHzyVQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E851" t="inlineStr">
+        <is>
+          <t>08149499586</t>
+        </is>
+      </c>
+      <c r="F851" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G851" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H851" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I851" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J851" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:900]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J851"/>
+  <dimension ref="A1:J901"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44168,6 +44168,2606 @@
         </is>
       </c>
     </row>
+    <row r="852">
+      <c r="A852" s="1" t="inlineStr">
+        <is>
+          <t>A52100017261</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Kishor Uddhav Nimbore Prorietor Of Dream House Solutions</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>A52100017261</t>
+        </is>
+      </c>
+      <c r="D852" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=XfWM30QAhIKL7qLKmH1sjNrFwsl6zpERLLd2TWzu1tdpj4tm1J3wpx8qLW4y0wiS4LqbkoeLt1e8YoGpvEe5Uv4vJqXgKEAmCjutFjbqszSrR2N6uPDh9SVj%2fW%2b8HiMcKmkRMCN17vTbBVWhG1PrkoabaaBj%2f75nbzqVDGyns0S26nmVMbYsDQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E852" t="inlineStr">
+        <is>
+          <t>02078881221</t>
+        </is>
+      </c>
+      <c r="F852" t="inlineStr">
+        <is>
+          <t>Boradewadi, Moshi</t>
+        </is>
+      </c>
+      <c r="G852" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H852" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I852" t="inlineStr">
+        <is>
+          <t>Aalandi</t>
+        </is>
+      </c>
+      <c r="J852" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" s="1" t="inlineStr">
+        <is>
+          <t>A52100017399</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Propertylogist Realty Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>A52100017399</t>
+        </is>
+      </c>
+      <c r="D853" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=9oaR%2bzV29h2bIU20jc8MAPAt5eF5WH4nRAI0PvoqmQLtXFrf8KBdZrNqImjVTtivJaCNmVNBucWXtgEVEzaUaRs3Uu%2fkgc39D9tw%2bn1tc2%2fvBmnebxNYg11b8MhwFjE0voHNvesBfC5f1JGfjLXrVZ26NDjZ3RVJ167cJ%2beGMcKefxRdSDOTEA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E853" t="inlineStr">
+        <is>
+          <t>02024484284</t>
+        </is>
+      </c>
+      <c r="F853" t="inlineStr">
+        <is>
+          <t>Shukrawar Peth</t>
+        </is>
+      </c>
+      <c r="G853" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H853" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I853" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J853" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" s="1" t="inlineStr">
+        <is>
+          <t>A52100002975</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Kishor Pandurang Mhaske</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>A52100002975</t>
+        </is>
+      </c>
+      <c r="D854" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bN1eH0zXrWl9fTzG386iVo4NEsQPWxdliQJwOW%2fMTm33AylOwbE2sHYilY%2fNT3FvRTZozMzI2lylTRHI6EYz3oLSIVDzGT14AjetRm9kGmpHBAvWHZ2w8USRARZJ82xB6I9olVldTZJUc1m9lfR74YV0Ub%2fIx%2f1O4h3Mb60hwxlQJXUX4xbSbA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E854" t="inlineStr">
+        <is>
+          <t>09834146127</t>
+        </is>
+      </c>
+      <c r="F854" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G854" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H854" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I854" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J854" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" s="1" t="inlineStr">
+        <is>
+          <t>A52100017328</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Pawan Ajit Choudhari</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>A52100017328</t>
+        </is>
+      </c>
+      <c r="D855" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=noHHoOvgghtxmJtPe0ujzk7fLtQxnEhnGGLCvFIqwe1jE4mh7L%2fV6lcqN0yb5Vt%2fk2pr7ig%2bEKL1o4zpAlH96mGUrHzBaTGA1jntDIR8CncPdVlFEFLm0I2mCrsZhymLNhOHxSwiyGWiqtfItbAD2yIQ7TOoMH%2fEnavnexSvMIYXFpgEBDXefw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E855" t="inlineStr">
+        <is>
+          <t>11111111111</t>
+        </is>
+      </c>
+      <c r="F855" t="inlineStr">
+        <is>
+          <t>Nanded City</t>
+        </is>
+      </c>
+      <c r="G855" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H855" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I855" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J855" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" s="1" t="inlineStr">
+        <is>
+          <t>A52100017456</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Pradnya Shantaram Shardul</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>A52100017456</t>
+        </is>
+      </c>
+      <c r="D856" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=L0HK5vpanII3z7Ky4q%2fHPZOlwL5JXZAuAsSPYC34UtPmzxQNpI%2bXH9njyN55jqchEFwm6ha4XCWSSgVGG6RiFMyJX780Z%2fTV5YESn%2bvcK4g60UwX5J6rKpI42Z7x%2bw3v8W2pnrBzGM5isjhLskZIuBs0RxjfszH5unjRf2btvVaeKyIgHjeI1g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E856" t="inlineStr">
+        <is>
+          <t>09421792651</t>
+        </is>
+      </c>
+      <c r="F856" t="inlineStr">
+        <is>
+          <t>Hinjewadi</t>
+        </is>
+      </c>
+      <c r="G856" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H856" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I856" t="inlineStr">
+        <is>
+          <t>Hinjavadi (Ct)</t>
+        </is>
+      </c>
+      <c r="J856" t="inlineStr">
+        <is>
+          <t>412115</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" s="1" t="inlineStr">
+        <is>
+          <t>A52100017214</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Pratik Vijay Puri</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>A52100017214</t>
+        </is>
+      </c>
+      <c r="D857" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Y9N4%2fExzBVo8JCI1ETbSnqE3FUQgjfAXjdy%2bxpkFer9UCxj4JQV9t5HVP1q8OAI6e7Txmd7Fs%2frKyaBzijaiRt3bd2y%2bxFLQrpFKfsG46lSznmm8V0gFVo82cyQgjlH%2flqlRGSEAt5xy4UZOG1X%2b4YvW4c3v20JOhBy9ooE%2flY7Xf1wktsJCHw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E857" t="inlineStr">
+        <is>
+          <t>09175192828</t>
+        </is>
+      </c>
+      <c r="F857" t="inlineStr">
+        <is>
+          <t>Katraj</t>
+        </is>
+      </c>
+      <c r="G857" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H857" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I857" t="inlineStr">
+        <is>
+          <t>Katraj</t>
+        </is>
+      </c>
+      <c r="J857" t="inlineStr">
+        <is>
+          <t>411046</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" s="1" t="inlineStr">
+        <is>
+          <t>A52100017845</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Ashok Shivalingappa Kalshetti</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>A52100017845</t>
+        </is>
+      </c>
+      <c r="D858" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QIOGDkSzT2RQ7lq4MtQoFir5M988%2fOI2HwEGrN6TxAkzUog0o4CijwOcxVqy1iP3XvXXZw0f0T7VnYgy6RF7kAixUH6TXwawILu1VQnniUMeVQA7WFEJYxMpUAq4zQ43eH8XMpXFUl7dGlfa0y2yteHbdT1GJPsHm5R%2ffOfDAlhFMgEYzWqwyQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E858" t="inlineStr">
+        <is>
+          <t>02041295992</t>
+        </is>
+      </c>
+      <c r="F858" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G858" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H858" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I858" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J858" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" s="1" t="inlineStr">
+        <is>
+          <t>A52100017472</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Neeta Vipul Parte</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>A52100017472</t>
+        </is>
+      </c>
+      <c r="D859" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=dLd3a4PtjNnvAMJqonNNKsdy3%2fAL6la4QVmQNVgU75N2Dhg2Fvinop4NH%2fdKH0Jybziac6pCNoKfeewfo1FrFH34dNWt9iPzuL6KTKFeNxzf7WG3T40CpsSIuB21ekrLulPMJk%2fhH6MAd4aIjPxR%2b%2fMm68BLMkALK58FL0nvxuTS5dI2nG6IYQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E859" t="inlineStr">
+        <is>
+          <t>08830237749</t>
+        </is>
+      </c>
+      <c r="F859" t="inlineStr">
+        <is>
+          <t>Bhairavnagar</t>
+        </is>
+      </c>
+      <c r="G859" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H859" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I859" t="inlineStr">
+        <is>
+          <t>Vishrantwadi</t>
+        </is>
+      </c>
+      <c r="J859" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" s="1" t="inlineStr">
+        <is>
+          <t>A52100017460</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Girija Nandan Kashinath Mishra</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>A52100017460</t>
+        </is>
+      </c>
+      <c r="D860" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=vWSgHZ9wn6%2f7SOLMEDtbi8sUqkTn%2b9LzySzsWgp%2fj3%2bMq%2bUMdz1U%2ffUJHDQAIXuFOJqU8lN4dskuNhMaUlpRgn6we1hWxTBv1P0ZHZyTA6SsKB1sF2JQO3Px%2fjhARJBFQQSEFPoGeY6pnQGNQQR36DJgIEtj8I%2fyfFm8MmohtQfJNuI4hGwD9g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E860" t="inlineStr">
+        <is>
+          <t>02012346302</t>
+        </is>
+      </c>
+      <c r="F860" t="inlineStr">
+        <is>
+          <t>Pimplegurav</t>
+        </is>
+      </c>
+      <c r="G860" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H860" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I860" t="inlineStr">
+        <is>
+          <t>Pimpale Gurav</t>
+        </is>
+      </c>
+      <c r="J860" t="inlineStr">
+        <is>
+          <t>411061</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" s="1" t="inlineStr">
+        <is>
+          <t>A52100017239</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Digvijay Dhananjay Parkale</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>A52100017239</t>
+        </is>
+      </c>
+      <c r="D861" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fwglTV45AJ1YN5oksKR%2bbqffNxVOF4UKLt%2frkDAzXgwzcykPuajtPojrHR1ya7JVr45XxarmzXLavvL7jK9Eq8lPFAwwbZuf5Jx5eRtZuJRA8buwYzF8rE%2bPJX09N3LYgkDoRMabl5Dutuo0mtvuUcc3b5Ww7rpgrzDuKOrOLgO6Kcgv2t%2f5Tg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E861" t="inlineStr">
+        <is>
+          <t>02025672009</t>
+        </is>
+      </c>
+      <c r="F861" t="inlineStr">
+        <is>
+          <t>Balewadi</t>
+        </is>
+      </c>
+      <c r="G861" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H861" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I861" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J861" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" s="1" t="inlineStr">
+        <is>
+          <t>A52100005186</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Dinesh Shriram Khandelwal</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>A52100005186</t>
+        </is>
+      </c>
+      <c r="D862" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=BGvdcGSgdbKJH7hnklZT1J%2bNEA6aIawjyZYtT0LvhlzBDn5ovPk0uxHloMluVp75Z7TrxW5XqfHA3bJJlPxcnU7eom0zOrVUpFwaa8rRrq4hEQMMqa5YoQPnFaBZy4EybEP7AqiCgp9esthQqGouM2pRroNxfAS4vJrvyN8KvOHfm%2bPOXLWKpg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E862" t="inlineStr">
+        <is>
+          <t>02024351056</t>
+        </is>
+      </c>
+      <c r="F862" t="inlineStr">
+        <is>
+          <t>Manikbag</t>
+        </is>
+      </c>
+      <c r="G862" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H862" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I862" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J862" t="inlineStr">
+        <is>
+          <t>411051</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" s="1" t="inlineStr">
+        <is>
+          <t>A52100017517</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Ashutosh P Joshi</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>A52100017517</t>
+        </is>
+      </c>
+      <c r="D863" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=4PGGd%2bYYuQCCTVb58QhD7VO2YV1Y0dK%2bvfS2UY1tqGKNnRlpcU67Jjl22OCT2%2fVJQofeqjquN%2bdOsfND2qYYh3Sg2hx%2f5uwJn3vfMMNXGeuLrFW8XQKl4dVM8NsGupVdoqt9lWnJMQaNSyhvA2qhYS4qBlP8KEArmV8FT9ex6X%2bv0vLy5MgFgA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E863" t="inlineStr">
+        <is>
+          <t>02026349793</t>
+        </is>
+      </c>
+      <c r="F863" t="inlineStr">
+        <is>
+          <t>Camp</t>
+        </is>
+      </c>
+      <c r="G863" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H863" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I863" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J863" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" s="1" t="inlineStr">
+        <is>
+          <t>A52100017423</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Prashant Malhari Kunjir</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>A52100017423</t>
+        </is>
+      </c>
+      <c r="D864" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MrIgbc06yPYK621PmTakkoj4hXCUz18onYyEup1EBg%2bFdfKtZl2Y2HpTcHJO%2fz1Hg7tRupUZJK%2bM4nr8S6pPVO1%2bYtqNfNsNi7Ax05cr8ZAKyNV9l8%2f9e3bftXz3QTldEx3SnX1yTkS75wrEbmrYXY0cUPl%2bFhXEKV0PxqXrEfoUSbJ4DhUQLQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E864" t="inlineStr">
+        <is>
+          <t>09730670000</t>
+        </is>
+      </c>
+      <c r="F864" t="inlineStr">
+        <is>
+          <t>Nigdi</t>
+        </is>
+      </c>
+      <c r="G864" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H864" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I864" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J864" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" s="1" t="inlineStr">
+        <is>
+          <t>A52100017405</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Saiphan Basulal Shaikh</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>A52100017405</t>
+        </is>
+      </c>
+      <c r="D865" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=HGJZq4qJbUfvekwTJ6fPpQJkiapb8a4y0DaUfd18FJYUEPQgE2JeFjatFv1iYvrtYOuWGFliuOO5AlzEHBWdOcL6i6GStGidLt2G16K0GJEIo0UV82gkC4e6rLAICOCqxNMvLHCwJjAytaciXLToxYCTJ9L%2bAw%2fAXCh4V5MsXRwe8DT0emRIDQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E865" t="inlineStr">
+        <is>
+          <t>02027515585</t>
+        </is>
+      </c>
+      <c r="F865" t="inlineStr">
+        <is>
+          <t>Sant Tukaram Nagar</t>
+        </is>
+      </c>
+      <c r="G865" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H865" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I865" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="J865" t="inlineStr">
+        <is>
+          <t>411018</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" s="1" t="inlineStr">
+        <is>
+          <t>A52100017685</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Jyoti Sachin Chakranarayan</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>A52100017685</t>
+        </is>
+      </c>
+      <c r="D866" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=jUaB21m2I0g%2buVUgf3P4tCTxwm5MUmN7s3EtvL4HLXCPTQmR5h%2bi6EYXrABDVBH4AtXH4ISJMSP%2fxePGyg2k3rzy%2bsrXBlh1yFP3lazjj3GaL5RL5ZEjjkVbAdx75KOkRYCHhPEKrEV9bDupaTUiK%2fOHdVdeUk%2ffkU7RIRaADvX7ECi1r80w%2fA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E866" t="inlineStr">
+        <is>
+          <t>09767033987</t>
+        </is>
+      </c>
+      <c r="F866" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="G866" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H866" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I866" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J866" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" s="1" t="inlineStr">
+        <is>
+          <t>A52100018182</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Prashant  Colvin</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>A52100018182</t>
+        </is>
+      </c>
+      <c r="D867" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=lCuiiSFaxoJT%2fEz7QOhu9lE7IXLY4EUUXTM21eHnlx5MuIC%2bH3auz9haWtaDbZ2oXJ8Nzkaspa4h4r2dw8SYaoLerGR9Cqc4acYwqtiDWJ0mHQJi0VkWI6lbhRo8IiFY0QPqxlpuANGXATpxVDcNAEk600CZg8cG1T3yTgtNTsJENidwgGsyRA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E867" t="inlineStr">
+        <is>
+          <t>09850847774</t>
+        </is>
+      </c>
+      <c r="F867" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="G867" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H867" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I867" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J867" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" s="1" t="inlineStr">
+        <is>
+          <t>A52100017330</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Alok  Kumar</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>A52100017330</t>
+        </is>
+      </c>
+      <c r="D868" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=P33hmiHSJymPIugKSMC1Ea2F5rH8dm9JlE5NP2l4Oh6q14d7%2f086ywQ1HFGWk3mnM3uTXEqcvDgg3dNgTrseo%2b6Cfne1I4z4XZ1V6cWoK24MQ4nVJgJ51zDLZc6lQ0c1FGAycof1FqSzIqTQwKp3JJMTZsV%2b%2fzRDhWETcsOOuvqVl%2bHfnGyE7Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E868" t="inlineStr">
+        <is>
+          <t>07004906134</t>
+        </is>
+      </c>
+      <c r="F868" t="inlineStr">
+        <is>
+          <t>Waghorli</t>
+        </is>
+      </c>
+      <c r="G868" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H868" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I868" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J868" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" s="1" t="inlineStr">
+        <is>
+          <t>A52100017774</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Rajeshri Rajaram Prachande</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>A52100017774</t>
+        </is>
+      </c>
+      <c r="D869" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5nYnwHtG6t4tPYM7U57CCBVaITYvQOG21SUyenrOq3RL%2b7d9AK5o8pnoRY00V%2bJccWn4ZHpWCAyYTlZx%2bKpaQIXvoE0j5lbmxkOT0SsszgMHEJr6Ga0UFt1ErMiX7FACxS7jMW2vmVqsYbhXD54a1YSO62z6FpI5F2XZ4iWk35FKvMCECWFBWg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E869" t="inlineStr">
+        <is>
+          <t>08108500888</t>
+        </is>
+      </c>
+      <c r="F869" t="inlineStr">
+        <is>
+          <t>Shivtej Nagar</t>
+        </is>
+      </c>
+      <c r="G869" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H869" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I869" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J869" t="inlineStr">
+        <is>
+          <t>411019</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" s="1" t="inlineStr">
+        <is>
+          <t>A52100017591</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Shradha Shripad Purandare</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>A52100017591</t>
+        </is>
+      </c>
+      <c r="D870" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KEUlLyDyJtFCNL42eC6Vc%2fZZpaiwVvct0qyiPRqvb3BrYqOn93vxKFsuOA2pT3zuvTNsyFcRTzZeVB1mT5euQa51LtvqgC1GfDKm0orCSH9IxzlsHQv3HVO14usQ3E3z7RugXWGsP9CPgpASrvOOfSGWkb1ihg%2bk0c5pO%2b5otlnI6LzIgglRAw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E870" t="inlineStr">
+        <is>
+          <t>09420256703</t>
+        </is>
+      </c>
+      <c r="F870" t="inlineStr">
+        <is>
+          <t>Sahakar Nagar</t>
+        </is>
+      </c>
+      <c r="G870" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H870" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I870" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J870" t="inlineStr">
+        <is>
+          <t>411009</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" s="1" t="inlineStr">
+        <is>
+          <t>A52100017814</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Lidwina Philip Joseph</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>A52100017814</t>
+        </is>
+      </c>
+      <c r="D871" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=FlZWDm7lOR6bEbru2uQX%2fM3psasB%2bEUTgUb4%2fEo4XIbAiJGfLsqOPy%2b0Z4g7wWphVm3wazLikUgMDTGzV2Yk9taaVvx1I%2brbHP9PDJCcMwVKaFxnBrfSL6Ltflj6zAZ1hCYPoVW5Uly%2bcFt5DbA%2fwOxbJcbqZM3FM68PJu0KuDlya1uwMB%2bHMw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E871" t="inlineStr">
+        <is>
+          <t>02026853622</t>
+        </is>
+      </c>
+      <c r="F871" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G871" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H871" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I871" t="inlineStr">
+        <is>
+          <t>Kondhwa Bk</t>
+        </is>
+      </c>
+      <c r="J871" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" s="1" t="inlineStr">
+        <is>
+          <t>A52100017556</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Vishal  Sharma</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>A52100017556</t>
+        </is>
+      </c>
+      <c r="D872" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hvxZ15dsJolf49kZrktHgDDryoOfCKNujO9oJW%2fxXvPkpAKDt%2b2ZaRoG4tHYb7gx6CbSYd6BGOk3uIgVjb40b5CqAL3ltUjxvsuGRseZixhsXiajwgMyEbiZgDUZxjJtOAfUCjMpx%2fvDybmL40bu9c0n8hRnNC8dFWODz1WIQ5M1DXeeAG7Jnw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E872" t="inlineStr">
+        <is>
+          <t>02026835698</t>
+        </is>
+      </c>
+      <c r="F872" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="G872" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H872" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I872" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="J872" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" s="1" t="inlineStr">
+        <is>
+          <t>A52100033300</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Nilesh  Survase</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>A52100033300</t>
+        </is>
+      </c>
+      <c r="D873" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MA5yRHnzxB1Ve1z7JiyOUefyIdrTkLTTFLmysh%2flHJqsvEioUNUPF7Ys8p4xKrgOwxJe2gJr%2f8ZvGcOfisuZQQTe8iOF2hgc8jLU1xm1qzVSU6YAiYxOYBJ%2bb6Y1jGz%2b3m5yu1aMmnf1jyFWENJNgzjf7TK8556a22JlLq0YUNPMpNZMGn3BfQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E873" t="inlineStr">
+        <is>
+          <t>09673087878</t>
+        </is>
+      </c>
+      <c r="F873" t="inlineStr">
+        <is>
+          <t>Walhekarwadi</t>
+        </is>
+      </c>
+      <c r="G873" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H873" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I873" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="J873" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" s="1" t="inlineStr">
+        <is>
+          <t>A52100017448</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Mdn Properties Private Limited</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>A52100017448</t>
+        </is>
+      </c>
+      <c r="D874" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=eTmsltTQmlMAn1NTe48qYpesLRj8ml1vuctNwv0k%2bTwIqibka6%2b5KF2j1SkzLu5ItRx2Q5FwLyeK1cpcAKB43CCS12cMT8hX1eWLcWh2216QNO8kc569MpcyGxVl7BWh314I6T81bte6i7fEji1ZCqcU1%2f05YDqGFXll%2fgFno%2frmwZE3%2fyFsCA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E874" t="inlineStr">
+        <is>
+          <t>02041004100</t>
+        </is>
+      </c>
+      <c r="F874" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="G874" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H874" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I874" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J874" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" s="1" t="inlineStr">
+        <is>
+          <t>A52100017309</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Mohammad  Asif</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>A52100017309</t>
+        </is>
+      </c>
+      <c r="D875" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=OJSO4IJBWBJyvZUNX7lZ09kISjwti5NUQ2MsLFq3gCaLJMOYy%2fUpx7486eaLLys84V%2fy5wMivlwFNyF1Sq1%2b5AKZ9TZUHvjZXP30l8Z%2bLHYFmds9xGOMj3LNyxDxxGu1GBaoYJ3zb5unNqaYgxwkmY9CFntl1%2fZwto%2bJCbCyc0OOOBVHH8gRiQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E875" t="inlineStr">
+        <is>
+          <t>02088057751</t>
+        </is>
+      </c>
+      <c r="F875" t="inlineStr">
+        <is>
+          <t>Koytewasti</t>
+        </is>
+      </c>
+      <c r="G875" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H875" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I875" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J875" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" s="1" t="inlineStr">
+        <is>
+          <t>A52100017333</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Pratik Popatlal Bafna</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>A52100017333</t>
+        </is>
+      </c>
+      <c r="D876" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=98INw3XDijGH%2bp%2ftjr%2bm55OGMPXDsKmK7zo167t0FZvoF1wWoXfQoMsgNdrlRz%2fLgKi2abSxMLWvisj0GDF15nI3t5xp7TzcKo8h%2f9nOGfz0tgyt37uRJwpSJUx7%2fUdyYe2s0mx%2feh6CGTCiJpuxwXzKR5haarqDnxrLWB3NPcsu%2fMueMXXOtQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E876" t="inlineStr">
+        <is>
+          <t>02024267100</t>
+        </is>
+      </c>
+      <c r="F876" t="inlineStr">
+        <is>
+          <t>Mukundnagar</t>
+        </is>
+      </c>
+      <c r="G876" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H876" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I876" t="inlineStr">
+        <is>
+          <t>Gultekadi</t>
+        </is>
+      </c>
+      <c r="J876" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" s="1" t="inlineStr">
+        <is>
+          <t>A52100017444</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Aakar Foundry Private Limited</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>A52100017444</t>
+        </is>
+      </c>
+      <c r="D877" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=XpOJQXEwjQBdpb%2br4eu5PhV1W8PEL0ilFuTaow6BFVSj04OcihH%2btfT74kqrd3JwvZXpkcSZlqMDAq2H3sxnVsJFbxahxxU7LkFf1m9ehaJqeZ%2b8jgTzUul2xbMkw1ppiLDyUkkvRJKh645rMP%2ftT1GNFLXZagWdLNJqYqoU%2fZtLfGTPb63kUQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E877" t="inlineStr">
+        <is>
+          <t>02067635555</t>
+        </is>
+      </c>
+      <c r="F877" t="inlineStr">
+        <is>
+          <t>Gultekdi</t>
+        </is>
+      </c>
+      <c r="G877" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H877" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I877" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J877" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" s="1" t="inlineStr">
+        <is>
+          <t>A52100017452</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Abhijit Sadashiv Jadhav</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>A52100017452</t>
+        </is>
+      </c>
+      <c r="D878" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=up%2bsYuixflwAdNBNb2HDUda2SLG7xXmxJhAGRwbSFXSwmxJay3isHb9H%2fdGZis7oUsnOiQ4ftp5WUSZcLBbNmVA1iSRu8Ywmkwk%2bceKo%2bYO8CxeGb4y1HMdnBaAgEWttnc2Vsm%2fd2mrriEY8klRdVq%2fgPrhvGPgbTl3x9EYkmdOOt8jJHzbcHg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E878" t="inlineStr">
+        <is>
+          <t>02049091210</t>
+        </is>
+      </c>
+      <c r="F878" t="inlineStr">
+        <is>
+          <t>Near Dsk Ranwara Nda Road</t>
+        </is>
+      </c>
+      <c r="G878" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H878" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I878" t="inlineStr">
+        <is>
+          <t>Bavdhan Kh.</t>
+        </is>
+      </c>
+      <c r="J878" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" s="1" t="inlineStr">
+        <is>
+          <t>A52100017285</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Mantrek Realty</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>A52100017285</t>
+        </is>
+      </c>
+      <c r="D879" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=XwrrmBCdTb%2fPIqtFyQ5Ld5sNBOtBrg3GSi0nAOiS1VqOL7v3oFanoALKtJgSB9nxmHZ4fIP%2bKomp4VJe7i00s4ew7JdBtd7vcYmwmhquyPLdxS%2bGn8%2ffixTSvaPfmjTsowAau5r5bJ96JxLy35eTGvIdQI58YAjr4h9pArefKUDSzKveYuJQRA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E879" t="inlineStr">
+        <is>
+          <t>02073044555</t>
+        </is>
+      </c>
+      <c r="F879" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G879" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H879" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I879" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J879" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" s="1" t="inlineStr">
+        <is>
+          <t>A52100018068</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Jash Nilesh Shah</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>A52100018068</t>
+        </is>
+      </c>
+      <c r="D880" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=vuxU9oabllZZCminywZy3hGzXKDEfvqX9AeD%2flxeSi0a%2fiCa5eTDO3bQFZ2Wyp2M2UuU8kQE8V0IVsR0NejEzlI0burLKLKhZFq7uwZwldpzNJloCfid%2b0Wb539p62UDEpshTFeSSolBhZUv7mk%2bIXLY4j8ptEPAXgwJaIn6HFB8%2bT%2beowrWXQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E880" t="inlineStr">
+        <is>
+          <t>02024475258</t>
+        </is>
+      </c>
+      <c r="F880" t="inlineStr">
+        <is>
+          <t>Shukrawar Peth</t>
+        </is>
+      </c>
+      <c r="G880" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H880" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I880" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J880" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" s="1" t="inlineStr">
+        <is>
+          <t>A52100018067</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Raj Nimish Shah</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>A52100018067</t>
+        </is>
+      </c>
+      <c r="D881" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=S%2bPirLNFKrWRuE6WlpPIYkwZA4DB0lVPziQq027BxWchdMkKR9qEPwNu1OkPAJUkWAcgJtt7DlOQGZDR9ZFKk2pZDAFE6OJbJKQI1ukYRwhDKqQjSYqcf2iYdbhr2yqphRJ28Drk%2fOqkSsQluihHo2OUFdvmPny19YgrzX4SNOKKXvCYC%2bOVBw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E881" t="inlineStr">
+        <is>
+          <t>02024464859</t>
+        </is>
+      </c>
+      <c r="F881" t="inlineStr">
+        <is>
+          <t>Shaniwar Peth</t>
+        </is>
+      </c>
+      <c r="G881" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H881" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I881" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J881" t="inlineStr">
+        <is>
+          <t>411030</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" s="1" t="inlineStr">
+        <is>
+          <t>A52100017415</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Nitin Subhash Patil</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>A52100017415</t>
+        </is>
+      </c>
+      <c r="D882" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=XVB5n6Pr3%2bEPGTfWdvlpYz2qtIUEHDnYE0K5EXggHBHzPyCKo4X3M3%2fBuqfsicu6HUfxFi5KxJT6p5Jbwgr4LOKGrmMkUaYx%2blnyjsRonw1ZrT3hFBFbCTCLtqyEx%2b7DVCATITMbPXUJKF3BS4gVe%2b5L3zqFkxn9SM7mxlqlmMKeEAhFdr5SYA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E882" t="inlineStr">
+        <is>
+          <t>09011920835</t>
+        </is>
+      </c>
+      <c r="F882" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G882" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H882" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I882" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J882" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" s="1" t="inlineStr">
+        <is>
+          <t>A52100017430</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Nagaraju  Kenchappa</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>A52100017430</t>
+        </is>
+      </c>
+      <c r="D883" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=BqK2t8ZjdIXZ1mzJHPqliZMn2Orc%2bD0Y91e1q%2bBOHr1btPPvCTPX4aTJNaG4o%2f271nEYsV410vfOyBwDZQxylbzFagXQygFX4qbOtPsLX2tqaKTm7qI%2bYpipAnKV0mzPIxA%2bPuOU5g6bBFm09aKRRY3QA5aGC07TRU06fawIaSOzKt%2bhkO2KOw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E883" t="inlineStr">
+        <is>
+          <t>09822043807</t>
+        </is>
+      </c>
+      <c r="F883" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="G883" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H883" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I883" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="J883" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" s="1" t="inlineStr">
+        <is>
+          <t>A52100017479</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Anand Arunkumar Paraswar</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>A52100017479</t>
+        </is>
+      </c>
+      <c r="D884" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=YacbagcC5rjEkcvnrpVa3FVGmVRwlTnE3jMK5A5TmGjrjhIMAkqdkNBvQrC%2fClwmlhaBUmQrtbWtcRYq0J8%2fO8lhDuJvRf7px5EgO0neLMTiF%2fSi%2ft4hRQLKhedNcSc2gxJkHZHc9eN3TLTC7irL62kQUoeFoo8AYXQm3PuRePvxeA6ntZAJLA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E884" t="inlineStr">
+        <is>
+          <t>09423218110</t>
+        </is>
+      </c>
+      <c r="F884" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G884" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H884" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I884" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J884" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" s="1" t="inlineStr">
+        <is>
+          <t>A52100024108</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Sandip Dnyanehswar Shedge</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>A52100024108</t>
+        </is>
+      </c>
+      <c r="D885" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=vr%2b492Qry8Ntvqz7zKfDrVR%2btTkLTDNtcIuhcVPtnQqNbXqn9iKJBYiXNXG0fjnmmduoWcpUugng%2fhqoa4OKjQ3t1Cm6%2ba49B9L0XLR4evbmLVsKIIwybqCL3tVWgVat79pMUoE0mf%2bAfOkkepUnnTNZ5y%2fypWYplZ47IC4M0I7uwe0n415UPA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E885" t="inlineStr">
+        <is>
+          <t>02067522533</t>
+        </is>
+      </c>
+      <c r="F885" t="inlineStr">
+        <is>
+          <t>Nanded</t>
+        </is>
+      </c>
+      <c r="G885" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H885" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I885" t="inlineStr">
+        <is>
+          <t>Nanded</t>
+        </is>
+      </c>
+      <c r="J885" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" s="1" t="inlineStr">
+        <is>
+          <t>A52100017483</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Nikhil Satish Patil</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>A52100017483</t>
+        </is>
+      </c>
+      <c r="D886" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QWkmp%2bJlplW3fn8yOQHmzmnHt7aG4DBH3DVAQF%2fbVpeIVCBz2l%2bObt7RYZ93Nwt2zMGW2AFLSVVkuQOyobRQvsydh9OUO60x0uU4KwynhFDl9WiKsvk0Vo%2fFltD9CQiGVYBoD1mX4eRbuNEa45BUzRnX8uqaU9SunjCrmWBrsaqtWt4EabIB7g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E886" t="inlineStr">
+        <is>
+          <t>09881363635</t>
+        </is>
+      </c>
+      <c r="F886" t="inlineStr">
+        <is>
+          <t>Bibavewadi</t>
+        </is>
+      </c>
+      <c r="G886" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H886" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I886" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J886" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" s="1" t="inlineStr">
+        <is>
+          <t>A52100017494</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Sonerao Satish Pandhare</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>A52100017494</t>
+        </is>
+      </c>
+      <c r="D887" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PP4s6CclhUfVtGreeK45LVnXHRWzb7akHYkP39Q6lMw6aYuhO77EcNBkEJ%2f7PQTh%2bWlrBQFGu4t0u88N5WKumaPD6nQdxlh7B8gCCkAgEFQYzgTquoikoyXzjUO1vMIgZ%2fIEsBBxdgYzz9Ut0q7zGcpojSwJwxZksxni7RwVpV0uCMH34rCk%2fA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E887" t="inlineStr">
+        <is>
+          <t>09975025384</t>
+        </is>
+      </c>
+      <c r="F887" t="inlineStr">
+        <is>
+          <t>Opposite Maruti Showroom</t>
+        </is>
+      </c>
+      <c r="G887" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H887" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I887" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J887" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" s="1" t="inlineStr">
+        <is>
+          <t>A52100017419</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Komal Harshal Navlakha</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>A52100017419</t>
+        </is>
+      </c>
+      <c r="D888" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=02tma3gur2BCk960rFdrdtC4JaAnQ35d%2fCzOQ0VrQPdLbOgaN7qmZ55pCTDja3TxUXLfe49fk6wHDXMkmIDgwlW%2fbA2v%2f5B1MAZlKhML7SN293CLma9DoIvZMr7LRdmCtFw6TmmP9QxuO54BqNb4nq0dCU2V64YvxfxQLkPpj85zJPzmbIqUVg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E888" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
+      <c r="F888" t="inlineStr">
+        <is>
+          <t>Shankarseth Road</t>
+        </is>
+      </c>
+      <c r="G888" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H888" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I888" t="inlineStr">
+        <is>
+          <t>Swargate</t>
+        </is>
+      </c>
+      <c r="J888" t="inlineStr">
+        <is>
+          <t>411042</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" s="1" t="inlineStr">
+        <is>
+          <t>A52100017623</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Manish  Gaur</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>A52100017623</t>
+        </is>
+      </c>
+      <c r="D889" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wgdwReYsrk5uAKuZ5T78ZaeL6OLQW8bEU0h6xvFRre5acahOaODhsrvDq%2fHzliadLGkp29EiN9%2frTLrIZ5aRDdazPDIbyN9ABlnBBkrfa1ir64mKy56yJX47iFPrm81VbQ05AfoZ6ApJy8zQkLqX9UerZY1pbSUAo2pjYqFqExvmAz0uJKhGFg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E889" t="inlineStr">
+        <is>
+          <t>08766762040</t>
+        </is>
+      </c>
+      <c r="F889" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G889" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H889" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I889" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J889" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" s="1" t="inlineStr">
+        <is>
+          <t>A52100017385</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Atul Chandramohan Khode</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>A52100017385</t>
+        </is>
+      </c>
+      <c r="D890" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=o%2blRXRy%2f3I3YWtlTNpXlFyKb0cxEwl4lYi4pS7hcPjjVRSKF17Q4jlNVT6Dw0ygVxVVmr4AR2elzF4Q6769uWp2LmdgrdwtUVcIHMmXc8mpRLHn%2b%2btZwefsBGz6S%2fgIHXQGNaSalQ3xbtAKfVcN57GW8QGUs3uNpQdp3r0SLwmXuzw0hsRQKIA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E890" t="inlineStr">
+        <is>
+          <t>09822609944</t>
+        </is>
+      </c>
+      <c r="F890" t="inlineStr">
+        <is>
+          <t>Anannd Nagar</t>
+        </is>
+      </c>
+      <c r="G890" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H890" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I890" t="inlineStr">
+        <is>
+          <t>Vadhu Kh</t>
+        </is>
+      </c>
+      <c r="J890" t="inlineStr">
+        <is>
+          <t>411051</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" s="1" t="inlineStr">
+        <is>
+          <t>A52100017522</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Raj Rajeshwar  Barhath</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>A52100017522</t>
+        </is>
+      </c>
+      <c r="D891" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Vu0SWVIdHbWFoefn4D5XREX4jElj8v2poiDI2Ld7surUBj92lCmDAFFSrMmCh5HMewd1MNcnMg98gHHmwMEG8j0O9l4QJSHi%2fK%2fd8uETy4B3fMJfC1wUMHv0GavYFj2Wt6xmKljcqoBaP07JuIp6YJrkVB3RCUn1axY9gLvKHUxCw%2fKR6fllEA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E891" t="inlineStr">
+        <is>
+          <t>02065220422</t>
+        </is>
+      </c>
+      <c r="F891" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="G891" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H891" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I891" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J891" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" s="1" t="inlineStr">
+        <is>
+          <t>A52100017425</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Samant Suresh Gadhavi</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>A52100017425</t>
+        </is>
+      </c>
+      <c r="D892" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=D6zH9H%2bxQ9ERQd7gZ%2fxTSMZW%2fRVQtxyN%2b90CKI0XH%2fnuKpo8MsN5RuSAavBYgzLHBLk4RqgD5MP7xskkVdQFuGJmfenW9Rtm5iP1I4yooqC1%2f14QDUqhpCsYjAo7vLPX5doyTphm3PcUld5GlwWWy00MM4PEQlndkx2%2fqkCMPYVag2mBKvc8fA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E892" t="inlineStr">
+        <is>
+          <t>09158786677</t>
+        </is>
+      </c>
+      <c r="F892" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G892" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H892" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I892" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J892" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" s="1" t="inlineStr">
+        <is>
+          <t>A52100017496</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Minakshi Yuvraj Patil</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>A52100017496</t>
+        </is>
+      </c>
+      <c r="D893" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3WbVFHfCPQZZ74tpMPXHWiFwUcMds0Z%2fYL7Qst73opuRJSpU4OU3Bue00A1bjSlLbILqRM1PSsLzwlEqDMaZ1I%2bfHU7kbqmUfaMuztXXOXpDWVqSKaLpopg6ZKuZ7ekaoMLX9LXg9tVqmbE4qVgXYbreVmLGxfxsk3zim3zGS8fz2ku1vD7GBQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E893" t="inlineStr">
+        <is>
+          <t>02512603028</t>
+        </is>
+      </c>
+      <c r="F893" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G893" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H893" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I893" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J893" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" s="1" t="inlineStr">
+        <is>
+          <t>A52100017469</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Anant Venkat Reddy</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>A52100017469</t>
+        </is>
+      </c>
+      <c r="D894" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6gN%2f8O3DP4D8TBKFE6Qf0ulSV7dmKzu7YSueY9korQDid6WJNcWyb%2f%2f3bGZbbmPXy9BokplR5%2bPb3PshV4HY5Oaq74Gil0k34q6MhmbUteXyym5ti78%2f3VbxFwwaRT0oBwp25oX9%2frwA1jWrfDnVhGlXIaUm%2f58HzkBRxlD3kOrvee5MnORWlA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E894" t="inlineStr">
+        <is>
+          <t>09545160160</t>
+        </is>
+      </c>
+      <c r="F894" t="inlineStr">
+        <is>
+          <t>Wadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G894" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H894" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I894" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J894" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" s="1" t="inlineStr">
+        <is>
+          <t>A52100017466</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Karan  Katariya</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>A52100017466</t>
+        </is>
+      </c>
+      <c r="D895" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Mc%2fOrXutiJ%2bTZHHg1lzyhhElcthaASUke4BphYjPaCi6lEtB0ybgmTWbIcI3zYfLNjiukWEOFXArUn9h5S3I8cLi8FpO7Fc70Ho7YZb8%2fgygTXdSFM7kvGm14oFP3B670KjRaDh4TOrqXcuSdbDxBtMEOZxtCQiRt95RSMVAiTqpAz6b8MvuKQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E895" t="inlineStr">
+        <is>
+          <t>02027472590</t>
+        </is>
+      </c>
+      <c r="F895" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="G895" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H895" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I895" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J895" t="inlineStr">
+        <is>
+          <t>411019</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" s="1" t="inlineStr">
+        <is>
+          <t>A52100017387</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Sachin Uttam Saykar</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>A52100017387</t>
+        </is>
+      </c>
+      <c r="D896" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=qqMN56R1l38rfpVKAP6r2%2fE9lvtYrhfkoDdXRoRJCZO5G6uo097js3CVTg2UypLFqj88mgz%2f7QzwHDH6qdHLm%2fTSyNzj7utcZxPWfwf4p0DObocTlLtYi61z50QsUcp9YdsOaCmJzk6%2bfCvc87yklaGwtOY9%2fk7DHcJdUGlUjxr6%2bf%2fYT7wWZw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E896" t="inlineStr">
+        <is>
+          <t>09921541414</t>
+        </is>
+      </c>
+      <c r="F896" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G896" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H896" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I896" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J896" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" s="1" t="inlineStr">
+        <is>
+          <t>A52100017542</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Vivek Dilip Patil</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>A52100017542</t>
+        </is>
+      </c>
+      <c r="D897" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2fyNsrRc8M7OcKHOKlkYvdp3Var1FJ6Qrnii1uOJjjtleVuKgFXolPR5v3uRT2Yi8tggDDvpTN1xBmS3aw%2fqPs5wiXAVEjSmfwghDGAWVnJbBk%2ba4VtCauyE5Sf1oKoNCPQwQT%2bEKJ5D1uisiqNkz7q7InYkrqPiMZMEgISslmar2a46tC8tvvw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E897" t="inlineStr">
+        <is>
+          <t>09604834872</t>
+        </is>
+      </c>
+      <c r="F897" t="inlineStr">
+        <is>
+          <t>Moshi</t>
+        </is>
+      </c>
+      <c r="G897" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H897" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I897" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J897" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" s="1" t="inlineStr">
+        <is>
+          <t>A52100017523</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Jameel Ahemad Ansari</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>A52100017523</t>
+        </is>
+      </c>
+      <c r="D898" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MgF981kFFouJJVrsrFigCw302CstmDrmdylmCcjCFCbWN5Vl%2bS471npz0GfD5smcaD%2f8JzqXGkVKekuM9eXbbzwy4eggsJsOYx0K%2fIKQ%2f3uT3NoTsUaaQ1PIkn%2bUYPAz4I%2bH5HVaAc7fhMQ5gndkWzt6Sq3QDO6At4CmB9Mk0mYVpqcMDfZrFA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E898" t="inlineStr">
+        <is>
+          <t>02026150066</t>
+        </is>
+      </c>
+      <c r="F898" t="inlineStr">
+        <is>
+          <t>Wadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G898" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H898" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I898" t="inlineStr">
+        <is>
+          <t>Chandannagar</t>
+        </is>
+      </c>
+      <c r="J898" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" s="1" t="inlineStr">
+        <is>
+          <t>A52100017447</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Mangesh Vijayrao Kawadkar</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>A52100017447</t>
+        </is>
+      </c>
+      <c r="D899" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=06vTWjLvecuZLHVnOyNYC9HxuxzIIQ%2bgiH0zvKQg5%2fypujiU2JQ3mDdPVwHOH9wTOhhoqrShxBO5SlNXg9vleho3neWYKGLmZR7nGTThU%2fVgvuSM4XVyg4aSUzs4Gr1DwsX2UaKKyNbZE2H9BFqbFZ%2bS0hmoESj5yyTa%2brIWsY0Ttqoect32tQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E899" t="inlineStr">
+        <is>
+          <t>02041404140</t>
+        </is>
+      </c>
+      <c r="F899" t="inlineStr">
+        <is>
+          <t>Balewadi</t>
+        </is>
+      </c>
+      <c r="G899" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H899" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I899" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J899" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" s="1" t="inlineStr">
+        <is>
+          <t>A52100017492</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Nitin Gajanan Raut</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>A52100017492</t>
+        </is>
+      </c>
+      <c r="D900" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=iqNI7TC7%2fDvcuCn45TXauZ0jjIeJB0zAeVrl7pzaiuRD%2fv1d2bL8C6LcX7vTXDQGBnOh0PYdkrMoeSG3w6EtInwZDMb2%2bydBYP9kOKadkbCfeX8KBSU9no5V9UR4bAZPXBvrnIAcUUoXrgulFefL3ZVJhwJe4i0S6oReJ5emWJPji2s5QG%2f4sw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E900" t="inlineStr">
+        <is>
+          <t>09823323345</t>
+        </is>
+      </c>
+      <c r="F900" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="G900" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H900" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I900" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J900" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" s="1" t="inlineStr">
+        <is>
+          <t>A52100017481</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Venkatesh Shantappa Patil</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>A52100017481</t>
+        </is>
+      </c>
+      <c r="D901" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=YMkUSkRj7uTnuYfdj6t%2fVVBBSjuYjVT2LNOqfwhlsaxY7cKJN98i5ykh5LRHuD7jtVN7tVxEbYlRlLHBOjB8FU8CFHKcNIi%2brwsiJT8gRSJ6SPHCP2gnwg%2f9Ya%2btTNh4aTDq2cva0JLEvQo0h%2frNPtYRQP0P%2b5QyQRbyVA%2bMtrSWqjJo%2bWZX7Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E901" t="inlineStr">
+        <is>
+          <t>09823029100</t>
+        </is>
+      </c>
+      <c r="F901" t="inlineStr">
+        <is>
+          <t>Vimannagar</t>
+        </is>
+      </c>
+      <c r="G901" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H901" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I901" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J901" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:950]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J901"/>
+  <dimension ref="A1:J951"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46768,6 +46768,2606 @@
         </is>
       </c>
     </row>
+    <row r="902">
+      <c r="A902" s="1" t="inlineStr">
+        <is>
+          <t>A52100017509</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Amoya Consulting Llp</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>A52100017509</t>
+        </is>
+      </c>
+      <c r="D902" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=YoXC16JAAUhkrS8PtsWqhNFk0NGwIqAs7Z8Of%2fBHLz6BEOQ1ale4ky71xWJrb1gn37NmwcnF7TomPecm5Mk9JGziMQurHFShaEHoWyutRm01GQwlsNXoob1qhR14Z6RTAJmAv2qXbRSx1o01hZxMgKxczEUWjhZHnM4vMf5Yld%2bCL5XQeFGPZQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E902" t="inlineStr">
+        <is>
+          <t>02066400173</t>
+        </is>
+      </c>
+      <c r="F902" t="inlineStr">
+        <is>
+          <t>Anand Nagar</t>
+        </is>
+      </c>
+      <c r="G902" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H902" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I902" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J902" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" s="1" t="inlineStr">
+        <is>
+          <t>A52100017578</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Sushant Bhagwan Jamkar</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>A52100017578</t>
+        </is>
+      </c>
+      <c r="D903" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=RTiFaLUrmI76KoDx2MzM3oCmxnYYKVggeK0gFBG%2b52usfzRsG%2fZ8%2bDo3pr%2fBtjAEhDDOV5bFpoD5VV%2b1WpcLyr6O77zMpb90ack9seEwT199eyWSH%2fmrV6I%2fpIKGv77mzeA%2bfBh37cRAH0gvLejOjy8DpWFYW5PD05U712XeB35cpWmGMXvyeg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E903" t="inlineStr">
+        <is>
+          <t>02025443361</t>
+        </is>
+      </c>
+      <c r="F903" t="inlineStr">
+        <is>
+          <t>Kothrud,</t>
+        </is>
+      </c>
+      <c r="G903" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H903" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I903" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J903" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" s="1" t="inlineStr">
+        <is>
+          <t>A52100017614</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Nikhil Uttamrao Nazirkar</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>A52100017614</t>
+        </is>
+      </c>
+      <c r="D904" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=U8JXhPFDyHiII7ro%2f45DAks4FZLjCZr%2bt3zOPuMO05dRzB2SFEFLCBOcBQhmBj3M7lFa9Wqky62QMudd1rDyZtaJSrrgYR4%2fzILVyWeqeyZSHjGKfB9yQ073z9kxLudFTc%2bo9EkOkYLC7Ch9ZwVVUl3Gwp4moomhzvhWX7idmAF2fyrsucsKWw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E904" t="inlineStr">
+        <is>
+          <t>09960448888</t>
+        </is>
+      </c>
+      <c r="F904" t="inlineStr">
+        <is>
+          <t>Near Little Flower High School</t>
+        </is>
+      </c>
+      <c r="G904" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H904" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I904" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J904" t="inlineStr">
+        <is>
+          <t>412308</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" s="1" t="inlineStr">
+        <is>
+          <t>A52100017994</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Atul Amrutlal Shah</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>A52100017994</t>
+        </is>
+      </c>
+      <c r="D905" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wb0JISVmBeK5%2f8GJvfxE6SgZUNi0qCvdSdsylz3VXAdOh7jY3RKinAd99pdCa0zoCNmmoV1F23XpUB%2fKn9h%2fLEPqT13TfIFBs1yDugj%2bu3S5ziffoHoK%2bAfHsd3KolKfjd2gJPliaZfa5xEaAeBDutcXSmK0ZVWLRTiRudGWOz0PIzwzeC1OHQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E905" t="inlineStr">
+        <is>
+          <t>09822066789</t>
+        </is>
+      </c>
+      <c r="F905" t="inlineStr">
+        <is>
+          <t>Mahesh Society</t>
+        </is>
+      </c>
+      <c r="G905" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H905" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I905" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J905" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" s="1" t="inlineStr">
+        <is>
+          <t>A52100017703</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Shashikant Wamanrao Panchal</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>A52100017703</t>
+        </is>
+      </c>
+      <c r="D906" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=DeggOIyqR0iZ0t2Z1t8lli5oZF6sM5V7aL3IqPeUT2rUkqkR69ac0hDwyRXCAOIT8p9HJd9F4ozgfVo2kr08BJlI8ONdMcrXGP%2fMX94y4S2kCxQepdA0%2bWBUZRBtc6EULoI93MFmw1eN2qKKYtT73znc4%2fpCgBEAHx4kNlLynBZeHOxTV5shpA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E906" t="inlineStr">
+        <is>
+          <t>09823111103</t>
+        </is>
+      </c>
+      <c r="F906" t="inlineStr">
+        <is>
+          <t>Swargate</t>
+        </is>
+      </c>
+      <c r="G906" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H906" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I906" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J906" t="inlineStr">
+        <is>
+          <t>411042</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" s="1" t="inlineStr">
+        <is>
+          <t>A52100017586</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Pushpak Madhukar Amodkar</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>A52100017586</t>
+        </is>
+      </c>
+      <c r="D907" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5KboBFl%2byz%2buGtxITsrSJl0mIIyoZ5Lqe4gxl4T%2frQlNjwptZUYlp1XtWRwC0YCuAeTx8%2bI0ZRm2pHJ1VS19%2fTdaGQfIEsz%2fHoyzsB1J0DIy7Zj9%2b%2fp48%2fjNEuV2x08UlYqZ8MDtVutna8a%2fnxmjKu6l2ARusDZwmO3gNeyFCJJbVrGkWuETpw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E907" t="inlineStr">
+        <is>
+          <t>08830202978</t>
+        </is>
+      </c>
+      <c r="F907" t="inlineStr">
+        <is>
+          <t>Satyakamal Colony</t>
+        </is>
+      </c>
+      <c r="G907" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H907" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I907" t="inlineStr">
+        <is>
+          <t>Talegaon Dabhade (R)</t>
+        </is>
+      </c>
+      <c r="J907" t="inlineStr">
+        <is>
+          <t>410507</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" s="1" t="inlineStr">
+        <is>
+          <t>A52100018529</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Yash  Khanapurkar</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>A52100018529</t>
+        </is>
+      </c>
+      <c r="D908" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=11Mdc66Me7VJtVLL5sNvZwB9SRmV%2fR28rt18p4Z9d18FTTWYvOU0jR%2f8%2fpZ%2fNI33j2JU%2bdrJew7gXy2lQ9PaLlsnyLM4Y6LxMuHd66B41amwzZpqv%2fefte4E264H3qXx3meh5t%2bgVs282WbwtV3n2Qc6HuwaLk2n90prRPE0lWQqnQXoZD3xOA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E908" t="inlineStr">
+        <is>
+          <t>08999647229</t>
+        </is>
+      </c>
+      <c r="F908" t="inlineStr">
+        <is>
+          <t>Sahakarnagar</t>
+        </is>
+      </c>
+      <c r="G908" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H908" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I908" t="inlineStr">
+        <is>
+          <t>Parvati</t>
+        </is>
+      </c>
+      <c r="J908" t="inlineStr">
+        <is>
+          <t>411009</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" s="1" t="inlineStr">
+        <is>
+          <t>A52100017588</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Geeta Nitin Kalraiya</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>A52100017588</t>
+        </is>
+      </c>
+      <c r="D909" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ysd%2fZdGirSaKOIejgP2lSOj8T2nHVHr5EdywzKeuhS%2fC42BrsMBxXQF1DaAEjWZw9YOCwP7hF0xmKzKxrAGHqbOxYyoxKOqaLlhArxTZ4mnZm2SWEp%2fJfyv9FcHhV5eZns1T6HL5lK5aMFyyYZkFDA9m%2bWH6%2bbzeMR7wPqrZG3F2fDnvi5RurQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E909" t="inlineStr">
+        <is>
+          <t>08208980214</t>
+        </is>
+      </c>
+      <c r="F909" t="inlineStr">
+        <is>
+          <t>Nibm Annexe</t>
+        </is>
+      </c>
+      <c r="G909" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H909" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I909" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J909" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" s="1" t="inlineStr">
+        <is>
+          <t>A52100017570</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Prasad Govindrao Deshpande</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>A52100017570</t>
+        </is>
+      </c>
+      <c r="D910" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=M75e5FL34b4JcP0o6zPz%2fev%2bpkoXtjY0fJzETULgH5kGxuTGuBFczy%2b3KjfZA7lckN8Rmqvf1qx6EN0oMaoSHd%2bzxrA3OrIKB8wCMZQcNFeVgf%2bd%2fD7uBaMrf%2bpTFtWUehauf61QXuX6ACOlzMxA40Ib77ZnUoeU6pyL9Wl9%2b9Gh6n%2bBQFmozA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E910" t="inlineStr">
+        <is>
+          <t>07030744646</t>
+        </is>
+      </c>
+      <c r="F910" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="G910" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H910" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I910" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="J910" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" s="1" t="inlineStr">
+        <is>
+          <t>A52100001680</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Alka Rishabh Jain</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>A52100001680</t>
+        </is>
+      </c>
+      <c r="D911" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=euH%2fHK49vl%2bLZ6OvfdNNJQxH%2f0aa6KgR7sbvt9gmAbSueaXH9OKkZFnrssd%2fkAIYQsCqAIF8faNkLB6D%2fK6lXHKGhX2YfXeV%2fpKVO%2bpMaxIvKnurqs1k%2fbzaCkr8otVkQTo1urOsfG4D5ZmGudS334kk1iG6jpWQ2jtqBg6UzQI%3d</t>
+        </is>
+      </c>
+      <c r="E911" t="inlineStr">
+        <is>
+          <t>02032343024</t>
+        </is>
+      </c>
+      <c r="F911" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G911" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H911" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I911" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J911" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" s="1" t="inlineStr">
+        <is>
+          <t>A52100018242</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Mohit  Singh</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>A52100018242</t>
+        </is>
+      </c>
+      <c r="D912" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LtyTbF2EPuvP9ouMrUprbSXzKQe0Gk2udw3Oz3LshurLUtR%2f8IC8sOiaVr1XfgsjaF9uQKL8m8walrzKx2VKEQPx8AzYkA9AtrOQDOfqj6fOzD%2b2%2fzJ34wDd0X%2bsw9jZjED3aXN35Y2vgo9dzoGQn%2bgCYWWioq5sHzM5C%2fumrtE7KPHAI04VsQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E912" t="inlineStr">
+        <is>
+          <t>08149422422</t>
+        </is>
+      </c>
+      <c r="F912" t="inlineStr">
+        <is>
+          <t>Tathawade</t>
+        </is>
+      </c>
+      <c r="G912" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H912" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I912" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J912" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" s="1" t="inlineStr">
+        <is>
+          <t>A52100017608</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Jude Anthony Lazarus</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>A52100017608</t>
+        </is>
+      </c>
+      <c r="D913" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=z%2fYapMPZweWTCfaONUmoFV8yRjyBB7OuNwbCTxG30BL5zWLLj4A%2flxh0LLVp33FLiLuHrlr876zNxoypfwzW1CW7edFsvn%2b5iMEgnRTkC8xjvgzhf4%2bkZr%2buk8JwHDtrPJPHWicvcucBpEUwO%2bhfiBwibCA4VVOoktxsU7aTLbFI079%2bUomHww%3d%3d</t>
+        </is>
+      </c>
+      <c r="E913" t="inlineStr">
+        <is>
+          <t>09890098195</t>
+        </is>
+      </c>
+      <c r="F913" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G913" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H913" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I913" t="inlineStr">
+        <is>
+          <t>Kondhwa Bk</t>
+        </is>
+      </c>
+      <c r="J913" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="1" t="inlineStr">
+        <is>
+          <t>A52100017633</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Manoj Govind Munguskar</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>A52100017633</t>
+        </is>
+      </c>
+      <c r="D914" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PgtBUcdZ0Avrg3YZlzN8E2jQpjcbPODxzuu5ZtHLzqg1hshqLkOu7OjylGaZ4U2JHbjG12BIRUjT6sWDcp%2f4GF%2fE%2fOw%2fb1NOhEa069aI9go9Riu5xCUlY45Gj5BESPOM3PyR9J1goj1Cxq9ahBdWaVQ41X8aRLbHoO7Bw%2b%2fHgz6DyYUKyAo9eQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E914" t="inlineStr">
+        <is>
+          <t>02060000000</t>
+        </is>
+      </c>
+      <c r="F914" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G914" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H914" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I914" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J914" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" s="1" t="inlineStr">
+        <is>
+          <t>A52100017576</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Tarulataben Diptesh Parmar</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>A52100017576</t>
+        </is>
+      </c>
+      <c r="D915" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=NknXg7D3v%2fAMqNm1IdpZFnsHIQD0D8kYHknqAFDI5xigVo3yL0FCKEY%2btjARZIL8N%2fMcpTboMHMezMlcFRpbfaRxQuHjM%2f6yTBVTxonYgIfZ7cE54BXVGhyBhc6YGlRwOXJC05hWEBAqwWn2McEGcZ14aipEgC8XC52zCpeOO%2bsAfBVOeNADmA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E915" t="inlineStr">
+        <is>
+          <t>02035467854</t>
+        </is>
+      </c>
+      <c r="F915" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="G915" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H915" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I915" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J915" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" s="1" t="inlineStr">
+        <is>
+          <t>A52100017615</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Salman Vazid Shaikh</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>A52100017615</t>
+        </is>
+      </c>
+      <c r="D916" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=XOiD3lVXMQu3KfTqXsrLuB7ps%2bqSOpZMkQz0WoCiDW7r6Ev3NTO1rB%2fOqhlmqrUs0GwvhcKUrLQVj33EP%2fSSPtiwGwKuvn31kcC4Et%2b9GugqNC8rjYrCFN%2bvnVfulZHtcowYtwnh1tbvFL0EwzjnA6J4JknlOCjmbJmcP533MvB%2b4mrue1XAzg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E916" t="inlineStr">
+        <is>
+          <t>08208412642</t>
+        </is>
+      </c>
+      <c r="F916" t="inlineStr">
+        <is>
+          <t>Near Florida Minis</t>
+        </is>
+      </c>
+      <c r="G916" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H916" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I916" t="inlineStr">
+        <is>
+          <t>Keshavnagar-Mundwa</t>
+        </is>
+      </c>
+      <c r="J916" t="inlineStr">
+        <is>
+          <t>411036</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" s="1" t="inlineStr">
+        <is>
+          <t>A52100017604</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Kishen Chhabaldas Milaney</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>A52100017604</t>
+        </is>
+      </c>
+      <c r="D917" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=TKDmV%2fjZzlo7hpIJ7dr1X31BdiE%2b9oMj6%2b6Gvs0ZuEuDNoZPA6S%2bSvOsEOFIg7mkSfRvXXg%2fg%2fWxlrPgNOIX9GG%2fXVvUPXcY%2f2l%2fEuOuevyVea4yQ1MhHlJIa2zX7Z3lqTgsEhTA0Lku6oLgteTvUCI1ZxXMtouie9YLMq7JMZG%2bLFF470QOLA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E917" t="inlineStr">
+        <is>
+          <t>02026835030</t>
+        </is>
+      </c>
+      <c r="F917" t="inlineStr">
+        <is>
+          <t>Lullanagar</t>
+        </is>
+      </c>
+      <c r="G917" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H917" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I917" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="J917" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" s="1" t="inlineStr">
+        <is>
+          <t>A52100017562</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Akshay Arun Kulkarni</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>A52100017562</t>
+        </is>
+      </c>
+      <c r="D918" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=XsK0xxPfoA%2bAGDWv2LEVqsM%2b4jiscpz%2bGHk3zwgV2CE4yHZJiYasch4%2f1FhN%2f58t%2f9KBCQlv8%2bsrMLu%2fVdwHwjjIvspYcb%2bhPp4Lmo7mMMRIiq%2f%2bxNK%2fQ5sB7apmuIIwghYFQOjWXeFjwLza4ArieTAUCuRAdn9jXvr5Vf5zPCXmdQUBSUkeuQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E918" t="inlineStr">
+        <is>
+          <t>09527557473</t>
+        </is>
+      </c>
+      <c r="F918" t="inlineStr">
+        <is>
+          <t>Bhugaon</t>
+        </is>
+      </c>
+      <c r="G918" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H918" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I918" t="inlineStr">
+        <is>
+          <t>Bhugaon</t>
+        </is>
+      </c>
+      <c r="J918" t="inlineStr">
+        <is>
+          <t>412115</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" s="1" t="inlineStr">
+        <is>
+          <t>A52100017560</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Pradeep  Parate</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>A52100017560</t>
+        </is>
+      </c>
+      <c r="D919" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=AaD6echv95htkrwEsEYNWVVpfugY4jw7XEDXRU%2fsxHGADcj3rzQWD3ued4t6mZLJQQWVhZu3YLJSMFqRinRbrEJqtMm51FKUfK3zLZ020uWl3yNGiAwLYE8R7kH6oLiADASdXgCHrm1Bsphvk5hQNt9G%2fpWQ5NREkp%2f8EUZFAhxhOmDMLIhMMA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E919" t="inlineStr">
+        <is>
+          <t>08999057103</t>
+        </is>
+      </c>
+      <c r="F919" t="inlineStr">
+        <is>
+          <t>S No 16A/2 Kondhwa</t>
+        </is>
+      </c>
+      <c r="G919" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H919" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I919" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J919" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" s="1" t="inlineStr">
+        <is>
+          <t>A52100017664</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Dinesh  Sirvi</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>A52100017664</t>
+        </is>
+      </c>
+      <c r="D920" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bN2Q%2b4eX6q2o9crujRrct8JrhhpdIEWA7Frw7QM3%2bClGqPJ79lsWOY2qnZkx6d35uxUDxVpz%2f9LWxahLsjtqy9g8c6a%2bPSlkBlS7pKVxYJuRxHxPJJVk7Z9AA1wBu0823v5vUzOsc78JhUmqqJEpvtZ6dqDyL1dCfBPLbJxKvrbF8aAZF27%2fBQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E920" t="inlineStr">
+        <is>
+          <t>02024307270</t>
+        </is>
+      </c>
+      <c r="F920" t="inlineStr">
+        <is>
+          <t>Bavdhan</t>
+        </is>
+      </c>
+      <c r="G920" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H920" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I920" t="inlineStr">
+        <is>
+          <t>Bavdhan Kh.</t>
+        </is>
+      </c>
+      <c r="J920" t="inlineStr">
+        <is>
+          <t>410021</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" s="1" t="inlineStr">
+        <is>
+          <t>A52100017724</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Gauri Arun Paste Proprietor Of Dream Properties</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>A52100017724</t>
+        </is>
+      </c>
+      <c r="D921" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=WvBCh3FhHHRBWbUyn55uEtcSenwl2%2fn2LWEkb5jnZ9jIIJgIt1b2pt9xAArCRGkAe8lX%2b%2bHJEx%2b%2fqvmU0KFo%2bP8GBv5cuFlaDUdtDWs9wkb2VmSKYttg5203XHEgY%2fRD%2b4zadPOcpEwMVIecOeymD4VjlchKA2IKC8juLduV1r%2fOK4vdg4ZqfA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E921" t="inlineStr">
+        <is>
+          <t>08600024427</t>
+        </is>
+      </c>
+      <c r="F921" t="inlineStr">
+        <is>
+          <t>Pimpale Gurav</t>
+        </is>
+      </c>
+      <c r="G921" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H921" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I921" t="inlineStr">
+        <is>
+          <t>Pimpale Gurav</t>
+        </is>
+      </c>
+      <c r="J921" t="inlineStr">
+        <is>
+          <t>411061</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" s="1" t="inlineStr">
+        <is>
+          <t>A52100017657</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Mahediali Farid Andagi</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>A52100017657</t>
+        </is>
+      </c>
+      <c r="D922" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=WLOZO5Ggu1k8vLHNB00HgacK%2bPI3IX6xW05Hek%2fOjo81TSEXAJaEj1aWo1omYA8l5vpvB%2fod%2fJPTkrZxNWuAbfsG8adlTtSJgi5wbz3QfGwHLJLo9Hy5VRts3EPt9cy4318UtYnYuOkyrbf8LgHOcsTUzsk33%2b5sDW6MTUklVPP12pnGQEkcag%3d%3d</t>
+        </is>
+      </c>
+      <c r="E922" t="inlineStr">
+        <is>
+          <t>09881360037</t>
+        </is>
+      </c>
+      <c r="F922" t="inlineStr">
+        <is>
+          <t>Kondhwa Khurd,Mitha Nagar</t>
+        </is>
+      </c>
+      <c r="G922" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H922" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I922" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J922" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" s="1" t="inlineStr">
+        <is>
+          <t>A52100017697</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Elite Infra</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>A52100017697</t>
+        </is>
+      </c>
+      <c r="D923" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=qFmMmbNBcbWFwhIhiu2nWFdbnlo46Av4JhalrEqQE2SemZ30dJyXSkVcsko5hbOluXM5vgFhlSJtmECH%2f7cwM08yVH4Sp66xNjjoEvFxwAUmzEgI9aKtnEXTJAzlM7gfgn3JKjqP4SPPB7I1C5kZC%2fkbeHCKqmPWgL0iySrfRSW82Dg7%2bZ1s5w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E923" t="inlineStr">
+        <is>
+          <t>02027650335</t>
+        </is>
+      </c>
+      <c r="F923" t="inlineStr">
+        <is>
+          <t>Nigadi</t>
+        </is>
+      </c>
+      <c r="G923" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H923" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I923" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J923" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" s="1" t="inlineStr">
+        <is>
+          <t>A52100017597</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Namrata Kanhaiyalal Goenka</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>A52100017597</t>
+        </is>
+      </c>
+      <c r="D924" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Xi%2fPgmOv6bw0D1M%2fYsCGuMQKqRYYcwE00DuB82uSjCf1YHDnR2%2bRhnbFm9uueyddl8NAxBX3sBhX2Nc7cd5gurPXA7Rk66jEJu8N%2fxANqM9ITcH0R%2bFI7nQ3RMIdzx1iIHNYcbpRfH0fmRSQd81xH0tzztldOL%2f%2bZVV6hvQGt3R%2b%2bpcZTlDtLw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E924" t="inlineStr">
+        <is>
+          <t>02228492046</t>
+        </is>
+      </c>
+      <c r="F924" t="inlineStr">
+        <is>
+          <t>Goregaon (E)</t>
+        </is>
+      </c>
+      <c r="G924" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H924" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I924" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J924" t="inlineStr">
+        <is>
+          <t>400065</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" s="1" t="inlineStr">
+        <is>
+          <t>A52100017632</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Chandrashekhar Gokul Patil</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>A52100017632</t>
+        </is>
+      </c>
+      <c r="D925" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=mjPUAc8Qgvt349iR0QM3xTyIcPi876BRT%2f2RWjmxGKotlM27wOPZfq41Rvpb%2brbPJLSPXmnMlslj5cucYzIpR374b4efFMAARA1TaA%2fc5dAOVz1Hh1875TGfp4sokZygL%2bEqRrjlyyz4lIKImmVQJf18aHWL9z5rSD0QSwWJdPe8VVZ1Tv80uQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E925" t="inlineStr">
+        <is>
+          <t>08888257024</t>
+        </is>
+      </c>
+      <c r="F925" t="inlineStr">
+        <is>
+          <t>Balewadi</t>
+        </is>
+      </c>
+      <c r="G925" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H925" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I925" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J925" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" s="1" t="inlineStr">
+        <is>
+          <t>A52100017710</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Arvind Waman Randive</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>A52100017710</t>
+        </is>
+      </c>
+      <c r="D926" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PSdUITMDaJP6Gy3Ovk0d9i%2bKQt%2f5wc%2b6Q5Oy2%2bb4xQb3INtORCtrvaI1loXJHp%2bIsPF5ySri2%2fmcLjm4ZYu%2bDwXvv%2bnXo65if%2fpJ6BpytNTdCUodfpwnApxMYS671eN7IbWwI8V3exEy74su2rNCtztTSMWnf8xAseb3yDpQZd2CZX6gQ4uU9Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E926" t="inlineStr">
+        <is>
+          <t>02024104155</t>
+        </is>
+      </c>
+      <c r="F926" t="inlineStr">
+        <is>
+          <t>Pimple Nilakh</t>
+        </is>
+      </c>
+      <c r="G926" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H926" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I926" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J926" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" s="1" t="inlineStr">
+        <is>
+          <t>A52100020212</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Ashish Sharad Kulkarni</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>A52100020212</t>
+        </is>
+      </c>
+      <c r="D927" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=t5gOzmseo6uJaxCLIDs5Bq5mCE1tQU0Sywdnc6JD1TmGTs04xroTGq%2bi2OwhC0OmRWwy%2fLUvDulUO7iGVDHcdzAX5%2bGVx80kt3gUr5%2by%2bSwRDsKEwfAtDjUjtt8kwVEFCu7vEetxnEEjxJ5hgUVGLnvlemSqAi%2bonQxAlO21GWT5VpF345J66A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E927" t="inlineStr">
+        <is>
+          <t>02097650419</t>
+        </is>
+      </c>
+      <c r="F927" t="inlineStr">
+        <is>
+          <t>Pigale Farms Koregaon Park</t>
+        </is>
+      </c>
+      <c r="G927" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H927" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I927" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J927" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" s="1" t="inlineStr">
+        <is>
+          <t>A52100017630</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Ravi  Lasod</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>A52100017630</t>
+        </is>
+      </c>
+      <c r="D928" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=A9Uwys4op%2b3gIITaItHaG24kDGeT%2b%2fS7y3jMJCOILWLzrJ%2fh7VW5kNtBwNGsVJJRutj7UxpTJ%2by6jAkzUNHdfT6N622b3KUpMCvCNdbiMMUAN2P0AR8M3pQ5vJcteHIcKRdCO%2f63FTraontUvBUmLo80fzhyRYrxqkZFI7xq2tETRkrEAfTP4g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E928" t="inlineStr">
+        <is>
+          <t>02029709930</t>
+        </is>
+      </c>
+      <c r="F928" t="inlineStr">
+        <is>
+          <t>Balewadi Phata Baner</t>
+        </is>
+      </c>
+      <c r="G928" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H928" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I928" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J928" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" s="1" t="inlineStr">
+        <is>
+          <t>A52100017920</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Pradeep Kumar Chaurasia</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>A52100017920</t>
+        </is>
+      </c>
+      <c r="D929" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=byDl9t54EwJep6vQRmMDUIzLFmIwFqjF4dxypoh1r%2fyMWmc9J%2fi%2bDbrkvraXqtiR5JV0HfgnXPaLWthyR66zryJcJ2wYNKU9xnfe6idPrhFGc%2bbY2Tu%2fkvaSuhwNSIU2NPY1p326cdU3uTx5VA%2fmg5i1noYF2DlnTBpAcakCm67E7qXyZssaRQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E929" t="inlineStr">
+        <is>
+          <t>02067990055</t>
+        </is>
+      </c>
+      <c r="F929" t="inlineStr">
+        <is>
+          <t>Ashthvinayak Society, Lohegaon</t>
+        </is>
+      </c>
+      <c r="G929" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H929" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I929" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J929" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" s="1" t="inlineStr">
+        <is>
+          <t>A52100017696</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Nilesh Babarao Chaudhari</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>A52100017696</t>
+        </is>
+      </c>
+      <c r="D930" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Fmo0sFW%2bLlXeU0JvFEROps81LOgCGlVdihfdrEJeFuPoAYy4N%2bZqcy73V8ySynS8XMK0H5RF0tO3t1z6vWXW9Yoze22ZAL676jzE8BChTS0uGhbwkoJIV8ajkVjftVeBZ7P2P1RucAv6654oDzlcBv0XKVElS%2fKPOkxvkI1gdpaT0nfsZzFp0A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E930" t="inlineStr">
+        <is>
+          <t>02048669823</t>
+        </is>
+      </c>
+      <c r="F930" t="inlineStr">
+        <is>
+          <t>Bavdhan Budruk</t>
+        </is>
+      </c>
+      <c r="G930" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H930" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I930" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J930" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" s="1" t="inlineStr">
+        <is>
+          <t>A52100017651</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Vitthal Jagannath Zanwar</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>A52100017651</t>
+        </is>
+      </c>
+      <c r="D931" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Rou9F9RXBt%2brqxXKGJhTK1KXluyz7JRkRAORnAXwE3r%2fPIvwwerc6spP5lxzwJ953WUzkA4SIhzZBi32JIGmH6zZ%2fB2EXNC1htQ19kQLwk0mV9iyygNGxAxcCCqMQr3g%2bfyUCJa3UgcetZ2cuB7Mt6OjLBDU4oSG42wiminVpqif1E%2fzK8Vrdg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E931" t="inlineStr">
+        <is>
+          <t>07588870854</t>
+        </is>
+      </c>
+      <c r="F931" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G931" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H931" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I931" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J931" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" s="1" t="inlineStr">
+        <is>
+          <t>A52100017676</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Rahul Ashokrao Ingle Proprietor Of Swaram Properties</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>A52100017676</t>
+        </is>
+      </c>
+      <c r="D932" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6q16JpN8JfS3A1KHF%2fR3Ypm%2bwgioea7vRCswCYItCa2sCxYml7cz7W1gQd1wb49NHtblrlvjxIVdVhvTtS2ezNos6Xbzpe7bkrfYRH77qPn0jcxVrS5znHhYCY2IKFXtLFU7HdLLOhuQeQIw8Mxgx%2f4HbJAMX1y07ZYm7QVzrv7hLZDYtMyDrg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E932" t="inlineStr">
+        <is>
+          <t>09823558000</t>
+        </is>
+      </c>
+      <c r="F932" t="inlineStr">
+        <is>
+          <t>Borhade Wadi, Moshi</t>
+        </is>
+      </c>
+      <c r="G932" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H932" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I932" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J932" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" s="1" t="inlineStr">
+        <is>
+          <t>A52100017786</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Vijay Narayan Barate</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>A52100017786</t>
+        </is>
+      </c>
+      <c r="D933" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Uh8%2fkUJ3bjIa9ywn8koCDS2iDcXu2BUCSeefjXbHGromS1Wp%2fYxALvuYb%2fMM85OFIFkdDBCZt3hIIVs%2b61ElHVTtB%2bSj6MJIktb%2fm7xzb0PlUuX9JSmAm1bEjUTjra64u3o0odKbDlB%2fI3ecF6b%2foMeTWc4JlWqhIkb6iVfZJY%2fDcrAddOU9cg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E933" t="inlineStr">
+        <is>
+          <t>02066000497</t>
+        </is>
+      </c>
+      <c r="F933" t="inlineStr">
+        <is>
+          <t>Gokulnagar</t>
+        </is>
+      </c>
+      <c r="G933" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H933" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I933" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J933" t="inlineStr">
+        <is>
+          <t>411025</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" s="1" t="inlineStr">
+        <is>
+          <t>A52100017686</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Hitesh Shivaji Avachite</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>A52100017686</t>
+        </is>
+      </c>
+      <c r="D934" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PTgDiFEPQvPeD7gDUm8bS%2fQWZUD9q42r4b%2bLg4%2bfRgZgwK6l0xfFuMdZlLhqHlbDyaQVGkx8BlwP3uubQoyQk2pbWGTF0SoCqGfo%2bRms7TnNLYThfqzoZdkt7dqGARFVY%2byuFs3tPzLA%2ftauGpdZigIQ3RJTaaJ04o6I0fz%2b80eeDptA5Al38w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E934" t="inlineStr">
+        <is>
+          <t>02060121664</t>
+        </is>
+      </c>
+      <c r="F934" t="inlineStr">
+        <is>
+          <t>Khadki</t>
+        </is>
+      </c>
+      <c r="G934" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H934" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I934" t="inlineStr">
+        <is>
+          <t>Khadki</t>
+        </is>
+      </c>
+      <c r="J934" t="inlineStr">
+        <is>
+          <t>411003</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" s="1" t="inlineStr">
+        <is>
+          <t>A52100017671</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Iqbal  Shaikh</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>A52100017671</t>
+        </is>
+      </c>
+      <c r="D935" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=lxfLRRCW4sWnCL6bP%2f43qtqLOUA6XeA0HRVRa2fugdjqGGgVlvURhZKd5vk9Cj2jgt%2bIGsmNtgFstS5LDrnateeYrUao0Xb18vehuVfYuzhg1jfnWiUVtImlqGZJL8iNf37CBQDCgJw0nLtroilla0zjQAtArSLDh2ToupLr3A4GStOXftKkww%3d%3d</t>
+        </is>
+      </c>
+      <c r="E935" t="inlineStr">
+        <is>
+          <t>09823511011</t>
+        </is>
+      </c>
+      <c r="F935" t="inlineStr">
+        <is>
+          <t>Near Ganga Village</t>
+        </is>
+      </c>
+      <c r="G935" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H935" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I935" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J935" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" s="1" t="inlineStr">
+        <is>
+          <t>A52100017755</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Dnyanesh Shriram Bijamwar</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>A52100017755</t>
+        </is>
+      </c>
+      <c r="D936" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=sb%2fX0UhNwcw9yg7TrzfYjQY%2bF1Sziao7PLROZyzmbtpcHjkIX48cXV9t0HzDaA0GTr9R8yZtvsJZlYh5jzqhrmt%2bX4pudBB0dv5t3lqEpzd39o%2bEG8MZMEu5zmhC21%2b0GQOJMDmDYENHnfK%2bq%2fdZMJwjeuXvC3kA82JzE8cYJchFWVX%2b5gLpJw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E936" t="inlineStr">
+        <is>
+          <t>02025450119</t>
+        </is>
+      </c>
+      <c r="F936" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G936" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H936" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I936" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J936" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" s="1" t="inlineStr">
+        <is>
+          <t>A52100017675</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Ankita  Mantri</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>A52100017675</t>
+        </is>
+      </c>
+      <c r="D937" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=mQ5aFTvosPg7fvT78%2bQ4zR169lM9oj%2bIHOTbjQGRSD7bXWYDQFhZdMrToHrYejR6KKhuLm%2b2484UPafS1bM9Q0zV%2bW7tEsxRPz0LAjIAZVeqPkgTH%2bNMg10EBpnKhLqf7zSJJUaau0YWPKu3TfCEl0%2fHJ2VoLG53XufGATRJnQYPMbK0fBRh5Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E937" t="inlineStr">
+        <is>
+          <t>02046711466</t>
+        </is>
+      </c>
+      <c r="F937" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="G937" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H937" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I937" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J937" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" s="1" t="inlineStr">
+        <is>
+          <t>A52100017749</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Sameer Sudhakar Nagarkar</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>A52100017749</t>
+        </is>
+      </c>
+      <c r="D938" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MbrGBqfOwC8VcQkh8dvpe0MqXJ8clXK7eQadPHreJZPj7FAysI%2fqECc0K7RL9VjV9lcxWvGFDUR0TZagLbwExzfNlsIcNaBAIw2MxtJ4Wu3siHmToHiwJ4JQdP4iTKHYNZ8kGnZzYVl2qyJLSbkyvK51mQerSjf%2fKQhvyBLmIMfggMIrKDxZGA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E938" t="inlineStr">
+        <is>
+          <t>02025511170</t>
+        </is>
+      </c>
+      <c r="F938" t="inlineStr">
+        <is>
+          <t>Shivajinagar</t>
+        </is>
+      </c>
+      <c r="G938" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H938" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I938" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J938" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" s="1" t="inlineStr">
+        <is>
+          <t>A52100017689</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Kizhakkum Shabeer Babu</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>A52100017689</t>
+        </is>
+      </c>
+      <c r="D939" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=gtHg%2badqJ7M57WCMJXKO3R1H%2fCx7t7FxbD3roB70zX76hHOFqrjnavSNw1Xs9jZVKYM0oLSsBxSi0zcIs0lrQAdTuJjwl15f9bUo2NmI0JIg6xy6iMomHpRkzZJjttD%2bL152%2bbPYdTqpH7znIjf4yl8pFvWu3PYE3Ds6%2bqMKI47iSNCTmQpdyA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E939" t="inlineStr">
+        <is>
+          <t>08806933933</t>
+        </is>
+      </c>
+      <c r="F939" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G939" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H939" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I939" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J939" t="inlineStr">
+        <is>
+          <t>511045</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" s="1" t="inlineStr">
+        <is>
+          <t>A52100018392</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Choudhary Manish Ram Kumar</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>A52100018392</t>
+        </is>
+      </c>
+      <c r="D940" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Lg%2fJ4kTKEfn9vl%2f%2fRAWA4Udcw%2ba%2fyh6R9NKI93yhW9JL0qtuArWdQcQKalAoCXDMNx7OarULA%2bbGApfHWI%2fEAtVeL7aP7jIhA8SzBVkjbZN3QIxOB0BQu0ijqiiXAWRX3AfpjR9apzgnZI242Kd6InZ9YF78TQz1R40eFQQJK9RZhseSYSL3ig%3d%3d</t>
+        </is>
+      </c>
+      <c r="E940" t="inlineStr">
+        <is>
+          <t>02030492005</t>
+        </is>
+      </c>
+      <c r="F940" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G940" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H940" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I940" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J940" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" s="1" t="inlineStr">
+        <is>
+          <t>A52100017668</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Santosh Laxman Chavan</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>A52100017668</t>
+        </is>
+      </c>
+      <c r="D941" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=pSCLrSuO1iZ0yCcATPhL9ccthBPP71Q0PqGB72y6jTyxz%2fr3Du%2bY9LtXZ9dVKuNNPtoP%2flIL1kvpzWhmUMS%2bd4fndyFUR%2big%2bDSbtpS0O8QBIRtzvGYws0FaHMpxw74dA0d6Bp4oI8efODqjBYZTgayELbSj5UMg%2fqstQxCPNJH%2bu4ZewXe46w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E941" t="inlineStr">
+        <is>
+          <t>99130002406</t>
+        </is>
+      </c>
+      <c r="F941" t="inlineStr">
+        <is>
+          <t>Chikhali</t>
+        </is>
+      </c>
+      <c r="G941" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H941" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I941" t="inlineStr">
+        <is>
+          <t>Chikhalgaon</t>
+        </is>
+      </c>
+      <c r="J941" t="inlineStr">
+        <is>
+          <t>412114</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" s="1" t="inlineStr">
+        <is>
+          <t>A52100017769</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Riti  Dwivedi</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>A52100017769</t>
+        </is>
+      </c>
+      <c r="D942" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fK%2bTNAJmJvFzDdkdFyKSlJq1O54R8ouFPAWLbtEL8w8CWm%2bO%2behQmxz2KmgHuUPsEXzjGQuY9jnfY2W%2bX3mwodPH5bRjbBgnGe5PJT0fgod3Z11raokzGPcthDAM5Sp0wm3BmQt5jZzYeqYrUja9BIrBPYNIkMUD2AFWfFWWk%2bAgusuBMog8XQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E942" t="inlineStr">
+        <is>
+          <t>07875626903</t>
+        </is>
+      </c>
+      <c r="F942" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="G942" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H942" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I942" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J942" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" s="1" t="inlineStr">
+        <is>
+          <t>A52100017881</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Emirus Realty Private Limited</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>A52100017881</t>
+        </is>
+      </c>
+      <c r="D943" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2b6wf0evY6DNdfZOvKPkUSRV6HFIqLJk6Esr2hYoGVozG0vVpta%2flviEmqZOKRAO9QcEFixJu3qtA7XwvJNLDSneWea5vxloW%2fL4qrlKc4AAUmtwbmlBmMyJNupLbE96ln0%2feN9miiEgjSLZ9CEGdZVQheoZKQMxlr9fWZUrrkYzztPC%2bCac4UA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E943" t="inlineStr">
+        <is>
+          <t>02048605588</t>
+        </is>
+      </c>
+      <c r="F943" t="inlineStr">
+        <is>
+          <t>Laxman Nagar</t>
+        </is>
+      </c>
+      <c r="G943" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H943" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I943" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J943" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" s="1" t="inlineStr">
+        <is>
+          <t>A52100017737</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Sagar Arun Ambhorkar</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>A52100017737</t>
+        </is>
+      </c>
+      <c r="D944" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=8DTIOzAeHdoVAuheBDNsAGYIzQm8H3WqHVzWj0oawm%2fL7StFuYD0K11PJ0NuOwbB3GcLAVrv5z%2f3RJDmbz3ZJQ4%2brWccXLkvNPZoPUNk9RKfjXeTJQKUCaBFDYEOx2ReotfPdITIzVBZC0MpZq6AVrf535FmaHswWZL0vQKv%2blyQ7bDRY8yATQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E944" t="inlineStr">
+        <is>
+          <t>08796752828</t>
+        </is>
+      </c>
+      <c r="F944" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G944" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H944" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I944" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J944" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" s="1" t="inlineStr">
+        <is>
+          <t>A52100017943</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Rahul Manoj Gandhi</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>A52100017943</t>
+        </is>
+      </c>
+      <c r="D945" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=8WZSmyOkqjPEl2qd80xKSn1gIUjGoMzg%2bkvHB1KcUhkvXVnXtpFurRQJHU%2b9sXkP8%2bq8%2bDLY1p5UTFagQe1%2fekEckNBhybB8fAukSlyrzrdIXkW1cJfz0aQmCMgVWnLslzClQSu9NIJBJHdtJuBRJueaJoAwJbNKbgZVFzrYj%2bP%2bpkm944igMA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E945" t="inlineStr">
+        <is>
+          <t>02024268549</t>
+        </is>
+      </c>
+      <c r="F945" t="inlineStr">
+        <is>
+          <t>Bibvewadi</t>
+        </is>
+      </c>
+      <c r="G945" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H945" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I945" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J945" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" s="1" t="inlineStr">
+        <is>
+          <t>A52100017688</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Onkarmal Amichand Jain</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>A52100017688</t>
+        </is>
+      </c>
+      <c r="D946" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=N96PqTepn2toSb8ponNywvz1bhtkPsdsFryqia7G%2bnh%2fFNMiBGxQ8JY6lKtXRtVGid3osfRK9qGfUB3iCPuBQAWL14pZ87oJTBek5GWtcuuHLTrom4mgErSA0cwVcTQyA0A28AaCZ9BGCHI3naZ6fA06H5kHdQGSt7tD9NS8lq6qNIjzjfSO1Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E946" t="inlineStr">
+        <is>
+          <t>02024270039</t>
+        </is>
+      </c>
+      <c r="F946" t="inlineStr">
+        <is>
+          <t>Guruwar Peth</t>
+        </is>
+      </c>
+      <c r="G946" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H946" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I946" t="inlineStr">
+        <is>
+          <t>Swargate</t>
+        </is>
+      </c>
+      <c r="J946" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" s="1" t="inlineStr">
+        <is>
+          <t>A52100017779</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Bhimashankar Mallappa Prachande</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>A52100017779</t>
+        </is>
+      </c>
+      <c r="D947" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=gJt1ulrNv74FgR7pbyYv8xpWMzPx%2fqJipLnOqEeZgFvdFEamdeVGjwBjhspIdGaJeN06cFy9daIGUyfjc77qPiumiXLBYALigcUwTIkadiaUYORGl6QBIQqcM7AGqc8md%2bhaFrij1395bxu2lLNMEu9GLsbWyrTAQZw883SE9vWMT%2fLfhh1JpA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E947" t="inlineStr">
+        <is>
+          <t>02096044442</t>
+        </is>
+      </c>
+      <c r="F947" t="inlineStr">
+        <is>
+          <t>Nr Balaji Mandir</t>
+        </is>
+      </c>
+      <c r="G947" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H947" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I947" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J947" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" s="1" t="inlineStr">
+        <is>
+          <t>A52100017809</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Uniwest Homes Private Limited</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>A52100017809</t>
+        </is>
+      </c>
+      <c r="D948" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Xm2RALUp2NI6zbF0mjMu0m23GGVp62lSl8%2bkpPJFzGdxRa%2bHzZWZ%2b%2bbHkGI1ntci3FkuecuABxQyeHYnyioh4PSjm7rTJeVVZqHt9zu1bGkM6AapSMGlfIX8HIjZ0WhHPDQm34hHUmPUELAgx%2b0XYX1XlDQZor9a6w3b%2ba%2bumtvTga5Vw1KIig%3d%3d</t>
+        </is>
+      </c>
+      <c r="E948" t="inlineStr">
+        <is>
+          <t>02026431721</t>
+        </is>
+      </c>
+      <c r="F948" t="inlineStr">
+        <is>
+          <t>Wanawadi</t>
+        </is>
+      </c>
+      <c r="G948" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H948" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I948" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J948" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" s="1" t="inlineStr">
+        <is>
+          <t>A52100017887</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Shreyash Deepak Shah</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>A52100017887</t>
+        </is>
+      </c>
+      <c r="D949" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=itE1BgLNF4i0mOPgmVZIdDz1kBsd9F%2fEETbuPPOOCNtqx%2fLYPUOJCRFaCrdFvnSvET0WlthagkncQdosx8nseZHfJPFgJ8xsOStKOUAUh0j6r4ZWG89wsOjbmBmAUpnJrog3rZfNcgTGaXh6OM%2b2%2bGDxen6W2wUWkHuIRNFnE2KR2mz9ti%2bhsg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E949" t="inlineStr">
+        <is>
+          <t>02462257104</t>
+        </is>
+      </c>
+      <c r="F949" t="inlineStr">
+        <is>
+          <t>Parvati</t>
+        </is>
+      </c>
+      <c r="G949" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H949" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I949" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J949" t="inlineStr">
+        <is>
+          <t>411009</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" s="1" t="inlineStr">
+        <is>
+          <t>A52100017705</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Sham Laxman Patankar</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>A52100017705</t>
+        </is>
+      </c>
+      <c r="D950" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=faTKVIFC2Q1%2bCPpPXNVNLLGxl3hWW3KeUSIV9UtehhAY9rxFst8VA2EF0XtsGzEv%2b8q%2b8Av3tHAZNb9yyUybjBZH5tKW%2frG230tNR91T6asm%2bo%2f6ipPmay903aGMMN8YzwvcvTvWoq2NOhPrsIg5kSlHHP4h1Edph%2fUy8LayfoNhAojMo%2bCPkQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E950" t="inlineStr">
+        <is>
+          <t>02022222222</t>
+        </is>
+      </c>
+      <c r="F950" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G950" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H950" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I950" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J950" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" s="1" t="inlineStr">
+        <is>
+          <t>A52100017915</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Ravi Kumar Gupta</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>A52100017915</t>
+        </is>
+      </c>
+      <c r="D951" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=37nI56P03YkQKTTWH4DekA8M68z%2fA3rD%2b2Hs%2bQN0dYmMG9312zcfLisKi%2bPG2qoLcmTWrY0sSKC7mnFO8EGWmnrOAiiCKBCXle5ZkHLfor6GdCeZbNIwYQXXyuqXYG%2fh7%2fLR6nUnQcpcCVkpMwvcY5QvMYdPlt%2bHyHJbuEQ9KgHvOhBuE%2brVfA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E951" t="inlineStr">
+        <is>
+          <t>02087652452</t>
+        </is>
+      </c>
+      <c r="F951" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G951" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H951" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I951" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J951" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1000]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J951"/>
+  <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -49368,6 +49368,2606 @@
         </is>
       </c>
     </row>
+    <row r="952">
+      <c r="A952" s="1" t="inlineStr">
+        <is>
+          <t>A52100017783</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Archana Ranjan Kulkarni</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>A52100017783</t>
+        </is>
+      </c>
+      <c r="D952" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xVBjyQmufid4o2ugxidIwq%2f22stJBbvm9ck1b2%2bfckZOpIF%2bFqxqBcAvYR1JX9XJhEjIYcTqVondn1w8QmD55sl1%2fbmTBNM5IUbbG6DjB7QVb6fBfJI6fqZONkLt4hWWdls9ErcdH3Msv7nzLW02ZyyySpbA2Fcs9zEbhbD3Pwcz5Li%2fAK8hrA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E952" t="inlineStr">
+        <is>
+          <t>09892165036</t>
+        </is>
+      </c>
+      <c r="F952" t="inlineStr">
+        <is>
+          <t>Police Line</t>
+        </is>
+      </c>
+      <c r="G952" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H952" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I952" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J952" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" s="1" t="inlineStr">
+        <is>
+          <t>A52100018035</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Naresh Ramesh Thakur</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>A52100018035</t>
+        </is>
+      </c>
+      <c r="D953" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=w5iIkc2ybLF7TtxN%2fNYMvXht9GlukebNAC4U8BmK4%2bQyq1QG%2b5463w1PRvRlWm%2fJnGMestXmsRTnnA92CnYrEcO9m5ckGSjubXY7Ex%2fxAq9jWOovQJL5IOd%2b6nDPXs%2b6ZlCDmjUfJ2estMbHql6PTONzriILP86Hx4XsbGuRijVI7sV2TJSVFg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E953" t="inlineStr">
+        <is>
+          <t>09225636523</t>
+        </is>
+      </c>
+      <c r="F953" t="inlineStr">
+        <is>
+          <t>Fatima Nagar</t>
+        </is>
+      </c>
+      <c r="G953" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H953" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I953" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="J953" t="inlineStr">
+        <is>
+          <t>411013</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" s="1" t="inlineStr">
+        <is>
+          <t>A52100017778</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Jasminder Singh Gandhi</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>A52100017778</t>
+        </is>
+      </c>
+      <c r="D954" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=XW4zYR3AiuglMmGcbsRtmFCdbolCF5Lpv%2fECaybNFVBbSljNa1X8hjfi2WU%2bBUp7%2f%2bNVZRVkz%2bGLoH0fCkvrlL00L%2fLKnYiG3gRmTxCV%2bmEb1yuyoVqOXkFurAvnVk8QSfzqHJA%2fy%2bqWSX7gl5mXPSKSUFR6iejvzD%2b9T4zuYWSRbqSJPV31WA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E954" t="inlineStr">
+        <is>
+          <t>20227051445</t>
+        </is>
+      </c>
+      <c r="F954" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="G954" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H954" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I954" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J954" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" s="1" t="inlineStr">
+        <is>
+          <t>A52100018210</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Shamiee  Sabharwall</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>A52100018210</t>
+        </is>
+      </c>
+      <c r="D955" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=qfT1VwfumXmDg8LvllntduEh6d5zuKrvH9QHZVYOxCMWTtybBTdWTpcu2cmINGRq88jlUT%2fmFIOIo9Npy7TX6Dlv6aFLWpI0eAQIZuUdB05xeW0IWs5hHAuQxTDh42KkzjwJgR5rZUuIlfbEVh4NDMB8MJU2IwXDT9VfEzFhQKKlhvGZ9TXrgg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E955" t="inlineStr">
+        <is>
+          <t>02026332553</t>
+        </is>
+      </c>
+      <c r="F955" t="inlineStr">
+        <is>
+          <t>Wanowarie</t>
+        </is>
+      </c>
+      <c r="G955" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H955" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I955" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="J955" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" s="1" t="inlineStr">
+        <is>
+          <t>A52100017727</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Maharoukh Ajay Bhosle</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>A52100017727</t>
+        </is>
+      </c>
+      <c r="D956" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=U%2faeefIm%2bQv1qZKKQicSTUtdlIltUb7wa89IbMX3p%2bTImyQAQZaCXMIHMAmtbd0PPCkZM7oM1WGcXFu0khA0ZuNASa%2fv%2fyuvOBq76b9uvGkZzjOcSQHA3%2fwURV%2f68XEoDi%2begoSZ9bPHE4%2fENtMwZHy4CmTCeRLzVzLpwRBOW9ARAn4FuQK1oA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E956" t="inlineStr">
+        <is>
+          <t>02026833465</t>
+        </is>
+      </c>
+      <c r="F956" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G956" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H956" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I956" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J956" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" s="1" t="inlineStr">
+        <is>
+          <t>A52100018069</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Vinayak Vitthal Gaikwad</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>A52100018069</t>
+        </is>
+      </c>
+      <c r="D957" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=qG4MvUtmL%2b0gUMO3FPN6Y2RAzZB%2bjRnOC0gCP4ltLmlGc%2fsP5HJRSOijhoVzwuGB8acS6%2bsAP98OZZrbF6lMvMiIgJj0AzBjmsFsAtEnOkPplDJgp73VbgiQVfiBGaUAnAOMIy9axV6R%2bpc5XtqBRgmUQ6BQyZVfh%2btFCe%2bvo3dPlpJyCVNZPA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E957" t="inlineStr">
+        <is>
+          <t>09096879685</t>
+        </is>
+      </c>
+      <c r="F957" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G957" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H957" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I957" t="inlineStr">
+        <is>
+          <t>Kondhwa Bk</t>
+        </is>
+      </c>
+      <c r="J957" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" s="1" t="inlineStr">
+        <is>
+          <t>A52100017760</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Sandeep H Sahasrabudhe</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>A52100017760</t>
+        </is>
+      </c>
+      <c r="D958" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=RmgomYQKz1cDGe%2fIOTxZu2zDHtJYj1qkjCYq5IbvVyfCF3gdUVp%2fOtmlXJ8GESy1i%2bW7JwFYgk6Ai0vSL5dScAOwoq8sFlNymC7DUdQ%2bFdvViFBDQsFu2p%2futcXehIEnq0M03EN%2b3IyEoS5BMKQSGozmn6BOHtl2k6gYSE0A29B%2b8IWw4geQFw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E958" t="inlineStr">
+        <is>
+          <t>02026437134</t>
+        </is>
+      </c>
+      <c r="F958" t="inlineStr">
+        <is>
+          <t>Bankar Road</t>
+        </is>
+      </c>
+      <c r="G958" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H958" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I958" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J958" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" s="1" t="inlineStr">
+        <is>
+          <t>A52100017721</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Nitin Madan Kulchandra</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>A52100017721</t>
+        </is>
+      </c>
+      <c r="D959" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hQ4HAifEuyFEDJ5NIcPFcMGj2Yy2W97TgItd5zJFR4YA9zkgFgoZWCG4c%2bmaXM2%2bnI8xpp5H16%2fYZvG%2bCc%2bpYeC7PPbMj6eCsqjeanuM4ZznJbwEuXoFTU1SMou6qWlJqzmrdxbniDKBSXMPeszySzDtPt%2b3zePZ31wxA%2fjEeoNe66O72HixDw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E959" t="inlineStr">
+        <is>
+          <t>09657027288</t>
+        </is>
+      </c>
+      <c r="F959" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G959" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H959" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I959" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J959" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" s="1" t="inlineStr">
+        <is>
+          <t>A52100017828</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Suresh Pandurang Phapale</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>A52100017828</t>
+        </is>
+      </c>
+      <c r="D960" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wgcoDTErUGssbznYv86yxeZ0Ec5xY1Mtua47Io%2bZaCStBZTqvkyoptLVOMS1ZkunXLu0e2iezKZya2Y6t%2faTRc61v4jImIT%2fY%2braui2ElDOq75ZIElTsC0DrIYxhT5pE0GtirDqxYND9kMlaUdwrHPmVEaED%2f69uRL%2fTWqng%2bFZnsNJJv5Dxaw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E960" t="inlineStr">
+        <is>
+          <t>09850500057</t>
+        </is>
+      </c>
+      <c r="F960" t="inlineStr">
+        <is>
+          <t>Charholi Budruk</t>
+        </is>
+      </c>
+      <c r="G960" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H960" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I960" t="inlineStr">
+        <is>
+          <t>Charholi</t>
+        </is>
+      </c>
+      <c r="J960" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" s="1" t="inlineStr">
+        <is>
+          <t>A52100017907</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Seema Kamlesh Parmar</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>A52100017907</t>
+        </is>
+      </c>
+      <c r="D961" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=EZdV7f52y1FRB%2f4LawfsZlLUqjSbouACk9TfYBpmsTV8ndDlBmvSbXFVnbew9mToanDJ%2fM8HztrJfjNbFk%2b2nBiwygETYZnsioi8RXcrbIKMm2HGCcnl%2f%2fiZthK%2buPm2mS1TbQChs9PiaqBW4%2bGxAYR8QjiWAfDcdhPcEDxChF%2bxAGc5Vbm1HQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E961" t="inlineStr">
+        <is>
+          <t>09371668620</t>
+        </is>
+      </c>
+      <c r="F961" t="inlineStr">
+        <is>
+          <t>Wanowrie</t>
+        </is>
+      </c>
+      <c r="G961" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H961" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I961" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="J961" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" s="1" t="inlineStr">
+        <is>
+          <t>A52100018004</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Raghav Arvind Somani</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>A52100018004</t>
+        </is>
+      </c>
+      <c r="D962" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Ur4%2fAWT3XYK3KTjcffI4rpdCtAK%2f7wqEmlnw3vUZSfWgljDn9eEJ0OLgTKrUQyn%2b6%2ffIY49AmDY7QvgZ4UIyudWlKgWGFzJqPkXbKpkWKg%2fPJfNdIrqe9TGR%2bU5D7SyWF%2fmw49pHRbnavxzieehMQwcG9t09iScCeRcgzhKOpBi106%2fT%2fE9U0Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E962" t="inlineStr">
+        <is>
+          <t>02026099000</t>
+        </is>
+      </c>
+      <c r="F962" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G962" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H962" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I962" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J962" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" s="1" t="inlineStr">
+        <is>
+          <t>A52100018083</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Pratyaksh Realty</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>A52100018083</t>
+        </is>
+      </c>
+      <c r="D963" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=vXcoM9%2fwwUnV9%2bSS1j0Fi9SJKexkWNvEb3F5FicI%2bDjov0T1zJI7HJU4p1kgYx%2bN8yzj%2bEyYUMtTRg%2foesTPmAISQpxSTwcS9icEyV2Ap%2bp%2fEJXDEDtSHQcb2aqqnyLj6dkrB341nfuQyu6CH64QM2OfesvZU6SojBC131KoYl1SAikf2wslBw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E963" t="inlineStr">
+        <is>
+          <t>02027292425</t>
+        </is>
+      </c>
+      <c r="F963" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G963" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H963" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I963" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J963" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" s="1" t="inlineStr">
+        <is>
+          <t>A52100001693</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Shekhar Vasant Walanj</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>A52100001693</t>
+        </is>
+      </c>
+      <c r="D964" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=U2JxVrsMDIA95WieDxMA56Udda1aA1F2AMwdx6avDKmCKmjZ77ORaGVgdVSOljNaLsJM33NMXr3W5fLiaXnYA8vib8SYb4PfdJBlSRfZ%2fR%2fIuUiaRp%2bAzySKH4FXd6Z%2fpodrgNmY6LILhC4oXIuICYYCODtS7hotUL4bV3QCCK0%3d</t>
+        </is>
+      </c>
+      <c r="E964" t="inlineStr">
+        <is>
+          <t>02024332995</t>
+        </is>
+      </c>
+      <c r="F964" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G964" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H964" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I964" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J964" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" s="1" t="inlineStr">
+        <is>
+          <t>A52100017821</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Jiten  Israni</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>A52100017821</t>
+        </is>
+      </c>
+      <c r="D965" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=dTZgVzRQNgu8L4g7StKOIB4MQVFirtw5pkUnBPuwHxVkEH7Je%2bQJYFAjhJ6rDNIxtIjxc2IPsUO%2fZe3t3%2f7ZqWa6Cur2BcdU9Oj%2fWVDYxKrbvyTrf8Ja4bw1iWbYW7ZB2XaY3O9INLrDnCy1tHst1c7TfgvzoPTFovkeUEfkJGZy5FkYXLaYUQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E965" t="inlineStr">
+        <is>
+          <t>09371089491</t>
+        </is>
+      </c>
+      <c r="F965" t="inlineStr">
+        <is>
+          <t>Keshav Nagar, Mundhwa</t>
+        </is>
+      </c>
+      <c r="G965" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H965" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I965" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J965" t="inlineStr">
+        <is>
+          <t>411036</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" s="1" t="inlineStr">
+        <is>
+          <t>A52100020642</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Vishal Rameshrao Ulhe</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>A52100020642</t>
+        </is>
+      </c>
+      <c r="D966" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=HOclkyhnQc4%2fErSVjQntaa%2b1IAjuysQM7umNTabgQnjJVVbFP7vZHhoGDBKIAyE6KtVP0B%2bFtrpvlWt%2fc%2fugKo%2bOG4b9CcaX8lAIYH2UiH41D78LReMNdQIVaqO46rAKfqsqfFkBZ3Vr7KLyEtAj2zGNd1SC%2f59s6EX8KnG3sQN6Vd3i%2bZ9Ovw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E966" t="inlineStr">
+        <is>
+          <t>09970364550</t>
+        </is>
+      </c>
+      <c r="F966" t="inlineStr">
+        <is>
+          <t>Hinjewadi</t>
+        </is>
+      </c>
+      <c r="G966" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H966" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I966" t="inlineStr">
+        <is>
+          <t>Dattawadi</t>
+        </is>
+      </c>
+      <c r="J966" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" s="1" t="inlineStr">
+        <is>
+          <t>A52100018167</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Vascon Engineers Ltd.</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>A52100018167</t>
+        </is>
+      </c>
+      <c r="D967" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hlFaRdhJN8g2tAXgRYkufYRAnTBj3DUjHW4sRyZwq8GBNJ195il21G5rgpbK74Xe5KTV2fU94eciqj7EcpQDfza26YV8WrvtkmhBtqyU6%2fFMY73IYlQio9WSdIMORBPJbGKDw53IIcTRU1adv6vzJZSRbDvQ4oW48duCb2W%2fG%2b1DgpEiy5jgvQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E967" t="inlineStr">
+        <is>
+          <t>02030562350</t>
+        </is>
+      </c>
+      <c r="F967" t="inlineStr">
+        <is>
+          <t>Vimannagar</t>
+        </is>
+      </c>
+      <c r="G967" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H967" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I967" t="inlineStr">
+        <is>
+          <t>Vimannagar</t>
+        </is>
+      </c>
+      <c r="J967" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" s="1" t="inlineStr">
+        <is>
+          <t>A52100017986</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Shubroto Debi Sikdar Proprietor Of Virtuous Realty</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>A52100017986</t>
+        </is>
+      </c>
+      <c r="D968" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=JsCjqdAqGFPqXmLln1Czvjji2%2bReD2E%2bAyBnHb%2bbre%2fdai%2bzKnKxynFUIgXHMsl1xHjBS0oGRV44laorvqbmZfE25oi7YCTXxd42Kw87NBxSQJjWraKeaBsfPm2utnrEBO3L2vbQr3QEkjfMlYhl1nMNyLS92l24E6d0zN9j7OqN3wQoBQ6N8g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E968" t="inlineStr">
+        <is>
+          <t>09766758548</t>
+        </is>
+      </c>
+      <c r="F968" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G968" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H968" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I968" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J968" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" s="1" t="inlineStr">
+        <is>
+          <t>A52100017810</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Prashant Somashekhar Sinfal</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>A52100017810</t>
+        </is>
+      </c>
+      <c r="D969" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1I57FEMWBs7CFsOe2BNiGDjXtoe8Yb3H9Lva2i2tdzyiozLkvYA1rtqhhstx%2fy0P4QFAqqTpVrBYdg%2fZm1556yQ5LkBJGc9tVJ1LL47ywR7AGeBvcEMMQqLDVIntQuMYm4k2EyhXf9nc%2b6NIAnrgKBPtWxi5issiZ7rJJN%2bYYAiPby5P41Fzpw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E969" t="inlineStr">
+        <is>
+          <t>02025871808</t>
+        </is>
+      </c>
+      <c r="F969" t="inlineStr">
+        <is>
+          <t>Gokhalenagar,</t>
+        </is>
+      </c>
+      <c r="G969" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H969" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I969" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J969" t="inlineStr">
+        <is>
+          <t>411016</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" s="1" t="inlineStr">
+        <is>
+          <t>A52100017891</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Satish Narayan Kestikar</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>A52100017891</t>
+        </is>
+      </c>
+      <c r="D970" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ExFvh3%2bIbI1vjHv3i%2fWfLxQVAgPAeFNVviJwU0nNJgJqCmD3YnXNybAWDfYAT3D4BlvSTUfYQG%2bkL4gof9F7UCFtx8uAspu68qt6gKCadoJV47%2fq1Wie4wcZAMr4cUwghaZ%2f1vbTaQDBxPSaOj9%2fR4ddBKabllwWgCoHyUyhV%2fxJQI%2fVDuWN3A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E970" t="inlineStr">
+        <is>
+          <t>08668843079</t>
+        </is>
+      </c>
+      <c r="F970" t="inlineStr">
+        <is>
+          <t>Shivtirth Nagar</t>
+        </is>
+      </c>
+      <c r="G970" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H970" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I970" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J970" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" s="1" t="inlineStr">
+        <is>
+          <t>A52100017835</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Maya Krishnajee Singh</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>A52100017835</t>
+        </is>
+      </c>
+      <c r="D971" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=asFAG7ZZygAuS7z7O1QqAZsKKVjQfHKV%2fKYOc47IFTNa69OAxXTD7XwKfq%2f2M%2bb28hCsOgBvZfQfSijQZAbkMBSqJu3VgxVQ8KOhtKoqHxyximb09hpigQ8Vk4jcjODj8LWp8yLFAHIq%2fRp8Es03WCQHT9Bm8LT%2buygxQ3d%2bK40K55OCzcv4Gg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E971" t="inlineStr">
+        <is>
+          <t>02000000000</t>
+        </is>
+      </c>
+      <c r="F971" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="G971" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H971" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I971" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J971" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" s="1" t="inlineStr">
+        <is>
+          <t>A52100017900</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Dinesh Dhanraj Oswal</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>A52100017900</t>
+        </is>
+      </c>
+      <c r="D972" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2NuE56xDuYBorT99nN%2f6gNdtvUEQPdJTyttYPDMhfebbrzeb48cHvSz3ar7ESWa0jbzzZjlH1VwovrpKfjosDCh30Ltt%2bKEvKC23cWPOvY%2fIz9XEwlqMPb1QMFgSOCOSs78xRJg6Zrv7XJE3%2ba%2bJGdKH54keSbnhNI%2fo49qH3crlwiYIZCTvUA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E972" t="inlineStr">
+        <is>
+          <t>02026381976</t>
+        </is>
+      </c>
+      <c r="F972" t="inlineStr">
+        <is>
+          <t>Bhavani Peth</t>
+        </is>
+      </c>
+      <c r="G972" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H972" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I972" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J972" t="inlineStr">
+        <is>
+          <t>411042</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" s="1" t="inlineStr">
+        <is>
+          <t>A52100018579</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Steadfast Energy &amp; Industrial Solutions Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>A52100018579</t>
+        </is>
+      </c>
+      <c r="D973" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=RUV2jvrUkZfC0KWK7oDgT3uu4mf73cSpujUqfRcXbrKe827mXG9G4gtILTOg7XBW5WIPCaAya%2fKqx1rUxfM1E3vCCNDr9GAgSArcoZbCMycZXpxER6iZUNoDtVkikblFFy8QM7wdmVLgUnrgrFcQ0AlA0gk9OwYBgVzzHqSAJmBtpy77McWvEA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E973" t="inlineStr">
+        <is>
+          <t>02026980014</t>
+        </is>
+      </c>
+      <c r="F973" t="inlineStr">
+        <is>
+          <t>Phursungi</t>
+        </is>
+      </c>
+      <c r="G973" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H973" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I973" t="inlineStr">
+        <is>
+          <t>Fursungi</t>
+        </is>
+      </c>
+      <c r="J973" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" s="1" t="inlineStr">
+        <is>
+          <t>A52100017890</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Payal Ashok Oswal</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>A52100017890</t>
+        </is>
+      </c>
+      <c r="D974" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=N7dwalhDN4f%2f%2fsRP8vIAHX67yTydkMVoRbg7TpPo7pcVgl4fKTN2DqANdDhZnnBfd%2ftX1dg8Fi0ljIPbv4J9NrIB%2f36ZuzlbobzOXz5m7s2xK8pVMMTikFHRM4iZ%2fg95H0n0rGgDrSdFbYyeObwEf%2fjhhPSEbhd9JXTjpc5xHgRbRhbaq80N%2fQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E974" t="inlineStr">
+        <is>
+          <t>02024241899</t>
+        </is>
+      </c>
+      <c r="F974" t="inlineStr">
+        <is>
+          <t>Market Yard</t>
+        </is>
+      </c>
+      <c r="G974" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H974" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I974" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J974" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" s="1" t="inlineStr">
+        <is>
+          <t>A52100018512</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Harshita Divichand Oswal</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>A52100018512</t>
+        </is>
+      </c>
+      <c r="D975" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=SxNey1ZZBj35BEafpinudo0hcdUVzYQG5dfBGDxydFdG5txaYWV8D9DQJGBRsqkb4lxY9ydOTtXdHGkbuwm%2fG2C5iunGoftGKP7O0e%2byafafW9%2fi4H%2ft2fuTiBlM%2bdRTTYJI%2fd795SgTRA1mMsnnBgHNJYE2RzKBOWQXRSPQgXLGYiFZ%2f01HPg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E975" t="inlineStr">
+        <is>
+          <t>02024241899</t>
+        </is>
+      </c>
+      <c r="F975" t="inlineStr">
+        <is>
+          <t>Bibewadi</t>
+        </is>
+      </c>
+      <c r="G975" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H975" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I975" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J975" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" s="1" t="inlineStr">
+        <is>
+          <t>A52100017863</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Raksha Ashok Oswal</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>A52100017863</t>
+        </is>
+      </c>
+      <c r="D976" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=V%2b4UUXLj47KSip2G%2bfls0YiP%2bBe8NU2jglDdT5LwSakuO%2b%2f9MKfg9%2b3%2bbqJgnLWdtNquOw6KR8dx9Mc3fj%2fmz5Q5qp%2fNidbUxjJVYgLJb4SN3zW7Ic0v8KN5tXapydL21J%2bjA1F7r0dtMx1qNU3NBe5F9d8%2b7nHrJv46NIEZ5LoXz%2fpg978Feg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E976" t="inlineStr">
+        <is>
+          <t>02024241899</t>
+        </is>
+      </c>
+      <c r="F976" t="inlineStr">
+        <is>
+          <t>Market Yard</t>
+        </is>
+      </c>
+      <c r="G976" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H976" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I976" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J976" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" s="1" t="inlineStr">
+        <is>
+          <t>A52100017901</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Ketan Arvind Ganechari</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>A52100017901</t>
+        </is>
+      </c>
+      <c r="D977" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=DgGUCHFhe%2fqQQ%2foXFhRTFLIkYk5Xp%2bXTAQtB251y3XA%2bbX2ixZjYsPCBYuOqi%2fetXkRn4KFs9qn22tkOODvhdS33xf5OKWdpoJcASLqOfC6fBpMstM2v2uOMa9tnrOR%2br35biir%2bH8XWgL8ZX%2fl9ET4iAwPhqcrMIvLMdPmBYGk0D2kB7sPsvw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E977" t="inlineStr">
+        <is>
+          <t>02024337766</t>
+        </is>
+      </c>
+      <c r="F977" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="G977" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H977" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I977" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="J977" t="inlineStr">
+        <is>
+          <t>411043</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" s="1" t="inlineStr">
+        <is>
+          <t>A52100017797</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Raj Ramchand Mirpuri</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>A52100017797</t>
+        </is>
+      </c>
+      <c r="D978" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=gqVI%2fmEjwo795Fidr%2fHJwf4g5%2bmO8LV0oXx5tQPGeyyzaGseVZbi5SQ3wfm1N3525%2bwSwscvniq3YAlkadGIuAJzIv3t3ZpBlcn6J38V28xOnRvU77WyAx2ILES%2fcr%2ftuSEb8VqxeCOChW7qCkHEW94UFNMrC2NlhdOeOwyfre8G7BrT7VKahQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E978" t="inlineStr">
+        <is>
+          <t>09819089805</t>
+        </is>
+      </c>
+      <c r="F978" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G978" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H978" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I978" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J978" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" s="1" t="inlineStr">
+        <is>
+          <t>A52100018108</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Pradeep Kumar Masand</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>A52100018108</t>
+        </is>
+      </c>
+      <c r="D979" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=gPj6S3ziAgvlSOvm2Omrhn6TrTHw3K1uvatFiLcqUVYa%2fiLnkD7z2W0MaKysIbttEzYgN6tbbTxsjn55zbutCwqILAe2KeZ82ohF9mY46ApOvCDl0A2AGTICxG3SnVcDGPFRmL%2faqBwAuE%2bYoon4SLkRdsgb4qoKR8FCnj1Apou6TGnbcnfzaQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E979" t="inlineStr">
+        <is>
+          <t>02226056262</t>
+        </is>
+      </c>
+      <c r="F979" t="inlineStr">
+        <is>
+          <t>Nyati County</t>
+        </is>
+      </c>
+      <c r="G979" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H979" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I979" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="J979" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" s="1" t="inlineStr">
+        <is>
+          <t>A52100017849</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Sagar Mukund Jadhav Proprietor Of Icon Real Estate And Buildcon</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>A52100017849</t>
+        </is>
+      </c>
+      <c r="D980" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=L3qRfdcklNcsr7dvNFeH%2bmqRksykZRrFXJ2gC6nHUr0PFxZn6KLmWg%2f5Y3gPkR2N4%2fi388z8qETY%2fSYhlgy3UwIYTQf2NeWIrzAaZ%2fVG64IPHgxzwKIoSonch29Ap2BkPyz5GjJ7H29zVKwEIFJyZKW5MZf%2bMv72MOz70j%2biHFlOOfb93rJzKw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E980" t="inlineStr">
+        <is>
+          <t>09011455555</t>
+        </is>
+      </c>
+      <c r="F980" t="inlineStr">
+        <is>
+          <t>Taleranagar</t>
+        </is>
+      </c>
+      <c r="G980" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H980" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I980" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="J980" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" s="1" t="inlineStr">
+        <is>
+          <t>A52100018124</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Alka Abhay Pandey</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>A52100018124</t>
+        </is>
+      </c>
+      <c r="D981" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=usA7Z0GiD1ss7T6F5Fm5ylutqOmQ7%2fTKBuhbNBMDzrovr1BNgwO1c9tcDHQyrCMCCZ47XEujJxzLCDakLOsw2Ik8TdR%2br%2fqtJrOoik8TK11WGg4%2blmN1AgOtgs7XJ2D962T7OAHDl5IDUKJrD9ifbq%2faSk%2frWWQOihWvpfOqXNayMvt4gx19gA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E981" t="inlineStr">
+        <is>
+          <t>09921563479</t>
+        </is>
+      </c>
+      <c r="F981" t="inlineStr">
+        <is>
+          <t>Katraj</t>
+        </is>
+      </c>
+      <c r="G981" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H981" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I981" t="inlineStr">
+        <is>
+          <t>Katraj</t>
+        </is>
+      </c>
+      <c r="J981" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" s="1" t="inlineStr">
+        <is>
+          <t>A52100017934</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Pravin Naresh Nethlekar Proprietor Of Om Sai Property</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>A52100017934</t>
+        </is>
+      </c>
+      <c r="D982" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xIamb0NNsEaIGZQhuTMc23xZt%2byhmIOKsyU82qMvw%2bEd4NWe1%2fCKm2BIk0xSZK%2bst9JDU0aisymsftE3M8I8irbwF54%2f0%2f%2b5BOugF7%2br6zkQf5WQmVsf%2fgLx4FMtOHiQM9pWfKgS2B66QjVwz3caRU%2fFcMP3h7L7KORv7sn3Ve1xAfbtpZCLNQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E982" t="inlineStr">
+        <is>
+          <t>09764687666</t>
+        </is>
+      </c>
+      <c r="F982" t="inlineStr">
+        <is>
+          <t>Keshavnagar</t>
+        </is>
+      </c>
+      <c r="G982" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H982" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I982" t="inlineStr">
+        <is>
+          <t>Mundhawa</t>
+        </is>
+      </c>
+      <c r="J982" t="inlineStr">
+        <is>
+          <t>411036</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" s="1" t="inlineStr">
+        <is>
+          <t>A52100018251</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Sanjay Marotrao Fulzele Proprietor Of Fulzele Nation Promoters And Developers</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>A52100018251</t>
+        </is>
+      </c>
+      <c r="D983" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MWlzzGkzdfQprCLeX1VmCOyPqZYExy%2f59AE2dlTX%2b5nArcQDBPWgr6X%2fTUNpYiHARGxNsPzeqfmlrs1nfRWa6jEkrk3VKux1RGpIj2X1knG6vHAmUr6biwSf1KxQBiCaJX4LM34tTA2RCPERrDdwc1KvyuCRd92%2fpzLJqriZjnVP4ka9KD%2fSIg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E983" t="inlineStr">
+        <is>
+          <t>09881080664</t>
+        </is>
+      </c>
+      <c r="F983" t="inlineStr">
+        <is>
+          <t>Marunji</t>
+        </is>
+      </c>
+      <c r="G983" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H983" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I983" t="inlineStr">
+        <is>
+          <t>Marunji</t>
+        </is>
+      </c>
+      <c r="J983" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" s="1" t="inlineStr">
+        <is>
+          <t>A52100017933</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Madhav Rameshrao Meshram</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>A52100017933</t>
+        </is>
+      </c>
+      <c r="D984" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=h14rIs7XAuElVFj4l94BLGUs%2bkW891TH6olVp%2bVpn%2btf114niP0l7HNmrDXsO0zonM8MqvD%2fjkZmN3yr7Mq5xHYaSOFwy0t5UJ34TIlroGsAP3br1Az3JddIuahGQgdBusd8Xn7sYKnQwfMMKYVBZQly%2fukWDxysdptpQmIiWBa5AinL%2bB8T1Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E984" t="inlineStr">
+        <is>
+          <t>09156962062</t>
+        </is>
+      </c>
+      <c r="F984" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G984" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H984" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I984" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J984" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" s="1" t="inlineStr">
+        <is>
+          <t>A52100019758</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Naveen Kumar Gupta</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>A52100019758</t>
+        </is>
+      </c>
+      <c r="D985" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=8PxXiugI4Il6P2hvpcTKJnPLnP8CS1WOZxJz9kJKOVQRyOD4NNcMy12fyH8jtCKKCyBweVbOQjnnaIo5Zf5ux2ebMvHNuMm1DYfmutuTVgnDRsJT2sf0IN62AP%2fRv4p8ad%2bHzW3ZQkoNjdLBv9NTKCNjyO1C5KrDgioJvCFQuPBiC5Tk%2fIKVow%3d%3d</t>
+        </is>
+      </c>
+      <c r="E985" t="inlineStr">
+        <is>
+          <t>05422635009</t>
+        </is>
+      </c>
+      <c r="F985" t="inlineStr">
+        <is>
+          <t>Shukrwar Peth</t>
+        </is>
+      </c>
+      <c r="G985" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H985" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I985" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J985" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" s="1" t="inlineStr">
+        <is>
+          <t>A52100018143</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Brickfolio Solutions Private Limited</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>A52100018143</t>
+        </is>
+      </c>
+      <c r="D986" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ulHTTBUtB5TZBHYUOV3aVsXDZ4H3lG9QVQFlifHkl%2fdIN8ipaktxhmkd8qZC%2fxqF4P%2f6Rh3nAAtypZA17iblkNaXWXBVDD5yEDGH%2fyImXhCEr2UrMzEdQuvssUqJYD8ggNUFRQ9GXSagfhePkWMPE5Q012LrObe5xac1Wp%2bv%2fyIXj%2fV345cHtw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E986" t="inlineStr">
+        <is>
+          <t>02049119119</t>
+        </is>
+      </c>
+      <c r="F986" t="inlineStr">
+        <is>
+          <t>Hissa No-1/2/3, Wadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G986" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H986" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I986" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J986" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" s="1" t="inlineStr">
+        <is>
+          <t>A52100017982</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Harit Ashok Shah</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>A52100017982</t>
+        </is>
+      </c>
+      <c r="D987" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fBRIgqt%2f9SARh8g%2bdrbvYqKcDahYdGKRvbBxSc7WPf9%2bpAzt7A9qleSyhUtXn7Wsw777JVSOPObZE9b3sNTdO3IK1ERITY2NgTl%2fgo%2fJKCB4nQohauwsIn8l4ofHUEVDXaQpz2OzAxdAuENzirjxGahLKwZNVmP3l30YNycHYyOrPfh%2bkjHwXw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E987" t="inlineStr">
+        <is>
+          <t>02061234567</t>
+        </is>
+      </c>
+      <c r="F987" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="G987" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H987" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I987" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="J987" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" s="1" t="inlineStr">
+        <is>
+          <t>A52100018073</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Omkishore  Singh</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>A52100018073</t>
+        </is>
+      </c>
+      <c r="D988" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wnAR%2ba85lj8V7GwmV8pjq%2f4AQt%2fnBduernNRJu8hSvQEx%2fV2jYqRTG%2fh%2bPrLv%2fy2ES4jlmUM2RqjV5LqKzfPnFZswfeKmUbIQysHLAylQdfAp7hCg6z3%2biIr2BD9d02EEUIsqh7Dr1DPCQiacMCMzH9XKaO1Cp%2fB8Go8XIcr%2fHQAzpl7febdaA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E988" t="inlineStr">
+        <is>
+          <t>09834983532</t>
+        </is>
+      </c>
+      <c r="F988" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G988" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H988" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I988" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J988" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" s="1" t="inlineStr">
+        <is>
+          <t>A52100017995</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Nitin Tukaram Shendge</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>A52100017995</t>
+        </is>
+      </c>
+      <c r="D989" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6c%2fpeOyA8HkDsw%2fomaDAqInVGsOp2kx3dNVGf1dmT5Imz0Fdz%2ftwAuN7j7o2tWIKUnKqlPOfY17h21UYd90B0H4MxuyvujcfV7MeWwBnG4CW64rDrVwqGTG7Y1MK%2f8K%2bxZiyNSbBSP27pWgqIrij7HkedGrKTsOaY4eWb23eqnofZZwfzTQENw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E989" t="inlineStr">
+        <is>
+          <t>02065207731</t>
+        </is>
+      </c>
+      <c r="F989" t="inlineStr">
+        <is>
+          <t>Yerwada</t>
+        </is>
+      </c>
+      <c r="G989" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H989" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I989" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J989" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" s="1" t="inlineStr">
+        <is>
+          <t>A52100018048</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Swapnil Annarao Ade</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>A52100018048</t>
+        </is>
+      </c>
+      <c r="D990" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=lLSikfj0koqzAc8uYHylYpUqZaUzENq7z1XWZ3W8Dwxp84z4kPixNwrgoo7LXbMlKu5dUXyWCWQe4hPWk1Wc8evZogp35JqjAQcC6s5H5k6uaxmEJ9bSmnYNZCBfU6RY%2fUKuqRKB1WsFLr43PNd2d27VXwWJWM79xJv24h4EsMIKzm%2fvEbZLig%3d%3d</t>
+        </is>
+      </c>
+      <c r="E990" t="inlineStr">
+        <is>
+          <t>09130124127</t>
+        </is>
+      </c>
+      <c r="F990" t="inlineStr">
+        <is>
+          <t>Bhugaon Daulat Petrol</t>
+        </is>
+      </c>
+      <c r="G990" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H990" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I990" t="inlineStr">
+        <is>
+          <t>Bhugaon</t>
+        </is>
+      </c>
+      <c r="J990" t="inlineStr">
+        <is>
+          <t>412115</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" s="1" t="inlineStr">
+        <is>
+          <t>A52100017946</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Mahendra Kachru Ovhal</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>A52100017946</t>
+        </is>
+      </c>
+      <c r="D991" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=AGJUjamAYfFgGSVErMsxa%2fIZeB13PY6QSOKwnNDavt7OUTWI5%2bWWCvhg9bG7SI9V0rqA8IvNgfAfCjup7Cx4CX0c3MrVoGuS%2b1wkkLzEoEaInwj%2bLiknyyHS5e8SrfJ3DmpIoi9U%2bFuGGgOvLEO8LfNY%2fU1bAsuV7K0P7m25BFeUWc3dqlee2Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E991" t="inlineStr">
+        <is>
+          <t>02046704868</t>
+        </is>
+      </c>
+      <c r="F991" t="inlineStr">
+        <is>
+          <t>Kamshet</t>
+        </is>
+      </c>
+      <c r="G991" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H991" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I991" t="inlineStr">
+        <is>
+          <t>Kamshet</t>
+        </is>
+      </c>
+      <c r="J991" t="inlineStr">
+        <is>
+          <t>410405</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" s="1" t="inlineStr">
+        <is>
+          <t>A52100018324</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Priyanka Chalu Ghugare</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>A52100018324</t>
+        </is>
+      </c>
+      <c r="D992" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Xh4h9nBc3k649UPswsitLOfsGeIJsDGaELN2EaqLpGDuFxT3VF1sfDrmTteszklHuMlFarA4sYyqhGeaUPEQNzFbVDq43reGd0%2bhSytLz2njpGqaMa5H%2bsMfBSqb%2fFuMSnrs0p5VDoBY7Ly%2bhAKLLxHcc2KyBr2Rrlov80HvmAqM8zDvzHPHPQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E992" t="inlineStr">
+        <is>
+          <t>08329970063</t>
+        </is>
+      </c>
+      <c r="F992" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="G992" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H992" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I992" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="J992" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" s="1" t="inlineStr">
+        <is>
+          <t>A52100017947</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Veeru Vedprakash Ohri</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>A52100017947</t>
+        </is>
+      </c>
+      <c r="D993" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=JP%2fwxwqAhq%2fMxfWXKa9UyiO6pf3QGlhE5Zd5QvrIzW7S8U5UytUYjG1IPzfvJpjVitV5FxdWCcoAOu%2bltcOxkD%2bdfy9o%2fvMKqsfSk6JSwAsp4jQfynkrqcJFfluBEa0bH1RjuqWYqM01QQUT0A5Zzh3ByRxEU6eLmPawr0e43hVmnlBR9EDnfQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E993" t="inlineStr">
+        <is>
+          <t>02068888903</t>
+        </is>
+      </c>
+      <c r="F993" t="inlineStr">
+        <is>
+          <t>Phursungi</t>
+        </is>
+      </c>
+      <c r="G993" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H993" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I993" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J993" t="inlineStr">
+        <is>
+          <t>412308</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" s="1" t="inlineStr">
+        <is>
+          <t>A52100001699</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Varun Devendra Mathurawala</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>A52100001699</t>
+        </is>
+      </c>
+      <c r="D994" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=cL%2b9x8L6cWRkEYzttb9yeDpAgGnGU7469YyGHZMNM5vcm4m8dTPWkwdF2zfO7GsUa8giUUU4F8dEtP4GOT5KV8Oysqyg%2ba9n5ypHn2cI%2fkSlXs2AHBYUJBuhjTTl1oIlo%2flyzWzHwUjA7vmNsFPS8zGI1Mx%2bd25XhawgrLtJeZQ%3d</t>
+        </is>
+      </c>
+      <c r="E994" t="inlineStr">
+        <is>
+          <t>02026346465</t>
+        </is>
+      </c>
+      <c r="F994" t="inlineStr">
+        <is>
+          <t>Wanowarie</t>
+        </is>
+      </c>
+      <c r="G994" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H994" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I994" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J994" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" s="1" t="inlineStr">
+        <is>
+          <t>A52100017989</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Eagleinfra Solutions Private Limited</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>A52100017989</t>
+        </is>
+      </c>
+      <c r="D995" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3NVHecEgsB8cqDis4a%2f8mtUIEpifQ7HRPAifmyKn0PwIy%2f2Cz66z%2fX4UzM6%2ffOa2ZtUnalqL6CBdWzyFeZvxE1ZOAfFUl5BXJqggITJ2TK1tVy8%2fGUXwNGMKpMoar4n1L7eeC2mpdY4N53Ub8iPwBG26i%2fblxgx5fZk3B%2bjnn5ND9NIYglS%2b3w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E995" t="inlineStr">
+        <is>
+          <t>02024486903</t>
+        </is>
+      </c>
+      <c r="F995" t="inlineStr">
+        <is>
+          <t>Spine Road,</t>
+        </is>
+      </c>
+      <c r="G995" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H995" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I995" t="inlineStr">
+        <is>
+          <t>Bhosari</t>
+        </is>
+      </c>
+      <c r="J995" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" s="1" t="inlineStr">
+        <is>
+          <t>A52100017940</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Azharuddin Niyazuddin Shaikh</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>A52100017940</t>
+        </is>
+      </c>
+      <c r="D996" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LxRPSy5UumZCLcrKhCbH7j5%2fsQQe6MAILtEcNfgjvCqs3%2bnQw1n6loFGVmwmNMNjI%2bj75nRnZpwHmkBWalqXWl5UQx8ZCcjE0is8YWm%2floS%2bsUSsc6ED8ygNO7xM4j5l7GL3Z%2fBRetYBBLata2oDJNgrSXnaASVbJL9VeSVsXn0hCFA29KcztQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E996" t="inlineStr">
+        <is>
+          <t>09850399993</t>
+        </is>
+      </c>
+      <c r="F996" t="inlineStr">
+        <is>
+          <t>Kondhwa Khurd</t>
+        </is>
+      </c>
+      <c r="G996" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H996" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I996" t="inlineStr">
+        <is>
+          <t>Kondhwa Khurd</t>
+        </is>
+      </c>
+      <c r="J996" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" s="1" t="inlineStr">
+        <is>
+          <t>A52100018012</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Deepak Vinodkumar Shah</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>A52100018012</t>
+        </is>
+      </c>
+      <c r="D997" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=SyQW3Yi4cGVMtkZYn1jxL6OJ13tSNKuiiHzcwkJBmhsePzJu9p37JJ79SyD9OzA317J9gUAww7y%2fCKNP3C1urKc3A7izaxXyjSRTraVyWWCfiq%2f7zH5uwwDp41yI0aP2gyuIMgzodf2mJvrVnMtaLLCiOpf15HuLrRf7kYJC8bK9CB44V8IUJA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E997" t="inlineStr">
+        <is>
+          <t>02114022615</t>
+        </is>
+      </c>
+      <c r="F997" t="inlineStr">
+        <is>
+          <t>Near Atom Plast</t>
+        </is>
+      </c>
+      <c r="G997" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H997" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I997" t="inlineStr">
+        <is>
+          <t>Talegaon Dabhade (R)</t>
+        </is>
+      </c>
+      <c r="J997" t="inlineStr">
+        <is>
+          <t>410506</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" s="1" t="inlineStr">
+        <is>
+          <t>A52100017951</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Vijay Balram Jodhwani</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>A52100017951</t>
+        </is>
+      </c>
+      <c r="D998" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2b1xVMqK6fhYEM%2b1Z4AMrPpwy5j1KMaWwEEZK%2b1vuBVVgNsb7yZhNPAg67fpdFkwSF%2br5tVfwp1llKovkwzLzCVIjp45jBVl1BNcVX%2f67f3ITCIkdORUd7EoMdyUuZRA0I8xN%2bCI7Clp3eNAAYWbATYhXEQCdVoRBG8nS4LjCqLZf%2foD3IQQe0Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E998" t="inlineStr">
+        <is>
+          <t>02024465837</t>
+        </is>
+      </c>
+      <c r="F998" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="G998" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H998" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I998" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J998" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" s="1" t="inlineStr">
+        <is>
+          <t>A52100019372</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Mansoor Saifuddin Talib</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>A52100019372</t>
+        </is>
+      </c>
+      <c r="D999" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=uaidPOdgao0lIO79VCNK%2frrHC19PQjX7ZFO%2fM1LEJISyT22f4nuNT14w6aMVcnRlXNi9D7s8VlOE1qHGKFsxcvV5JtfKnfa%2bUNl6KuULKfGbb5XlrAtlQQ8Vi%2br9s84OkmPbvkUfmwzKCL2utvhZg6BpdtGmHEX5qQvyOO9dvcREKFwMCeavOw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E999" t="inlineStr">
+        <is>
+          <t>02026343177</t>
+        </is>
+      </c>
+      <c r="F999" t="inlineStr">
+        <is>
+          <t>Market Yard</t>
+        </is>
+      </c>
+      <c r="G999" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H999" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I999" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J999" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="1" t="inlineStr">
+        <is>
+          <t>A52100017965</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Anil Vasantrao Tingre</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>A52100017965</t>
+        </is>
+      </c>
+      <c r="D1000" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=SgJeXLtkHWJEw4nki0012RvMTWBNkmX0Y4NMvssuASBngQG2YkjJRl4AvI7LfyiVLbcMJG9qEGdqCWN4d1y1Mi8bxyPfAtTpQz3jeLw0NkmoT0g7NKSaBTu1xHVzOkmCSETYYNKqoYhYboRM5DsTCTi3WVbADDNx64OJBIkdoo7IB2z0r2IThg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1000" t="inlineStr">
+        <is>
+          <t>02041241818</t>
+        </is>
+      </c>
+      <c r="F1000" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="G1000" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1000" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1000" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J1000" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="1" t="inlineStr">
+        <is>
+          <t>A52100018041</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Nitin Jagannath Tamboli</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>A52100018041</t>
+        </is>
+      </c>
+      <c r="D1001" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=GGRYvewRZasftnrt8WKJpterevMAxyQxnBE3ZKRaAgvgG412LC2xCaQHe7y2XKqo6T%2bVXEaHoDlWSXHwmsyQTfbP6jlRjqjz56Pra%2fnEq6BcUP1pGJpHC692slEE%2f%2ffyOjbWL9XPZrKmv6NU%2bOkpgLB%2bSHVBtTqmGwTc3lQ%2fzaAY0c3XP5atmw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1001" t="inlineStr">
+        <is>
+          <t>09822111390</t>
+        </is>
+      </c>
+      <c r="F1001" t="inlineStr">
+        <is>
+          <t>Sant Eknath Nagar</t>
+        </is>
+      </c>
+      <c r="G1001" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1001" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1001" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1001" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1050]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1001"/>
+  <dimension ref="A1:J1051"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51968,6 +51968,2606 @@
         </is>
       </c>
     </row>
+    <row r="1002">
+      <c r="A1002" s="1" t="inlineStr">
+        <is>
+          <t>A52100018086</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Trupti Jayasing Salunke</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>A52100018086</t>
+        </is>
+      </c>
+      <c r="D1002" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=0MJY%2fX%2bRUCfuy21TNN5XdVh1pw6UY5TNBKxopt%2f9q7BOLWk8jIsVsy4RAnaD9KJE8%2fNzQxVxb9COQXCYUESqc5PjXXCbu4LQF09L5naaNcala%2bEnKazZH5VE9pSGMp6nJLUIRwi6%2ber0xIlLsfJvbIS17OAateMq6oWcNDE3U5%2fIDLnY%2bBbq%2bA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1002" t="inlineStr">
+        <is>
+          <t>02000000000</t>
+        </is>
+      </c>
+      <c r="F1002" t="inlineStr">
+        <is>
+          <t>Vidhya Nagar</t>
+        </is>
+      </c>
+      <c r="G1002" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1002" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1002" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1002" t="inlineStr">
+        <is>
+          <t>411032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="1" t="inlineStr">
+        <is>
+          <t>A52100017976</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Pratik Arjun Tamhane</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>A52100017976</t>
+        </is>
+      </c>
+      <c r="D1003" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Fin97ZuJTO6v7xu6zSWtmzGVEKaQgTCPiFPhrMS%2b4k02roMgE1REVzsHfAyXNrOL7ELh2y38rciejN7CFwjKp7%2b5zf8dJwZcIaEyTNXzQzslzMYfQtjUX1gKW%2fa6L0PqHGjsKoJhtMj1vjBVXEDGnRDdnRPmo7QAUK9ALB3%2fb8c9bGrhPOixFg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1003" t="inlineStr">
+        <is>
+          <t>09923502020</t>
+        </is>
+      </c>
+      <c r="F1003" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1003" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1003" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1003" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1003" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="1" t="inlineStr">
+        <is>
+          <t>A52100018013</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Sharangdhar Padmakar Kulkarni</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>A52100018013</t>
+        </is>
+      </c>
+      <c r="D1004" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Xj0Tarp%2fno8Gj%2fOJNb0njP3s1nUIASa29%2bbIWTgCwazhkb%2f0geG4SINOnB3DQWi6FEZ2wjYv8yvGZH6Q0d7Gz13HRsSQBQhKczJAYCtWD3jb9GjNXDBhTD%2fAWWRPbXdT6qSCdyQ6PUR2XxNVcMMVTU5wZRPW3U8JU2KI7nERp2rpcHgSd6DtIA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1004" t="inlineStr">
+        <is>
+          <t>09822098921</t>
+        </is>
+      </c>
+      <c r="F1004" t="inlineStr">
+        <is>
+          <t>Erandvana</t>
+        </is>
+      </c>
+      <c r="G1004" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1004" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1004" t="inlineStr">
+        <is>
+          <t>Peth</t>
+        </is>
+      </c>
+      <c r="J1004" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="1" t="inlineStr">
+        <is>
+          <t>A52100003370</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Piyush  Agarwal Huf</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>A52100003370</t>
+        </is>
+      </c>
+      <c r="D1005" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wufki9DWJ5Pi8U3%2fZNFgIlCgBD43fiNbR0LHl1o3UvRaUfMY335zCJiDk5EnCrjwlvaB1Zpj3%2fjUfIukzHmERZHbAc0SYUl0wlJ7WaNK2BNkm4fA8HjmTw48o%2bA2N%2b%2fjN8MmHQVDZ20IIwFPe4gJ79cXry4qitLs0jqT09swDlPFmKyDjirFoA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1005" t="inlineStr">
+        <is>
+          <t>08600030244</t>
+        </is>
+      </c>
+      <c r="F1005" t="inlineStr">
+        <is>
+          <t>Hinjewadi Phase3</t>
+        </is>
+      </c>
+      <c r="G1005" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1005" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1005" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="J1005" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="1" t="inlineStr">
+        <is>
+          <t>A52100003454</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Dharmendra Kumar Shahi</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>A52100003454</t>
+        </is>
+      </c>
+      <c r="D1006" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=zUqFRs4QF4EA%2b1niXAsOJjdn9NPDvtZJTLrpCtdjaILgUhgN0iC3Gu%2bDEo%2bHjVvxLuh%2b9KDK1RQ8u4WqvE4FnIJb9G%2fzqdosAjEA1DBwIMSWtFKLnogtt6mmDn%2bBlc9tz2ZYD0sNmFjisASZ9fojWQUBmHwMkGs3qSKMoE6vlPlPzzkPt%2fQAtQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1006" t="inlineStr">
+        <is>
+          <t>07775083355</t>
+        </is>
+      </c>
+      <c r="F1006" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1006" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1006" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1006" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1006" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="1" t="inlineStr">
+        <is>
+          <t>A52100018154</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Kishan  Singh</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>A52100018154</t>
+        </is>
+      </c>
+      <c r="D1007" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=n9p1WtpH05ET3MxEDdHtLKNCvW%2bCd6FpVerUeA8bOb7jRiJgBbYfBxYvLLtnyn61Qkgq3a%2fAXEnfCY0BOua2TtlkOUXNZhsBn8oKVTdw89xiom0M7Rog1shyiCJXyvi6PSgXBoLXhQvL7RAZTAZ5WM2SBcxJ1nFgNJCg8sGvT6CbXctjeSUMvw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1007" t="inlineStr">
+        <is>
+          <t>07892450518</t>
+        </is>
+      </c>
+      <c r="F1007" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1007" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1007" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1007" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1007" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" s="1" t="inlineStr">
+        <is>
+          <t>A52100017973</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Wasim Najir Attar Proprietor Of Pearl Properties</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>A52100017973</t>
+        </is>
+      </c>
+      <c r="D1008" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=BQLUgbRgAgYBzGnQaB5mEi6r6KzfDwnUYVDxG9lzW25BoQ5MXyn9NC9hnoh50u2yhW9NImkLpLn0%2b9P0so5KlVmCpvkWMURiH8CX8cO6yCQ6pV2Rl9AzuN69XQXctkIk6IPKGUfxseb6xzBtG7kgfMhTzwFDNhnIh%2brxrGnh2%2bTbaH2Qvz1DXw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1008" t="inlineStr">
+        <is>
+          <t>07447642293</t>
+        </is>
+      </c>
+      <c r="F1008" t="inlineStr">
+        <is>
+          <t>Parvati</t>
+        </is>
+      </c>
+      <c r="G1008" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1008" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1008" t="inlineStr">
+        <is>
+          <t>Parvati</t>
+        </is>
+      </c>
+      <c r="J1008" t="inlineStr">
+        <is>
+          <t>411009</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" s="1" t="inlineStr">
+        <is>
+          <t>A52100018010</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Kegrock Realtors Private Limited</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>A52100018010</t>
+        </is>
+      </c>
+      <c r="D1009" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xHmTCDCXyIM6S3Q2nWfPOhCs00cw6zyZhzWicPCK9MrXz%2bIzRhl4%2f0iIX6786d%2bkWWzv0FM2aeGP4HyhcE6q82qGNKNEKHx91kfws6xzMkZ97z0Dtr2xCLDmlM3wiezzIxfQbdQhwF6SFbRhdpBpbdqCrxXw2zbsEBoV9SmUa1h10XAT31iGTw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1009" t="inlineStr">
+        <is>
+          <t>09156803935</t>
+        </is>
+      </c>
+      <c r="F1009" t="inlineStr">
+        <is>
+          <t>D.P Road</t>
+        </is>
+      </c>
+      <c r="G1009" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1009" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1009" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1009" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="1" t="inlineStr">
+        <is>
+          <t>A52100018031</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Global9 House Hunt Llp</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>A52100018031</t>
+        </is>
+      </c>
+      <c r="D1010" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=qI4N41EVpZD4MZqvywcKrNpaEnkK7alxNvIk7sMZeSwBIgCEiVamLS2w6cYeqV%2fuEe2HXWzFiQYyKlDsaRGJb1BsNnTFOKL4UcCupsfG4P3W1zK%2fFGHNIis%2fJrO9JpJJKggNvL%2b8YbcGjoNJXH%2fIb9Cr2op1v1G0qZZKE1rLaZTc0swdzTKtUQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1010" t="inlineStr">
+        <is>
+          <t>02026890634</t>
+        </is>
+      </c>
+      <c r="F1010" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1010" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1010" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1010" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1010" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" s="1" t="inlineStr">
+        <is>
+          <t>A52100018096</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Santosh Datta Kale</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>A52100018096</t>
+        </is>
+      </c>
+      <c r="D1011" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=d1%2b33gZISTGvtQX1g2DEvS5FMNB6WlZXUIOK57HUu15jnJ84xTQoenndiX9vRX3JXDPHrflhC7NfIHJo1yVDYAFjl6JHtmRV63SOLYxUuoav%2bV%2frazw%2bBg3r2ZpkPA6UJlpTSend6i9t%2bPIBMdiA44X2t006JoHKWX5wUWdCk9nnVbFGrORY4g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1011" t="inlineStr">
+        <is>
+          <t>08888493049</t>
+        </is>
+      </c>
+      <c r="F1011" t="inlineStr">
+        <is>
+          <t>Hadpsar</t>
+        </is>
+      </c>
+      <c r="G1011" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1011" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1011" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1011" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" s="1" t="inlineStr">
+        <is>
+          <t>A52100018023</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Ravindra M Pawar</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>A52100018023</t>
+        </is>
+      </c>
+      <c r="D1012" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=h9o5St8RDGUd7dRLN4vhGSpWPXuyJw1miAhgVJdeHbt64iP5cqOffy5gIBzQxE%2fVHw7hdyDRWCeZEmlTcBCoD%2bkFFsiwY5nUEZJzw1Y9quBPVau6n25eYafLdob6dw%2fV3KBpzRhrr2upWtzSfd71%2bE55rB9jszNF7YZzRpoKzipNHbsIp9jKsg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1012" t="inlineStr">
+        <is>
+          <t>08668531557</t>
+        </is>
+      </c>
+      <c r="F1012" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="G1012" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1012" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1012" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="J1012" t="inlineStr">
+        <is>
+          <t>411043</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="1" t="inlineStr">
+        <is>
+          <t>A52100018163</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Pravinkumar Namdeorao Shinde Proprietor Of Property Consultants World</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>A52100018163</t>
+        </is>
+      </c>
+      <c r="D1013" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=aGyo%2bmqrlMYHqkOgZ%2b8dCcImgLvnt2qmMgssOKpiwlWlC3sfl1sFPSGUCsTwQ%2bZkJFuAk6HizojN7HHrswbwQDiGXpTiiXT52benGAYjvDZ7Lza4V3q5fxwjfTUFWdAAzsdRFR5o%2fF4O51ijC1hakkMwodBOnFvvEn2QyfdijSlugsvNY3OfzQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1013" t="inlineStr">
+        <is>
+          <t>09422012074</t>
+        </is>
+      </c>
+      <c r="F1013" t="inlineStr">
+        <is>
+          <t>Bhosari</t>
+        </is>
+      </c>
+      <c r="G1013" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1013" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1013" t="inlineStr">
+        <is>
+          <t>Bhosari</t>
+        </is>
+      </c>
+      <c r="J1013" t="inlineStr">
+        <is>
+          <t>411026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="1" t="inlineStr">
+        <is>
+          <t>A52100018003</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Prashant Vasantrao Kalbhor</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>A52100018003</t>
+        </is>
+      </c>
+      <c r="D1014" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=BNksqVJzZGqDHCXrqBzlNky6s%2fOOX1NyQtmzAelo43Bep0x5jmns%2b3XIltd9ZzVNneS3XxIh2323q9NDuShRZJZpNRBAfUPft3wnicxdjdJEn7V7Lonwcu98kPollb%2fbLKf%2fHlIsEIIYRQa2SIsGzDcGIlM7THyLf1W9p1sfGMvQ6uwjZKt%2bFw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1014" t="inlineStr">
+        <is>
+          <t>09011191122</t>
+        </is>
+      </c>
+      <c r="F1014" t="inlineStr">
+        <is>
+          <t>Kadamwak Wasti</t>
+        </is>
+      </c>
+      <c r="G1014" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1014" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1014" t="inlineStr">
+        <is>
+          <t>Kadamwak Wasti</t>
+        </is>
+      </c>
+      <c r="J1014" t="inlineStr">
+        <is>
+          <t>412201</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" s="1" t="inlineStr">
+        <is>
+          <t>A52100018001</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Navin  Motwani</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>A52100018001</t>
+        </is>
+      </c>
+      <c r="D1015" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=rS81tez%2bzU1lidWjewcrPyx0Cf7Oc4bZd8gggctYOenlgN%2fimOc6cWXi1Pllxhv2x8zzd5%2fFUXOlaVTwLVpkrBm2J%2bD0fDClBJWqeXJf%2biTK3UO4grwJfTd%2f31JlMDtLlO3XWY9q2wVVMWfr9hRAnR0xilZaAZQi%2fw2xoMncFaQZP8gFN%2box%2bw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1015" t="inlineStr">
+        <is>
+          <t>08369128126</t>
+        </is>
+      </c>
+      <c r="F1015" t="inlineStr">
+        <is>
+          <t>Malad West</t>
+        </is>
+      </c>
+      <c r="G1015" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1015" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1015" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1015" t="inlineStr">
+        <is>
+          <t>400064</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" s="1" t="inlineStr">
+        <is>
+          <t>A52100002245</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Sonal Siddharth Lodha</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>A52100002245</t>
+        </is>
+      </c>
+      <c r="D1016" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=L4LUjFSHQom%2baiq5kOuyjmoq6NDICo5Qiu13JKf189SJnzkHKjbZeE6VLpporwbLE73dEB4aKwB%2b0NbYcddmDLEPXXcfHPX%2fYqI41qt2LwzB7x88oHQpBuuDWZLUzzUhhVqUuceJNDl581%2bK%2bES8s9boQ5LrdrRjQyILa5hXJX4%3d</t>
+        </is>
+      </c>
+      <c r="E1016" t="inlineStr">
+        <is>
+          <t>02065110025</t>
+        </is>
+      </c>
+      <c r="F1016" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1016" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1016" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1016" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1016" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" s="1" t="inlineStr">
+        <is>
+          <t>A52100018165</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Prashant Pawan Singhaniya</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>A52100018165</t>
+        </is>
+      </c>
+      <c r="D1017" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CIXKX2yO0C%2fIwlO2lXJhxBS3J5Ur54h0G7myv%2b9m9piRG4xIry620rNWPJYiEmpuk3H%2bYXLTc8Ymme0lT%2f%2bWsRTP3Zqr9GzVGt8OxKVsKRCCgErH7ez9Rc87RYA6wHsGpA5y9BA%2biaQ3Mlt90AuyG5UECNUuXYvD%2bLhk4owC4ZL3nm0Q9E3JfQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1017" t="inlineStr">
+        <is>
+          <t>02024443447</t>
+        </is>
+      </c>
+      <c r="F1017" t="inlineStr">
+        <is>
+          <t>Narayan Peth</t>
+        </is>
+      </c>
+      <c r="G1017" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1017" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1017" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1017" t="inlineStr">
+        <is>
+          <t>411030</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" s="1" t="inlineStr">
+        <is>
+          <t>A52100018381</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Sibasish Ajit Bhattacharya</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>A52100018381</t>
+        </is>
+      </c>
+      <c r="D1018" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=zEy%2bx3Nnk9vkb0kfm8UANt9NUQM81mbcM9J7ZGNcxcpdnFaQB8TjvFYxCOyk45f3ejpWucWX5vtjIqnkq11wD%2b6Y0178FfILUvxefVbcZAP0Uf%2b6ei%2bfNTt4AJ6gwkz50MPp709QiuotSm1scsLySL51aVTOS0YDvXiENBPI9BwR6aN5TWK10g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1018" t="inlineStr">
+        <is>
+          <t>09665872530</t>
+        </is>
+      </c>
+      <c r="F1018" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar, Pune</t>
+        </is>
+      </c>
+      <c r="G1018" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1018" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1018" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1018" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" s="1" t="inlineStr">
+        <is>
+          <t>A52100022196</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Vibhavari Pravin Survase</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>A52100022196</t>
+        </is>
+      </c>
+      <c r="D1019" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1QP2nwVqUsF8xHyvmjS5uodZYUQDwnHugmy80HKOB8EIUYZ%2fMaGVLkSlgdAqK%2bkHFVkykCSAWGaql%2b0pcdAwz8S6AJmkI%2bVIWu8KDrfjCh8j5P33BdkP8BLaqwALKXFAtJNq6%2bDERPvmnFE80Kxa9%2fay30VMVsnesKjlE1%2b5BzkJxVqUPTFIkA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1019" t="inlineStr">
+        <is>
+          <t>02029700860</t>
+        </is>
+      </c>
+      <c r="F1019" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G1019" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1019" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1019" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1019" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" s="1" t="inlineStr">
+        <is>
+          <t>A52100019250</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Prashant Krishnarao Wankhade</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>A52100019250</t>
+        </is>
+      </c>
+      <c r="D1020" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=izY%2boibShUAg5a2iTb3AIksEg9P0z3nj8%2bqoam%2fzXFbnVxYKb10vRiLXdQUW%2bSNyDQq1UYn5FPj1AwfJXnnJ8ek9OsrdqQoshq5BHb%2fltyT6GXuoPqT2tQWJsKg35hv9F73rMHR9aMiRSZ7Bb4iXzCa7tHN4ugG%2bNdkXr1jaZ42SfubXdDtmXw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1020" t="inlineStr">
+        <is>
+          <t>02022222222</t>
+        </is>
+      </c>
+      <c r="F1020" t="inlineStr">
+        <is>
+          <t>Ghorpadigaon</t>
+        </is>
+      </c>
+      <c r="G1020" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1020" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1020" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1020" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" s="1" t="inlineStr">
+        <is>
+          <t>A52100018437</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Shyamkant Ravindra Kasar Proprietor Of Sk World Financial Services And Property</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>A52100018437</t>
+        </is>
+      </c>
+      <c r="D1021" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=YH241Mk1qv1g04zLUfdfKQKPCvSE19dfl7ScXkZvzC5ZzqSIEZrQs7A%2fGTazyIgBJUJOPTxtoA9yjVmrc4aKhLuGn7hXIt9UPeVpagcHtawMVOdRDq9ek3bc7y2Z32wsfcxETKlHbCU5KvBw3vhF8sxqBnUTpkPiN62rd2OCcaJUkgzyLvLgUQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1021" t="inlineStr">
+        <is>
+          <t>07020669232</t>
+        </is>
+      </c>
+      <c r="F1021" t="inlineStr">
+        <is>
+          <t>Hadapasar</t>
+        </is>
+      </c>
+      <c r="G1021" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1021" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1021" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1021" t="inlineStr">
+        <is>
+          <t>422008</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" s="1" t="inlineStr">
+        <is>
+          <t>A52100018027</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Vikas  Baravkar</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>A52100018027</t>
+        </is>
+      </c>
+      <c r="D1022" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=dwvJvLuREObB4qEMqrWzBD9aWnNiVHBITZa859nJE%2fzfC%2fc1Do9ukMIq38umkJJnorn56KetXZVt3o4KLYKCc5bzotZSWujWY4MEAuUkHUwKYiE7XKEMA7fPD1RN%2fi%2bBuxj5tyV4kEF7L5K%2fDkrteBP1p2xYCGpMmWQMKNEZrSsV5YdXj8Mfow%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1022" t="inlineStr">
+        <is>
+          <t>02083080658</t>
+        </is>
+      </c>
+      <c r="F1022" t="inlineStr">
+        <is>
+          <t>Phursungi</t>
+        </is>
+      </c>
+      <c r="G1022" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1022" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1022" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1022" t="inlineStr">
+        <is>
+          <t>412308</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" s="1" t="inlineStr">
+        <is>
+          <t>A52100018287</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Sanjoy  Das</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>A52100018287</t>
+        </is>
+      </c>
+      <c r="D1023" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ppjQ9af5B6amMeDB13Kcxh%2b5iK%2bztktjGyEEq%2fRPUA09%2bRGRoj19qlMRRbZNzQ7L2Sesw1qAW409WTcNtQMaz%2femcofyOfIL95FnvytuDk6PvmDxP6JD0dXqmHiYy%2bgmqXSmFkq2QjyWzuvS5peI2PXw2qga6nkqLlSUs5FjYGOKj0br22R%2bxA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1023" t="inlineStr">
+        <is>
+          <t>09158738942</t>
+        </is>
+      </c>
+      <c r="F1023" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G1023" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1023" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1023" t="inlineStr">
+        <is>
+          <t>Kondhwa Khurd</t>
+        </is>
+      </c>
+      <c r="J1023" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" s="1" t="inlineStr">
+        <is>
+          <t>A52100018236</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Sunil Prabhakar Desai Proprietor Of Prime Spot</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>A52100018236</t>
+        </is>
+      </c>
+      <c r="D1024" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5baOW4PfwxHRZKhkXoTJXOKHoFkgEiFTZ7%2bXuNn0TpbajGHI7wcJkqibRGguYI8fSPugwwYD3O9f78MuvwU%2f6I%2bjro2ib9CYTEVWxe3BDO75unKKJLsgKZc5TJJQOh5r4nkpT%2bGbOR3GlZCF5xqSl3lW7uSFFquZusEax4XGZ4TmkDGEm%2ffVKA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1024" t="inlineStr">
+        <is>
+          <t>09890336417</t>
+        </is>
+      </c>
+      <c r="F1024" t="inlineStr">
+        <is>
+          <t>Pune University Circle</t>
+        </is>
+      </c>
+      <c r="G1024" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1024" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1024" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1024" t="inlineStr">
+        <is>
+          <t>411016</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" s="1" t="inlineStr">
+        <is>
+          <t>A52100018028</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Sandhya Vinod Katariya</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>A52100018028</t>
+        </is>
+      </c>
+      <c r="D1025" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=aFT7c7D6fJh6yk9KkN8MsPV%2bpKPYoupxlQ8PMzb733KJH0JnP9qv9%2fqiX88%2fTYmWAmny9yh7fDDy034bV8u%2fdChGXYDId8KXnr0SkFjEieuB2QMjfjI8DNrXCQbYpk1YEpiT7qwLHbr4Sn0D6MjTHvnGmPb5o5Nrnq7sSWDKI4nYxjh7bRle9w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1025" t="inlineStr">
+        <is>
+          <t>99404709900</t>
+        </is>
+      </c>
+      <c r="F1025" t="inlineStr">
+        <is>
+          <t>Market Yard Bibvewadi Pune</t>
+        </is>
+      </c>
+      <c r="G1025" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1025" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1025" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1025" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" s="1" t="inlineStr">
+        <is>
+          <t>A52100020855</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Mayur Shrikant Malwadkar</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>A52100020855</t>
+        </is>
+      </c>
+      <c r="D1026" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LzAg9OKKElOu%2fUTpfhN1YBbY3azMuroVxRPeU2waCKNr8eleMQmnFRCp4j%2faMxbQzzpA1kVmZ5e6tiqKSIL3Ks%2fuwSOL4kYePEEmHoERe8%2bnJyFQodlOq%2fnp1f6U3wHvlOZPCmS51Zprr2cqhLARPQeTvEe5XS4OHjPo0xOw6fYTUwhyOzWd3A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1026" t="inlineStr">
+        <is>
+          <t>09822846744</t>
+        </is>
+      </c>
+      <c r="F1026" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="G1026" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1026" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1026" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1026" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" s="1" t="inlineStr">
+        <is>
+          <t>A52100018123</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Ashish  Bharti</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>A52100018123</t>
+        </is>
+      </c>
+      <c r="D1027" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CoBugnDP7xbvhuAZ1yzb1Ig02QH7nYiNSKzqXjOq4JRSGxWfXQR58QUn%2bZPc9jTxmj363O8m6%2baSdvieZtqRKb71SOXGpq7tvP6d8YRA875eF8sSTm8RaaBH1H6uHIzdqjdHVizsY%2bIbT2E425iisX4lDUgDlKWmJBCzxA0mHskw2GyvdjaeZw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1027" t="inlineStr">
+        <is>
+          <t>08697558480</t>
+        </is>
+      </c>
+      <c r="F1027" t="inlineStr">
+        <is>
+          <t>Walhekarwadi</t>
+        </is>
+      </c>
+      <c r="G1027" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1027" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1027" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1027" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" s="1" t="inlineStr">
+        <is>
+          <t>A52100024208</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Sanjay  Salvi</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>A52100024208</t>
+        </is>
+      </c>
+      <c r="D1028" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ZwsS%2bVd6WZUazbUdhiXUQchhxPciJOdBRH3%2bj1kgAU7AzmlHyOGdQvLWp4XJmD%2biONSgnWx59KBOUIXqFaQ6jouCXNL1MuoFj5m7RIjPB%2bZS3TfZfSMHICDoMMDpsxnA0UMeVUhywWYFLaPflfiM88YH2T3gW4DY5%2b%2bSFECGAD11JkaxWxifiA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1028" t="inlineStr">
+        <is>
+          <t>02026618079</t>
+        </is>
+      </c>
+      <c r="F1028" t="inlineStr">
+        <is>
+          <t>Kalyaninagar</t>
+        </is>
+      </c>
+      <c r="G1028" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1028" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1028" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1028" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" s="1" t="inlineStr">
+        <is>
+          <t>A52100018144</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Kailash S Gurav</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>A52100018144</t>
+        </is>
+      </c>
+      <c r="D1029" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=BbYyyS4gjMe3F6rQ4sdjXBUAvdwcZ1x9UWS9J66iTpAgMdd5qTZfuDw6GUfgcVDNOYgp%2b5IVJQ%2fDq0CAjzRwBrVy8R5r0i076b0OAsabORXUJn5YhLb5wjhZSQnTFfD0fHHL8sK0ly%2bDu0s46yBKvpDgg2TLfHv0xR3D5VTAvVeRHaIBtKQgxQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1029" t="inlineStr">
+        <is>
+          <t>09822571620</t>
+        </is>
+      </c>
+      <c r="F1029" t="inlineStr">
+        <is>
+          <t>Sus Gaon</t>
+        </is>
+      </c>
+      <c r="G1029" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1029" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1029" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1029" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" s="1" t="inlineStr">
+        <is>
+          <t>A52100018065</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Taher Hussain Kanchwala</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>A52100018065</t>
+        </is>
+      </c>
+      <c r="D1030" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hY6Stv7OsM0hPLcRvzuNgRsXbUXXxNQCnNr24TSiqUpO3XxVMg%2ff3kO45J1QIBxs2TqIkWFT9RZ9vxpW7evKS3JEl78hNSKib8qawQ%2fJesOis9c8vYY4%2fHfWYmZgc%2fKr6m4i8YxO1SRdEfNYA5IV6svPjIyyvxuq6C%2fhehmbu5ldUbeQLJwp3w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1030" t="inlineStr">
+        <is>
+          <t>09922321025</t>
+        </is>
+      </c>
+      <c r="F1030" t="inlineStr">
+        <is>
+          <t>Sanjay Park</t>
+        </is>
+      </c>
+      <c r="G1030" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1030" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1030" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1030" t="inlineStr">
+        <is>
+          <t>411032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" s="1" t="inlineStr">
+        <is>
+          <t>A52100018062</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Shilpa  Shankar</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>A52100018062</t>
+        </is>
+      </c>
+      <c r="D1031" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=qkhPNT4lTmfE2wBTttJtCUVGYQOu3WVDRhoasih79CJw80Gfhb%2bp0PdE%2bgviwcUV2jSrA23eGt08a9rIAcDKQ9wyMtAFUvAKeHXmaLWACkFi4MQHlKIXTL2dkt5X1RaHTaxeLjSbO1ZAeLL%2bqN481%2f6WS%2fthAJYM21aAOYsQnn%2bFEiG1bW3zfA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1031" t="inlineStr">
+        <is>
+          <t>09920922351</t>
+        </is>
+      </c>
+      <c r="F1031" t="inlineStr">
+        <is>
+          <t>Paud Road,Pirangut</t>
+        </is>
+      </c>
+      <c r="G1031" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1031" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1031" t="inlineStr">
+        <is>
+          <t>Mulshi Kh.</t>
+        </is>
+      </c>
+      <c r="J1031" t="inlineStr">
+        <is>
+          <t>412115</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" s="1" t="inlineStr">
+        <is>
+          <t>A52100018057</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Rahul Chintaman Joshi</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>A52100018057</t>
+        </is>
+      </c>
+      <c r="D1032" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=U9jOaVfSLVMQ%2b9wpXir43NIM4Jkvwk4BHdD9AAnxZsY2rDIEmKZ6MNbi6nyCqAH%2b1jM4k8tVUDlC3N2nw%2bWRetPDMLUKd7brJbOmnXBFljC%2bOCHFALj23OlC%2bn7R2daF2GKeSR0YSE1JkX2rmm3BsSLhydi4kZohd0pconpleQJPzdX3XEOUlQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1032" t="inlineStr">
+        <is>
+          <t>02027515575</t>
+        </is>
+      </c>
+      <c r="F1032" t="inlineStr">
+        <is>
+          <t>Bibavewadi</t>
+        </is>
+      </c>
+      <c r="G1032" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1032" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1032" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1032" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" s="1" t="inlineStr">
+        <is>
+          <t>A52100018095</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Narendra Jairamdas Mansharamani</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>A52100018095</t>
+        </is>
+      </c>
+      <c r="D1033" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=EENyutZkH7QnFj0tH2gN6IAYmW29ifHNhY%2bJpVajzuHsWAjvKqcr0ZScTjE9ioGgkWb8bEMC3nvm7k517rCn9Q3In9s5GIXIlqDR%2fX%2fdVHyDVumDniOAbKI0r4N2tQv1adyNVruucdzIU6u6zQcfEcnHQiwqOwYsfy2%2fvFVAXoIhdmEsWpVHhA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1033" t="inlineStr">
+        <is>
+          <t>02048618624</t>
+        </is>
+      </c>
+      <c r="F1033" t="inlineStr">
+        <is>
+          <t>Wadgaon Sheri</t>
+        </is>
+      </c>
+      <c r="G1033" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1033" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1033" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1033" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" s="1" t="inlineStr">
+        <is>
+          <t>A52100018220</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Ratnadeep Cosmos Guldevkar</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>A52100018220</t>
+        </is>
+      </c>
+      <c r="D1034" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=8LmFtfYwNGZJtsRI2gqOY3%2fFbtU0t6zB3yLpnVni9szaG6ba2wICMiVE96NWfTBbnurbb%2fY4YtaeDyfgiiwL9JFztaKQiMdSB5LC0p0giAr68ZrcIvpNd6UOuue1goRlD0XONDjde1nz6SlRuWs8dpNm%2bGfcOvwdpLmGJaQVIXmOMT7O%2fAC7KA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1034" t="inlineStr">
+        <is>
+          <t>02026687800</t>
+        </is>
+      </c>
+      <c r="F1034" t="inlineStr">
+        <is>
+          <t>Wadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G1034" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1034" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1034" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1034" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" s="1" t="inlineStr">
+        <is>
+          <t>A52100018239</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Mangesh Ekanath Bhosale</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>A52100018239</t>
+        </is>
+      </c>
+      <c r="D1035" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=szzoJqs2ZdznsxrWhxVQGlxpgzQ3hazbTnyfNq8czZFImQribNfW2F2lrUCBY6VbbPtEmPIJYlLG2UjvZHHCq5my1dqeZkYUXdnz31aJadUVH84Vp0sXUZG4YMDWrDO19cCG3%2bQQgAsgNQQuCoAcRdq%2fq7xhpsK2fs6eOTCq9osNi6xAUGv2Zg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1035" t="inlineStr">
+        <is>
+          <t>02026140913</t>
+        </is>
+      </c>
+      <c r="F1035" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1035" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1035" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1035" t="inlineStr">
+        <is>
+          <t>Charholi</t>
+        </is>
+      </c>
+      <c r="J1035" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" s="1" t="inlineStr">
+        <is>
+          <t>A52100018149</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Ganesh Manik Tapkir</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>A52100018149</t>
+        </is>
+      </c>
+      <c r="D1036" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KLzoHeICQjqGGeDZPbPHfIK7Gp65t%2fwWbv2oi9wwVAVYEm3Z9TNaLzZ3%2fBqeu13VR6M94JJ63sIm8gLakGEdzC3HjOcN4Lb0BtASG6qYCGlF7mzG22C5zS5sN5AaljyHKaOXIivYoxWsb8GLmBJL%2bDCMirTkZOZ%2fEC%2bkxGQ94375rP%2bsPCBQWA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1036" t="inlineStr">
+        <is>
+          <t>02026140913</t>
+        </is>
+      </c>
+      <c r="F1036" t="inlineStr">
+        <is>
+          <t>Alandi Devachi</t>
+        </is>
+      </c>
+      <c r="G1036" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1036" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1036" t="inlineStr">
+        <is>
+          <t>Aalandi</t>
+        </is>
+      </c>
+      <c r="J1036" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" s="1" t="inlineStr">
+        <is>
+          <t>A52100018098</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Balram Laxman Purohit</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>A52100018098</t>
+        </is>
+      </c>
+      <c r="D1037" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=rIMDZB1zWdcc8e5ig3%2bFA0VlzTDG0xpIatwkWNlTRzfnSRh3i369wDMXCxGYUnQHbEeGdqa14DHrI3NWfwLzgsCawK8gpDMIE0jsladIFXfv%2b4vyTki9lnpKpIhX5CeKwkU6S7GsAouRWypAR0URmOvD9pbjEonqgOnmii09eM%2fqieYYa8OXEA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1037" t="inlineStr">
+        <is>
+          <t>02025281687</t>
+        </is>
+      </c>
+      <c r="F1037" t="inlineStr">
+        <is>
+          <t>Bhusari Colony, Kothrud</t>
+        </is>
+      </c>
+      <c r="G1037" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1037" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1037" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1037" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" s="1" t="inlineStr">
+        <is>
+          <t>A52100018359</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Prashant Kumar Singh Huf</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>A52100018359</t>
+        </is>
+      </c>
+      <c r="D1038" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=T%2bV%2bjac8XIwSApIfnqvXbGwE1BDXg%2fZ%2bq82xSJIE6eh9mcPEQhpj37SMGLsJ8q5NE8LOM4s%2f313muD37uX9SvxjGiXsEZYb8jktcsqKu2Tlgt0VEXF3Kh4jdD8XZu2FSvHfn3EIE4EtitbLhzmv2%2fiKqVB%2fotxvfh7Fc32VyX2Zfo3B9DUmJmg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1038" t="inlineStr">
+        <is>
+          <t>07299005395</t>
+        </is>
+      </c>
+      <c r="F1038" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1038" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1038" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1038" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1038" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" s="1" t="inlineStr">
+        <is>
+          <t>A52100018131</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Priyanka Chandrakant Jawalkar</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>A52100018131</t>
+        </is>
+      </c>
+      <c r="D1039" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=C5H2VMxQTVfaJVELavqYcmdbuyqiV8ewRD4eAyqe3NNZH0e4wmQZ4zeqtO4uRTqCWAmjNKkmGfF35QKp7dZAuUmdJGW3au7mKnDUM%2fUTuN8Dltpq%2bgbyzpHWuWbXAVGClpeqO2m0VD8qjW%2bHUaGMEOSxQ8BWoYoM4vgDsMmGSES9AwCIQbrzIw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1039" t="inlineStr">
+        <is>
+          <t>02024272427</t>
+        </is>
+      </c>
+      <c r="F1039" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1039" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1039" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1039" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1039" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" s="1" t="inlineStr">
+        <is>
+          <t>A52100018125</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Pankaj Somnath Thorat</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>A52100018125</t>
+        </is>
+      </c>
+      <c r="D1040" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=n%2fDvYnRSJYFQd8TVN1%2b0lLNbrNJIn4G2WLVx79HfrXtHMGsns1PepUy7BOZtOgUqKhk%2fZfG6FTDMF4QgqVJPY11uXWzGdisALWQUhtsXwyHPWcDw%2bgAPdGgM9bsHSaHRMnYYTAzroZWJWHgBKCONNrmZsxXxICbhBR5fe%2bRO90Ty0ggKuLNHzQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1040" t="inlineStr">
+        <is>
+          <t>02027350195</t>
+        </is>
+      </c>
+      <c r="F1040" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="G1040" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1040" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1040" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1040" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" s="1" t="inlineStr">
+        <is>
+          <t>A52100018186</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Kapil Bipin Pathak</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>A52100018186</t>
+        </is>
+      </c>
+      <c r="D1041" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=rLX6ubgFnlr1j2bwRFghlXozijODv0BOrc6zQq%2btKE1bsFyKbUtAiy4m41cUuE896aWTAhP3USfD1ZnXPi0zDozT7nkjKUqI%2fvNukalxULMmjkk6kZYdJeKVvc8OiTd%2fQNoXE%2bRcifmE2sbstRKEg6fEaCM2LBEewJWX1tkHgP9cOizXiMzvHA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1041" t="inlineStr">
+        <is>
+          <t>02026687800</t>
+        </is>
+      </c>
+      <c r="F1041" t="inlineStr">
+        <is>
+          <t>Kalyani Nagar</t>
+        </is>
+      </c>
+      <c r="G1041" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1041" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1041" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1041" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" s="1" t="inlineStr">
+        <is>
+          <t>A52100018117</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Ganesh Sukhadeo Sanap</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>A52100018117</t>
+        </is>
+      </c>
+      <c r="D1042" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=rJ2xt0ZGYGDI4n6bdwcglnPqlUgKHjdSUfHBZj5uE5gfonSmy4%2bjTFEd9VoTxelnaSv8LAN%2fKxoe4CLy5Y2Tzq9%2bhDyC1N20w8NXjnBPBnyFlKrLSdHXj7UUIJelJ1V4M7iVG7gZvVFopsyTio%2b%2b0p087Ciup1kWlx01OTthH8genOtQH9zqkg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1042" t="inlineStr">
+        <is>
+          <t>09579374237</t>
+        </is>
+      </c>
+      <c r="F1042" t="inlineStr">
+        <is>
+          <t>Pride World City</t>
+        </is>
+      </c>
+      <c r="G1042" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1042" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1042" t="inlineStr">
+        <is>
+          <t>Lohgaon</t>
+        </is>
+      </c>
+      <c r="J1042" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" s="1" t="inlineStr">
+        <is>
+          <t>A52100001739</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Sachin Bhagwat Thorat</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>A52100001739</t>
+        </is>
+      </c>
+      <c r="D1043" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1NDI%2fr5GPn0IFDxInPawfg5GB45kwryM9LDX%2b8L8MqyhLpKij4Q3V6J%2fjqWr8CyxI0CyuDXRGRERomqA58PSWo0E3ThCdSeyQNSX22PwrhqZYJcMlmB%2fHQj7N%2ffiqw5TSC7ggL6K5Wv3X44fWYcWvZ8PGWOmhBUTo5Ool8NYs0TmGZp3MfDViw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1043" t="inlineStr">
+        <is>
+          <t>08379909555</t>
+        </is>
+      </c>
+      <c r="F1043" t="inlineStr">
+        <is>
+          <t>Hinjawadi Phase1</t>
+        </is>
+      </c>
+      <c r="G1043" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1043" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1043" t="inlineStr">
+        <is>
+          <t>Hinjavadi (Ct)</t>
+        </is>
+      </c>
+      <c r="J1043" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" s="1" t="inlineStr">
+        <is>
+          <t>A52100018388</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Propmates International Private Limited</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>A52100018388</t>
+        </is>
+      </c>
+      <c r="D1044" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=iuAnx%2fgSa38W3hUeS0ZytI9YMMiaILkfVhkvzVQ6m%2bbub6l%2bhgshxdOBUjuRZP%2fI9%2bBO0DG8Ewp86jtMgfs8vIJ1z4dMqg17y1bObr69vSZFJOOVW3v34N5cFipCy7JJ5CxQdF%2fv3zFtfvByXR%2bsJXJrH%2beD9U9aYkjpPdaq9KyLz4UmQUiA4Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1044" t="inlineStr">
+        <is>
+          <t>08412900047</t>
+        </is>
+      </c>
+      <c r="F1044" t="inlineStr">
+        <is>
+          <t>Shivajinagar</t>
+        </is>
+      </c>
+      <c r="G1044" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1044" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1044" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1044" t="inlineStr">
+        <is>
+          <t>411005</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" s="1" t="inlineStr">
+        <is>
+          <t>A52100018295</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Nasreen Kadar Patil</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>A52100018295</t>
+        </is>
+      </c>
+      <c r="D1045" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2fUTwz3%2fYL6v%2bv7V4J9XBqzkieJkcAPLQoZWD3%2fdfQK1n0v%2bXPsNwCSzSJkGAdH4CcR03HfuOj3VcpbAFQ2aL7E21iyEvDWUaGVYsprjpMvEa0tJXZCm5J54e7ntiIW%2fxADZgRUdJ2h9T%2bbaBmmAs0m99qxFhfsxasTcDXBK%2f4uDQ9aODRXXWqQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1045" t="inlineStr">
+        <is>
+          <t>08352277853</t>
+        </is>
+      </c>
+      <c r="F1045" t="inlineStr">
+        <is>
+          <t>Lohegaon</t>
+        </is>
+      </c>
+      <c r="G1045" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1045" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1045" t="inlineStr">
+        <is>
+          <t>Lahagaon</t>
+        </is>
+      </c>
+      <c r="J1045" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" s="1" t="inlineStr">
+        <is>
+          <t>A52100018171</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Vikas Shahuraj Patil</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>A52100018171</t>
+        </is>
+      </c>
+      <c r="D1046" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=faE920mLYE7BGRByT7R85Wt1%2fDVJ5naKoPEmyfbPEY1bgUZ0tGAAHFfgpDjuQ0BayzMCxskWPpcLm7kp9wlofvKUDsyuBl%2btNjpPc1fxFtnO%2fuWRacs%2bNeq61BC88Zco2fxJU3tKcvJnT408AaHBa6BXK7UQ4tEZOb7EincaFXOP6JWPHZZ8cA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1046" t="inlineStr">
+        <is>
+          <t>02025471111</t>
+        </is>
+      </c>
+      <c r="F1046" t="inlineStr">
+        <is>
+          <t>Erandwane</t>
+        </is>
+      </c>
+      <c r="G1046" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1046" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1046" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J1046" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" s="1" t="inlineStr">
+        <is>
+          <t>A52100018261</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Divakar Bharat Mirajkar</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>A52100018261</t>
+        </is>
+      </c>
+      <c r="D1047" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fRIh3qsk4sJNAlsNxuAQWQ5ZdJN2SqHgsbIz%2bGdBOkEyRLOd8hd%2bEeRL1thMdI%2fWUq%2b7DjNcUR68Fm%2bUINBW5Nhzbhc24DtSyNthgQ5L2aim122gkYpLs8ku%2bVM2vY7s%2fFJ9KMIiCHEN7%2bQU4nVDTTYZ5zOmer025W5JERXqNKsXMsbjYFXXDA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1047" t="inlineStr">
+        <is>
+          <t>20123456789</t>
+        </is>
+      </c>
+      <c r="F1047" t="inlineStr">
+        <is>
+          <t>Koregaon Park</t>
+        </is>
+      </c>
+      <c r="G1047" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1047" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1047" t="inlineStr">
+        <is>
+          <t>Koregaon Park</t>
+        </is>
+      </c>
+      <c r="J1047" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" s="1" t="inlineStr">
+        <is>
+          <t>A52100018332</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Abhishek Arun Bhukan</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>A52100018332</t>
+        </is>
+      </c>
+      <c r="D1048" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=7SDeOV5Uy8qKlTvmjLPvzjmmen854Sy7cMVll2oXjr4lRs7JzBCnk%2bc3aeEU4LSHv6mh6JrakR5XnT3k2ewSg3Dmw80rkQ7S6KVFh4pDHZRgM6mwYCnGegTQC4Nf9ow0KP%2bMBYbbsKDzGdoBqz%2bmhPIdSkN2FhWC6cpytZzc%2bE5QfhoPWdIm6w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1048" t="inlineStr">
+        <is>
+          <t>08956998108</t>
+        </is>
+      </c>
+      <c r="F1048" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1048" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1048" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1048" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1048" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" s="1" t="inlineStr">
+        <is>
+          <t>A52100018402</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Varun James Datt</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>A52100018402</t>
+        </is>
+      </c>
+      <c r="D1049" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=HIocum1qS%2f1By5m%2bowP1JMse%2bwm7zctdaELKu%2bsBUMBWDw05X7zxdz3hAPh%2ft1e9bnvaxXhkaEOkNQ1ZtXH%2fI0cEQ3tJUIAf0Vk5xNkbYIeK9pGuIDiggoQoR3mEdz8P7K0Erq1Scf3PFSO9jSbv2k9M%2bw3MNusWaYetpuATPEDRb2hdTynPCg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1049" t="inlineStr">
+        <is>
+          <t>09503022229</t>
+        </is>
+      </c>
+      <c r="F1049" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1049" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1049" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1049" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1049" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" s="1" t="inlineStr">
+        <is>
+          <t>A52100027600</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Kamleshkumar Kantilal Shah</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>A52100027600</t>
+        </is>
+      </c>
+      <c r="D1050" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=iLnrEux0NLbQ%2b6Ma5187lJ9Rio5ZVlrMVqADS3q3QkDdT5eS5u3wfhVm%2fByA1lG6OQS3fLjE%2b4aO3F3LkyJTJnsWwxRJzPDa2044mYzBS0MailawfXcOBckFYFM63oV8rOGYIm4QrThEarqIDQWiOQv%2fqk21x85KnWWwU9aQexYMYWDO4LsDDw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1050" t="inlineStr">
+        <is>
+          <t>02024264666</t>
+        </is>
+      </c>
+      <c r="F1050" t="inlineStr">
+        <is>
+          <t>Gultekdi</t>
+        </is>
+      </c>
+      <c r="G1050" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1050" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1050" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1050" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" s="1" t="inlineStr">
+        <is>
+          <t>A52100018275</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Yashpal  Singh</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>A52100018275</t>
+        </is>
+      </c>
+      <c r="D1051" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=OBjPgjottembHO3pJxItofBu9mtn7mjYZBhhZey9NRpUid%2bU1zjlvy60e%2fxQAwYo51yvOx9eYAFB%2f%2fm4KH88sysFjlTBSdmEAnkmL1Ct1VmXLEhYTa705HEQZVCrOO84n9GHCO12Hyi3DnWu6r87G%2fZpjGFyW%2fVByMeop3IhkJEpesYK5Hw1EQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1051" t="inlineStr">
+        <is>
+          <t>08007402829</t>
+        </is>
+      </c>
+      <c r="F1051" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1051" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1051" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1051" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1051" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1100]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1051"/>
+  <dimension ref="A1:J1101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54568,6 +54568,2606 @@
         </is>
       </c>
     </row>
+    <row r="1052">
+      <c r="A1052" s="1" t="inlineStr">
+        <is>
+          <t>A52100001791</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Chandan  Kumar</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>A52100001791</t>
+        </is>
+      </c>
+      <c r="D1052" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=jSGhS0YZZMurJ1XtnS%2fR8Jc%2beWdev4RSRaAwF%2fIBZQnPJSo5H3cuUJ8Vq96CdYyVWKvMPmLdXhbEL7%2f30yM693Pa9GLuWAxv15n4y1p3dgaPIoPAbtT2GYFfFN8ddFEs%2fd5QElTcsiL3IMibS%2b%2fI%2fBRXDxHjTmGD%2bJkCpnLPd%2fk%3d</t>
+        </is>
+      </c>
+      <c r="E1052" t="inlineStr">
+        <is>
+          <t>08446522666</t>
+        </is>
+      </c>
+      <c r="F1052" t="inlineStr">
+        <is>
+          <t>Jivan Nagar</t>
+        </is>
+      </c>
+      <c r="G1052" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1052" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1052" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1052" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" s="1" t="inlineStr">
+        <is>
+          <t>A52100001880</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Vivek  Kumar</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>A52100001880</t>
+        </is>
+      </c>
+      <c r="D1053" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2qdIwgAoewkIPXgcqqq%2f39plYpKbLpmrVaawGko%2brR04X1ePnNoSrOJrQ%2bP6Zlwie56Ch7qgNJJDpN87sn6uWXZAKROZ4OTSglV7AUmgxFiILjECfRtyPz6O4EPx11ws3yPlKT5oCBtHe9b5znRDuR1JIquRSQc4l9AgEd%2fQH%2bY%3d</t>
+        </is>
+      </c>
+      <c r="E1053" t="inlineStr">
+        <is>
+          <t>08657802233</t>
+        </is>
+      </c>
+      <c r="F1053" t="inlineStr">
+        <is>
+          <t>Sutarwadi</t>
+        </is>
+      </c>
+      <c r="G1053" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1053" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1053" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1053" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" s="1" t="inlineStr">
+        <is>
+          <t>A52100018224</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Mina  Bhowmick</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>A52100018224</t>
+        </is>
+      </c>
+      <c r="D1054" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2blWkacqOEAIrBcoI%2bYj9ZVR9VNc4WFa8t8DZjWJRFVZ2CLrkEnp4Em3lKcgAyK4AmoOAgg487U9EoVqmHvPs9rQdiHoZrGyUPyg1E1WlOxcy19IWpzrVCfo6XoPn08u694oBppMx5isButibYmXAF%2fMrnQdhtnNltM9SeHfSCrb5ekzywi1UKg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1054" t="inlineStr">
+        <is>
+          <t>03325914368</t>
+        </is>
+      </c>
+      <c r="F1054" t="inlineStr">
+        <is>
+          <t>Vimannagar</t>
+        </is>
+      </c>
+      <c r="G1054" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1054" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1054" t="inlineStr">
+        <is>
+          <t>Vimannagar</t>
+        </is>
+      </c>
+      <c r="J1054" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" s="1" t="inlineStr">
+        <is>
+          <t>A52100018366</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Dnyaneshwar Ganpat Nehatrao</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>A52100018366</t>
+        </is>
+      </c>
+      <c r="D1055" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=StqB%2fELy4B%2fqKjxbZD2gv5fA6khGWi%2fatOcyR8rg7kLuL5Gckw2SZ3AeXevbZDmFHZ5uTgDqa62fN8uU8ZHcYb3VBXJ783RzBHgDMgDnn6qwGgv%2fN7rc4dlZwDiC3zZpgta9godlr4qLAjRvo9eUu53l8K2akcxDqdVwktKZT3zBzaTjZRAj5Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1055" t="inlineStr">
+        <is>
+          <t>09226111809</t>
+        </is>
+      </c>
+      <c r="F1055" t="inlineStr">
+        <is>
+          <t>Talegaon Station Road</t>
+        </is>
+      </c>
+      <c r="G1055" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1055" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I1055" t="inlineStr">
+        <is>
+          <t>Talegaon Dabhade (M Cl)</t>
+        </is>
+      </c>
+      <c r="J1055" t="inlineStr">
+        <is>
+          <t>410507</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" s="1" t="inlineStr">
+        <is>
+          <t>A52100018203</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Sandeep Prataprao Bodhale</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>A52100018203</t>
+        </is>
+      </c>
+      <c r="D1056" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=GRa44wUWuyRtSu09yM6xVnkCfosi1BIm8f0%2fgokzWoXFTm6yu8WsJHDIGgGb%2btbeQkdUoAWaBKauTcFRTaJ%2b%2bOWSL9qRWO%2bp4%2b%2bhc7phJHmZda5FQU6jLV1cmlBUrfO%2ftuzCpiGNcUGDNAR6KArFG4ObboszA8wUqzZDm3H7aJEvNitFZY5CTw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1056" t="inlineStr">
+        <is>
+          <t>02024443394</t>
+        </is>
+      </c>
+      <c r="F1056" t="inlineStr">
+        <is>
+          <t>Sinhagad Road</t>
+        </is>
+      </c>
+      <c r="G1056" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1056" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1056" t="inlineStr">
+        <is>
+          <t>Parvati</t>
+        </is>
+      </c>
+      <c r="J1056" t="inlineStr">
+        <is>
+          <t>411030</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" s="1" t="inlineStr">
+        <is>
+          <t>A52100018282</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Binod Kumar Alok</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>A52100018282</t>
+        </is>
+      </c>
+      <c r="D1057" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CjZPUGZbWwy0t31TyOXRFzDzEgQ4MeV39UlftSw7YGhMI6hW5qeD4R6gXRTZEKA9vK8dmD6uk%2fzotLJsSISNOnS%2fkN3XhHar8lW84ZBl4ZdfQPhx7OfdVDEhg3C2WV0Eu1Gbug70Eae6eKgm4Zx4F6MmXF%2fDudPszXIF72HgLCEoMECneet9Tg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1057" t="inlineStr">
+        <is>
+          <t>02046306556</t>
+        </is>
+      </c>
+      <c r="F1057" t="inlineStr">
+        <is>
+          <t>Hinjewadi</t>
+        </is>
+      </c>
+      <c r="G1057" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1057" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1057" t="inlineStr">
+        <is>
+          <t>Hinjavadi (Ct)</t>
+        </is>
+      </c>
+      <c r="J1057" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" s="1" t="inlineStr">
+        <is>
+          <t>A52100018208</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Mangesh Ganpat Chavan</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>A52100018208</t>
+        </is>
+      </c>
+      <c r="D1058" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=80V%2f5xTwRAdZrEJiYTA96cCMRr1hRcV1cl5KLUcUdxEjw%2famNpQ%2bJ3vYPw0osNkA0lvgEpK2eZGR3KrR5weiQKgEtpmw58QR4jkJKC0ft4JUPIE75OAA2q%2fxbm1kgFoJv5QYdDwUPoiMaPbTkWGrlbP1NieSsawBOvu28OFgQ0j%2bUcnKHoR6og%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1058" t="inlineStr">
+        <is>
+          <t>08087388080</t>
+        </is>
+      </c>
+      <c r="F1058" t="inlineStr">
+        <is>
+          <t>Right Bhusari Colony</t>
+        </is>
+      </c>
+      <c r="G1058" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1058" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1058" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J1058" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" s="1" t="inlineStr">
+        <is>
+          <t>A52100018866</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Amazon  Realty</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>A52100018866</t>
+        </is>
+      </c>
+      <c r="D1059" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=w76dfR1BCOl7CMGhGp0u0jfKxA9PfRsLWTul114i0a36bvBGpFl1aBrCN4eKRrrPvKN8l9kSSc917hOZ1EFHz90qauN0PAKDL6lD%2fRYKaCb2SxQARtJbygL%2febkf6hkupp8Dc96zU1z6Fl4IBuJsVzcvuquZKr7Z9AUBv6WUzBJN4PvlHT5OlQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1059" t="inlineStr">
+        <is>
+          <t>01234567891</t>
+        </is>
+      </c>
+      <c r="F1059" t="inlineStr">
+        <is>
+          <t>Chandan Nagar</t>
+        </is>
+      </c>
+      <c r="G1059" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1059" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1059" t="inlineStr">
+        <is>
+          <t>Chandannagar</t>
+        </is>
+      </c>
+      <c r="J1059" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" s="1" t="inlineStr">
+        <is>
+          <t>A52100001904</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Sheela  Thomas</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>A52100001904</t>
+        </is>
+      </c>
+      <c r="D1060" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2b5hu4%2bbnA2dFOZVVGLgqs2jrQxkjmIkjfUkLN2%2bN715MhF1mzuAUOuwU%2fDBr0%2fKa8tTSf3U4OqEnhmm%2b3oTg9KgVt5ZzLkXuVpXg6y%2fXNNn2ugDFL%2bPp4gXJJ8%2fJSKNs1f9EhOdM3qPmL1VXlQzJTkXF3ZMUegBB8r3LID2Ah2c%3d</t>
+        </is>
+      </c>
+      <c r="E1060" t="inlineStr">
+        <is>
+          <t>09765393140</t>
+        </is>
+      </c>
+      <c r="F1060" t="inlineStr">
+        <is>
+          <t>Bhavdhan</t>
+        </is>
+      </c>
+      <c r="G1060" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1060" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1060" t="inlineStr">
+        <is>
+          <t>Bavdhan Kh.</t>
+        </is>
+      </c>
+      <c r="J1060" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" s="1" t="inlineStr">
+        <is>
+          <t>A52100018376</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Vineet  Khanduri</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>A52100018376</t>
+        </is>
+      </c>
+      <c r="D1061" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=P7qqJdU%2bIk8TbR%2fwSffBiFyOhnycgYJqEkvpr33545r%2b3L8SM9Rhx124Ra%2bbka14HxPXXAEARChVJZ8NXV4BxmqvFLMIV%2f%2fI%2f25Vw2qayX%2fWwrMvHzuXYeNlqwMt0u2E%2bLB%2bh7opKn2py8SG9vrj%2b%2bY5xT9IajqfBgK17AYucmYUkOKBXx%2f%2bhw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1061" t="inlineStr">
+        <is>
+          <t>02041229012</t>
+        </is>
+      </c>
+      <c r="F1061" t="inlineStr">
+        <is>
+          <t>Wadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G1061" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1061" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1061" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1061" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" s="1" t="inlineStr">
+        <is>
+          <t>A52100008114</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Amoi Arun Dhas</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>A52100008114</t>
+        </is>
+      </c>
+      <c r="D1062" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=DObcbG0f7avD%2bO3isfpSKHYDlLmvcZx738fj9NXJpBgAIrxpB9cIkYt%2bIPENHphJr%2bNiN3hRnFBNEGIK%2bYKqVjlEocGGau5TOGrz57f7EyxCO90IEUHz6LeiLQJJlNXvBkKw3GO3irKUNvnzjBXVWDcYpMywbKsPz4j6wVY%2bQFrJMWUsZ7wPAg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1062" t="inlineStr">
+        <is>
+          <t>08380099333</t>
+        </is>
+      </c>
+      <c r="F1062" t="inlineStr">
+        <is>
+          <t>Dhanukar Colony</t>
+        </is>
+      </c>
+      <c r="G1062" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1062" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1062" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1062" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" s="1" t="inlineStr">
+        <is>
+          <t>A52100018253</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Madhav Kumar  Yadav</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>A52100018253</t>
+        </is>
+      </c>
+      <c r="D1063" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1WP5uGO2JTh53chkWQya9i%2fZ1wn2sVxnaoR1XbaTMjLS5mjujP4n2NgXl3PFtCd%2fssTWy0JSbYDsVG1t0kLcsiITpMyOIr44LBpvJykktfpqIMsG4cvyhOwaoe3d4iEQ9PYUEduYPM90ii%2fL3mrPc9N06%2f1i4UArMbKvzAyYsxP5uU5TMaqnBg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1063" t="inlineStr">
+        <is>
+          <t>08825181406</t>
+        </is>
+      </c>
+      <c r="F1063" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1063" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1063" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1063" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1063" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" s="1" t="inlineStr">
+        <is>
+          <t>A52100018313</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Ameya Arun Kulkarni</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>A52100018313</t>
+        </is>
+      </c>
+      <c r="D1064" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=nLw8tJHH1lkvVCV4LwRA07mtfu3Z2ykRqB2J7ikh3BGCPkxncbByQQgtxJn1Gr6urTFTBiEhZaLHWL5sq43rTg4EbV2LZ9St3ilE0rsvzUTg3TAlWqwAl9RoZw%2fgkfsge9MiqBkua1uV7aF%2fV44VTdMwYecUNVLhVrqn6PQNsEOiKei8B2KcvA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1064" t="inlineStr">
+        <is>
+          <t>02025462447</t>
+        </is>
+      </c>
+      <c r="F1064" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G1064" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1064" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1064" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1064" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" s="1" t="inlineStr">
+        <is>
+          <t>A52100018256</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Mayur Suryabhan Kanawade</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>A52100018256</t>
+        </is>
+      </c>
+      <c r="D1065" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=S09tJUBEVNRH6e22QrpZpTz9nTTU6ziUTlFr3eb5VQbB0RTkMogMein68uVQZ%2bwaiZ3C6cuGKLSi0HYrnvxbXHUZVJ7ZvY76v4UbyFxPzpPEbC9rSooeMf57W5vB7jASgJAyzaF2%2bLkblTPPcSwtG3TPGZYFiiY%2bImGWyNoXUjErTxe27ZOjRw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1065" t="inlineStr">
+        <is>
+          <t>09561587775</t>
+        </is>
+      </c>
+      <c r="F1065" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1065" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1065" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1065" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1065" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" s="1" t="inlineStr">
+        <is>
+          <t>A52100018269</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Prabhanjanakumar  Patra Proprietor Of Lotus Landmarks</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>A52100018269</t>
+        </is>
+      </c>
+      <c r="D1066" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=iqjFj7ZvB82WzcFuKGuNqfLykagBysFdAYofwF6LKBrOwmmF64OnETfMTA5UgVnntyVIIzRNA56ZrL4chSQGfD%2bd%2f3ajLU2CWL3Y6Hc78q7Oo07Sap938NmO2L1e2VsGDiM4WxD9vRWVBy5zezJ1Dag04bqP7NyDR%2fOEs83ZMin9SZpCJ54NiA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1066" t="inlineStr">
+        <is>
+          <t>09881748383</t>
+        </is>
+      </c>
+      <c r="F1066" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="G1066" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1066" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1066" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1066" t="inlineStr">
+        <is>
+          <t>411018</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" s="1" t="inlineStr">
+        <is>
+          <t>A52100018450</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Deepashree Umesh Pawar</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>A52100018450</t>
+        </is>
+      </c>
+      <c r="D1067" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hsV2DyMD0wVfm6TNaq36BaE%2fXCi5Cj%2f0L4jWkbijJhN8M2IkcrwT3j2ZAO7yImQnSqEY3YSiNgRqbcJEkTDheS6l6WDLMBK9IXayTxkO6f%2bMng3e0DUObkJ4tabf6cHtbyhnbQVbs20xfVDPBmLXLsMfXCeM1MnhUMZkh9mjl4QWUTO4rIeGXQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1067" t="inlineStr">
+        <is>
+          <t>08379842663</t>
+        </is>
+      </c>
+      <c r="F1067" t="inlineStr">
+        <is>
+          <t>Bhugaon</t>
+        </is>
+      </c>
+      <c r="G1067" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1067" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1067" t="inlineStr">
+        <is>
+          <t>Bhugaon</t>
+        </is>
+      </c>
+      <c r="J1067" t="inlineStr">
+        <is>
+          <t>412115</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" s="1" t="inlineStr">
+        <is>
+          <t>A52100018396</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Kunal Vinaykrishan Dhingra</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>A52100018396</t>
+        </is>
+      </c>
+      <c r="D1068" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=tX6teGEbQIgEa6zD0PFwXU9Qjup8lvFwS8%2fLnFxvOaP0kVI9trXiQ5rS%2bsoc0zChFJ2aF1Di9XV5nGQzDWsOnV4M82k%2fDcD1Jqf02J6d2rMTi9C0mvN3OeV2j8SNvlVTWu0jG9KjOPnDG793Ujup5y6Dp2%2f0cIk4ez6ki5MNujkfkqRXpDijCg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1068" t="inlineStr">
+        <is>
+          <t>02040090972</t>
+        </is>
+      </c>
+      <c r="F1068" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G1068" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1068" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1068" t="inlineStr">
+        <is>
+          <t>Kondhwa Bk</t>
+        </is>
+      </c>
+      <c r="J1068" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" s="1" t="inlineStr">
+        <is>
+          <t>A52100018321</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Arpit Brindayan Chouksey</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>A52100018321</t>
+        </is>
+      </c>
+      <c r="D1069" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=pCKce7SlGwBhqOUiF0qYMfG07yl0yOkvxcZj7EA%2fIECEKT0JGJv1WEn7lsGt%2bHqC9p3XZBe%2fG95YU2K1LYoa%2bgzuzNmHHBhzpVgHNNJReAf6ICpEFqANaeVjrWyUv9hcjquf9O%2fQr79x8oemhYYhbjqY9YLv2Wm04fX88K4VaYK9y5DF2TzY4Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1069" t="inlineStr">
+        <is>
+          <t>09112720484</t>
+        </is>
+      </c>
+      <c r="F1069" t="inlineStr">
+        <is>
+          <t>Bavdhan Budruk, Haveli</t>
+        </is>
+      </c>
+      <c r="G1069" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1069" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1069" t="inlineStr">
+        <is>
+          <t>Bavdhan Kh.</t>
+        </is>
+      </c>
+      <c r="J1069" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" s="1" t="inlineStr">
+        <is>
+          <t>A52100019456</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Ekta  Behera</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>A52100019456</t>
+        </is>
+      </c>
+      <c r="D1070" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=kk83DnPPIDUJFZviar7DNx%2fTGR%2bOnuKUW8FZyisxAIf2IZSWGKKEghg6LE9PK9Hy6ls0KOmK70KlgqkvBhDB%2bKZMku7HaZKDqBN%2b4pF01ImpkgkR7U25Ola6vtegU0Du8QULDMXjI%2fwodgLuHUuQSmV6WZc6TBo0xjoHWpP2hTde46d0ZZJZJA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1070" t="inlineStr">
+        <is>
+          <t>02066788505</t>
+        </is>
+      </c>
+      <c r="F1070" t="inlineStr">
+        <is>
+          <t>Mahadev Nagar</t>
+        </is>
+      </c>
+      <c r="G1070" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1070" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1070" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1070" t="inlineStr">
+        <is>
+          <t>412307</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" s="1" t="inlineStr">
+        <is>
+          <t>A52100018298</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Prakash Manika Shinde</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>A52100018298</t>
+        </is>
+      </c>
+      <c r="D1071" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fAcJoIk8AtLGiWWs5YFCgdZbP0nS7oNIv5GbJAEAbwTGUi1z%2bOpUulFjVZ38UC4dUibxZQ7C42AKhpaFHnImy%2bG0pQJcL%2bLBMtEnWT1scf8un2oVw9%2b8rin0IV0S%2fleuVMKH465JVL8Sta30uTK9AqeYueWUwuiMqu3RohRP1wgN8Gmh%2bYfDsg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1071" t="inlineStr">
+        <is>
+          <t>02022361112</t>
+        </is>
+      </c>
+      <c r="F1071" t="inlineStr">
+        <is>
+          <t>Yerwada</t>
+        </is>
+      </c>
+      <c r="G1071" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1071" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1071" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1071" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" s="1" t="inlineStr">
+        <is>
+          <t>A52100018296</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Albasquare</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>A52100018296</t>
+        </is>
+      </c>
+      <c r="D1072" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=kloyI%2bf8UkymvesKVC%2fakgRVEXUv4xRf3wC%2fqgipXkh%2fEbGuHrnAtNuF48SW8LDr7Qfbc3cds6umtoYcrIX88mOxAqoE%2fnPv38Uva2YQVOnqCbkmu4tmtzmqSzoU0EtxZsnRUxp4Z1oNcq0JyEk8ZZescpdVXP5sFqgOFXTdPU8xDMkZOAphag%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1072" t="inlineStr">
+        <is>
+          <t>09881748383</t>
+        </is>
+      </c>
+      <c r="F1072" t="inlineStr">
+        <is>
+          <t>Yerwada</t>
+        </is>
+      </c>
+      <c r="G1072" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1072" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1072" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1072" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" s="1" t="inlineStr">
+        <is>
+          <t>A52100018284</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Suryakant Dayaram Thakkar</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>A52100018284</t>
+        </is>
+      </c>
+      <c r="D1073" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=H6WN5EzPWn%2f%2bG1FftrPkZm84KFVKf8%2bKZ3I15%2fYu90QIEW4RM%2b1SVQQsPH718AL3R%2bcenumiCDOPFlvgCqtOPKfcLnR8dH2MGkAFk1OlgIqCM87ehYHCPdRebuMK3ZDZBZ26TKpNTjlXRl1BMYGhOvtcvd%2f65BJAjybQ5EQjPUzuWZ86E36Gcw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1073" t="inlineStr">
+        <is>
+          <t>02224142315</t>
+        </is>
+      </c>
+      <c r="F1073" t="inlineStr">
+        <is>
+          <t>Matunga Mumbai</t>
+        </is>
+      </c>
+      <c r="G1073" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1073" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1073" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1073" t="inlineStr">
+        <is>
+          <t>400019</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" s="1" t="inlineStr">
+        <is>
+          <t>A52100021429</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Suchit Vijay Sarsar</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>A52100021429</t>
+        </is>
+      </c>
+      <c r="D1074" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=4hE5Q5TZ3Owu5NXLTK3Ccr8sCcHgoUUGgHqYZH6ZwALF9ex73VZAlnkIEYGvMy2dTfW%2fel1M2eq%2fKwARWJZ5VkJyU6WDxLm9ixue7ogp2VSn0gTbepFkwv31%2b2lu1PmQbodpEYf1dEVcy7gj86pQ1inImhB7zheGOzGjMspAWAFNKJi8dGe7jQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1074" t="inlineStr">
+        <is>
+          <t>02265221248</t>
+        </is>
+      </c>
+      <c r="F1074" t="inlineStr">
+        <is>
+          <t>Ghorpadi Gaon</t>
+        </is>
+      </c>
+      <c r="G1074" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1074" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1074" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1074" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" s="1" t="inlineStr">
+        <is>
+          <t>A52100018317</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Kiran Suresh Tipe</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>A52100018317</t>
+        </is>
+      </c>
+      <c r="D1075" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PMlV6OhVyywZpWW9%2fVJZu4GkGo5IGQp1UeFqz8vFAeM7qxKLCeLvDjy8vmMymDH%2fdwEl%2bpaPuviF2IIgZAvhLLa48MtuLfg1M3vfMViyyALX4xCqdCXBJZmodu7XDy9Sgh0GTCMDrLdWBMc4yMnfb5e00iXUTsuDj3Js9jwnCVCxEVKgnIJP%2bg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1075" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
+      <c r="F1075" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="G1075" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1075" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1075" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="J1075" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" s="1" t="inlineStr">
+        <is>
+          <t>A52100018315</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Abhijit Keshav Kapase</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>A52100018315</t>
+        </is>
+      </c>
+      <c r="D1076" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Szff8zClKck6CyrwF1lG1Es%2fCz9QvVk2JPgTxzdYhwBYr4mb2bMGvWdNqweT0%2fVlRqfn4Y3BUh5awDgifkRscjkxxQQLcnUixa%2b%2b3dV5d0mNBXC8Ol%2f8dlrr%2bVgxIxxVkzTbEi33qup9hLPutoWh%2fvRHds9QhLhu6HluJkJqZW4sku0FtMntqA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1076" t="inlineStr">
+        <is>
+          <t>09607711122</t>
+        </is>
+      </c>
+      <c r="F1076" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1076" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1076" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1076" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1076" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" s="1" t="inlineStr">
+        <is>
+          <t>A52100018344</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Sukesha  Wadalia</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>A52100018344</t>
+        </is>
+      </c>
+      <c r="D1077" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=HegsgzJzLDm7XE3QSwNuMSocGE2xHhwu4V6fIZcTt1myIQOaOkv2a4YMkO49%2bIaCPV3VddHE6MIAVkVLhhtpPkmgDUXPkv8%2fOQovGoYs8Sdjda5e7g1Y1OCmYNWAemg6Dsy1LkSrDzV%2f6UYZJt8ML0zJxo5n2A5L332f%2bP0K5DobSIov8uB%2feg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1077" t="inlineStr">
+        <is>
+          <t>02041241818</t>
+        </is>
+      </c>
+      <c r="F1077" t="inlineStr">
+        <is>
+          <t>Lohagaon</t>
+        </is>
+      </c>
+      <c r="G1077" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1077" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1077" t="inlineStr">
+        <is>
+          <t>Lohgaon</t>
+        </is>
+      </c>
+      <c r="J1077" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" s="1" t="inlineStr">
+        <is>
+          <t>A52100018307</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Tarannum Shamshuddin Mulla</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>A52100018307</t>
+        </is>
+      </c>
+      <c r="D1078" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=4wI0%2fEjhWG28kAPwW0vbfDYmjFLEjv%2fG4KCG9w0murC17nELAZseNbt7FFgq%2fjckoS%2ffVuVpFy8%2fUCQ9pK%2fDZN7jrUrIRjV%2bbjwLQ4WvMPUeYf44EZ97V9SqKZYzp%2f72tQ2TDurB%2fQQLiLRMZPoQR2Bwhtj3FSkvI60w3zjWpvbyUiZJvDs1cg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1078" t="inlineStr">
+        <is>
+          <t>09822975444</t>
+        </is>
+      </c>
+      <c r="F1078" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="G1078" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1078" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1078" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1078" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" s="1" t="inlineStr">
+        <is>
+          <t>A52100018378</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>S Golakanath Patro  Patro</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>A52100018378</t>
+        </is>
+      </c>
+      <c r="D1079" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=S5j48Rch2Y1yJyVtrUQlbqe5Ojg6PwgATnSldobo7EaByjDt6LqykME8oT9F0HJ5vmeTgLUgxVZGHgE%2ft67ysnHkEmaEthf0lnUNh6sogXm73ONAT7cW1XupoRheLbAhbR%2b8cP4flUuzkFeloDvKHiUVwSUUR%2fzdr2pDjcd1zYXV2vn1fgrJtw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1079" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
+      <c r="F1079" t="inlineStr">
+        <is>
+          <t>Marunji</t>
+        </is>
+      </c>
+      <c r="G1079" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1079" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1079" t="inlineStr">
+        <is>
+          <t>Marunji</t>
+        </is>
+      </c>
+      <c r="J1079" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" s="1" t="inlineStr">
+        <is>
+          <t>A52100018356</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Payal Jagjit Vora Proprietor Of Pv Realty</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>A52100018356</t>
+        </is>
+      </c>
+      <c r="D1080" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2fzT2gf2fzBuk4DRShWuXqT%2bvqBoVDeX4fu8xx%2fsopxQ3mS8gHUwKbP%2bnpZ2Kr7gMfoDxR7VQ0Frc6%2f9lCB06rE21obEVXPYp9RTER43IglwlHm6Ua5i6Dlna4flNDKtnfuyvxwlIchmio8V5beQbafIBwvvHqb31OaTQIOC7pLLGyfpVXZNk5g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1080" t="inlineStr">
+        <is>
+          <t>09970577766</t>
+        </is>
+      </c>
+      <c r="F1080" t="inlineStr">
+        <is>
+          <t>Sahakar Nagar No 2</t>
+        </is>
+      </c>
+      <c r="G1080" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1080" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1080" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1080" t="inlineStr">
+        <is>
+          <t>412009</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" s="1" t="inlineStr">
+        <is>
+          <t>A52100018350</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Dattatray Rambhau Bhogil</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>A52100018350</t>
+        </is>
+      </c>
+      <c r="D1081" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=E%2b3Gvc%2fD6XextG%2f4HNHmJBDH59YF9ah2gdTPM8HLxSesyqUW1lAscU05gKiLD1n4luk4ad%2bJDWs%2fcBJSOVupiLT4vuPH06Tqv%2bqK2O8Mts53sS4ar3S15itWLZsiaG2OpDfvdmX52w%2bBQi7O47iGIikI5j4AC9P5q0iiakzKOuADPRvhx37UEw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1081" t="inlineStr">
+        <is>
+          <t>02067082813</t>
+        </is>
+      </c>
+      <c r="F1081" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1081" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1081" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1081" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1081" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" s="1" t="inlineStr">
+        <is>
+          <t>A52100018454</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Kishan Ganesh More</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>A52100018454</t>
+        </is>
+      </c>
+      <c r="D1082" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Hzgh5SrAsbS5EAEqv1PbnLq0iILvh7pxvkvesemPd21Q0Z6cjmgPafNwiZhsrXh7TZELnZYtyE1smTGu4Jc%2fTSBsN7GFgJOpDTnOGReFnKY8pGa8JqCeQud6VhaqaFiQPyku7jIpvnu5jB7X5XZvNwbUyj7VBRDWLWW29WLFY2vAMGIFXTowrw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1082" t="inlineStr">
+        <is>
+          <t>02026410200</t>
+        </is>
+      </c>
+      <c r="F1082" t="inlineStr">
+        <is>
+          <t>Kondhawe</t>
+        </is>
+      </c>
+      <c r="G1082" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1082" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1082" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1082" t="inlineStr">
+        <is>
+          <t>411023</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" s="1" t="inlineStr">
+        <is>
+          <t>A52100018386</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Sanjay G Makhani</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>A52100018386</t>
+        </is>
+      </c>
+      <c r="D1083" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=UEj3Zl4iiqh5Ro%2b2xqTjTDgqdnnRdo9QwtNpzN1FjvFfiaOphI42b8%2fuIwAo2rVhU9EXEfNY8ZNyrauKIyMOXRP8AP57C7z%2fo7i4DJjUNPcdhKImM9xgb5mOevwgv9j7GIbI5ohu6AhbCC%2f0nMYOg%2bkFK%2bgV2dMRk7pxmOUGPUZyuQfozxZXmg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1083" t="inlineStr">
+        <is>
+          <t>02025661992</t>
+        </is>
+      </c>
+      <c r="F1083" t="inlineStr">
+        <is>
+          <t>Balewadi</t>
+        </is>
+      </c>
+      <c r="G1083" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1083" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1083" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1083" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" s="1" t="inlineStr">
+        <is>
+          <t>A52100001887</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Yogesh  Thakkar</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>A52100001887</t>
+        </is>
+      </c>
+      <c r="D1084" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=HL4%2bVANNlVX%2fR9%2bD6ueLqHb%2fzmozsLofrkeBvgQAl1V8zCRnzPfe8P0nIzwNOrddIqeCu4yN0oj%2f4CcKo2JeJXNzUfFmbPcfr0q%2bSUeDza7zfL2OH6jl%2b9cuoNo5EfBP%2bJc1AtSVvXrWOf5WGJzNZJmJ90EFoi0D2bPpmQdTQ8E%3d</t>
+        </is>
+      </c>
+      <c r="E1084" t="inlineStr">
+        <is>
+          <t>02026153630</t>
+        </is>
+      </c>
+      <c r="F1084" t="inlineStr">
+        <is>
+          <t>Koregaon Park</t>
+        </is>
+      </c>
+      <c r="G1084" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1084" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1084" t="inlineStr">
+        <is>
+          <t>Koregaon Park</t>
+        </is>
+      </c>
+      <c r="J1084" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" s="1" t="inlineStr">
+        <is>
+          <t>A52100006230</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Amanco Realtors Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>A52100006230</t>
+        </is>
+      </c>
+      <c r="D1085" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=oUklvH8bNXuGIN57m2ZKA4Ap8gTnGNIoODDk238c4B4TtnXz3pmyYgzrKF9rSvTvIHwc86azWS9DwgTIeOq7eIlvmEmE16k4gIbR5O28B5jzTFGKUIRdzkbS6VHBT2StSJy0jMw21SQboSEy%2fd3zEikDY01GizvYKRiXWSOhQQWmkoyS9KGSrQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1085" t="inlineStr">
+        <is>
+          <t>07507114400</t>
+        </is>
+      </c>
+      <c r="F1085" t="inlineStr">
+        <is>
+          <t>Sinhgad Road</t>
+        </is>
+      </c>
+      <c r="G1085" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1085" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1085" t="inlineStr">
+        <is>
+          <t>Wadgaon Bk</t>
+        </is>
+      </c>
+      <c r="J1085" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" s="1" t="inlineStr">
+        <is>
+          <t>A52100018361</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Kiran Dilip Jamdar</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>A52100018361</t>
+        </is>
+      </c>
+      <c r="D1086" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KXHLJeKfs0bvoRj9RJP%2blhTbKpN4A2REV1%2ftwZkwFueU5CnwrwVVav8nrUlOkbZWsrBaeVMBNbX3tksVHOHU71ZUWQj7LyKHC5BNsettqRA9mh1hNdlj3mEsLOvaen%2b%2bdMK3vGGYw4dwMDXicvgLvCbrobzWskuK4IpMmgiTk2acm7xf8EWQIg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1086" t="inlineStr">
+        <is>
+          <t>02026992888</t>
+        </is>
+      </c>
+      <c r="F1086" t="inlineStr">
+        <is>
+          <t>Bhagirathi Nagar, Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1086" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1086" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1086" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1086" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" s="1" t="inlineStr">
+        <is>
+          <t>A52100001772</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Sagar Ashok Patil</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>A52100001772</t>
+        </is>
+      </c>
+      <c r="D1087" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2LNvBRbN4nVFz0J%2fxGRirOFpqEtRJ%2fwef5M%2bOVDh76DO6G%2bI6A1i%2b7wSjPn7oRtF55ZWns43UekbGgY%2fe%2b8XIezjYOI3FMDL583mmbjd1p6K5apj3ulEsr1jHswDk8924lUTdXiFgXMgUEK06Wt6ge7Sf%2fPa1ZyWjH5RFEOgcy4%3d</t>
+        </is>
+      </c>
+      <c r="E1087" t="inlineStr">
+        <is>
+          <t>08380944844</t>
+        </is>
+      </c>
+      <c r="F1087" t="inlineStr">
+        <is>
+          <t>Bhosari</t>
+        </is>
+      </c>
+      <c r="G1087" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1087" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1087" t="inlineStr">
+        <is>
+          <t>Bhosari</t>
+        </is>
+      </c>
+      <c r="J1087" t="inlineStr">
+        <is>
+          <t>411026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" s="1" t="inlineStr">
+        <is>
+          <t>A52100018404</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Sagar Sanjay Kolapkar</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>A52100018404</t>
+        </is>
+      </c>
+      <c r="D1088" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=sQcgNiQaBpp5jEnrY5XU9kXrjAjSpP7viFfGehqNPPt%2fLz0s3%2fsaUb502OLlJwNyPZ54SPJeilMglqEcPQY7sQBEx8Xtvx6boH2eO974W5VZX3SY%2fbJw7J%2fS%2f8kR4Qco5nxZ1E4ywrhNSvSX2lPMk%2bUVcm62ljLN70rqiyl2ZoGTg09yCJvBUw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1088" t="inlineStr">
+        <is>
+          <t>00000000005</t>
+        </is>
+      </c>
+      <c r="F1088" t="inlineStr">
+        <is>
+          <t>Katraj</t>
+        </is>
+      </c>
+      <c r="G1088" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1088" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1088" t="inlineStr">
+        <is>
+          <t>Katraj</t>
+        </is>
+      </c>
+      <c r="J1088" t="inlineStr">
+        <is>
+          <t>411046</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" s="1" t="inlineStr">
+        <is>
+          <t>A52100018827</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Vijay Narayan Darekar Proprietor Of Sadguru Properties</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>A52100018827</t>
+        </is>
+      </c>
+      <c r="D1089" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=C8rqIVHPvOj9p3USK6lpE%2b6zYHV4S81SQAeS5378vsDz4tpJEkqauOV1ZvJA1ceyy59SS9BmqUPQy56rJXsF0YGRpcI1ht2jNgX1jXa%2bGI0tFeCYBNpIHRd1GZq4%2fEXiSObsUdfsbdlUvhTUXoH2DAaSprF8lQrtxk2MUV44t0M5gCvt8M57dQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1089" t="inlineStr">
+        <is>
+          <t>08956642636</t>
+        </is>
+      </c>
+      <c r="F1089" t="inlineStr">
+        <is>
+          <t>Keshavnagar, Mundhwa</t>
+        </is>
+      </c>
+      <c r="G1089" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1089" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1089" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1089" t="inlineStr">
+        <is>
+          <t>411036</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" s="1" t="inlineStr">
+        <is>
+          <t>A52100019052</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Vinod Sadashiv Pisal</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>A52100019052</t>
+        </is>
+      </c>
+      <c r="D1090" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=l91ocpKln%2fvb1u98XLRoUCt3JMO0tmNPePAH6JMwcDBwTiE074zVuTPE8CidVpYH%2f20zmydShwov0UCxyU6jvHAvvLyOqq%2f14%2fXPmNkPgMMOXf7p2y7E86hB7BhpdXwPspzNpCucrk2mi12kXTJRrzJYgmZB54dpncvylRscuQdFIZl%2fKzYtww%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1090" t="inlineStr">
+        <is>
+          <t>02012345678</t>
+        </is>
+      </c>
+      <c r="F1090" t="inlineStr">
+        <is>
+          <t>Dattagad Nagar</t>
+        </is>
+      </c>
+      <c r="G1090" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1090" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1090" t="inlineStr">
+        <is>
+          <t>Dighi</t>
+        </is>
+      </c>
+      <c r="J1090" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" s="1" t="inlineStr">
+        <is>
+          <t>A52100018436</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Raj Satpalsingh Rajput</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>A52100018436</t>
+        </is>
+      </c>
+      <c r="D1091" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=t064aEDcmPdUUDA4Ymql33pKWJLGguqoBUI4knVC178JxT9JKDE1G2Wveg%2f%2fyF9svIJ37f3ne6fV4siMRlbtXeNMwt3a3a1qsFVyU5YsdvrLHHvo8FmMX%2fP3RDJY%2bdyw9C2%2bGg%2buPePp1dnCC8nvqWDaxBZ8tmDVbbH80uTmWRFNCtANrMXLBw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1091" t="inlineStr">
+        <is>
+          <t>91751743916</t>
+        </is>
+      </c>
+      <c r="F1091" t="inlineStr">
+        <is>
+          <t>Wadgaon Budruk</t>
+        </is>
+      </c>
+      <c r="G1091" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1091" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1091" t="inlineStr">
+        <is>
+          <t>Wadgaon Bk</t>
+        </is>
+      </c>
+      <c r="J1091" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" s="1" t="inlineStr">
+        <is>
+          <t>A52100018518</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Shyam Suresh Punjabi</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>A52100018518</t>
+        </is>
+      </c>
+      <c r="D1092" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CyHU2iOQuBZsIAM1IkS7HgjYFQCwkZRo5Hl5D4ChhR1C5Ban0haDWxnisj8xDOcQREWcWPwfNH6r3NysEHDcSAv7MvfjgZdtL904BrtNp6s0VKB8HFtnnWa7rdcV7sUUQTgUfXta%2fulpw8%2bGrFQHRVgmf54RxULZ1yK3Qdxz%2bqVDPNzDBrRj6Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1092" t="inlineStr">
+        <is>
+          <t>02027515575</t>
+        </is>
+      </c>
+      <c r="F1092" t="inlineStr">
+        <is>
+          <t>Pune Camp</t>
+        </is>
+      </c>
+      <c r="G1092" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1092" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1092" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1092" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" s="1" t="inlineStr">
+        <is>
+          <t>A52100018794</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Ganesh Shankar Salunkhe</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>A52100018794</t>
+        </is>
+      </c>
+      <c r="D1093" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=B1eIKta%2fKzG1hijW0KwPXyXiJdTP3Jfw0qz3%2fFUgM1LbWHxYPHlsP4eHVgx4%2fzoox%2bgsuZLYYGpFoFzNSTdbRY3Ot1b6tfnKhCyE1kjCNxqk2WTN6Alol8bha1FvjQhTfuDc%2bKlAZL0AfEbwMpn%2fbIqqgi%2btr7pZ2Rs%2fPjZIhCmtBOxOBK6gMQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1093" t="inlineStr">
+        <is>
+          <t>02052341289</t>
+        </is>
+      </c>
+      <c r="F1093" t="inlineStr">
+        <is>
+          <t>Viman Nagar,</t>
+        </is>
+      </c>
+      <c r="G1093" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1093" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1093" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1093" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" s="1" t="inlineStr">
+        <is>
+          <t>A52100018463</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Darshan Anil Parakh</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>A52100018463</t>
+        </is>
+      </c>
+      <c r="D1094" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=78%2fyBP2s7ncOTAjXqX8s58EL7%2fS5vTwPB3mMxqyd%2bulTJSwizg%2fEClAHZPZwOZBsdgpze6pfLX103sv02pi2QQwo%2fyEncQzQe7wboRCYpwIwdOOuFwmNcAyxtl7B%2f%2bLxp4T9XA9vMTUTWUQfIRoIs1buLrKr92SwVWUJmuMp1Ax9J4HoC01paA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1094" t="inlineStr">
+        <is>
+          <t>02026358536</t>
+        </is>
+      </c>
+      <c r="F1094" t="inlineStr">
+        <is>
+          <t>Nana Peth</t>
+        </is>
+      </c>
+      <c r="G1094" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1094" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1094" t="inlineStr">
+        <is>
+          <t>Peth</t>
+        </is>
+      </c>
+      <c r="J1094" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" s="1" t="inlineStr">
+        <is>
+          <t>A52100018416</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Rahul  Kapur</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>A52100018416</t>
+        </is>
+      </c>
+      <c r="D1095" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=NrjqKatTSKi7xLx7lvNcRtMdma%2bPfwGalU4wBp%2b37bCpB%2fyOzyPhMu%2bf6yKsrwNRZF5BjOsfAXSHNhG78RhB0uOrfz0mXsYYIzWP4N%2b8L%2bWwLEEyX3PskMbQGTgvdlmJEvavlV4r82xTrXi1TFyZHLgm5%2bUpKjImHCXPgjNmMQZoz6ElSqWzhg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1095" t="inlineStr">
+        <is>
+          <t>09766690809</t>
+        </is>
+      </c>
+      <c r="F1095" t="inlineStr">
+        <is>
+          <t>Koregaon Park</t>
+        </is>
+      </c>
+      <c r="G1095" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1095" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1095" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1095" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" s="1" t="inlineStr">
+        <is>
+          <t>A52100018473</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Girish Mukund Dabholkar</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>A52100018473</t>
+        </is>
+      </c>
+      <c r="D1096" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6PX%2fEL6ElL17eLvSgb%2bLQ%2fSZJwiMX41ck3A%2fejTSRdjk6SQQjlCrQKp5f2C6Nt%2bCjQm5cMrkouI%2beZZVAfHDD77Xv9I22DoJ6Bc3%2brC9YPrWGSM8ClHPDUCYw8sR%2bv9oJTzC1mJVXs7vp4RZoV1TM13mn%2fxDusEZHmxlsK03fe5Tly72wzQaBg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1096" t="inlineStr">
+        <is>
+          <t>07507317780</t>
+        </is>
+      </c>
+      <c r="F1096" t="inlineStr">
+        <is>
+          <t>Shivajinagar</t>
+        </is>
+      </c>
+      <c r="G1096" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1096" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1096" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1096" t="inlineStr">
+        <is>
+          <t>411005</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" s="1" t="inlineStr">
+        <is>
+          <t>A52100018673</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Yogesh Devidas Biradar</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>A52100018673</t>
+        </is>
+      </c>
+      <c r="D1097" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=NN7iy5McYK%2fzpzPEIIEloaqobIh88B4GHnFBhak0oUZA3UrbrZjq1lfR6voFROCR0KsAO2Mc3F225I5kBXmtnNSBzYaHceIJ3gJ8RXwwChmyRtqbYmKpyIsJi4ND1oztoeiyMlnoMOo6itz1qgmG%2b3u0ygiw%2ftEFkrCXK%2bSIpr0LdMGa8sOmbw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1097" t="inlineStr">
+        <is>
+          <t>08208394270</t>
+        </is>
+      </c>
+      <c r="F1097" t="inlineStr">
+        <is>
+          <t>Warje Malwadi</t>
+        </is>
+      </c>
+      <c r="G1097" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1097" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1097" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J1097" t="inlineStr">
+        <is>
+          <t>411058</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" s="1" t="inlineStr">
+        <is>
+          <t>A52100018458</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Satyam  Pawar Proprietor Of Fd Home Realtors</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>A52100018458</t>
+        </is>
+      </c>
+      <c r="D1098" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=smlXiuVZxiJqMhLEzMRrOf30tG59Qf6lFCCUFO6nw7lwhzJiTi0AiyQrChMVL%2frcpscyweNjn4udiFAjE9TktXumaGo78l91SciNJVA%2fi677lpyjDHV3Piu9Vq5O5UZ0HEQBOTt0U68ToFxHDmpwEw88deHmajIr%2fXd9x61LIWhtjfKemN%2feEQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1098" t="inlineStr">
+        <is>
+          <t>09860208817</t>
+        </is>
+      </c>
+      <c r="F1098" t="inlineStr">
+        <is>
+          <t>Bavdhan Burduk</t>
+        </is>
+      </c>
+      <c r="G1098" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1098" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1098" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1098" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" s="1" t="inlineStr">
+        <is>
+          <t>A52100018468</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Chandrabhano Chandrika Singh Proprietor Of Nash Convergent Solutions</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>A52100018468</t>
+        </is>
+      </c>
+      <c r="D1099" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=eMW%2f9OyKCLLhCJqTAG6iZhQzBzye579jASLxZr0UgZ7ABHaJvHJRYzAcSro23uQ9xRnXuLxowiXgondkf5n%2fNcePZTwIqzNkkzkA2No62mmlkMgVzNMwujgqP8YbEjiIE07JhuzR3ZlIRGMgRs7LZ76ERHUzsdqAJCKxGEAbEzbFJQR5eaVivQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1099" t="inlineStr">
+        <is>
+          <t>09145155979</t>
+        </is>
+      </c>
+      <c r="F1099" t="inlineStr">
+        <is>
+          <t>Viman Nagar</t>
+        </is>
+      </c>
+      <c r="G1099" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1099" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1099" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1099" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" s="1" t="inlineStr">
+        <is>
+          <t>A52100018523</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Ravi Trambak Avhad</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>A52100018523</t>
+        </is>
+      </c>
+      <c r="D1100" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=taPA%2brFw%2f6Q6jqBn2yt7%2bOEVSUlkKszT%2bv6heZMj1%2fgm0Uzc7mX6MwvLnRPziLs%2bEdYjIdmruusm1t3LInglRIbavybgMI5jkn%2bmBrnR5mYMR0uSNFspRkBwW24ByTmiKkpdxxYi%2bsyvA0I4OzCfv840ObUoZXgFUKmsXWmfiugBXOVEndIOxg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1100" t="inlineStr">
+        <is>
+          <t>08459564127</t>
+        </is>
+      </c>
+      <c r="F1100" t="inlineStr">
+        <is>
+          <t>Shivaji Nagar</t>
+        </is>
+      </c>
+      <c r="G1100" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1100" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1100" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1100" t="inlineStr">
+        <is>
+          <t>411005</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" s="1" t="inlineStr">
+        <is>
+          <t>A52100018697</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Nilesh Shamrao Tungar</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>A52100018697</t>
+        </is>
+      </c>
+      <c r="D1101" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=k2k%2btGTYJIGg0CIIQPgm7gp4NtBSHQYkmQH35ez%2fW%2fLxdeuZBfI5KCN%2fRojxS%2bNnldjSWOk1n9csv56INc1ixyY56pql4ubaCZf21SCkNpX5r6X5eCQJUH%2bnLeJv%2bX84dk883oBxbSEjOrkhVLgOoxJZjxI5rS9rpj5Suva7WMNxMD6TgELwPA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1101" t="inlineStr">
+        <is>
+          <t>09921921818</t>
+        </is>
+      </c>
+      <c r="F1101" t="inlineStr">
+        <is>
+          <t>Near Sai Baba Mandir</t>
+        </is>
+      </c>
+      <c r="G1101" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1101" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1101" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1101" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1150]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1101"/>
+  <dimension ref="A1:J1151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -57168,6 +57168,2606 @@
         </is>
       </c>
     </row>
+    <row r="1102">
+      <c r="A1102" s="1" t="inlineStr">
+        <is>
+          <t>A52100018451</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Manoj Chandrakant Shalu</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>A52100018451</t>
+        </is>
+      </c>
+      <c r="D1102" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Z%2bc26BgpOlfAZElKKvAZL%2fYsmAYphoY0DUDTIOeuG87KyhHNECliVLNOS5KaoEELFEIrZ%2bLazXefKWy2h52kCHSC%2bSMILt%2ff8bXNM6%2bk9nncIIROXQfMAJhrnvAEouYZs6XyDjYlaI%2bOxeiixpmyREm9RrV33G%2b%2f5p6kpiP3Akb6rYJhG37T5Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1102" t="inlineStr">
+        <is>
+          <t>09881061421</t>
+        </is>
+      </c>
+      <c r="F1102" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="G1102" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1102" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1102" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="J1102" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" s="1" t="inlineStr">
+        <is>
+          <t>A52100018430</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Dinesh Dattatray Khatate</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>A52100018430</t>
+        </is>
+      </c>
+      <c r="D1103" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ElE1qVYc05O%2b0GHHMIyHk8Qadn5rNJYfPf3Z%2bwc9pEHz%2bUKeKrZO7iTksco3GLoqvrQuRvEGPa0hNL3goLAiwZBp4agDDz3DDGoAVdKtHRThbavVYrPkwjUuHcaKd5xEyaStnNlOFJYDgIvtwHP8acH%2bfURmO3ipkbwmiBBNWqGExnFFpPpiQQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1103" t="inlineStr">
+        <is>
+          <t>02022065353</t>
+        </is>
+      </c>
+      <c r="F1103" t="inlineStr">
+        <is>
+          <t>Near Kranti Mitra Mandal</t>
+        </is>
+      </c>
+      <c r="G1103" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1103" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1103" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1103" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" s="1" t="inlineStr">
+        <is>
+          <t>A52100018543</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Abhijit Vishnu Jadhav</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>A52100018543</t>
+        </is>
+      </c>
+      <c r="D1104" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6dCiYB1N1UeGTTAmKPyKrCnMiNxsA674DxrG9u1XXFWqoXqCUZiR3y7wRc6Jsa%2fTL9pbQKSHQaCZqHdLGghnuRFJ9NwNMPiYXT6WpYu1lL2ewPshf36Lyda9lm9F%2bP0M%2bDt3%2fLiSoyuvXe7TDYUqsKBdG33wM7RNQGWDhhNZ7Pa7nCf2%2fCYMpQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1104" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
+      <c r="F1104" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G1104" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1104" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1104" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1104" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" s="1" t="inlineStr">
+        <is>
+          <t>A52100018452</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Abhijit Tarachand Dungarwal</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>A52100018452</t>
+        </is>
+      </c>
+      <c r="D1105" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=UX0JysoFlWWMtS%2fgQVCua4xiAG41%2bhlGXavELR62BTJlRdu4agcK5O4WUgBdsgdy8LGjFUiG7tOANUw7VhWUhaYsvYZ8HpiOo3ijyracJhW4YbG80lNbQ70qdYXz78Ylk0nNMRj2VPql2wPbZ1vJMqKac6Lhnp91ulc1do8FTKEYxUp%2f2p7DmQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1105" t="inlineStr">
+        <is>
+          <t>02026963108</t>
+        </is>
+      </c>
+      <c r="F1105" t="inlineStr">
+        <is>
+          <t>Sukhsagar Nagar</t>
+        </is>
+      </c>
+      <c r="G1105" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1105" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1105" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1105" t="inlineStr">
+        <is>
+          <t>411043</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" s="1" t="inlineStr">
+        <is>
+          <t>A52100018914</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Satpal Rampalsingh Mourya</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>A52100018914</t>
+        </is>
+      </c>
+      <c r="D1106" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2fk1hgMkh6jKOMmZFy87RYFtyq0Zkud2Jm%2f90tRw35dvtkU28TAH6UcVmpVKbzjHRHDtuMzy3mpDh8fnXnjqkHCRd9Wfvjab7bZLxv%2brYod%2fciFfPj6CzjvOk4aLBxIOS5okVn7QGYWG20PJTTJbXU0yv8KvA9p7JWuNSp5ZKUi8SylGesDfD9A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1106" t="inlineStr">
+        <is>
+          <t>02066763226</t>
+        </is>
+      </c>
+      <c r="F1106" t="inlineStr">
+        <is>
+          <t>Hinjewadi</t>
+        </is>
+      </c>
+      <c r="G1106" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1106" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1106" t="inlineStr">
+        <is>
+          <t>Hinjavadi (Ct)</t>
+        </is>
+      </c>
+      <c r="J1106" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" s="1" t="inlineStr">
+        <is>
+          <t>A52100018611</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Jigarr Jayant Vyass</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>A52100018611</t>
+        </is>
+      </c>
+      <c r="D1107" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Ry3xHaxcny%2ftLWiqRsn3XAv%2f0wzqdPF7kaLUmCGnIJYSrpb%2f%2fBik%2fOfUBHkQXsmI2RDeMsxa9xh5%2f5BV6wQqISMBW66hOyXecCqrDKtkmNjc37J6D8RWQd9v7rPWNk7EvKgtz9%2f9h4zTj%2fHD5848qv5zUIOIGAk%2fN89loW5cnrs0Z%2ffoyvfy2A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1107" t="inlineStr">
+        <is>
+          <t>02065106510</t>
+        </is>
+      </c>
+      <c r="F1107" t="inlineStr">
+        <is>
+          <t>Chakan, Midc</t>
+        </is>
+      </c>
+      <c r="G1107" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1107" t="inlineStr">
+        <is>
+          <t>Khed</t>
+        </is>
+      </c>
+      <c r="I1107" t="inlineStr">
+        <is>
+          <t>Bhamboli</t>
+        </is>
+      </c>
+      <c r="J1107" t="inlineStr">
+        <is>
+          <t>410507</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" s="1" t="inlineStr">
+        <is>
+          <t>A52100018733</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Umeash Vasant Gaikwad</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>A52100018733</t>
+        </is>
+      </c>
+      <c r="D1108" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=AOvOxIIHo1FEIEZPXRQLWYr2%2b%2bGDm%2fQMPqPC5KoUq5aJXZBI5QLHiAy0dTSyTYrULYAVeOFCrfpKZm6dqD8LY8wQ9HhqKZB3proQSzw1RjlLN7ervtTd1n1T0%2bZvHjyS%2brdNNbUca%2bXW08c4g2sZhSTt8EyZbv7PQPBx0LUdrD0kSDFNu8DBTg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1108" t="inlineStr">
+        <is>
+          <t>09579007377</t>
+        </is>
+      </c>
+      <c r="F1108" t="inlineStr">
+        <is>
+          <t>Indrayani Nagar</t>
+        </is>
+      </c>
+      <c r="G1108" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1108" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1108" t="inlineStr">
+        <is>
+          <t>Bhosari</t>
+        </is>
+      </c>
+      <c r="J1108" t="inlineStr">
+        <is>
+          <t>411039</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" s="1" t="inlineStr">
+        <is>
+          <t>A52100018507</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Sameer Vinayak Ubale</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>A52100018507</t>
+        </is>
+      </c>
+      <c r="D1109" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=y0zM4Mz1ic4HE2w6wngYbhtNN5kV%2ff%2fslBWJQLS8Pli%2b46GYY9HAl3mCKq7P2FPK3JNY3M%2fHzSoPFElDxEB0q39f30muDYBytUDcfHX%2bPIu9geDzk65mVYbd%2bsHORfPjZlWizsSRTc5gkdRypURtmQAybAvQ8fwbPAeF%2bP28lgaWEXDqXK%2f5nw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1109" t="inlineStr">
+        <is>
+          <t>08669992323</t>
+        </is>
+      </c>
+      <c r="F1109" t="inlineStr">
+        <is>
+          <t>Dehuroad</t>
+        </is>
+      </c>
+      <c r="G1109" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1109" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1109" t="inlineStr">
+        <is>
+          <t>Dehu Road (Cb)</t>
+        </is>
+      </c>
+      <c r="J1109" t="inlineStr">
+        <is>
+          <t>412101</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" s="1" t="inlineStr">
+        <is>
+          <t>A52100018484</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Eakanath Baliram Igave</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>A52100018484</t>
+        </is>
+      </c>
+      <c r="D1110" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Vua45c%2b40m3cjDP6bkogoy6Giiarf4y4oOQLeZJy1bHBPK%2bhg%2brXBfr0hIK%2fCEJUQl3GLcMkNNb8pCW%2fZDnyzx4EqrGNc8MXcou4Tedr9JHcdoOb9l3NPQSlPgxL%2f9EooA4R4bsVN2TaSDwyiHspQ0OhXKAXCOs3UBVfw1qKjf2PatxW6LKzGw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1110" t="inlineStr">
+        <is>
+          <t>09284839027</t>
+        </is>
+      </c>
+      <c r="F1110" t="inlineStr">
+        <is>
+          <t>Bhekrai Nagar</t>
+        </is>
+      </c>
+      <c r="G1110" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1110" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1110" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1110" t="inlineStr">
+        <is>
+          <t>412308</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" s="1" t="inlineStr">
+        <is>
+          <t>A52100018989</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>G: Corp Developers Pvt. Ltd.</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>A52100018989</t>
+        </is>
+      </c>
+      <c r="D1111" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=L8o6rG3HguvT04HKAo%2fu3thz%2f0JHjCLMXDURiXuYyB1hWYdV6XKcAjXy9mFkDbZmGcjkY5or3P8kVtosdJTn0SXiBaQQf15Hy39yYPP69M9ba08X7fiZO6mnskrNqo3eDOgx%2f4c6SbhIyd31adPpfnv8YQvLQRSwgQR8mBKcIpqn1xJCnu0ffg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1111" t="inlineStr">
+        <is>
+          <t>02049046555</t>
+        </is>
+      </c>
+      <c r="F1111" t="inlineStr">
+        <is>
+          <t>Camp,</t>
+        </is>
+      </c>
+      <c r="G1111" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1111" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1111" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1111" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" s="1" t="inlineStr">
+        <is>
+          <t>A52100018501</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Fmg Real Estates Ltd</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>A52100018501</t>
+        </is>
+      </c>
+      <c r="D1112" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CulgWC8sPPyqqb09soWGBuvc62CGx3qxPa3kpaKzdOmo74edaz4P9EZ%2bNTy%2fBytWVqPh7eTOTVo%2f%2blCkcVQtjo2DsiCWNTB5tO7sNFux2dwgXro3A86dBGzgP9AhQhbb0Kv%2bgWhmW5E6ehKtwhgnKR96j8e5DHpZ%2fB1VPvB0YQ8cR97G0%2fZt2A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1112" t="inlineStr">
+        <is>
+          <t>09311705433</t>
+        </is>
+      </c>
+      <c r="F1112" t="inlineStr">
+        <is>
+          <t>Down Town</t>
+        </is>
+      </c>
+      <c r="G1112" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1112" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1112" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1112" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" s="1" t="inlineStr">
+        <is>
+          <t>A52100023070</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>The Brand Lance</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>A52100023070</t>
+        </is>
+      </c>
+      <c r="D1113" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=oamRVutuiAW7AxyrprK1rZsAX1wHe095HGDMdsXEPx1FT%2b3Uokr3iscEdZUD7iNgcpU5yCeRgFH4HZqs6KlIoTuj7zvRCj3Ng7691lz%2bV8SQ%2fs9YLdlGj1wiTlYWun7KDmryCq8SX%2fuf1lDOb82xdheAurevJU1vGvYLjePIolJ%2bZEXwbGn8YA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1113" t="inlineStr">
+        <is>
+          <t>02026717033</t>
+        </is>
+      </c>
+      <c r="F1113" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G1113" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1113" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1113" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1113" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" s="1" t="inlineStr">
+        <is>
+          <t>A52100018594</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Pooja Ravi Shetty</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>A52100018594</t>
+        </is>
+      </c>
+      <c r="D1114" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fGDZynp1cjUgjK%2bHpsVXx4KnNqTM9MWpEE8uc7isxOHV63MURiuJcePBjRBqH6SJtarWULlzLAkx%2fyHSfx%2bub%2fCLmHIMWpStQc1E5hhVc5EbqgqXvZf9B%2byOy9DCZWqHSWqD9XOqvqhl12vHLHYuf8u8rfhzhUCR3WkRnXF8CZCueoTNBnIqzw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1114" t="inlineStr">
+        <is>
+          <t>09673387790</t>
+        </is>
+      </c>
+      <c r="F1114" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="G1114" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1114" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1114" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1114" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" s="1" t="inlineStr">
+        <is>
+          <t>A52100018535</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Joharsingh  Malhotra</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>A52100018535</t>
+        </is>
+      </c>
+      <c r="D1115" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=oLO%2fGuxgXX3U62iZ%2buygWyyLgDdi23Sl7yq0%2fV4bU7mcoKkz7WIBsNInx0YrRNcYLh3MfvAgj8P6%2brEOKCxgHfa74qypb%2fQz3J7Hf6mnRRqPABbsjcNjJJ8IRQ95QfOpejmhNfltzD1N5oMVAJ0ooI9Zmr3MjqltJmDqiTma14PWTczzB%2fsPqw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1115" t="inlineStr">
+        <is>
+          <t>02212345678</t>
+        </is>
+      </c>
+      <c r="F1115" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="G1115" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1115" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1115" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="J1115" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" s="1" t="inlineStr">
+        <is>
+          <t>A52100018498</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Sanjay Dattatray Jagtap</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>A52100018498</t>
+        </is>
+      </c>
+      <c r="D1116" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=guTplmuJ33mf8ovmiVIBxv8JXmchMVOvzBhlKF6ez6NhspeaKio4s%2fdJv8qQoLIKnIDz9784GmRwNGwM%2fm5j8DKnvp0mNOglZD%2fgduj14qH3fSQw98HvCXDAEnxs%2fOG6JPCZhYlVjLpTUoVVDJeGyc0E%2f7ltEW%2f8F%2bVCQpCiDE%2b%2bzbwL96XZIA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1116" t="inlineStr">
+        <is>
+          <t>08149230372</t>
+        </is>
+      </c>
+      <c r="F1116" t="inlineStr">
+        <is>
+          <t>Talegaon Dabhade</t>
+        </is>
+      </c>
+      <c r="G1116" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1116" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I1116" t="inlineStr">
+        <is>
+          <t>Talegaon Dabhade (R)</t>
+        </is>
+      </c>
+      <c r="J1116" t="inlineStr">
+        <is>
+          <t>410507</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" s="1" t="inlineStr">
+        <is>
+          <t>A52100018803</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Murad Hussain Tol</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>A52100018803</t>
+        </is>
+      </c>
+      <c r="D1117" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KHEcDwNKP09y6Xbcc%2f60PzbryN5Fzq6Vp7IHhsPdospyrcKy7HcVnHpA%2bn5uQlzgtVqTWQKbwfLTlm05ZuGwyEnM55Epw%2fo%2fn1ZE76ccLOTuJyosG%2foEINji9Aob3DYWMFkQjvaAoVekw8GQzkmYC%2fe7tNtT8ZMVYHXbzNUErxOs9NMsu5wiEA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1117" t="inlineStr">
+        <is>
+          <t>08830072187</t>
+        </is>
+      </c>
+      <c r="F1117" t="inlineStr">
+        <is>
+          <t>Kondhwa Budruk</t>
+        </is>
+      </c>
+      <c r="G1117" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1117" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1117" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1117" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" s="1" t="inlineStr">
+        <is>
+          <t>A52100019302</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Pranav Dilip Gupta</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>A52100019302</t>
+        </is>
+      </c>
+      <c r="D1118" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=jXnQ860fUzWF7gqeh%2ff7Bd9r7NxgV7rWVWBqiNHhMXLwLbRZtzY%2fUGsjAbZQkqiqyWzI9x6ZIyZK3jvhb1VImWGz34avqz1ZxB%2bjJxZ%2bZALxD8VlEWkwwrQTOLwmJS0q7RuvZbiPSpVFODgeMQYZ6REiudT5zWDtoFrF1GXlYNUnoufmWXLpXw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1118" t="inlineStr">
+        <is>
+          <t>02027652775</t>
+        </is>
+      </c>
+      <c r="F1118" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1118" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1118" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1118" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1118" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" s="1" t="inlineStr">
+        <is>
+          <t>A52100019236</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Siddhant Dilip Gupta</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>A52100019236</t>
+        </is>
+      </c>
+      <c r="D1119" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=WItAidUx0FTvQgz%2bfhxbbzap8rCJqbbUcG0%2ffvi7vJWD9hQ%2baazAwuwGNDqVUaocoxvjE6e8qWPlAkThPTTOjN5m6zBBVbcXjjtl7wy6oPImGm4B96yqgmmdNVDQbp%2blXlYwlIzXEopq3jcdu7qCGTHvWublbkDNadicWFwLmGDwtTTmbHrYhQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1119" t="inlineStr">
+        <is>
+          <t>02027652775</t>
+        </is>
+      </c>
+      <c r="F1119" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1119" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1119" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1119" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1119" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" s="1" t="inlineStr">
+        <is>
+          <t>A52100018732</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Rohan  Chaturvedi</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>A52100018732</t>
+        </is>
+      </c>
+      <c r="D1120" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Nu90tBo%2fkP1%2fRtVX%2f2WmJ%2bgfGbhJiC0gyq1qQ%2bMI4h4SqAcVOFclu54p1GsYRV97%2b5h5bcvnCM4N033H7za%2fWG4vT5lkabwFrziosF2ItEOk3aPrC8SOJBWeBSkJPJgoOnHkEtSl%2b%2fWwkB6QWDQ1XUkS6%2b9U7YDEB9Y3Wu%2fuB7rMp7VpQh3ZNg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1120" t="inlineStr">
+        <is>
+          <t>02026870347</t>
+        </is>
+      </c>
+      <c r="F1120" t="inlineStr">
+        <is>
+          <t>Manjari</t>
+        </is>
+      </c>
+      <c r="G1120" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1120" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1120" t="inlineStr">
+        <is>
+          <t>Manjari Bk</t>
+        </is>
+      </c>
+      <c r="J1120" t="inlineStr">
+        <is>
+          <t>412307</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" s="1" t="inlineStr">
+        <is>
+          <t>A52100018945</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Smita Samuel Chavan</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>A52100018945</t>
+        </is>
+      </c>
+      <c r="D1121" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=JYXbouZ8RqUmKNm%2fayu3Q5VUZ3T2o8nRjp76QRMMfG3RKsDXgcMA%2fxczowzA3crNAEmeYe%2bNv04HdBuVN8PvB1i2wQBmmi9diE2mMwJkyRMzncK3JDgt5yqsNmTpustSlOSWEFAus6qpEVqeutUwCSHV%2fHnLXBR9jO1cm%2bE3foG6Ab5ysu6tCw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1121" t="inlineStr">
+        <is>
+          <t>09921215605</t>
+        </is>
+      </c>
+      <c r="F1121" t="inlineStr">
+        <is>
+          <t>Ramtekdi</t>
+        </is>
+      </c>
+      <c r="G1121" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1121" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1121" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1121" t="inlineStr">
+        <is>
+          <t>411013</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" s="1" t="inlineStr">
+        <is>
+          <t>A52100018766</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Alka Arvind Chapalge</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>A52100018766</t>
+        </is>
+      </c>
+      <c r="D1122" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=yUYjWCRpl%2f1P5OmUmV7va5uV%2bzVpyv5hLw%2fAHk1g26N0la0WL6yddDm3d93A4Io4aneVHDvr1C6%2fc8Vp5sUI34ywy81G4NX136egbU9F0cpegFhBIzXMiPW1ShEqj4rtSJ3TQ67%2fEzrGC2pV%2f0CJUzp6WIkZPPE3QWNHr4zYC%2f4uSvT%2b%2fpQG6Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1122" t="inlineStr">
+        <is>
+          <t>09226121500</t>
+        </is>
+      </c>
+      <c r="F1122" t="inlineStr">
+        <is>
+          <t>Balewadi</t>
+        </is>
+      </c>
+      <c r="G1122" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1122" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1122" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1122" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" s="1" t="inlineStr">
+        <is>
+          <t>A52100018493</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Nandkishor Bhagawtrao Sampate</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>A52100018493</t>
+        </is>
+      </c>
+      <c r="D1123" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wW5QLZDRhvNGXhKj%2bCQuJ7Lr6pTxjXJkWucynJ%2b7t7vtQH%2blRupolLtuJ7%2fNVGse%2fEh9pse2aYV9yw9amjrJuUydxvA7Ib7XTEj04ePhDr75P%2b%2f8a%2fG0BYwdUc9wOfGRf4J2q%2f03viTT%2fRiBuhye1nQzavPUYQFeXywUfUUVIlIXs0jCMOXLNg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1123" t="inlineStr">
+        <is>
+          <t>02041000000</t>
+        </is>
+      </c>
+      <c r="F1123" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1123" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1123" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1123" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1123" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" s="1" t="inlineStr">
+        <is>
+          <t>A52100018672</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Nikhilesh Kumar Dubey Proprietor Of Ashoka Properties</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>A52100018672</t>
+        </is>
+      </c>
+      <c r="D1124" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=0iULsENEsUiTOf7Oz99KdUCI3lP%2fnWx955LMB%2bmI9BlIE3hHb%2bqJcggONDiSutnn3A0yeW3WFJyYF9lA9YsXgmpQ2qoHkY8C9F0ppv6OH%2fYh4txWxWTdwDeFMaee0dMvAZz1KMqt4Yb4qU9BoMMHohc%2bY246jlud1GD4ppbOMca2WmTdNgifhQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1124" t="inlineStr">
+        <is>
+          <t>08237759239</t>
+        </is>
+      </c>
+      <c r="F1124" t="inlineStr">
+        <is>
+          <t>Sarkar Chowk ,Atul Nagar</t>
+        </is>
+      </c>
+      <c r="G1124" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1124" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1124" t="inlineStr">
+        <is>
+          <t>Marunji</t>
+        </is>
+      </c>
+      <c r="J1124" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" s="1" t="inlineStr">
+        <is>
+          <t>A52100018561</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Narayan Shankar Sabale</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>A52100018561</t>
+        </is>
+      </c>
+      <c r="D1125" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=f4%2b7NAU1fEe0ZNmILYp30DBcsCTYnDlfVHR%2b7duZjNCdAV0YYtQxfbvxksoQFfoFTaB9c6n4%2b1JvtRg%2b35D4a3A38XbBAppSqjyGUkJeaEPg258%2b2kyGMVXNCmZvTHsCyi%2biTJn21kZpoVIdCi6vK3z6abuFD2Ru3ac3mCfCA1Jjv8KZ7wtGvA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1125" t="inlineStr">
+        <is>
+          <t>09822842389</t>
+        </is>
+      </c>
+      <c r="F1125" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1125" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1125" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1125" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1125" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" s="1" t="inlineStr">
+        <is>
+          <t>A52100018725</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Sadashiv Laxman Panchal</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>A52100018725</t>
+        </is>
+      </c>
+      <c r="D1126" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=b%2bff7jTMnPETEeZQw4jV55%2fkk33HDSzP%2bgCcncxsCoCDJbOn2wxYNTWarmgq2A3UnFyyKCDiPRGApaZ9lSlj84QmqbS3GD9p4VVD%2bM8uVwTrc3H74CNQyzXhGfva46mmM7VWxWULfrudJbcrv0E485LP2z48WRX1fd4ZL2Bi7u%2b0mhkQ3wFY9g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1126" t="inlineStr">
+        <is>
+          <t>09923316229</t>
+        </is>
+      </c>
+      <c r="F1126" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="G1126" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1126" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1126" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J1126" t="inlineStr">
+        <is>
+          <t>411058</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" s="1" t="inlineStr">
+        <is>
+          <t>A52100018983</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Nishant Laxmanrao Dighade</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>A52100018983</t>
+        </is>
+      </c>
+      <c r="D1127" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2Tct4MSzI1dEkLQT9DLGpVjpt98MJ4DbFsOZmGdBEU3S%2ftbqnKNdQQNvnfj1fG21dtHHJB1jhCPcNyR8c0zILzuT%2bHC8SJU3F1xnK2g9TxLI3t15Fg7ywTC%2bjU3nZcgVvan%2briyQwOamVliGbi%2bmNP69iH92d7z6Igiq5JjJzQa4WDsfxf0Dzw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1127" t="inlineStr">
+        <is>
+          <t>09028739525</t>
+        </is>
+      </c>
+      <c r="F1127" t="inlineStr">
+        <is>
+          <t>Wanowarie</t>
+        </is>
+      </c>
+      <c r="G1127" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1127" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1127" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1127" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" s="1" t="inlineStr">
+        <is>
+          <t>A52100018556</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Sumit Ghanshyam Swami</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>A52100018556</t>
+        </is>
+      </c>
+      <c r="D1128" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=k0bAWrHcKrd26zHRKLQ5ff0bnlTLyzBYQxO%2bYx%2bR4Q7po6jlW3Q78E%2f2qcTdxW2PDui72GeUs1foUaCtVPWmitq3XPT0Dp2DzaHVeCkq%2fEczJIAns4MsBJ7zndTnODgpFlCxnmA5WZilp59aNeMHnVhRE9troDHoisDLgfHIGEIBybq1I74DvQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1128" t="inlineStr">
+        <is>
+          <t>08668455087</t>
+        </is>
+      </c>
+      <c r="F1128" t="inlineStr">
+        <is>
+          <t>Viman Nagar</t>
+        </is>
+      </c>
+      <c r="G1128" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1128" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1128" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1128" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" s="1" t="inlineStr">
+        <is>
+          <t>A52100018540</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Indu Narendra Mansharamani</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>A52100018540</t>
+        </is>
+      </c>
+      <c r="D1129" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=zjJQIs87RRSrYlXCnVLmZ%2ff%2bpbm2in0id5eysTuXhmpnn8AQFak8UEBH1pjDKRlOPqsU0pVUtOOMr4rOIVCqqNcJl9DgqPzzCn5xqKG2u63zoCYMCB8VPJOZUkbxkLyvrsfDVjGW65azmQwoJMvonl7kXHvdwAwRe8mqRgxX1qvMJ5Jvf8l%2bTQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1129" t="inlineStr">
+        <is>
+          <t>02026687801</t>
+        </is>
+      </c>
+      <c r="F1129" t="inlineStr">
+        <is>
+          <t>Viman Nagar</t>
+        </is>
+      </c>
+      <c r="G1129" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1129" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1129" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1129" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" s="1" t="inlineStr">
+        <is>
+          <t>A52100018746</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Anil Laxman Mugale</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>A52100018746</t>
+        </is>
+      </c>
+      <c r="D1130" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=vkMV7KPhTiN6UrKRH7An%2bsAekTMGEOCpSi%2btSDvlLAnFap8kIk6jIxmVjK4nxf7H52GmE5m9I8XkI1WShgiYosMalZcOlzqSefForSQHdcbgy%2f1mT4CkzmwK5OaM%2b9KDmn505QTpt9KjXNZfYV19C8HV4L1LSYywFQl3kNcWCTDiuudOoz2w4A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1130" t="inlineStr">
+        <is>
+          <t>02024458768</t>
+        </is>
+      </c>
+      <c r="F1130" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="G1130" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1130" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1130" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1130" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" s="1" t="inlineStr">
+        <is>
+          <t>A52100018577</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Vishwesh Madhukar Kulkarni</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>A52100018577</t>
+        </is>
+      </c>
+      <c r="D1131" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MY11c7Wvydkq8GQKEfogMn23CGgcCwILdWs3VNBgT1uTSo5%2bP07QsNdA3P4SSmdmCru8aIyvYKyzx34w6sXCJ3arqyANmKSI0Wbs2hug3X9ooB%2f%2f%2fgCB8Nzw07UiUkJktIp2D3%2bLP0t10BN1dP9kaxYprdRMX0lhfyKwzGCTg02HtAFDtfo%2fsA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1131" t="inlineStr">
+        <is>
+          <t>09028022747</t>
+        </is>
+      </c>
+      <c r="F1131" t="inlineStr">
+        <is>
+          <t>Lagadmala</t>
+        </is>
+      </c>
+      <c r="G1131" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1131" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1131" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1131" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" s="1" t="inlineStr">
+        <is>
+          <t>A52100018602</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Sanjay Basappa Kumbar</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>A52100018602</t>
+        </is>
+      </c>
+      <c r="D1132" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=erJOdrRMAcZBbVd1Mh1W4Ki0fT7pmTMBSW2DzjwGROpWD9fdaxxxttXJNfpokKdbrlgzeDHJz9%2f9BjzypL14vxKGSiBAjY4AsiI45lNDwGhRm9Wt4MEcIUudEDWhSmzbDIkAEidaDk%2bdYJOLK%2fQS%2bMufOXQrP66hsposa8VJZVBz%2fM3F5YoTAw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1132" t="inlineStr">
+        <is>
+          <t>02000000000</t>
+        </is>
+      </c>
+      <c r="F1132" t="inlineStr">
+        <is>
+          <t>Wanowarie</t>
+        </is>
+      </c>
+      <c r="G1132" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1132" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1132" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1132" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" s="1" t="inlineStr">
+        <is>
+          <t>A52100018704</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Ajay Vasant Patil</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>A52100018704</t>
+        </is>
+      </c>
+      <c r="D1133" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=OMNO6YbNgvD6KHFZRTPDM9XmEcdSM7WP%2bDyiDcgj4ewxyiu8uWIN0kVmwFp%2ffw33LPUpZC1Tr4RwC7hlYSEVM0MOZDfasTSqe7k7oRy6hlG1b5sjHAIZKUDCrsNWneRWaw3gaoyQXppTaMIwnF04xr0pvTRKYXxt3LXMPB6XbniSNjrWA0mN1w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1133" t="inlineStr">
+        <is>
+          <t>02046700833</t>
+        </is>
+      </c>
+      <c r="F1133" t="inlineStr">
+        <is>
+          <t>Bijali Nagar</t>
+        </is>
+      </c>
+      <c r="G1133" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1133" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1133" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1133" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" s="1" t="inlineStr">
+        <is>
+          <t>A52100013285</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Sameer  Jain</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>A52100013285</t>
+        </is>
+      </c>
+      <c r="D1134" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=T63ii2Ws8eH3w8q76183puFkiV1ILKDQMFrAMGBmWcXHBrPpNbDM%2ffFBdQFOrtX%2fGqj1COR%2bUevPPgeBtVqHw6ptaIL0GIyyC3io66Ze5aGeB2yU%2fQlS7UzCPsmwXPpv63jDj%2fyCJRqkH6B9tmglSKH5gWh8KYIIVNbdOMiHjgxMmjv70H5EJA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1134" t="inlineStr">
+        <is>
+          <t>02041215001</t>
+        </is>
+      </c>
+      <c r="F1134" t="inlineStr">
+        <is>
+          <t>Koregaon Parl</t>
+        </is>
+      </c>
+      <c r="G1134" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1134" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1134" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1134" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" s="1" t="inlineStr">
+        <is>
+          <t>A52100019368</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Sheetal  Pardeshi</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>A52100019368</t>
+        </is>
+      </c>
+      <c r="D1135" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=kMoltikgkx1JoVd32EY5vMtdf0kMUsB0lGk9fo7TpBfpKS6KI9Y0zcOB41TnfZaVsO%2bw9OlGhZExCR43QRSKpB8vOop0NvbFkS0EPvWpWNNkQzD9aEx2L8Mueps9dPyc8ej13WCPgaZsFHq8CztTx%2b7PfixqGi5B6jOwJM7XBvBs05IE2e8tkA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1135" t="inlineStr">
+        <is>
+          <t>02027652775</t>
+        </is>
+      </c>
+      <c r="F1135" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1135" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1135" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1135" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1135" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" s="1" t="inlineStr">
+        <is>
+          <t>A52100018552</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Pravin Bapurao Gaikwad</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>A52100018552</t>
+        </is>
+      </c>
+      <c r="D1136" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CJ8553PmFtm8mRzRLRkogNtA12k7C8r7XXsq4CBG2lkdMMctrhewnvBm8OuW6NwpXLly4ErpG4ezyK42wC8FOJb%2bsg447ZYIUQ8TO%2fP7duVCNzsUUF3OmNL2ZLHRFjDt3sRDHmzKUdlbjRSJA6HeAv15g09nL%2braFzWojY1uhE0iaCrh1P%2fa4Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1136" t="inlineStr">
+        <is>
+          <t>09890237001</t>
+        </is>
+      </c>
+      <c r="F1136" t="inlineStr">
+        <is>
+          <t>Vishrantwadi</t>
+        </is>
+      </c>
+      <c r="G1136" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1136" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1136" t="inlineStr">
+        <is>
+          <t>Vishrantwadi</t>
+        </is>
+      </c>
+      <c r="J1136" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" s="1" t="inlineStr">
+        <is>
+          <t>A52100018633</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Ajay Jethalal Kukadia</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>A52100018633</t>
+        </is>
+      </c>
+      <c r="D1137" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=0o1aGhiJPQmTCI7Q5C5%2bTRnFmPYThhSkWfjrphDczl4C5ghI4F3Q1cqdDwTH7PAKTxBy9p%2bRYg6jAaf8E5DyidvTv3EsytoEoikkDRB1uPQotWucZxCFAGoFd6E91RQRK%2b2HFx3GQFDNBYqatXLZMlfE%2bdBdAEW4DWqQkhUIXoneNUqI4IQKRg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1137" t="inlineStr">
+        <is>
+          <t>09607791166</t>
+        </is>
+      </c>
+      <c r="F1137" t="inlineStr">
+        <is>
+          <t>Vadgansheri</t>
+        </is>
+      </c>
+      <c r="G1137" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1137" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1137" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1137" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" s="1" t="inlineStr">
+        <is>
+          <t>A52100018595</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Krishna Sunil Kumar Sugla</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>A52100018595</t>
+        </is>
+      </c>
+      <c r="D1138" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=NxbLh3GpPD0F7CoLpUE1cJgRM%2b5vjAlnJVnZTAY7hY05yuU6PKjJMb12%2fvfgNCIpBM1OVnEb5m8fF%2bqT%2bE9k9NEpH3k%2brrRzde5oQmGU0WHSBRudA6OXfvo3YPv%2fAXNPn0asMJ9teWe%2fwyCYRi8eEgkxItv19Ov5bt8Z%2fGn0eVzU8%2fvidZFRMg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1138" t="inlineStr">
+        <is>
+          <t>08888990087</t>
+        </is>
+      </c>
+      <c r="F1138" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1138" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1138" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1138" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1138" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" s="1" t="inlineStr">
+        <is>
+          <t>A52100003385</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Manas Madannlal Parik</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>A52100003385</t>
+        </is>
+      </c>
+      <c r="D1139" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2z9%2fkrS3uqYj1VNMDOAaw%2bLyHVz8rUWL7e7g5Q%2bPTTThsoYAyYyh0ZfJCr6o6cdr%2ffLapEWw6EVZ%2bRvItZ9J3JmmQbgktXp9j114KwCiFXYL1bWEHyluJl93PPHXCN8yJbEKSM7w9cjb3SB%2frDlCChlH0kOHDqvCVwX%2brCxTat7rPeSFJDJAoA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1139" t="inlineStr">
+        <is>
+          <t>09850633126</t>
+        </is>
+      </c>
+      <c r="F1139" t="inlineStr">
+        <is>
+          <t>New Sangvi</t>
+        </is>
+      </c>
+      <c r="G1139" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1139" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I1139" t="inlineStr">
+        <is>
+          <t>Sangavi</t>
+        </is>
+      </c>
+      <c r="J1139" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" s="1" t="inlineStr">
+        <is>
+          <t>A52100018618</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Sumeet Ramesh Shinde</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>A52100018618</t>
+        </is>
+      </c>
+      <c r="D1140" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ZicMG%2b7nKbnApo6%2fWU7BJlwRtIKdA7z7ilcTVJRS4uheooEog%2fL%2bacSai918J6vdZVNNPPQBpI6BqqB%2bVHkBz%2bktyEB4093lSsJuzW7j1YArPQSlm3gKgr%2fkMYfcrPXAZ8r13ljggzLQVNEWyDJ9bsfcCyGgrQzxQVBG9L7YSid%2fOe1aq07e3A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1140" t="inlineStr">
+        <is>
+          <t>02027515575</t>
+        </is>
+      </c>
+      <c r="F1140" t="inlineStr">
+        <is>
+          <t>Kivale</t>
+        </is>
+      </c>
+      <c r="G1140" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1140" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1140" t="inlineStr">
+        <is>
+          <t>Dehu Road (Cb)</t>
+        </is>
+      </c>
+      <c r="J1140" t="inlineStr">
+        <is>
+          <t>412101</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" s="1" t="inlineStr">
+        <is>
+          <t>A52100002287</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Vinod Inderlal Jessani</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>A52100002287</t>
+        </is>
+      </c>
+      <c r="D1141" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=py5FET%2bdOM8R05F%2bj4hpZdS%2fjzG9tMz39c36RzAnnRt3LuOUtyANsGsOjX%2fK8gQ8oRQ%2fZkvcYM5vBdTRGfU2IbYxiRdKnPedGD%2bcethh%2bQlhXREGMN%2bCfO2JfkD2F4wX5XxVA4nMwKSx3bdl5ZIHD%2fy9oTOhEkIwP19wQZdGosX1N1krKDvpKw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1141" t="inlineStr">
+        <is>
+          <t>02026341486</t>
+        </is>
+      </c>
+      <c r="F1141" t="inlineStr">
+        <is>
+          <t>Camp</t>
+        </is>
+      </c>
+      <c r="G1141" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1141" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1141" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1141" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" s="1" t="inlineStr">
+        <is>
+          <t>A52100002562</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Ravindra Vitthtal Tapkir</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>A52100002562</t>
+        </is>
+      </c>
+      <c r="D1142" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=eNV3RthwWyTzNGK2pLpX41no0QcEy41cqI273Iw%2bAUhi%2fuqqt%2bUGTkGQPLbPHwN%2fCUTHhWC3qHfQTREUOFD9Hr82%2fpVclpiccNfj1wZk6%2fN40GH73%2bvZLEJGoxyYYxsXJJ3x5R6xzAHpeFqbQP41MSjcMPwAQaQerU3Dxz22Lc0aw69NqtJ1TA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1142" t="inlineStr">
+        <is>
+          <t>02027011289</t>
+        </is>
+      </c>
+      <c r="F1142" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1142" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1142" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1142" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1142" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" s="1" t="inlineStr">
+        <is>
+          <t>A52100002815</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Sailesh Motilal Nain</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>A52100002815</t>
+        </is>
+      </c>
+      <c r="D1143" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CovYV73L4d7hWAsZOcFjJWJ8%2b%2fs3fXjNu%2fRtzmEN2vKGc5zhTehQAJWud8TUgSsDDpYD4pBcfcDLdkBIqdsY0HSSPhmQNN9Gb0FYhz%2fSywgJu3O%2f5264lADPaFqISA5qGFP5M%2bKBiI0PhI%2fUROiA%2f31SaFcArWOZ77W59R6lRDLpT4d%2bUS6oWA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1143" t="inlineStr">
+        <is>
+          <t>08806273428</t>
+        </is>
+      </c>
+      <c r="F1143" t="inlineStr">
+        <is>
+          <t>Koregaon Park</t>
+        </is>
+      </c>
+      <c r="G1143" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1143" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1143" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1143" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" s="1" t="inlineStr">
+        <is>
+          <t>A52100002277</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Suraj Prakash Kamale</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>A52100002277</t>
+        </is>
+      </c>
+      <c r="D1144" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=kmX44um60d2EaKSJ8LYIjB0b%2fZMuNWUTmzbuQSUdXe9tQOKuqGcnp0f9siPxkOs7HsTf2dZ2RUVVxBBMyoGdd%2bSHK5A56YuXVpIgI%2bu%2bBsRhRHVdEvAYWzBw2eQbB61u4MWIXBXcjSmMPnhEPqUJJt20%2fKT4GMKjORRsi34HYOo%3d</t>
+        </is>
+      </c>
+      <c r="E1144" t="inlineStr">
+        <is>
+          <t>02025881593</t>
+        </is>
+      </c>
+      <c r="F1144" t="inlineStr">
+        <is>
+          <t>Hinjwadi</t>
+        </is>
+      </c>
+      <c r="G1144" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1144" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1144" t="inlineStr">
+        <is>
+          <t>Hinjavadi (Ct)</t>
+        </is>
+      </c>
+      <c r="J1144" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" s="1" t="inlineStr">
+        <is>
+          <t>A52100011345</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Vipin  Deshmukh</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>A52100011345</t>
+        </is>
+      </c>
+      <c r="D1145" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KCSXtRBMUiCWBv07eyDyxSoAoe%2feynvMOYlgULFszzWyZ%2bud2b5Wk9NkRIYTVLlbVHM5vZudOqP%2fmNeN4NDVTmjb6LQ1%2f%2fo65p1QUY0zoo5ejGREElYRcL8bApIVQi0y7H67u1TZdRBJnLvBslv0M7g6W3gHSmvkKRyLf8yC2WUdLKL1E%2fzh9A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1145" t="inlineStr">
+        <is>
+          <t>08407911234</t>
+        </is>
+      </c>
+      <c r="F1145" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="G1145" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1145" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1145" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="J1145" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" s="1" t="inlineStr">
+        <is>
+          <t>A52100002328</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Santosh  Kothari</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>A52100002328</t>
+        </is>
+      </c>
+      <c r="D1146" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5Iikk0eHqaY4s%2b5pg6xtow2ENIB7VfLjEcglvUPB63ubCpJUyyHICqA97vwwcXg0algzhDJ7310FRGhELfXzEYUGY%2fTePbhLqe%2bukHi1EqVu4UC%2f78zCjJwG0KlVbD1KcBKPRrDyD2MWHiP98Qk9KHWMzmk%2fyuUd6rMMqUvLRrk%3d</t>
+        </is>
+      </c>
+      <c r="E1146" t="inlineStr">
+        <is>
+          <t>02024267191</t>
+        </is>
+      </c>
+      <c r="F1146" t="inlineStr">
+        <is>
+          <t>Market Yard</t>
+        </is>
+      </c>
+      <c r="G1146" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1146" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1146" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1146" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" s="1" t="inlineStr">
+        <is>
+          <t>A52100004390</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Sagar Suresh Sinkar</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>A52100004390</t>
+        </is>
+      </c>
+      <c r="D1147" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=L82apdIT26qegcfl2y2YORvQZ131snflK8W7oduw%2fJPCfZyCeUXh9vmBxdG3GvqNnHv3LpLMAJQXuhFmnAUIL8RLZzFz8TwosycvkfI79Q9pLV6DroQObPbO0MeGYZEf5%2btOdvJGLylytHbDDrEU73l%2bi8%2fYTVu9ed0JY%2fRTFkuhrTD%2f2w1giw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1147" t="inlineStr">
+        <is>
+          <t>09923227022</t>
+        </is>
+      </c>
+      <c r="F1147" t="inlineStr">
+        <is>
+          <t>Sadashiv Peth</t>
+        </is>
+      </c>
+      <c r="G1147" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1147" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1147" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1147" t="inlineStr">
+        <is>
+          <t>411030</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" s="1" t="inlineStr">
+        <is>
+          <t>A52100013438</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Vivek  Hapse</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>A52100013438</t>
+        </is>
+      </c>
+      <c r="D1148" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6KEIsPSoVcy%2bl18FQzcBqFKeLOJU2qS9VAtUS6hzM3c4FCr0ONa3%2fsI9u1yozY6LkLqlEUY95mkmMZIDYqx7wXY5jdfNPBf%2bGpBZ05hPNRSRzy%2b2CZWIK585842eh3CjiYmrRbwY4HpQAfgnTrkhsND72sP%2bQirbitCin%2fyNzu2DjYEaL6ahuw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1148" t="inlineStr">
+        <is>
+          <t>02041209290</t>
+        </is>
+      </c>
+      <c r="F1148" t="inlineStr">
+        <is>
+          <t>Viman Nagar</t>
+        </is>
+      </c>
+      <c r="G1148" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1148" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1148" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1148" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" s="1" t="inlineStr">
+        <is>
+          <t>A52100001998</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Paras Hiralal Katariya</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>A52100001998</t>
+        </is>
+      </c>
+      <c r="D1149" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=mw%2feHSxuUCdNcL%2b5zwmOhs3qMWAGd9qrXZsWjAYqX7cYpd8i1Q1WyqmdWjihXwfb6izZy7zid%2fAwUs0%2f0RE0ZNCepTw0jvqFkiJfi8jtwkqPRXCQO6%2fZQEB6Qo%2b5jOs5L8R5xs4k%2bdSzt21sw5cna%2f0Ybz%2fc%2bFolbqWBHw0tDksACUB946FcyA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1149" t="inlineStr">
+        <is>
+          <t>09890027959</t>
+        </is>
+      </c>
+      <c r="F1149" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1149" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1149" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1149" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1149" t="inlineStr">
+        <is>
+          <t>411067</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" s="1" t="inlineStr">
+        <is>
+          <t>A52100002342</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Yugantar Vishwas Ballal</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>A52100002342</t>
+        </is>
+      </c>
+      <c r="D1150" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=jcL3mejsxHxvlOFEC%2bW3urh0k%2b7d4gEZ%2fJ4ptoA9bCagDjA3J80aFcl8ouRZrmVQP%2bCJTTH%2bcR5b9DUb00uJ4VB3M%2fXiQY0t5JckDDWsaioexPyDAe2Q%2b%2f6nN8df1BzmzOtMd8FRDNGFE2M9m6p5xoIq2pkMXsO15AYHbcBRdfE%3d</t>
+        </is>
+      </c>
+      <c r="E1150" t="inlineStr">
+        <is>
+          <t>02048604751</t>
+        </is>
+      </c>
+      <c r="F1150" t="inlineStr">
+        <is>
+          <t>Yerwada</t>
+        </is>
+      </c>
+      <c r="G1150" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1150" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1150" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1150" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" s="1" t="inlineStr">
+        <is>
+          <t>A52100002012</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Vitthaldas Badrinarayan Maniar</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>A52100002012</t>
+        </is>
+      </c>
+      <c r="D1151" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QK6rDN4DMIyJpHf6Dm6PyaZgGPvf7o005F31Ptac5%2fFFrGO8lhTGyAag%2fPIjD2MyP%2fXQMd%2bpi8FSLXs6cOLLsbk0WjmPiPZeecbTGE4NO8Mty8mIRD3i7bEW8V%2bSc5yUk9nIb1NiXPtyT4PR2gMK%2b4cY0Tl6%2bxtyxnedljTF%2bvI%3d</t>
+        </is>
+      </c>
+      <c r="E1151" t="inlineStr">
+        <is>
+          <t>02025519015</t>
+        </is>
+      </c>
+      <c r="F1151" t="inlineStr">
+        <is>
+          <t>Nana Peth</t>
+        </is>
+      </c>
+      <c r="G1151" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1151" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1151" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1151" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1200]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1151"/>
+  <dimension ref="A1:J1201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -59768,6 +59768,2602 @@
         </is>
       </c>
     </row>
+    <row r="1152">
+      <c r="A1152" s="1" t="inlineStr">
+        <is>
+          <t>A52100001933</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Aarti Ajay Chaube</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>A52100001933</t>
+        </is>
+      </c>
+      <c r="D1152" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PnfeLmQ0KDKOD1q2H7U2yjfBeQ3NRQya1mbVoW3NDdz5Sxlem97qukJu%2fK4uLpo2koeOAdR16p5Nlq0C%2fONqQQOlBtvBIiqhZHd6KrUno6cunsF65Z8%2fLqtmVxV0hcocpX7dxYizS%2fw5%2btndrXm3UGH1atfQzNwTJuAKX%2f5u6oY%3d</t>
+        </is>
+      </c>
+      <c r="E1152" t="inlineStr">
+        <is>
+          <t>02000000000</t>
+        </is>
+      </c>
+      <c r="F1152" t="inlineStr">
+        <is>
+          <t>Wadgaon Sheri</t>
+        </is>
+      </c>
+      <c r="G1152" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1152" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1152" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1152" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" s="1" t="inlineStr">
+        <is>
+          <t>A52100002268</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Ajay Gendalal Jain</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>A52100002268</t>
+        </is>
+      </c>
+      <c r="D1153" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KdyFSuWoe6K1wo%2fU4vpVdxwg6gjiSRGYQd8UfF%2bRoQWEkFpmmBwWa65PW4bCrSuP%2bYQtIa8IQuLBi5cZ2979kYoMFIjZPpNfXOjCbaeahqRWFeuMRwF%2bfEoINo1Mzh5uWktT0JJJfYURiD2l0yNydk7gr0%2f4kyp1S7EUWnbxHQ4%3d</t>
+        </is>
+      </c>
+      <c r="E1153" t="inlineStr">
+        <is>
+          <t>02027290333</t>
+        </is>
+      </c>
+      <c r="F1153" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1153" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1153" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1153" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1153" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" s="1" t="inlineStr">
+        <is>
+          <t>A52100004190</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Manish C Kankaria</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>A52100004190</t>
+        </is>
+      </c>
+      <c r="D1154" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=nDTNSfSeMurwxPhTM0Gbx5YwzU%2fjmdxKW%2byw4pCWSqA%2f2BQBaZLP4OmJjagSINNR6R4Ar4EkeeyCJWtNiHDhQQh%2fWdffbm4uFXBCvIcTCQi%2bc%2fpjtIhSu60eiOj6qVNjvwnJ0EwmCXhio7PMy2OzvKPHiZh42NbF%2b5eR3PJHr8uZz3M4t2LACA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1154" t="inlineStr">
+        <is>
+          <t>02026342831</t>
+        </is>
+      </c>
+      <c r="F1154" t="inlineStr">
+        <is>
+          <t>Camp</t>
+        </is>
+      </c>
+      <c r="G1154" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1154" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1154" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1154" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" s="1" t="inlineStr">
+        <is>
+          <t>A52100002231</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Sucheta Manoj Adkar</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>A52100002231</t>
+        </is>
+      </c>
+      <c r="D1155" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PKI2rLfmYf4L%2bKI1JOJYYrp7%2fY7FiHXuI7qGvNi6%2bg8%2brSvJZAKrCHMOBQj%2bPqHkoxJNUXPK5s5x87BVEZtfVxrRSscUVwqw%2bg50cW6L6qmsD%2bsK%2bvWSOnlor4mEwcfL%2bZOZAvVSeiMhHwIZRSJZc45ucbB8m1%2fhYbF5Ka6lbOh7gxLl45d%2bng%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1155" t="inlineStr">
+        <is>
+          <t>02025387729</t>
+        </is>
+      </c>
+      <c r="F1155" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G1155" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1155" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1155" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J1155" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" s="1" t="inlineStr">
+        <is>
+          <t>A52100002165</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Amol Prabhakar Musale</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>A52100002165</t>
+        </is>
+      </c>
+      <c r="D1156" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3DhMwnRQILsXYH9heY%2fEsgxvN35J9oVOfN%2bwdV9udhDEEFdG5%2fIqyIbPAIZ4fU%2fiDFHSL9IEXvjUXtNmkfe5wCYjDQBkpXPYu%2bI78HbEP0OGV72zIsSD00ZKRGu4aMjncV%2fIt4xPe%2fnIJFop5qXGTHBGaEIbgmJS6TNVdCpEwXk%3d</t>
+        </is>
+      </c>
+      <c r="E1156" t="inlineStr">
+        <is>
+          <t>09545000721</t>
+        </is>
+      </c>
+      <c r="F1156" t="inlineStr">
+        <is>
+          <t>Rahatni</t>
+        </is>
+      </c>
+      <c r="G1156" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1156" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1156" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1156" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" s="1" t="inlineStr">
+        <is>
+          <t>A52100003869</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Kingdom Key Enterprises</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>A52100003869</t>
+        </is>
+      </c>
+      <c r="D1157" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MBnF17OK02CwLDl8ckB2pWV0Q6cX3Bg4I95fj0fL5VwzXe5RG1%2f7mBZsH0MvYF%2fljOFsZmFaDpKehZCOMBEGv6HlUtupcX0jF%2f8DG%2bqZ8wdS8W58pFiKVx3ZY0BXArBExoY9WTUafCaWxL4uoG2eScMQ8N2puXeVV1JGugbndH%2fPwPmeWDFtUg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1157" t="inlineStr">
+        <is>
+          <t>02065333425</t>
+        </is>
+      </c>
+      <c r="F1157" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1157" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1157" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1157" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1157" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" s="1" t="inlineStr">
+        <is>
+          <t>A52100009189</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Ankur  Gupta</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>A52100009189</t>
+        </is>
+      </c>
+      <c r="D1158" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xvqkAldAO5XO6G7RV94RsTEesDmaOcPf%2bb0XwoSom1BMuuugrE6djGM6u4ghJhr6iggDC%2fNG58nPdjeO2J%2fdrQrZASOkX72By%2b5kNl0j4hk3HE%2bQPgspJB5XRCC1laIquryL37c2gcWkqwVX9fVzNWbSiEDsO02zbXm5hyiYIEIkTj2NBtii7g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1158" t="inlineStr">
+        <is>
+          <t>09763911189</t>
+        </is>
+      </c>
+      <c r="F1158" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1158" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1158" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1158" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1158" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" s="1" t="inlineStr">
+        <is>
+          <t>A52100003147</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Manan Rohit Raja</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>A52100003147</t>
+        </is>
+      </c>
+      <c r="D1159" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Z9EHLx2zMb2f9bSQPzRtJG%2fB8h1N2Y0t12XW6vmP2ri%2fZ2GvasU48CKs2NnshZqSBFiFPpCRCxJ52ZNt6Qm6orVIC5yw5hlNw3xOBnQ2qQdGDxj1AwR%2faHyGnTcvi0tSYV6Uvm5UBGr39AsEI%2fNxguMG8A2tEuUMz%2fL07Kesh2eMqNqV46AIFA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1159" t="inlineStr">
+        <is>
+          <t>09579780081</t>
+        </is>
+      </c>
+      <c r="F1159" t="inlineStr">
+        <is>
+          <t>Bibvewadi</t>
+        </is>
+      </c>
+      <c r="G1159" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1159" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1159" t="inlineStr">
+        <is>
+          <t>Birobawadi</t>
+        </is>
+      </c>
+      <c r="J1159" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" s="1" t="inlineStr">
+        <is>
+          <t>A52100007877</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Suman  Thakur</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>A52100007877</t>
+        </is>
+      </c>
+      <c r="D1160" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=jHX%2fnXycttpqsc2YdTYSo1J%2b3%2f4SKmKtWg1f38PINPXfHxLSxIKt%2bsoyKPGzrVETlfcGxA%2f%2bEtvjez7UCN88f4qH5XOYgNmQ7pwCFT00R2bY5fdmQheMSJ%2bl8RDKqhJsMzdVgWIa5Ph75GF%2b2a9XoeeGlAUVoXH5QX1JHJUtj%2bfg64gzZJIhpw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1160" t="inlineStr">
+        <is>
+          <t>02025718118</t>
+        </is>
+      </c>
+      <c r="F1160" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G1160" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1160" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1160" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1160" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" s="1" t="inlineStr">
+        <is>
+          <t>A52100001915</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Rajendra Kashiram Chavan</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>A52100001915</t>
+        </is>
+      </c>
+      <c r="D1161" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ESGuZQgbQuUfXmJlHeVBOai2ygCJyFpbVnj6Mj3OoiyYy7MnCG%2bV8s0rELfTDh%2b70rTfnULHnWAS%2fjmq29QnjBXycr7vyi65%2fCYpd5xgOAfyCD%2f5Q0gISWi94LU%2bGX86pRsivVgsWRdw407xe6%2fLzE6HIfnWhH9fHp0h%2b5S9%2b0lijA9bwFY9EQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1161" t="inlineStr">
+        <is>
+          <t>09823054645</t>
+        </is>
+      </c>
+      <c r="F1161" t="inlineStr">
+        <is>
+          <t>Kasturba Society</t>
+        </is>
+      </c>
+      <c r="G1161" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1161" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1161" t="inlineStr">
+        <is>
+          <t>Vishrantwadi</t>
+        </is>
+      </c>
+      <c r="J1161" t="inlineStr">
+        <is>
+          <t>411032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" s="1" t="inlineStr">
+        <is>
+          <t>A52100002555</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Ajinkya Ravindra Oza</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>A52100002555</t>
+        </is>
+      </c>
+      <c r="D1162" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=A4IY1aaADM4RqEhTC8TL4eeLspM6XjdPhhUpqTN9P3u%2bYHUZhBkRGqdlGZtKgH%2b%2bLDqsvOtZ94BE2yEHo%2fOjgkI4ptwOql184bPvRCD4hs7E%2fl8mXQLXXvOd%2bYz26jHY%2bnDnE4h5WO60ZrFF5dYdw%2bOu4YdUmcLSkr939btG38prGaaxGuLRgw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1162" t="inlineStr">
+        <is>
+          <t>02026443434</t>
+        </is>
+      </c>
+      <c r="F1162" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1162" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1162" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1162" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1162" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" s="1" t="inlineStr">
+        <is>
+          <t>A52100038069</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Hitendra Panditrao Choudhary</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>A52100038069</t>
+        </is>
+      </c>
+      <c r="D1163" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=yTJJWif90TTxjl%2bK4gTQyxQR7V3Jkhksmd3vVibtd%2bq3l1C5TdlgHSPKk0uaNVGvDfWeyhGYDLXpma797Yt4DF2A706tsE2GntjQbpBO87djnay2MR3LbOrgxekU9jmBLEEb1YzlcdEeG%2feCHtIYlPP%2fcQblyFHTAgZI%2fsl9BCfjA72JFQa8rA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1163" t="inlineStr">
+        <is>
+          <t>02025897575</t>
+        </is>
+      </c>
+      <c r="F1163" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1163" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1163" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1163" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1163" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" s="1" t="inlineStr">
+        <is>
+          <t>A52100002922</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Vanessa  De Souza</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>A52100002922</t>
+        </is>
+      </c>
+      <c r="D1164" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=nj460iJw7Rz9JLjkU1OqceNXGkPOQw3Ui2mnzbkg%2f9lpd%2bqszHlT7AGqHMwvIU%2fcYdzVtCJzwp5uScCKn%2bGHwDPXDmA3CcdMCQ4DK1HL0Yj5587IVdDxD1YUct89oOtChEabUFnHjqPauBNoQB3DZa4xdcB3787zrl2LJamGFXSchAslLopfZQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1164" t="inlineStr">
+        <is>
+          <t>02026113024</t>
+        </is>
+      </c>
+      <c r="F1164" t="inlineStr">
+        <is>
+          <t>Pune Camp</t>
+        </is>
+      </c>
+      <c r="G1164" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1164" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1164" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1164" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" s="1" t="inlineStr">
+        <is>
+          <t>A52100004147</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Amol Maruti Phirange</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>A52100004147</t>
+        </is>
+      </c>
+      <c r="D1165" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wWMTxRcdAmQwcQU6fzZCqPMosRx8pxXRDfGlurwr5HbkeYlV3vmihsqvDhJrAXxZ1gyK2a8AjsImmMOeWu%2f12Ys7iU16TrKlxR2oPdlYGm9hc0pQ6Mg9fIHcg2IKgjQpOvQueFZMangMFGqV6BPRcljcRCby5LL%2bakHdrSkft66O5W8tuyaLyA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1165" t="inlineStr">
+        <is>
+          <t>09823206944</t>
+        </is>
+      </c>
+      <c r="F1165" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="G1165" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1165" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1165" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1165" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" s="1" t="inlineStr">
+        <is>
+          <t>A52100002467</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Lalit Jawarilalji Bafna</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>A52100002467</t>
+        </is>
+      </c>
+      <c r="D1166" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=4we2I5xuoTQrTD36qf1P6urYh1C93MCazx%2b3bXQO0g69dHD7gEjbfCfNXQePFcgWmKJt2fIGy1E6vPhWF9enpthXe1O1djpKPBDtxjhlIpumtI34aXFmGOZc8LWU9nkulcrR45yhT6KKyOG%2f7z%2bPjspIYzRFCpEu%2f6BitQz0LKNy5Z3pkIIhcg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1166" t="inlineStr">
+        <is>
+          <t>02069704646</t>
+        </is>
+      </c>
+      <c r="F1166" t="inlineStr">
+        <is>
+          <t>Narpatgiri Chauk</t>
+        </is>
+      </c>
+      <c r="G1166" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1166" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1166" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1166" t="inlineStr">
+        <is>
+          <t>411011</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" s="1" t="inlineStr">
+        <is>
+          <t>A52100000363</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Ajay Patwardhan Sharma</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>A52100000363</t>
+        </is>
+      </c>
+      <c r="D1167" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=pbwoWXG4IPfpe%2fo4%2fEfvGusPo5xLDSGPDR6EjFUWBuioE%2ff5d5JM%2ftyliA%2bzSG1UK69b0gIz5swQUwduCf8Phb4LyRT2UE%2bXyh83SnD5x1WQkb12HI79MhBsBK6wte1KiVaFkEry%2fa36dpcI%2fJOuxyL4uwv4U1EjXyqkUrLFMP0%3d</t>
+        </is>
+      </c>
+      <c r="E1167" t="inlineStr">
+        <is>
+          <t>02027410484</t>
+        </is>
+      </c>
+      <c r="F1167" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="G1167" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1167" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1167" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1167" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" s="1" t="inlineStr">
+        <is>
+          <t>A52100002033</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Raghav Bhagwat Kulkarni</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>A52100002033</t>
+        </is>
+      </c>
+      <c r="D1168" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=zMYz364lgpu92oF%2bjTyZGEcnZQVOtEqMqw2XZBe1LSYbu8MJKEhrWcbDF6Idww1mz33c9iAvCbzFeQvbhVb3dSMnXL338i3u8540vbJSHGcKsQ5L9c%2bTrofh2GyIXeJ%2fEGInbvo2fqlkT8s7813BdRY876hkZIWPtwPuILhFXgc%3d</t>
+        </is>
+      </c>
+      <c r="E1168" t="inlineStr">
+        <is>
+          <t>02020251115</t>
+        </is>
+      </c>
+      <c r="F1168" t="inlineStr">
+        <is>
+          <t>Erandavane</t>
+        </is>
+      </c>
+      <c r="G1168" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1168" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1168" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1168" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" s="1" t="inlineStr">
+        <is>
+          <t>A52100005910</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Jaypalsinh Daulatsinh Shinde</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>A52100005910</t>
+        </is>
+      </c>
+      <c r="D1169" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=7OgZTQQPWhgWkCkCk4CdQaFxzRKG4Rw6I%2bxMPOnMRN9JlKcUbQZ8DtmqlQp%2bCDwlVRx1y9Qh3LIwSAB0XPi%2bqQGbPc%2fvsKBemLvZSC%2bKq7TKVtRvqEFE5Q70tV5BBJ7h0lE7Lj6gjnRSeQz1%2fkqVDv5xJfar87jrqhb%2bpTFtFyVOJPs5po%2fDGg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1169" t="inlineStr">
+        <is>
+          <t>02067030844</t>
+        </is>
+      </c>
+      <c r="F1169" t="inlineStr">
+        <is>
+          <t>Vishal Nagar</t>
+        </is>
+      </c>
+      <c r="G1169" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1169" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1169" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1169" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" s="1" t="inlineStr">
+        <is>
+          <t>A52100004685</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Aarti Rohit Shaha</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>A52100004685</t>
+        </is>
+      </c>
+      <c r="D1170" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=e8Usr3pEooj768wr2DskyO0wxnzqTK2V%2bFs2PmfFtFK7j5prTQgvWgiXFDo0KaPc2XV7eYDfUVImirKvTQkzKmXQ3QYAM5scQmNeSl%2bdXbNCdDcksqOoKsQW0jPX0UIKEU7AhAMLIpXMD6%2bIGICEMsihVAqk4ZRMpU5GDhAw8phZWsFMbgUTtQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1170" t="inlineStr">
+        <is>
+          <t>02027171727</t>
+        </is>
+      </c>
+      <c r="F1170" t="inlineStr">
+        <is>
+          <t>Bhairavnagar</t>
+        </is>
+      </c>
+      <c r="G1170" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1170" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1170" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1170" t="inlineStr">
+        <is>
+          <t>460215</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" s="1" t="inlineStr">
+        <is>
+          <t>A52100002224</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Sujit Kumar Sinha</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>A52100002224</t>
+        </is>
+      </c>
+      <c r="D1171" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Oii9x%2b0IWYYS%2bs4eGUP1FECVMWFIqCG%2bC98Q1l6ih4UH9tOVSsCEfbSrzFYX5M8REqhFqnMRnHld0XXbsU5es1S%2fNi5ceQNEg2NaH%2fth4UgoQq7goydakVXBhaoOvakIDFYNm%2fk5mdLyoaNWh0PlctOLItHzgbPhtCx9YdO44jQ%3d</t>
+        </is>
+      </c>
+      <c r="E1171" t="inlineStr">
+        <is>
+          <t>02065200505</t>
+        </is>
+      </c>
+      <c r="F1171" t="inlineStr">
+        <is>
+          <t>Lohegaon</t>
+        </is>
+      </c>
+      <c r="G1171" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1171" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1171" t="inlineStr">
+        <is>
+          <t>Lahagaon</t>
+        </is>
+      </c>
+      <c r="J1171" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" s="1" t="inlineStr">
+        <is>
+          <t>A52100011008</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Rajendra  Kisanrao Kokate</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>A52100011008</t>
+        </is>
+      </c>
+      <c r="D1172" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1UxHdrx6imijjPsfn3KslcwschR5VwuB4SoxgWV625Pr6RAs1OHUnCjhizXiHx4v%2fVkhGQmFqhGQsnbe45TTnkqrKMYRkXW592bRg4Sy2sQCH9Dz9d3oOWzqpyJ8owPFo%2fz0AwuGivouGTyq0qiLf04GVJJVpfQypPrS1%2bhkzeKlXJc1AHs2zw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1172" t="inlineStr">
+        <is>
+          <t>02027286026</t>
+        </is>
+      </c>
+      <c r="F1172" t="inlineStr">
+        <is>
+          <t>Sai Chowk</t>
+        </is>
+      </c>
+      <c r="G1172" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1172" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1172" t="inlineStr">
+        <is>
+          <t>Pimpale Gurav</t>
+        </is>
+      </c>
+      <c r="J1172" t="inlineStr">
+        <is>
+          <t>411061</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" s="1" t="inlineStr">
+        <is>
+          <t>A52100003125</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Rajivranjan Ajaykumar Dwivedi</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>A52100003125</t>
+        </is>
+      </c>
+      <c r="D1173" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=k3E99Mka9fydILTgIM0nXNzWfuwfIhB92mER5tqS1Cc0xgevoTV31u6A7IVnmZ9LHd0EvDI22QipYvIo7B0U6lS4zVHSMfagXiPbzJ1JPZYuGHB3tKm%2bGnXJUAumQjCoAmT9pWYAUqFsWsRS8Tc78NZsu75h7MKtjoxIdCmEzW9hURLIqZwb5g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1173" t="inlineStr">
+        <is>
+          <t>08928919999</t>
+        </is>
+      </c>
+      <c r="F1173" t="inlineStr">
+        <is>
+          <t>Nalstop</t>
+        </is>
+      </c>
+      <c r="G1173" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1173" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1173" t="inlineStr">
+        <is>
+          <t>Karve Nagar</t>
+        </is>
+      </c>
+      <c r="J1173" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" s="1" t="inlineStr">
+        <is>
+          <t>A52100000755</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Santosh  Mishra</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>A52100000755</t>
+        </is>
+      </c>
+      <c r="D1174" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3ue9jhEKd77%2fqe%2bY2MwVkRIej%2b3RUZIIp4Wc8TAm3rj3T44%2fABSmzix9fLXXErGQvmscWxowE01o1J7pSNlnXrIFlgwun1ljsfIxw3uOXJifBLdah3sL6oteUb6NLPbR0mCb3YVjeCttcXR5LOiNh6kYtvFtShz69fdah1d%2bAyBn%2bRK%2fXIqZBw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1174" t="inlineStr">
+        <is>
+          <t>02032324252</t>
+        </is>
+      </c>
+      <c r="F1174" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G1174" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1174" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1174" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1174" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" s="1" t="inlineStr">
+        <is>
+          <t>A52100038894</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Prashant Shahurao Lande</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>A52100038894</t>
+        </is>
+      </c>
+      <c r="D1175" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5QFiTF4oKn15mCSF20gwTP5bDIzNtHWMar0vRRpjXkVHhxzGJhOpI5B6wuv40P%2fSbwY2QmdATL8zRHisvmUX%2f%2btHg0xklwBcrdxHWDNA%2bu7TtqcL8VwhBkar%2fEJbjCOHXJ7H8wjtsarzPJzr1hSnHl8%2fSugvMvhZ%2foD9nvF00owGBVMl4bSL3A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1175" t="inlineStr">
+        <is>
+          <t>02026830599</t>
+        </is>
+      </c>
+      <c r="F1175" t="inlineStr">
+        <is>
+          <t>Wadgaon Sheri</t>
+        </is>
+      </c>
+      <c r="G1175" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1175" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1175" t="inlineStr">
+        <is>
+          <t>Vadgaonsheri</t>
+        </is>
+      </c>
+      <c r="J1175" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" s="1" t="inlineStr">
+        <is>
+          <t>A52100002150</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Suunil Shatrughana Pawar</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>A52100002150</t>
+        </is>
+      </c>
+      <c r="D1176" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=nHFmiyDgMh0AtElxGgzF6ng%2fxzjozWLZx%2bBpnl7sDOgPB8wqPtzXxOCV%2bIAWNgKbm6Vj7oP9SRQ33YcekblfXgB4efaCC%2bktGYo6tdIloVQX1r0fxGVwYlcirYi9sHMlNnuO5rNFNO5Y7BHGr04WiA8DTI%2f7rfO3AJnYu72Swu2gUoGEztUZLA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1176" t="inlineStr">
+        <is>
+          <t>02024430505</t>
+        </is>
+      </c>
+      <c r="F1176" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1176" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1176" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1176" t="inlineStr"/>
+      <c r="J1176" t="inlineStr">
+        <is>
+          <t>411043</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" s="1" t="inlineStr">
+        <is>
+          <t>A52100002037</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Galaxy Properties</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>A52100002037</t>
+        </is>
+      </c>
+      <c r="D1177" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=pui5D55Lbup3FYxVY6ePrfJyV7PJpFH0PqnghFx9%2bxFIFe1nzaKSE3OwHbX6K5APnMGL%2b3RbzMKhX%2b629m9rnrQ1uYzJQ5EGxsgEN6g8eR4lI%2f2ANk3ZIwsy6HggE2kxQTQxopc6BqBO9%2bSHvNR190rWgvGBaEIcSuD9rFD3H0o%3d</t>
+        </is>
+      </c>
+      <c r="E1177" t="inlineStr">
+        <is>
+          <t>02065005547</t>
+        </is>
+      </c>
+      <c r="F1177" t="inlineStr">
+        <is>
+          <t>Chandannagar</t>
+        </is>
+      </c>
+      <c r="G1177" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1177" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1177" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1177" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" s="1" t="inlineStr">
+        <is>
+          <t>A52100002818</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Paras Vivasvat Parekh</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>A52100002818</t>
+        </is>
+      </c>
+      <c r="D1178" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=yOXRAu4S5BnY2slVoGcz0uDQFx%2fDkUZOnsY5aZjtXRqUc5EVLQ87CBg5tAXf%2bqgWxHEslmQI98ne7SmHTbXnRsiBXFCM2evEdW1YKoR%2fxNXtxlVXT5%2bYBPLcbNKVXeYNOx3mUaCXsfwkm9EBooV5UHSCHFOSlgvASFw%2fS7nijKqoRX0xIaQolA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1178" t="inlineStr">
+        <is>
+          <t>02065330200</t>
+        </is>
+      </c>
+      <c r="F1178" t="inlineStr">
+        <is>
+          <t>Wanawadi</t>
+        </is>
+      </c>
+      <c r="G1178" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1178" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1178" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1178" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" s="1" t="inlineStr">
+        <is>
+          <t>A52100016365</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>2Wings</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>A52100016365</t>
+        </is>
+      </c>
+      <c r="D1179" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=UjF8uF%2f8j8UfpBgErYeCPnoOTx%2be2D7lEwPX5OGrBrEkY4Xf91vcLklBmDTyXrwwMe%2byTRbGh4EB5aLppjGNB4UZemQHEfgmyb0xdxK27LP4dLT1LbLSqJ%2fp21QqJqdMGQ2MxJDNeec0Q2EO2WfImjQ9Zu1h8nZwGKf1vIIKTbBDpBhTnT0D9A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1179" t="inlineStr">
+        <is>
+          <t>02069853675</t>
+        </is>
+      </c>
+      <c r="F1179" t="inlineStr">
+        <is>
+          <t>Viman Nagar</t>
+        </is>
+      </c>
+      <c r="G1179" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1179" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1179" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1179" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" s="1" t="inlineStr">
+        <is>
+          <t>A52100004302</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Paresh Gokul Chapke</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>A52100004302</t>
+        </is>
+      </c>
+      <c r="D1180" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=oQAxbeGoQtT23rULaKBuRig4u%2fguUDPBpJ1qDJbeU7E1vCdn1xZP1%2bWCftqxZLk0Yl7841XoR9BEfXRZ1qmWpzq2PObhqtGCWJNN3ipj5yDcXwIGZKK0%2fF%2fUWkheO7hsLMbEIxQ1cNqiOxQmY0rndF50nTF%2bNblqPjf75p7AZNdMqiNOG%2bOhOQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1180" t="inlineStr">
+        <is>
+          <t>09561791613</t>
+        </is>
+      </c>
+      <c r="F1180" t="inlineStr">
+        <is>
+          <t>Bibwewadi</t>
+        </is>
+      </c>
+      <c r="G1180" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1180" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1180" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1180" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" s="1" t="inlineStr">
+        <is>
+          <t>A52100002499</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Yezdi Sorabji Mogal</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>A52100002499</t>
+        </is>
+      </c>
+      <c r="D1181" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=j3LvbQF1sGzde92m%2bbdTrpNX0dbCmzfKsZvPLKqUmc3ojf7hV7jJXe7F0f1IUWwt6ML6prEiG81udALlqH7fRH51KYB84uvg%2bfE2%2bxlRnZB0%2bgNzDMpfWBksQ61cYQ6G%2fDJ9NqBBmXbnte20luyXn4vSbO3D1u9krT%2fWgT5pKUeetT9W2VIrlQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1181" t="inlineStr">
+        <is>
+          <t>02026804677</t>
+        </is>
+      </c>
+      <c r="F1181" t="inlineStr">
+        <is>
+          <t>Mohamadwadi</t>
+        </is>
+      </c>
+      <c r="G1181" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1181" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1181" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="J1181" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" s="1" t="inlineStr">
+        <is>
+          <t>A52100003506</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Ketaki  Zagade</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>A52100003506</t>
+        </is>
+      </c>
+      <c r="D1182" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CKKF9nUZWS5jMlcGjGCw5bIji4BTw1sMjMiOQJsEaqmhPsm%2bjLkrO7RMjsOZcLbYzuDWNu60dlUrWumUFlc3L%2bhE5maKI8j%2fv20E4V2mXHV8vDVXzwB3T%2bX0d11VtQAlaIYiNOQ95Q2WgkeSGvtX2QORFI9sOmrXz64%2f7s7PcOH%2fvLlq1q22zg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1182" t="inlineStr">
+        <is>
+          <t>08983562852</t>
+        </is>
+      </c>
+      <c r="F1182" t="inlineStr">
+        <is>
+          <t>Rahatani</t>
+        </is>
+      </c>
+      <c r="G1182" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1182" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1182" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1182" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" s="1" t="inlineStr">
+        <is>
+          <t>A52100002491</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Ramesh Popatrao Karpe</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>A52100002491</t>
+        </is>
+      </c>
+      <c r="D1183" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=EVQEgSJZAxKt3NPBWzPG8LcZEBxc1rfDcYuho8YJ%2fH9s9gYwnwrCAaIhOgdErlaEIZ7qKKlr%2fw32pH8cv0ebDEBW5SvwctQpZjFPOJsLf70wlxiF7A120UmCqwNelpl%2f8pQLtnZqr6XuzIlP2OT6vVmzz%2bSGgZ6gHQXGos5i7dj6u830peVwgg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1183" t="inlineStr">
+        <is>
+          <t>08378992729</t>
+        </is>
+      </c>
+      <c r="F1183" t="inlineStr">
+        <is>
+          <t>Neharunagar</t>
+        </is>
+      </c>
+      <c r="G1183" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1183" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1183" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1183" t="inlineStr">
+        <is>
+          <t>411018</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" s="1" t="inlineStr">
+        <is>
+          <t>A52100018616</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Avinash Srichand Tejuja</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>A52100018616</t>
+        </is>
+      </c>
+      <c r="D1184" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=M4Pgt%2b%2btEEaDVYQknL3PX45Spx7h4WWid0iwA7hUaGYaW%2fAQNiyWHVcIsyqjWYa8Tq3e2h17iymrNvey6ibt%2fz%2bpnW5yZgN5nSRVXrw%2fFE9dcH%2fjImQQSDAdAxcZpHL%2f1QDOc6KHjqEWDq2ydhWVSADKNOZjvHZq1izY9zV72%2fukoMBhvWn%2fGA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1184" t="inlineStr">
+        <is>
+          <t>02226855247</t>
+        </is>
+      </c>
+      <c r="F1184" t="inlineStr">
+        <is>
+          <t>Kondhwa Khurd</t>
+        </is>
+      </c>
+      <c r="G1184" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1184" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1184" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1184" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" s="1" t="inlineStr">
+        <is>
+          <t>A52100018617</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Biswajit  Nayak</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>A52100018617</t>
+        </is>
+      </c>
+      <c r="D1185" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=lHDlUeZsTOYywUS7CB2tGZFVhcAjIifagC9TBTURNmki60Erkb4fkh3kkHxlARw3cfth2y6%2byTjlmFEVdUNs7S9EBHXwPi3Ig2%2fVl%2f0ylwjMkxEtLq733LkNccKvytRT%2feKPF58BSlLQ9opryrp9iQzbcZAX7v54NlvlTYun39BK8z0DBwwlGw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1185" t="inlineStr">
+        <is>
+          <t>02029706482</t>
+        </is>
+      </c>
+      <c r="F1185" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1185" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1185" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1185" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1185" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" s="1" t="inlineStr">
+        <is>
+          <t>A52100019002</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Propertybuddy Consulting Llp</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>A52100019002</t>
+        </is>
+      </c>
+      <c r="D1186" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2fmxnweOfn0NJzflRMphX8kMbnIuYcHJRm%2flRX8fcDint%2f6J9UmD4AwBjyMjZrSB2zWpPwAYx1SZp1exuYitUjb28Mb%2fREwEsiZ8APtneMI4GvEW6hdPsCUl%2bFjeZB5%2bDnL0fawyW4Qe8ocY1%2bbQUkWKduuFNm2G3CEe0%2b%2fpTjsN8JkI7cdIC%2fQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1186" t="inlineStr">
+        <is>
+          <t>9021159135</t>
+        </is>
+      </c>
+      <c r="F1186" t="inlineStr">
+        <is>
+          <t>Ward No 8, Aundh</t>
+        </is>
+      </c>
+      <c r="G1186" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1186" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1186" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1186" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" s="1" t="inlineStr">
+        <is>
+          <t>A52100018637</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Ravi Uttam Chavan</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>A52100018637</t>
+        </is>
+      </c>
+      <c r="D1187" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=GrxAH9EoalxPHRkm%2bcjm0w2lZUWvPxm2wazJOQCUkzjh5dPrOi93t9udPuOiC4lplcSl%2blgKg1ZUsg2o1V%2bkf1gl6dXqHMEmzG2nFtv06lJggKghnbYZsxP1n%2bNDnRnmowGrfv12IEs1lDGaWDRGb4HV3bdE2ELpgXcuqvLtKwqMzvMNaFVFhQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1187" t="inlineStr">
+        <is>
+          <t>08983740004</t>
+        </is>
+      </c>
+      <c r="F1187" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G1187" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1187" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1187" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1187" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" s="1" t="inlineStr">
+        <is>
+          <t>A52100018651</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Saif Noormohommad Shaikh</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>A52100018651</t>
+        </is>
+      </c>
+      <c r="D1188" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=TbnGaxRNWvwL4Ql4W5qXJPEOyob2fyIGbVwA2sIIlj%2bzkq04S8FC%2bIj6Dmm%2b73wtmRSAlVu%2bAGf71EpEVgmQc%2fmAIbsZZ1OL3lTVHPJfEd38uE3NzjbXIcy7AUc39y%2f%2bUXAYir%2flVHjmmk2BQFBam2SqG%2bwXiPuXem2CPDtCvIgsjASjaIObxA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1188" t="inlineStr">
+        <is>
+          <t>02012345679</t>
+        </is>
+      </c>
+      <c r="F1188" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1188" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1188" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1188" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1188" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" s="1" t="inlineStr">
+        <is>
+          <t>A52100018636</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Ashish Nagorao Valekar</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>A52100018636</t>
+        </is>
+      </c>
+      <c r="D1189" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=0HrxpXUUG9ZPHIo9tmSxtd0VQN5Es6dSLy2f4DDC0lPAtW3Jw%2f9KnfuGCaYM4oUpCGs86Z0kAaOqDblq5y%2fMzCucd5fkivBvaf1Mh6bXkO413YEYYWYtyYw4D7UK49W9blx5fBOu7n%2byUuA%2blm0HOEQ8v%2f1d7rAYssyeM70yz1N2%2fFa0KN6gFA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1189" t="inlineStr">
+        <is>
+          <t>02025432121</t>
+        </is>
+      </c>
+      <c r="F1189" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1189" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1189" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1189" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1189" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" s="1" t="inlineStr">
+        <is>
+          <t>A52100018798</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Aktarbadshah Miyasab Jattagi</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>A52100018798</t>
+        </is>
+      </c>
+      <c r="D1190" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bU2cJXni9adDTzPoUgzXgaFwWxZqeLrQ35RPrHmFv7lb0uRx2k7G7OzCfIKjXMXHixjWIpgHdxqAe32m2esmAXMsVp761p1KHkFITG8CGAWkWh2F2T0AbZhGm8wQJMNObvyDHn4jyIQsPqh8I7zxNXnBSt4spAWC5qk4nNhX9cfOtvcq69%2bFZw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1190" t="inlineStr">
+        <is>
+          <t>09822106981</t>
+        </is>
+      </c>
+      <c r="F1190" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="G1190" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1190" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1190" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1190" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" s="1" t="inlineStr">
+        <is>
+          <t>A52100019044</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Gurcharan Singh Sheehanth</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>A52100019044</t>
+        </is>
+      </c>
+      <c r="D1191" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=70pnx8BMi9w3rd%2f4S48U23hPdY8y73s9rmhJ4ejJOM5Qa7K8%2fU2vtESnOr%2bm3e9eQJneAkyPP3SP2pkqibhguhUdxOspAFsbPW%2bp2xc6rBVygGhtFS43fkbPknPhHLu%2f3rWmzFz9UvKzhAJiuqadvtgQUj2iTvucVXLaB1xuouQ5NjNtnWjnZg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1191" t="inlineStr">
+        <is>
+          <t>91989088073</t>
+        </is>
+      </c>
+      <c r="F1191" t="inlineStr">
+        <is>
+          <t>Kalyani Nagar</t>
+        </is>
+      </c>
+      <c r="G1191" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1191" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1191" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1191" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" s="1" t="inlineStr">
+        <is>
+          <t>A52100018875</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Nyati Builders Pvt. Ltd.</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>A52100018875</t>
+        </is>
+      </c>
+      <c r="D1192" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=17EwGQcCEAEq4ky%2fAtA2ASZ4OqJoSw7Q%2f%2bpeJb4AuLuixps700HsGiuboFeoha9Hx55rzFVfLwhq4qTbPvnCzXBy5oF0Mo6l2T6kQqfmvxseReHm%2fubplihszWTUi4h9JkroCEn1WOCc1izVGVH9XOUeLkk%2fvLibJQJDFsWg0orzw59O6POCvw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1192" t="inlineStr">
+        <is>
+          <t>02066863333</t>
+        </is>
+      </c>
+      <c r="F1192" t="inlineStr">
+        <is>
+          <t>Yerwada</t>
+        </is>
+      </c>
+      <c r="G1192" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1192" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1192" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1192" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" s="1" t="inlineStr">
+        <is>
+          <t>A52100018683</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Reshma Chetan Shinde</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>A52100018683</t>
+        </is>
+      </c>
+      <c r="D1193" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1lsu9ljvnbd79KDpyNalDGImZVE5ZWhCnBpTusUlRF4X5OymoYJg%2bp2t7NVvoZ2Hi8a1QE02hMzFLfBhG%2f%2bzOfbycKV1AxJFZO6chAeDi9F74b6JuV6KXukplYawIf3CTmVGQ41HWfwqlp0KPhbJuHhA0Rwd89G3kmte3qdGveOvZ6Uz3parAg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1193" t="inlineStr">
+        <is>
+          <t>02027281883</t>
+        </is>
+      </c>
+      <c r="F1193" t="inlineStr">
+        <is>
+          <t>Juni Sangvi</t>
+        </is>
+      </c>
+      <c r="G1193" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1193" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1193" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1193" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" s="1" t="inlineStr">
+        <is>
+          <t>A52100018690</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Iqlakh  Chouhan</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>A52100018690</t>
+        </is>
+      </c>
+      <c r="D1194" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=aMEiJGITWH01lv%2b4hrAMc7xdvzF8iT0NXgL0koq6ACy%2feoWjqEdpuoiws4ozDcvMbJbpdDjKYhQNnTkHmz6mrzUhBRQCVYI3Az0Y9MKN6ti1kaMhQBB9x%2fYI%2fdALEZSNpat1ZwEN5iNyiXUJB4Loa5VRh3oe2tSQHsto5BL3BihDIdLoUjbrKw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1194" t="inlineStr">
+        <is>
+          <t>07722015556</t>
+        </is>
+      </c>
+      <c r="F1194" t="inlineStr">
+        <is>
+          <t>Survey No 14</t>
+        </is>
+      </c>
+      <c r="G1194" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1194" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1194" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1194" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" s="1" t="inlineStr">
+        <is>
+          <t>A52100018694</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Nitin Ganpat Atigre</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>A52100018694</t>
+        </is>
+      </c>
+      <c r="D1195" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=koZJRlkjH8%2bmthGgaReRrgaHV3U8jHppIXWKr9fEE3FgXga8JNn8pjV0GMtSk1SNnYIk1Tx0IwixLYIzpgpmgy3MDJ5sNzcb42c6Ai2ARa9GsGU5Tl17ONxIsT8EOzVHsp4gm81mLQPETrr5EV4fAnBXYMqyHGo0gpxsjNEOg8iKkaNim%2f73%2bA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1195" t="inlineStr">
+        <is>
+          <t>09168246699</t>
+        </is>
+      </c>
+      <c r="F1195" t="inlineStr">
+        <is>
+          <t>Bavdhan (Bk)</t>
+        </is>
+      </c>
+      <c r="G1195" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1195" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1195" t="inlineStr">
+        <is>
+          <t>Bavadhan Bk</t>
+        </is>
+      </c>
+      <c r="J1195" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" s="1" t="inlineStr">
+        <is>
+          <t>A52100018691</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Shilpa Suhas Mankar</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>A52100018691</t>
+        </is>
+      </c>
+      <c r="D1196" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=apcRxVWV4eJ1a%2fzT3UGPmIo%2fUExF0AONOS50F7pU7j1inFCc8aiGVjs9s84CyjY%2beKKj2RO01wzRlQ3bSCFw9KmKIdS6KB33WpNDIs%2fVmtWFtvyO4OWje2Kl4%2bRAq%2fa9liUP3%2f2J824n5jEwJaMPE1xeUGdASKTHybaLpQ%2bU1gk58SOYcO19hw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1196" t="inlineStr">
+        <is>
+          <t>09309153658</t>
+        </is>
+      </c>
+      <c r="F1196" t="inlineStr">
+        <is>
+          <t>Pimple Gurav</t>
+        </is>
+      </c>
+      <c r="G1196" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1196" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1196" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1196" t="inlineStr">
+        <is>
+          <t>411061</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" s="1" t="inlineStr">
+        <is>
+          <t>A52100018703</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Chandar Jethanand Nathpotani</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>A52100018703</t>
+        </is>
+      </c>
+      <c r="D1197" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LBb2P5Zv3sevhYzHexBPUOlvUQCLhmyaqGD1nrqhtYCTeYfgYyZSJ6mXPa0E5SpRAj%2bziwew2sMyh7cft8YY2Gw8hVhe43l96cC5U4ppvPXblzJ8UaFtveT0D5EKIUCAh0jkv6GoNZb3woADsFzjzYSfu7zSxjEexYaOnCSpxNNXapn7%2fdQY9g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1197" t="inlineStr">
+        <is>
+          <t>09822187597</t>
+        </is>
+      </c>
+      <c r="F1197" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="G1197" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1197" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1197" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1197" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" s="1" t="inlineStr">
+        <is>
+          <t>A52100019041</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Santosh Kedarnath Survase</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>A52100019041</t>
+        </is>
+      </c>
+      <c r="D1198" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=YsIWZEu6%2b5B4E47%2fUv%2bPk8tVdyZcxLLN90TQGwnGnQkeansqLLxOYVC2Y125cB6d2C9pL%2fZd%2fCFYoYPPoAQS%2bxM4hMQvrG1n76rCDGAUoLbT8G69BrW4aN15a77Pi6m%2budDXwUCXM662O7b%2bhVPO2Z8qLqZ5853j5gR2UdNhpNuWooM2yctsGw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1198" t="inlineStr">
+        <is>
+          <t>09823115797</t>
+        </is>
+      </c>
+      <c r="F1198" t="inlineStr">
+        <is>
+          <t>Whalekarwadi</t>
+        </is>
+      </c>
+      <c r="G1198" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1198" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1198" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="J1198" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" s="1" t="inlineStr">
+        <is>
+          <t>A52100018756</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Jagadipa Finserv</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>A52100018756</t>
+        </is>
+      </c>
+      <c r="D1199" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=OkwCTMFkwU0BYh2DdjusmuWRuKTiEpfZOhzs57ApMHeJcOyH8QZ6Aj%2bONQZZf6irvVtAj%2b7I5O9Xgz7%2bDUCl%2b%2beaFd174z64n5HEsvvpSrmVcX0WFKDAszceL9Q%2f%2f%2f5VhZtbivU1HLeceKZSY%2foidSQEVMh0S8wl6ptbkWvKa1SKVHk2pvuT7w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1199" t="inlineStr">
+        <is>
+          <t>02024269065</t>
+        </is>
+      </c>
+      <c r="F1199" t="inlineStr">
+        <is>
+          <t>Market Yard</t>
+        </is>
+      </c>
+      <c r="G1199" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1199" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1199" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1199" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" s="1" t="inlineStr">
+        <is>
+          <t>A52100018947</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Mahesh Ramhari Kangle</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>A52100018947</t>
+        </is>
+      </c>
+      <c r="D1200" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=TnVzHv6Av07hQ6sXFMmdO8Cn55%2b7fs0ex%2fI2mUJ98bUikjAxmN6X4m4WNwH5Yrovk6x5Pii%2bYP%2fQTxZKSUxbXKJtqsQVV69Lei5RUh%2fY7wKHE%2bZ1pVGhH6kJ8fynHiQ4EzTKtiBdqMg9DVlpZyW7CsrprL7EFd%2b3%2bm4SXvodQ7huGtWhohi5ng%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1200" t="inlineStr">
+        <is>
+          <t>09082596857</t>
+        </is>
+      </c>
+      <c r="F1200" t="inlineStr">
+        <is>
+          <t>Punawale</t>
+        </is>
+      </c>
+      <c r="G1200" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1200" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1200" t="inlineStr">
+        <is>
+          <t>Punawale</t>
+        </is>
+      </c>
+      <c r="J1200" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" s="1" t="inlineStr">
+        <is>
+          <t>A52100018719</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Rekha Vishal Agarwal</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>A52100018719</t>
+        </is>
+      </c>
+      <c r="D1201" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=qUnr2c%2b62aYO0Iu8uC0BPCm%2fzf39LW1yz%2fEUo%2fs7Rf2HpHhLnF4nZemrg6oudq9sgbMOWYY7aWBDRK9inyqq%2f0I7y0Oyk9waTK7HqW4QE%2f3kARsT18YFfzHbecVt%2byCSpDTYLjtCd%2boEkSQjrjxWpSMfWHFqloweIMjozXdI7e%2blvU4pu867LA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1201" t="inlineStr">
+        <is>
+          <t>91202700924</t>
+        </is>
+      </c>
+      <c r="F1201" t="inlineStr">
+        <is>
+          <t>Wadgoansheri</t>
+        </is>
+      </c>
+      <c r="G1201" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1201" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1201" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1201" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1250]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1201"/>
+  <dimension ref="A1:J1251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -62364,6 +62364,2602 @@
         </is>
       </c>
     </row>
+    <row r="1202">
+      <c r="A1202" s="1" t="inlineStr">
+        <is>
+          <t>A52100018696</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Rajiv Kumar Singh</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>A52100018696</t>
+        </is>
+      </c>
+      <c r="D1202" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=kRzfBwUn8vWwWC2P7FXkYexFB2mtLAyGXdPSEzn0l3IqvskiIgFjXO63WUZtbM4ZOnCFbUPQeYDSyucJ8sQGnSsJn6M177nJVYcqQK7N4w47WtZHlHzULVV%2fd3azWBwwkByuZ7p2Y%2bNCS%2bkxygKXAXdQRmPzTXmfC0vPBwCIWqgvowQMprrbxQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1202" t="inlineStr">
+        <is>
+          <t>09011069676</t>
+        </is>
+      </c>
+      <c r="F1202" t="inlineStr">
+        <is>
+          <t>Kamal Park</t>
+        </is>
+      </c>
+      <c r="G1202" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1202" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1202" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J1202" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" s="1" t="inlineStr">
+        <is>
+          <t>A52100018755</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Poonam Harishchandra Rai</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>A52100018755</t>
+        </is>
+      </c>
+      <c r="D1203" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=RkP65coCfRmoo74oWql30MbYF4byMcii5re0vMHP1n%2fongfn91%2fENoScGKiVGx66yvdq5YasiY204gjkT40v49DCGtYHbz4XmA955%2fHOHmRjjBErEeicDfZz2wK83I%2fafK0kUTC1vsibhm4%2bKM9Bs3KEdmIp6WS0hTR1g7xr9j5X8KYY%2fOiw7g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1203" t="inlineStr">
+        <is>
+          <t>02020000000</t>
+        </is>
+      </c>
+      <c r="F1203" t="inlineStr">
+        <is>
+          <t>Wanowrie</t>
+        </is>
+      </c>
+      <c r="G1203" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1203" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1203" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="J1203" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" s="1" t="inlineStr">
+        <is>
+          <t>A52100018742</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Priyanka Sanjay Agarwal</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>A52100018742</t>
+        </is>
+      </c>
+      <c r="D1204" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1SF%2fMkJa3I%2bVMGrqa%2bbqoX6SBfhdCvUyV99C6Rg1PZxb%2bOWerkWlD%2fqnnWg5OILm5d4f07hfziwbxsbcNy0DB1bLjlHCLLpm8oHQH7HChHux19yKBgn1d2sRP%2bXKGX2E%2fnzw%2bJbEL94Vghusv6SJvfqcQcwimnJt04KQN5fHiae8k%2bIVao3S5A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1204" t="inlineStr">
+        <is>
+          <t>02026124958</t>
+        </is>
+      </c>
+      <c r="F1204" t="inlineStr">
+        <is>
+          <t>Mundhwa</t>
+        </is>
+      </c>
+      <c r="G1204" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1204" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1204" t="inlineStr">
+        <is>
+          <t>Keshavnagar-Mundwa</t>
+        </is>
+      </c>
+      <c r="J1204" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" s="1" t="inlineStr">
+        <is>
+          <t>A52100002387</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Priya Vikram Ghorpade</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>A52100002387</t>
+        </is>
+      </c>
+      <c r="D1205" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=smk02p8YFVrWBjIp5J7wCzr1Tn34w2cQX4tIO7LzvUUncpFyt%2fOTs71%2bBFMiOFxtDXNIlBrcMFYP60s6V2vywsyYjaqrdlqgQQR38hyrFgyBcF7cWRDIwZzrP8rG0CIPNGdv901cDh0e%2fc0hro%2f56T178KaNknetUIEXYAC6Sgh%2b3oVDjz57IQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1205" t="inlineStr">
+        <is>
+          <t>08788152246</t>
+        </is>
+      </c>
+      <c r="F1205" t="inlineStr">
+        <is>
+          <t>Bavdhan Khurd</t>
+        </is>
+      </c>
+      <c r="G1205" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1205" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1205" t="inlineStr"/>
+      <c r="J1205" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" s="1" t="inlineStr">
+        <is>
+          <t>A52100002502</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Salman Mansoor Shaikh</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>A52100002502</t>
+        </is>
+      </c>
+      <c r="D1206" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=IZkNrCK5OSy90rifR1J9qwAWYwmm5lw%2bE%2bEnU%2fazWTRZegbHqBvUWl5mCW4BQu59z%2f9fjl42yGJib%2f5XALpg0ewu5fXl7EcVf2b4BpEyKRkcRvkZq2nSOKNbSM1IILbDM7LMjoZPf36vrxVHBzbfebZ2%2bMqxt1akUPbs%2bjZxkhIl4w%2fFxQKpvA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1206" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
+      <c r="F1206" t="inlineStr">
+        <is>
+          <t>Ghorpadi Gaon</t>
+        </is>
+      </c>
+      <c r="G1206" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1206" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1206" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1206" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" s="1" t="inlineStr">
+        <is>
+          <t>A52100004356</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Vishal Jatin Thakore</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>A52100004356</t>
+        </is>
+      </c>
+      <c r="D1207" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2bsAJ32pC75OkRNdoK1wLLD67FGVdX9J7pjetpZTvk5CvXsxkYnKLmCH2%2fwUmyzwC8PD1ZJsaS2SpemN6Dwdjyn%2bdAkEgOBdW2%2f3pvJ8Efd8VRC2Ao%2b2HrXemCDodWaqg8RayzEOEYtrvkiFEC%2fUQYmSdqRr2B5BHMUQP5H78n6J5nCT2SQvVzw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1207" t="inlineStr">
+        <is>
+          <t>02026451855</t>
+        </is>
+      </c>
+      <c r="F1207" t="inlineStr">
+        <is>
+          <t>Gultekdi</t>
+        </is>
+      </c>
+      <c r="G1207" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1207" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1207" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1207" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" s="1" t="inlineStr">
+        <is>
+          <t>A52100001996</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Chandan Kamalakar Mayekar</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>A52100001996</t>
+        </is>
+      </c>
+      <c r="D1208" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=dob50v5nutv%2bVYik6gXVORISq%2fmkxTR9fTmGO90PjEmeD%2boq51DiZ9N5Kw9ro1gY0hhvOEvV28LrbxQr5A5h7qlmCYkly7cMGhYlJPA1VQJxUkH7bj%2brx6%2fHUCsibfTUeo4FPquxp2lwr1hqOFUJGP7X96gfShcRjw8HlGktibI%3d</t>
+        </is>
+      </c>
+      <c r="E1208" t="inlineStr">
+        <is>
+          <t>02065110029</t>
+        </is>
+      </c>
+      <c r="F1208" t="inlineStr">
+        <is>
+          <t>Dange Chowk</t>
+        </is>
+      </c>
+      <c r="G1208" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1208" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1208" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="J1208" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" s="1" t="inlineStr">
+        <is>
+          <t>A52100002022</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Malan Sambhajirao Karpe</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>A52100002022</t>
+        </is>
+      </c>
+      <c r="D1209" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KnSdpDwTvp8W%2f3OQuZxLlD04erWpJmihmkHwgZtfA9hmkwmue1j8NKZ6%2bGnAVfhTKnVX3HRZfmOfkYJvWAbtKLCmeAyN27UoULUAGnvL9CtN%2b24VzrpM5Sc1%2f670cRxw7L7sT8sOAS9wqa0gQj71wwUfuyY%2fzEWxQ%2fQMotbiyDU%3d</t>
+        </is>
+      </c>
+      <c r="E1209" t="inlineStr">
+        <is>
+          <t>02000000000</t>
+        </is>
+      </c>
+      <c r="F1209" t="inlineStr">
+        <is>
+          <t>Chandannagar</t>
+        </is>
+      </c>
+      <c r="G1209" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1209" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1209" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1209" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" s="1" t="inlineStr">
+        <is>
+          <t>A52100004446</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Yogesh Bharat Gandhi</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>A52100004446</t>
+        </is>
+      </c>
+      <c r="D1210" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Pn7nxnYElh1Opt%2b1y090twEk6qj2LqPgH96h8apuQzFH2uGI5m5MazWb2IWKTdvEhtnlNUg07ujlCjgyLpVHDZMm21p8uOWJAfhjHD4Hav8Dz9KwvM8WJyJPQtfDNxsKtwZmIXdALcs1ndxULR5jQTnHpTvCZHmGD9h4NKRWn4LAyDCN2G0HNg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1210" t="inlineStr">
+        <is>
+          <t>02025655748</t>
+        </is>
+      </c>
+      <c r="F1210" t="inlineStr">
+        <is>
+          <t>Sadashiv Peth</t>
+        </is>
+      </c>
+      <c r="G1210" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1210" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1210" t="inlineStr">
+        <is>
+          <t>Parvati</t>
+        </is>
+      </c>
+      <c r="J1210" t="inlineStr">
+        <is>
+          <t>411030</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" s="1" t="inlineStr">
+        <is>
+          <t>A52100001945</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Tejaswini Vijay Nikam</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>A52100001945</t>
+        </is>
+      </c>
+      <c r="D1211" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6%2bTD1pxUmUf1siLFNME9MSeP9pbnwiU6VPNrQ2OtW23BXjw5RZVyO4bkC75CF8zRR%2bw8ULW62gaZrtpHvUtC8wogt8KmAx5cK%2fP8MIPHq7pIuyHJBI%2beyD3edTQlrDDCivVly2MxO8PU2TL7OA4fzZpdmgxnj%2f5VG6Ak%2ftV35HI%3d</t>
+        </is>
+      </c>
+      <c r="E1211" t="inlineStr">
+        <is>
+          <t>09870202118</t>
+        </is>
+      </c>
+      <c r="F1211" t="inlineStr">
+        <is>
+          <t>Bharti Vidhyapeth</t>
+        </is>
+      </c>
+      <c r="G1211" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1211" t="inlineStr">
+        <is>
+          <t>Ambegaon</t>
+        </is>
+      </c>
+      <c r="I1211" t="inlineStr">
+        <is>
+          <t>Ambegaon</t>
+        </is>
+      </c>
+      <c r="J1211" t="inlineStr">
+        <is>
+          <t>411046</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" s="1" t="inlineStr">
+        <is>
+          <t>A52100001960</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Verindersingh Sardarsingh Oberoi</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>A52100001960</t>
+        </is>
+      </c>
+      <c r="D1212" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=JkGQEuR6L05CGK%2bAuTosQjDEXXG%2bz2YxHSTy197jxGzywAeEdnLXoqM%2bqaJ13mUnydAQ0kf5U95JbhF93%2bkl%2fxfZ9RtVMrrVvPSG57HsgW%2bq%2fhzD2B2uXqoybaUU%2bs%2fXXLRu5YAV3SrJVoz6%2bQw8dfICgMEw1rSbJeuAktiZWRE%3d</t>
+        </is>
+      </c>
+      <c r="E1212" t="inlineStr">
+        <is>
+          <t>02026164116</t>
+        </is>
+      </c>
+      <c r="F1212" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1212" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1212" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1212" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1212" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" s="1" t="inlineStr">
+        <is>
+          <t>A52100001969</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Apurva Bharat Sanghvi</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>A52100001969</t>
+        </is>
+      </c>
+      <c r="D1213" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=lUve%2bTLFb%2b5KSIBc2oa3o0rJITZpMwlP6NNoltlruEnzS7ADS5OdlHFXe2f03LU2NT0CuQOk3P3yzXRximYwG8NkrflGwmkZ4E9ZZVB1Bx2RmuCqfqXCN%2b%2fFMJmES2%2b9WJl4w55Yx%2b9Gvu98utx206XEqlE9qlwrr3q%2fSE6CvQU%3d</t>
+        </is>
+      </c>
+      <c r="E1213" t="inlineStr">
+        <is>
+          <t>09370720756</t>
+        </is>
+      </c>
+      <c r="F1213" t="inlineStr">
+        <is>
+          <t>Camp</t>
+        </is>
+      </c>
+      <c r="G1213" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1213" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1213" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1213" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" s="1" t="inlineStr">
+        <is>
+          <t>A52100007510</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Vishal Yashpal Sabarwal</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>A52100007510</t>
+        </is>
+      </c>
+      <c r="D1214" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=adQKhRtbdIHgn9kbGqT1Z96gxvQJF4C7JwgM5lhrDcEqrJLOMcsdhHgS32g%2btVmYfTYQHHwI%2fSseGUQvRSyysBNndfeXd1QHPZ1j2swza6kcrAeUsgMjM5VWLJT%2bAtwTh7I%2fMlxDAZxIO31abU6ATVgtJEWxT6O1CWgovtGbgNXYam8WFqmfjw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1214" t="inlineStr">
+        <is>
+          <t>02025812621</t>
+        </is>
+      </c>
+      <c r="F1214" t="inlineStr">
+        <is>
+          <t>Aundh Road,Kirkee</t>
+        </is>
+      </c>
+      <c r="G1214" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1214" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1214" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1214" t="inlineStr">
+        <is>
+          <t>411020</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" s="1" t="inlineStr">
+        <is>
+          <t>A52100002422</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Sham Ramrao Biradar</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>A52100002422</t>
+        </is>
+      </c>
+      <c r="D1215" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=eLfeoKDq06oUOdc3QdmfI7fAZZphvhvhaQtW%2ftnPCRkHTN4OmDcn%2f7CPkgLPVZMyAWUG36hvgffBefcVTT2ViojOJgWCuGhn4asdwjtAgLI8Xckrf3U2Fjp9CRnscPekAP8S039l%2fcYx3RgxoFBHjtw8Hyo9ZgxiXMKYPlRFsCR%2fNaTjc7K06w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1215" t="inlineStr">
+        <is>
+          <t>02065110056</t>
+        </is>
+      </c>
+      <c r="F1215" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="G1215" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1215" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1215" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1215" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" s="1" t="inlineStr">
+        <is>
+          <t>A52100003741</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Bhartarinath Subhash Nale</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>A52100003741</t>
+        </is>
+      </c>
+      <c r="D1216" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=jC5n%2bXdG9qA3iXRZnaaTQV0HE4XV7g9Nk3ijPWd%2fqcAX3yJoE4oUyTl2t17IPstb6i0GBdoG1t%2fXfsHg4wPKT5BrBsUoT0MzD9AaUoiWQpa68DbA3qIQoE2cuFK5fviBHF1vo534tbsS%2brXZsP8NlFkbUatym14%2bQcFYSYmbTq1OOaopLXU8Bg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1216" t="inlineStr">
+        <is>
+          <t>02060601777</t>
+        </is>
+      </c>
+      <c r="F1216" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1216" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1216" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1216" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1216" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" s="1" t="inlineStr">
+        <is>
+          <t>A52100003261</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Lalit  Kaushal</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>A52100003261</t>
+        </is>
+      </c>
+      <c r="D1217" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Jer5IhnPoT8%2fLaw88URty1Noq2SWCQuGRuJH%2bY6PitvogLH4NzDW7FRUwxd0WF1n3sV4TuUmpeWN6qjDSWwoz1P1sR2u2WNSuMFHdzbP%2bs8XKXggZMjkzaCihFv%2bHt5OtGKXeJQS7mV4JvCpHfrY%2bu50UEB2GQzleQPjTv1%2fmZARFHf6hN8ATg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1217" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
+      <c r="F1217" t="inlineStr">
+        <is>
+          <t>Lohegaon</t>
+        </is>
+      </c>
+      <c r="G1217" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1217" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1217" t="inlineStr">
+        <is>
+          <t>Lohgaon</t>
+        </is>
+      </c>
+      <c r="J1217" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" s="1" t="inlineStr">
+        <is>
+          <t>A52100007204</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Bluenest Properties Llp</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>A52100007204</t>
+        </is>
+      </c>
+      <c r="D1218" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=8k17Z9ol%2fRBpDBVqY1DGa%2fHHPDM%2fEdLdLv6lQUSnnIkQuZj04UpYiyUN0I0baUPleJTIuwceOXfK%2b0qVebDrDMVfxtEzClAqIv9YCTeizNrN8OQybrt6lqpmjrwKsUMI25fmkL0tc4jnkS%2fJJpkvNZooXs27kBTA4Hz7hoHMLbNQG9VWBXsvtw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1218" t="inlineStr">
+        <is>
+          <t>02065104999</t>
+        </is>
+      </c>
+      <c r="F1218" t="inlineStr">
+        <is>
+          <t>Warje Malwadi</t>
+        </is>
+      </c>
+      <c r="G1218" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1218" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1218" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1218" t="inlineStr">
+        <is>
+          <t>411058</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" s="1" t="inlineStr">
+        <is>
+          <t>A52100006714</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Rakshak Infrastructure(I) Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>A52100006714</t>
+        </is>
+      </c>
+      <c r="D1219" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KgnEXdOHNDJodCjaGogA7RXyUjH1PYB%2btLhLFPNms97nx44JrHaCf2kogJw8NLjwdiDPojx0V5EHDo5ah8ffBuSlEQMb8yUY7%2bJMFXvTlgAkMgdMU8BIEoOr1vx9EIdoCV%2bxl%2bgRtMT0ECMJeV8oDlKyCSTHyhYAeA64gXGpP%2b9z0k0LyXPT7Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1219" t="inlineStr">
+        <is>
+          <t>02069333357</t>
+        </is>
+      </c>
+      <c r="F1219" t="inlineStr">
+        <is>
+          <t>Viman Nagar</t>
+        </is>
+      </c>
+      <c r="G1219" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1219" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1219" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1219" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" s="1" t="inlineStr">
+        <is>
+          <t>A52100011673</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Vikram Ashok Pore</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>A52100011673</t>
+        </is>
+      </c>
+      <c r="D1220" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=9M6OJowGfezQW%2flncJuY8F1KD1L2%2b9bTLNaXk1yiafco1CBpdA488LMkFneud3h%2b0SNh53j7F9xXxIGjOgc21vcZFizveynBPTJgNslZBAWVQDXMhx%2fZ6KPY4jVH%2bdRY2lqtNycry6b3YHWxNSDG1sT57vlZlMXZb9zmxa92LCznbS9clRQIqw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1220" t="inlineStr">
+        <is>
+          <t>02067231516</t>
+        </is>
+      </c>
+      <c r="F1220" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1220" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1220" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1220" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1220" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" s="1" t="inlineStr">
+        <is>
+          <t>A52100002038</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Ankur  Lodha</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>A52100002038</t>
+        </is>
+      </c>
+      <c r="D1221" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=UBGW%2fylpmVjg%2bynMdIy8BeB%2bXRl51xOT1kYH3bJgl7QjslJ6ViysmUaBXip39666bxrIPmkXhfDEQawbeHytT5OMLji0PVJpG%2bgx5foMvxZx28axbwF8AMsALDXYXj9y9xGZddQFKSjjBbx83wLHLdi%2bOx9DraA3bvGR8mx2Y9g%3d</t>
+        </is>
+      </c>
+      <c r="E1221" t="inlineStr">
+        <is>
+          <t>02046502684</t>
+        </is>
+      </c>
+      <c r="F1221" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1221" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1221" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1221" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1221" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" s="1" t="inlineStr">
+        <is>
+          <t>A52100004740</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Shilpa Sohan Bharade</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>A52100004740</t>
+        </is>
+      </c>
+      <c r="D1222" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=E4HBhsCsosnyySgKufKUGTOlba%2f9PV2Dj7WR9ABHnwQWakFKnXixTMlSZ9hWuBEMv4fukqqHbhZ2%2bYPVzPFkFX%2fMmf0MEMjCj6iWPdKUmHy6SUI%2bLXzHUi1MylcQL6C6TYND9fYjfRHmeN3i7wBb3MTwK3MPGYXjhYIb6r4N9qJ%2bIlNat4QxsA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1222" t="inlineStr">
+        <is>
+          <t>02070306181</t>
+        </is>
+      </c>
+      <c r="F1222" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="G1222" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1222" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1222" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1222" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" s="1" t="inlineStr">
+        <is>
+          <t>A52100002556</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Dheeraj Mahadeo Shejal</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>A52100002556</t>
+        </is>
+      </c>
+      <c r="D1223" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QnqwKETzqjV2GN0aKlLV0%2fH7UZ%2fdldObeYjjoH2yTX3eCKluECsC2jU6gb0mIv47A1R8W26P2qQkviH9%2fddQPgKwT4cnyOL0xrztXX45ZirSCRvIso32tTDmvR8dc%2f7clKR4tKjoqDXPUsLiPW7JMeNf5QYbgQLi%2bU19xtn3eustD7nUV2PkkA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1223" t="inlineStr">
+        <is>
+          <t>07350734040</t>
+        </is>
+      </c>
+      <c r="F1223" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="G1223" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1223" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1223" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="J1223" t="inlineStr">
+        <is>
+          <t>411043</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" s="1" t="inlineStr">
+        <is>
+          <t>A52100002613</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Sachin Chandrakant Gaware</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>A52100002613</t>
+        </is>
+      </c>
+      <c r="D1224" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LPpw%2b5PQkeTHLbg%2fNR59Go%2fC6y2zqEX2KXzrSuRjxikPkCE0zYmTx7Kr1P4n405BCgFJ0AtlOICL8dtTyIDycR7CPJ9v0cWa%2bvFHWmMhL7KIBixYR4ZrU3zsTLvpPGmQnBBb2g2QhbPlsRAYBU2IxbPDY0S2%2f4WsNtfZPIN%2bkWCtCw4lhnVaqg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1224" t="inlineStr">
+        <is>
+          <t>02026331520</t>
+        </is>
+      </c>
+      <c r="F1224" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1224" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1224" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1224" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1224" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" s="1" t="inlineStr">
+        <is>
+          <t>A52100002004</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Rupinder  Singh</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>A52100002004</t>
+        </is>
+      </c>
+      <c r="D1225" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ZeWT50AsRp3n41Dru8rqQrhSygi97ulgIw%2br6eu4qzjz1VNymGL4yzCGvI5U2qOa6zsrqT%2brLqScDFCQPHVEaL0Gp9bwai7Z7jOeR0A8A02fpE0kA7vqUPeYeJPkuD%2f2e7aNzy95uoVg%2bqS%2f9l7XfRwk1ootLqXcMDG4tB5drdU%3d</t>
+        </is>
+      </c>
+      <c r="E1225" t="inlineStr">
+        <is>
+          <t>02060121664</t>
+        </is>
+      </c>
+      <c r="F1225" t="inlineStr">
+        <is>
+          <t>Wadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G1225" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1225" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1225" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1225" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" s="1" t="inlineStr">
+        <is>
+          <t>A52100002389</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Ankush Krishanlal Bansal</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>A52100002389</t>
+        </is>
+      </c>
+      <c r="D1226" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bhrBEfyFXx2jLYASqNEm7wNqoOfB8KXY9cOXPN4WwlUqDCOKcjQhxvOOBSrn%2fB%2fpp8HrLXtPIzhf0gUhWpiovkQ1WohQKz%2fsHxgPIZ%2fMqJ4qoLWkVTQEmfwd%2ft7p3jlKiLri9IRJYH36EhKZTHuE9PORSy7RscB1%2fUf5i%2bPu2XvvdlTtNIqEjA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1226" t="inlineStr">
+        <is>
+          <t>02027479205</t>
+        </is>
+      </c>
+      <c r="F1226" t="inlineStr">
+        <is>
+          <t>Nigdi</t>
+        </is>
+      </c>
+      <c r="G1226" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1226" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I1226" t="inlineStr">
+        <is>
+          <t>Nigade</t>
+        </is>
+      </c>
+      <c r="J1226" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" s="1" t="inlineStr">
+        <is>
+          <t>A52100002478</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Pervez Phiroze Mehta</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>A52100002478</t>
+        </is>
+      </c>
+      <c r="D1227" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3MNuUdfquKfDJ66V8Lcd5FCsdk0vJSD7CI1fU%2bh2FGBuuquWpWinHLwG47%2bOWhdbeG%2bdDPJ1rbalvAQPoIvtV2YvdUblyrGX2wJ92t1OKqdHUC6t394V1Mp7d4JiWIZIFN2axapo8yxReTNpFxKYRPjQCgM%2bONL3zNETKW%2bEJxB0L7MP18mwpw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1227" t="inlineStr">
+        <is>
+          <t>02098907548</t>
+        </is>
+      </c>
+      <c r="F1227" t="inlineStr">
+        <is>
+          <t>67-B</t>
+        </is>
+      </c>
+      <c r="G1227" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1227" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1227" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1227" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" s="1" t="inlineStr">
+        <is>
+          <t>A52100001889</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Abbas  Faiz</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>A52100001889</t>
+        </is>
+      </c>
+      <c r="D1228" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=8Gd8jnMyjKME6Tv0DO5g5%2bAZOOAIPScoRuvyRutFAavrFsCsZCF4dFxVxpMRLJmpJxdtgvVIeid4FZs78mhCm6HwqN%2fvk3lCinKdDY0l76SWAbmVUZl9FFBGKW87Cw6ix%2bdezo03tL5TQ4Rz3%2bkZVQoX34kizTgUjjguviB3q5bFevDctLQtSg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1228" t="inlineStr">
+        <is>
+          <t>02041223402</t>
+        </is>
+      </c>
+      <c r="F1228" t="inlineStr">
+        <is>
+          <t>Sn 1A/1/2</t>
+        </is>
+      </c>
+      <c r="G1228" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1228" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1228" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1228" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" s="1" t="inlineStr">
+        <is>
+          <t>A52100002434</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Homi Minoo Kalyaniwala</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>A52100002434</t>
+        </is>
+      </c>
+      <c r="D1229" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6Tm8gTDkhWlPm6hiU84t9uRb4bn5%2bddtTNVdm28jL%2fsI%2bUxmYtpZ4C8T1MjI9TabJA8cuOZxSy1XVvq6QgYkrn0DRBuqFAhZ1CHT1AbQdq0DVwo%2bFH%2f4Kr0hI3TSJLyQ%2fiOlfdtcnIVTd6BbgTmhK1wrraQJjHBCVuP51nDMZFunAubKB%2fyCxA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1229" t="inlineStr">
+        <is>
+          <t>02098900079</t>
+        </is>
+      </c>
+      <c r="F1229" t="inlineStr">
+        <is>
+          <t>Opp Iqbal Classes</t>
+        </is>
+      </c>
+      <c r="G1229" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1229" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1229" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1229" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" s="1" t="inlineStr">
+        <is>
+          <t>A52100002854</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Nitesh Kumar  Singh</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>A52100002854</t>
+        </is>
+      </c>
+      <c r="D1230" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LBTVx7bI7GW%2buo0S3GhQuWjUdypyawjv5Fd9iRsI0ac%2bM4t8vVKfN4MgWZLslScoorPA76h98Ebl1DK%2bFblkJqSJpZen%2fTjTtfSpEHTxJa0Im%2fsdr6AxVY1kTN4Tsb9toPYbpH2vEXRE4yAoPG%2bVAHKmrp1vy%2f7CkOlfgQyHVtjd5v%2fmFW4lfQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1230" t="inlineStr">
+        <is>
+          <t>08169418838</t>
+        </is>
+      </c>
+      <c r="F1230" t="inlineStr">
+        <is>
+          <t>Magarpatta Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1230" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1230" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1230" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1230" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" s="1" t="inlineStr">
+        <is>
+          <t>A52100001206</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Prashant Prakash Karnawat</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>A52100001206</t>
+        </is>
+      </c>
+      <c r="D1231" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ro4c591uc8XkEWmtwLl2rtgmB1ywYSZmFJUViXTK%2forQ488g9%2flneClYOreyJhTIoae7r1TVhKRzu1VsGop3l5%2b48bohqBbZ1eXEzPYYG%2bOgGzpqxoVtXrwzsjfIvy0CY040upZS2AMFLDIntw%2f%2bp86txUdDOuID2oW%2fYJ03boIg83zFVcgclA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1231" t="inlineStr">
+        <is>
+          <t>09168044344</t>
+        </is>
+      </c>
+      <c r="F1231" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1231" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1231" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1231" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1231" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" s="1" t="inlineStr">
+        <is>
+          <t>A52100003710</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Raghuprasad Ramchandra Pawagi</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>A52100003710</t>
+        </is>
+      </c>
+      <c r="D1232" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=NZL5rpdq08kyjahkE8BWLS4O10JPJKwUhOvKnawQYNAktkhPGQ%2bkCCctvyaD9aEJlJLs%2fNeHUUcFU0n2nbGyZUUegQ%2bVik0kRPNm2xEcA6%2fnvX77guLLruQp%2f1RtrdUiqg0VAqZd0VxGJWL3o9jU4J0eEJ2I8BVEzl28t3SPFLK6hwUADbCyog%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1232" t="inlineStr">
+        <is>
+          <t>02024477486</t>
+        </is>
+      </c>
+      <c r="F1232" t="inlineStr">
+        <is>
+          <t>Near Hatti Ganpati Chowk,</t>
+        </is>
+      </c>
+      <c r="G1232" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1232" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1232" t="inlineStr">
+        <is>
+          <t>Peth</t>
+        </is>
+      </c>
+      <c r="J1232" t="inlineStr">
+        <is>
+          <t>411030</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" s="1" t="inlineStr">
+        <is>
+          <t>A52100005792</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Nirmaladevi Prataprao Satav</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>A52100005792</t>
+        </is>
+      </c>
+      <c r="D1233" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bEKhOtVVSF32yO2I7uxjMiQZMpKhQtgc5pWJ7NYmzgKkA17o1ModYUkkU3EIoCFzNiWnqYNI0dA0Le59He6lcnNDKKuuPU%2b2Jqh2hxAsbZd7G8MRH0BySNm3r3gEZJJTXlYc201QKmws9vTnpc30UCxO7p2d%2fqflaKVzACHH6umaO3M3oPyF9g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1233" t="inlineStr">
+        <is>
+          <t>02025529472</t>
+        </is>
+      </c>
+      <c r="F1233" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1233" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1233" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1233" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1233" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" s="1" t="inlineStr">
+        <is>
+          <t>A52100020018</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Deepali Sunil Tembe</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>A52100020018</t>
+        </is>
+      </c>
+      <c r="D1234" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=moxcEOeaAmeAkubPo8sHL3JioN6dFMse7pZvpiztEu6o%2fPyMhc%2b4yNX3NzkrwZq9G7VCGWUuKdYEwPpMLOujC9pC%2fnfTOEZOZvV02jmwgiAJ9yjl%2fBMbSH1J9DgMeHrZAqiQwbSX9jhrBSHlJfUUcQbTIpIxEBj7LzhQmGRM88WDmciHPFnGqQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1234" t="inlineStr">
+        <is>
+          <t>02025445468</t>
+        </is>
+      </c>
+      <c r="F1234" t="inlineStr">
+        <is>
+          <t>Rambaug Colony</t>
+        </is>
+      </c>
+      <c r="G1234" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1234" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1234" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1234" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" s="1" t="inlineStr">
+        <is>
+          <t>A52100002075</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Ashish Ajit Vengurlekar</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>A52100002075</t>
+        </is>
+      </c>
+      <c r="D1235" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=K3acXQy4DMHkyfhLiIyP%2fp8uD1UUG4UGjJWCTAWVREYfGaNWA0PrtQd3zYExwg%2f%2flywBgRAjj3LphYZFd8LGs5v%2fZ0zd9IRaHwmd%2bMy7PHqXC8LhwEiLoEoMDxtvRYfqKRu4FAhEQMrgpv6pDzQx0OgC1l4hpI8YT%2bNhXRHXJ%2fahlv4depv16g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1235" t="inlineStr">
+        <is>
+          <t>02099999999</t>
+        </is>
+      </c>
+      <c r="F1235" t="inlineStr">
+        <is>
+          <t>Kalas</t>
+        </is>
+      </c>
+      <c r="G1235" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1235" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1235" t="inlineStr">
+        <is>
+          <t>Kalas</t>
+        </is>
+      </c>
+      <c r="J1235" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" s="1" t="inlineStr">
+        <is>
+          <t>A52100000356</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Rahul  Daga</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>A52100000356</t>
+        </is>
+      </c>
+      <c r="D1236" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=U8W%2bgJBxmsvBXv%2fNTH%2bhjlp5GE9sjKQ%2fAaLq42HI5erglkiK3PVCB4rW74c4HxrD3wcnEikw1cUCV6Dd2%2fBw3ArHyvDP8vcm%2bQLcDof4ipJpusNCT9oMErMxfsc8jU23dsVigZg0DvX%2fSciIuxVxSxXc%2buO%2bG3v3WuFi%2fMZkKd9axaI9rjKsIg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1236" t="inlineStr">
+        <is>
+          <t>02026881487</t>
+        </is>
+      </c>
+      <c r="F1236" t="inlineStr">
+        <is>
+          <t>Mundhwa</t>
+        </is>
+      </c>
+      <c r="G1236" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1236" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1236" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1236" t="inlineStr">
+        <is>
+          <t>411036</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" s="1" t="inlineStr">
+        <is>
+          <t>A52100001884</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Santosh Hanmantrao Kadam</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>A52100001884</t>
+        </is>
+      </c>
+      <c r="D1237" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Mp%2bIjHXBbr5aoBY9sMv9mXYOWXKSZe%2fKPRfophFomIeyVMVT2JeCRiHvcYRgO0z8cxtl%2fAS0btHggEzwkVIjGJaHMJxi2RLovekA2ld3ELL1sta4GXKAtcXqCQfKPpUU8UADocuaYujjROPF1Pylk10ywoyRkFfk1Kz4GQ88j3s%3d</t>
+        </is>
+      </c>
+      <c r="E1237" t="inlineStr">
+        <is>
+          <t>02069738111</t>
+        </is>
+      </c>
+      <c r="F1237" t="inlineStr">
+        <is>
+          <t>Lohegaon</t>
+        </is>
+      </c>
+      <c r="G1237" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1237" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1237" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1237" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" s="1" t="inlineStr">
+        <is>
+          <t>A52100001939</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Pankaj Haribhau Sutrave</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>A52100001939</t>
+        </is>
+      </c>
+      <c r="D1238" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=eajauZ3B8TSK2odvZAMCVDjKq9uNH0eX5KvkcO2qwA65pejM5eqYD77a6Xb0Pw0R3nkj1%2bey1vC8%2f98c8b6XvvwKbr7Ii0eLPSeRAf34zsE5FEZQo5F%2fUKoG1VEnyboMo076IW1B34jk9NAZjlPLnqXDuG71ghVoWeq8cC%2flGww%3d</t>
+        </is>
+      </c>
+      <c r="E1238" t="inlineStr">
+        <is>
+          <t>02025382842</t>
+        </is>
+      </c>
+      <c r="F1238" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G1238" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1238" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1238" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J1238" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" s="1" t="inlineStr">
+        <is>
+          <t>A52100000028</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Vijay Purshottam Manakikar</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>A52100000028</t>
+        </is>
+      </c>
+      <c r="D1239" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=HRUqki3wzfwQfootn9rB%2fRHGGWz2kVcM1lGgN5p0y4xcVPQ5hb2MgnFUj8aZsVpHBiF56TLuU2MSJo%2fDZFyzoX%2bNXrRriObZeIAJBrF%2bkUY7lqDe%2fOvqYFp1%2byDxDMjl38hkpTLP79dlg9OKXYs8jCKnvQMazizX3wKcsgYKfOU%3d</t>
+        </is>
+      </c>
+      <c r="E1239" t="inlineStr">
+        <is>
+          <t>09623009793</t>
+        </is>
+      </c>
+      <c r="F1239" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1239" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1239" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1239" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1239" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" s="1" t="inlineStr">
+        <is>
+          <t>A52100002585</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Honaji Balasaheb Sanas</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>A52100002585</t>
+        </is>
+      </c>
+      <c r="D1240" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LeoAbcNdMeSoj0LrGittEVor9L7XwHrwVh3uay%2fmrxmf1G8TVt3s7l77NoMSbRWxSLX4pnONa6VGD1SQ2PDOVcq9Ek1b%2bwj1zA9OxRJC2eE6GEycuJa%2ftfdyl71wQ8C1zk6J6%2b7uIjvNFAoeKq7w9Y%2fIXnZYj%2bdEzuYH60mCWX6ms%2f2QTJfXyQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1240" t="inlineStr">
+        <is>
+          <t>02041233377</t>
+        </is>
+      </c>
+      <c r="F1240" t="inlineStr">
+        <is>
+          <t>333 Koregaon Park</t>
+        </is>
+      </c>
+      <c r="G1240" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1240" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1240" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1240" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" s="1" t="inlineStr">
+        <is>
+          <t>A52100018734</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Sagar Samuel Parmar</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>A52100018734</t>
+        </is>
+      </c>
+      <c r="D1241" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=9Hp4zQ%2fycoR%2bemyzH4nNGBbdj%2bNBxVmHuaodcyQ1QDuW%2bdCv0csDFUPKzHkK%2fHWMgaCOQ7VARVa3ywpHq%2bMLuH9tfFP1oRYCfhtHhMGO67C9yqATyJf7tBJytkeLh%2fY95%2fX03E2oTFKw0F1%2fgFzO5Pul9ocTAkJvXhXu3R6OWBQZ4EUm2dOphw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1241" t="inlineStr">
+        <is>
+          <t>09881078294</t>
+        </is>
+      </c>
+      <c r="F1241" t="inlineStr">
+        <is>
+          <t>Old Sanghvi</t>
+        </is>
+      </c>
+      <c r="G1241" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1241" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1241" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1241" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" s="1" t="inlineStr">
+        <is>
+          <t>A52100018826</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Shashi  Shekhar</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>A52100018826</t>
+        </is>
+      </c>
+      <c r="D1242" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=rrpQnruMOdSqpmhGirEOW7zng9PRcSQGHoo4i0qQ7gpck9sv7egjGG2Cwf8ghJkPjNAh742%2bDNxubro4FVKzZv5xJKo8OHLBsMjjS7waoouyTHarNtIhuv7zg9NdkgH3Qw2zzzWsKGN6b6OMpPmDEWBBamnw4Ars4fm5GFwq6loRNIBPbXIrTA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1242" t="inlineStr">
+        <is>
+          <t>02064012422</t>
+        </is>
+      </c>
+      <c r="F1242" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1242" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1242" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1242" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1242" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" s="1" t="inlineStr">
+        <is>
+          <t>A52100018805</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Sanket Nagnath Sutar Proprietor Of Unique Properties</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>A52100018805</t>
+        </is>
+      </c>
+      <c r="D1243" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ig1VT2lfcvpwWziDRkdUng9UFuiucrPI%2f%2f3%2b3mwZUL%2bjOQ%2fHLGNvCDf2AQnZDb9SFkM8R2LHXxUGGFaYxseYV%2bZMYlxlQUU1YPMYci2Pb3zjaLZkENvXdzPPLp9rV%2fQr9PmOgtnvmozDUs5wOmOaf%2bus9iIBDAROIWE91EPrFoloyxIsTi8tzQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1243" t="inlineStr">
+        <is>
+          <t>08888222473</t>
+        </is>
+      </c>
+      <c r="F1243" t="inlineStr">
+        <is>
+          <t>Walhekarwadi</t>
+        </is>
+      </c>
+      <c r="G1243" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1243" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1243" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1243" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" s="1" t="inlineStr">
+        <is>
+          <t>A52100019352</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Mangesh  Kashinathan</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>A52100019352</t>
+        </is>
+      </c>
+      <c r="D1244" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=IxGHtDED34gdvx9kS%2bidc7rEu2VsUVqnez6uIzEn5UJ2Yck%2fTAH%2fdtOZxj6qdmv32VUpKcCuSioa%2bcS7ihOAuDnRA%2fwBWR4UtEi2mcNNsF8j0iKX%2bczEmJUiAbtJMLK7LlKLGHYCDx5fD5cCxxKxDp5kqE%2bmCj6PSmlK%2fcyP%2bK9T%2fqySSDqWqg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1244" t="inlineStr">
+        <is>
+          <t>02027203157</t>
+        </is>
+      </c>
+      <c r="F1244" t="inlineStr">
+        <is>
+          <t>Near Sbi</t>
+        </is>
+      </c>
+      <c r="G1244" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1244" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1244" t="inlineStr">
+        <is>
+          <t>Pimpale Gurav</t>
+        </is>
+      </c>
+      <c r="J1244" t="inlineStr">
+        <is>
+          <t>411061</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" s="1" t="inlineStr">
+        <is>
+          <t>A52100020166</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Rajeshree Yogesh Shah</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>A52100020166</t>
+        </is>
+      </c>
+      <c r="D1245" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=gViWuIjV0nsU%2fawLOQhe%2f5r56P9wkaji%2bnreVRtzgxqQZgFkR9eQJzgNUzRKW8HMPYcYlw03DrtnPfGPkiX9kFJuSnco66%2bQyaZLWZ6kYM5AO44NgT8qkVyTSjs5awAYb9pXKTG0cb9z5ciHALMfmQvgGeP%2fJAyIOcxiaWtLOt1KM2Ir7oLWmQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1245" t="inlineStr">
+        <is>
+          <t>02024478208</t>
+        </is>
+      </c>
+      <c r="F1245" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1245" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1245" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1245" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1245" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" s="1" t="inlineStr">
+        <is>
+          <t>A52100018868</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Ankush Jayprakash Agarwal</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>A52100018868</t>
+        </is>
+      </c>
+      <c r="D1246" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=DJmeE5zCJGrNbNsVlEtgUW50mKxOGsFpzy2wGQ5dfK8HKJfDyRe3%2fQnutjeF86G5NJjR%2brKMqIAAO7HwMhHYKLo01V5NyiP8%2bOA3W2aU%2bl%2b723nsVkO%2frYh%2f7%2b8o4ux9ZLgbkDs%2bqfLVmaq%2fGRO%2fUYGE1NGfbF5amy%2bozKmHnxHZH874D2z1bA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1246" t="inlineStr">
+        <is>
+          <t>02041240013</t>
+        </is>
+      </c>
+      <c r="F1246" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1246" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1246" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1246" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1246" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" s="1" t="inlineStr">
+        <is>
+          <t>A52100018781</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Yogesh Pradyumna Aphale</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>A52100018781</t>
+        </is>
+      </c>
+      <c r="D1247" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=geg7b2JynAHuihmSRJgbarikNC3n7jcUJ0gbXjCJGT3e7DCPctjkwHM0ztNnmgMyA2rFcBPWEhTt8BkWZi5BVnsbuxaoMVg149CMSBtIbTt8%2fflZfIOUCJDNIyt5rnuR%2brFHb5pt1j2V88AQ0TFvhjis5GDk65fAOEQFV0kBmHXEZ6OBaRVIVQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1247" t="inlineStr">
+        <is>
+          <t>02024269563</t>
+        </is>
+      </c>
+      <c r="F1247" t="inlineStr">
+        <is>
+          <t>Maharshi Nagar</t>
+        </is>
+      </c>
+      <c r="G1247" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1247" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1247" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1247" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" s="1" t="inlineStr">
+        <is>
+          <t>A52100002630</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Mahendra Nirmal Badgujar</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>A52100002630</t>
+        </is>
+      </c>
+      <c r="D1248" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=waHkRcDKf9Zr9BN%2fdxZiZjwCkQ8OAxgAHYRKhXM0Dg4J599twtP3PlB%2frRTshIbHBS0YA1fg20xVhkUqrQZwF6zg0KsGHRwawpQtvlq4LYYWmRX%2bdLzHmI9CLU%2fNBU%2bsmj3TDCtTiDKxQbIHvZMI6ibS%2b3eTllShd%2fUjK6zyvd979YoWSguaMw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1248" t="inlineStr">
+        <is>
+          <t>02026722082</t>
+        </is>
+      </c>
+      <c r="F1248" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1248" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1248" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1248" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1248" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" s="1" t="inlineStr">
+        <is>
+          <t>A52100002582</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Natasha Nitin Mahindrakar</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>A52100002582</t>
+        </is>
+      </c>
+      <c r="D1249" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=N2CATIdUscWLC1cTXqn2KkXtrvbnjy4C2AdSdgiNtdR6f4hKwR2ICKDo4oZsTJ%2fSqBDlDdCaaZgrz3taq4qDWP1zIG%2bKoirQwlyf9hBUxTXAW6hjX%2fGxNMq6e0dHwdJpKmlyFjh2AmtbpFC0TfMjzLKgieXInggU3troxeLA90T3ARYtAhNH2w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1249" t="inlineStr">
+        <is>
+          <t>02030204887</t>
+        </is>
+      </c>
+      <c r="F1249" t="inlineStr">
+        <is>
+          <t>Wanavadi</t>
+        </is>
+      </c>
+      <c r="G1249" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1249" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1249" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1249" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" s="1" t="inlineStr">
+        <is>
+          <t>A52100002093</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Reetu  Singh</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>A52100002093</t>
+        </is>
+      </c>
+      <c r="D1250" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=yTdnFyGKi7gD7Wt5HoodSW%2fbq0PtleTNTzSSqZK32ilBULBv5lpp1z3LOBUZQKx7oLrEztzI4mNhqkJkigtL0SP5Jz5GnD7quFNyb113c%2be9LD6KuF9o7YboUR2%2butt1ZGTJ2O6%2fVG%2bw%2bDeXMsPy4eXFcrBSn%2bh%2fyUWiC%2fjuxU9gFs78IvPQJQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1250" t="inlineStr">
+        <is>
+          <t>02026683156</t>
+        </is>
+      </c>
+      <c r="F1250" t="inlineStr">
+        <is>
+          <t>Lohagaon</t>
+        </is>
+      </c>
+      <c r="G1250" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1250" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1250" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1250" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" s="1" t="inlineStr">
+        <is>
+          <t>A52100003017</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Mukund Subhash Kshirsagar</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>A52100003017</t>
+        </is>
+      </c>
+      <c r="D1251" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=yIAuXAcO2axDetu5uW%2fO1kuDLATcbFIK6DRfoKTDZBxzfE9ggLQRWH3a8h0e%2bdR9XzcLqeTVTIqRm0kua2Wm2eD4%2bz9EeJ%2f8aKPyyUg9iT%2b5xlrIpdL%2brJNS%2bdxz42S1DBADfApmwZzpQ5kraE5bTv8FhOU37F0mTP%2bADPaVeZQUgxYn%2bSUZYw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1251" t="inlineStr">
+        <is>
+          <t>09689917835</t>
+        </is>
+      </c>
+      <c r="F1251" t="inlineStr">
+        <is>
+          <t>Wanawadi</t>
+        </is>
+      </c>
+      <c r="G1251" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1251" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1251" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1251" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1300]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1251"/>
+  <dimension ref="A1:J1301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64960,6 +64960,2606 @@
         </is>
       </c>
     </row>
+    <row r="1252">
+      <c r="A1252" s="1" t="inlineStr">
+        <is>
+          <t>A52100004278</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Estatemint Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>A52100004278</t>
+        </is>
+      </c>
+      <c r="D1252" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=iGdJOvmC5Tzgf0S8g4BnM2MIJDmALqMqTBCbQBsc6l3FDtQS3imcVzkNC5vYWUDB1r4IyRUpdoUgQqSPmHL9vtvw8MN9lHW57Nv6BZ9B7KVPdfhzOwS1bBpqGaOAOt4BhtvjgJw6wcEJ0oTauSKTMIE7vDNIkqPRxBnQoIOR0cAuPnuH2Us91Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1252" t="inlineStr">
+        <is>
+          <t>02066895996</t>
+        </is>
+      </c>
+      <c r="F1252" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1252" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1252" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1252" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1252" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" s="1" t="inlineStr">
+        <is>
+          <t>A52100002474</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Saghher  Jhalaani</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>A52100002474</t>
+        </is>
+      </c>
+      <c r="D1253" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=BC%2fxT8LE1GTzH2nL6cQMtGzt7NaBzuFtjdrS7lS5pP6alfItJ8LamX8irrRxuLaKFMlu0BUBqoZ4SDAJ4hbfxU2EQQVdxrYA5gSyo9G7tcrOPzcXqEGcOuPcD4ALdN2MatZgA2xwrIbZwl1xLkpDtTIo8elV%2bvoR1vOy5G0WHrfUFJVaSp4rjw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1253" t="inlineStr">
+        <is>
+          <t>02067274103</t>
+        </is>
+      </c>
+      <c r="F1253" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1253" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1253" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1253" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1253" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" s="1" t="inlineStr">
+        <is>
+          <t>A52100002993</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Deepak Choithram Budhrani</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>A52100002993</t>
+        </is>
+      </c>
+      <c r="D1254" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=HDTTU3Qe8Bl4aNOwRt%2bOjFXttJ80D7I1J90%2bApp110cuZapMfEsl17Sc1lUQ9FAKFgUUtr%2b%2fFYS5hMThHMVD5AHbddjHEIC5FT5jiWcSgycn%2bkW5qrXcqRiyrl3PIXE3zESsas6HcmOPcErgm8ZV2HMELPybrL6LRba66g6RNsKuXvD3eBTtHw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1254" t="inlineStr">
+        <is>
+          <t>02026158013</t>
+        </is>
+      </c>
+      <c r="F1254" t="inlineStr">
+        <is>
+          <t>Koregaon Park</t>
+        </is>
+      </c>
+      <c r="G1254" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1254" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1254" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1254" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" s="1" t="inlineStr">
+        <is>
+          <t>A52100003833</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Sameer Arvind Vakharia</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>A52100003833</t>
+        </is>
+      </c>
+      <c r="D1255" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ZH%2fvjfVxzJDspvTPy64icYydEOOdWY7DjfMHCoJcogErbqHKWtOolCpv%2bKnFgGa5eXs3bPQ8tMOI2EyjENfAe5zaNpj0LiMcjfhOnsgCjbQWGKM9zjWtUPzmrmF2%2fYkgzQW85L4Nv9r3WNQh6LDAqJXXnC6UvYrXhI8YGyWpIYdi8E%2bFpvdcHA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1255" t="inlineStr">
+        <is>
+          <t>02027201020</t>
+        </is>
+      </c>
+      <c r="F1255" t="inlineStr">
+        <is>
+          <t>Rahatani</t>
+        </is>
+      </c>
+      <c r="G1255" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1255" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1255" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1255" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" s="1" t="inlineStr">
+        <is>
+          <t>A52100002996</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Govind K Shewani</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>A52100002996</t>
+        </is>
+      </c>
+      <c r="D1256" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ogX5irDuXhLv2xCsPnV%2fQiktoT%2b3x20qzHrDj5h3Vrdvu7cmMsOPbcCah5SMqhpRYI0tHiEJLnXpAPfUkQiRr6K%2fH4idsZWYxsp%2bCU0RIJMY8BMsrwSGZqPsX6PuOXYQyvfxLh22%2fft6a8ccnB3K3r7Tx4nPO1MNCA0lD34MN9fJf8ME3UeeLg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1256" t="inlineStr">
+        <is>
+          <t>02040092485</t>
+        </is>
+      </c>
+      <c r="F1256" t="inlineStr">
+        <is>
+          <t>Wanowrie</t>
+        </is>
+      </c>
+      <c r="G1256" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1256" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1256" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1256" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" s="1" t="inlineStr">
+        <is>
+          <t>A52100007344</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Kushagra  Soni</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>A52100007344</t>
+        </is>
+      </c>
+      <c r="D1257" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=77vMAxoK8bEGZMaki4flwE8lQpx68FPOQORc6zsAfIgIdY67%2bojBT1b85fUQE7Tx2EEDtW5C5qwvcIJFnpMvJgQL2hiRkYKUDJKxSU0iSBjD%2fpGm8W7jd3ik6%2f3UL2ev09c0EriMasB9weoYOm5RLANmFqivPxxdC27sB483MAAYMNomrnvCrA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1257" t="inlineStr">
+        <is>
+          <t>09960870070</t>
+        </is>
+      </c>
+      <c r="F1257" t="inlineStr">
+        <is>
+          <t>Ghorpadi</t>
+        </is>
+      </c>
+      <c r="G1257" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1257" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1257" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1257" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" s="1" t="inlineStr">
+        <is>
+          <t>A52100007332</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Ravi Ranjan Kumar Gautam</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>A52100007332</t>
+        </is>
+      </c>
+      <c r="D1258" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=nOnsoo%2fB5rqSkLXt95tC9%2bpUb%2fd3pL0jd%2fujIeLgo2kSHJrpkSJRECaUsokFp7ZolQiPssCII8ourbR%2bVQjEgnREPcvU6HIjH7klrX12PuV2xCHH1brn6SUwG5OcVUFyA%2fAtV7VTsAURPIGph6n83TjFeMPJuMD97IYs6CfkmTrjMYew9BkuSQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1258" t="inlineStr">
+        <is>
+          <t>09834162225</t>
+        </is>
+      </c>
+      <c r="F1258" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1258" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1258" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1258" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1258" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" s="1" t="inlineStr">
+        <is>
+          <t>A52100003785</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Yogesh Mohan Sutar</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>A52100003785</t>
+        </is>
+      </c>
+      <c r="D1259" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ZYGffib5uMTmUbK5eNNhvcj0hvTc5c7MXFKYg02kWtbykf5X7LTvu%2bD9rflZT2qwZZdEWWNlCCJjLx4pwTcktXLR38KSJDzjjG1DxetgQG%2fakilgfRVGriibi%2b2V3hlUAvAIt7F%2fdUnVwfmcYQFDaok7gYr227b%2bT3ZxF6bjw%2fURhZI4wT8Uwg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1259" t="inlineStr">
+        <is>
+          <t>02065222375</t>
+        </is>
+      </c>
+      <c r="F1259" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="G1259" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1259" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1259" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J1259" t="inlineStr">
+        <is>
+          <t>411058</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" s="1" t="inlineStr">
+        <is>
+          <t>A52100002367</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Sharmila Swaminathan Iyer</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>A52100002367</t>
+        </is>
+      </c>
+      <c r="D1260" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wqlerROzjIC4N15IzISrPfLnRPUFCFSsP11tMO4bLHwP48NM6VdXRcNasZGsm2HrKraZUGJBTOvDJZ5OQLUMpStRe4eMWrfSTKKx4Py6lOaas692nS89%2fAFQm5av9JBNVETmF0AUgRQ27xvAgsNsFklrxDB5Sya9v9lulsgf2MC8zDqXvaE2nQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1260" t="inlineStr">
+        <is>
+          <t>09225420247</t>
+        </is>
+      </c>
+      <c r="F1260" t="inlineStr">
+        <is>
+          <t>Tathawade</t>
+        </is>
+      </c>
+      <c r="G1260" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1260" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1260" t="inlineStr">
+        <is>
+          <t>Tathwade</t>
+        </is>
+      </c>
+      <c r="J1260" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" s="1" t="inlineStr">
+        <is>
+          <t>A52100002705</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Sudhir Devidasrao Deshpande</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>A52100002705</t>
+        </is>
+      </c>
+      <c r="D1261" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Q%2fw7FsvXEx%2bAYMSZloojWgCToazOM4DlCeCTcyqK%2bV2SYGwfkktQywPP5dfQIBGFh5atrOL2jX1%2b5hY1vpAIHP9cbh85PPln8XYYV7hB2Ze1jN%2f8lqWnxRdlHz%2fg5vNlJaA8aV3WqFzDrJDQe7kVjiMm3m7zz9M6Uw4nQroXDEo41ZAQaReU2g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1261" t="inlineStr">
+        <is>
+          <t>02024347600</t>
+        </is>
+      </c>
+      <c r="F1261" t="inlineStr">
+        <is>
+          <t>S.No 14,Wadgaon Bk.Anand Nagar</t>
+        </is>
+      </c>
+      <c r="G1261" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1261" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1261" t="inlineStr">
+        <is>
+          <t>Wadgaon Bk</t>
+        </is>
+      </c>
+      <c r="J1261" t="inlineStr">
+        <is>
+          <t>411051</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" s="1" t="inlineStr">
+        <is>
+          <t>A52100008304</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Saroj Vinod Jain</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>A52100008304</t>
+        </is>
+      </c>
+      <c r="D1262" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Q1fRDJ3w5yXmEqGYz1Enk2j4SmrpUuhwFTqvyladSZK9Mb%2b8na1h9Ky1ZdgHqTa9FGgR1Sk5S%2fYGuLE%2fXwJDJiewehh1%2b%2bn5qfGDGYw%2fRAFDeYe1VmMjSw%2fmwODvk%2f71aFcicdRCIN02ynhb0blMxsdiAs63yONmvisheczljc0KDIA2PEdHzQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1262" t="inlineStr">
+        <is>
+          <t>02032341008</t>
+        </is>
+      </c>
+      <c r="F1262" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1262" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1262" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1262" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1262" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" s="1" t="inlineStr">
+        <is>
+          <t>A52100008409</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Santosh Vasant Patil</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>A52100008409</t>
+        </is>
+      </c>
+      <c r="D1263" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=60TXRaB73Wp%2bYBjXYqHPuQwqMaloFtX2f7bsfMxK1Ki%2bay6ZzGAS6mweJAVHW1tHMBWE6J7i02Wc%2f5wTTQRVQ973oo4pv7HecVB8WBKcRfYPuOZf38XdF1tdXVTNH5NGU%2b4OYkoXPszs2TJyRWpDUOrrFK%2bm%2b8D7w81WA8vK3nNBRfkuFKSEWg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1263" t="inlineStr">
+        <is>
+          <t>02025888866</t>
+        </is>
+      </c>
+      <c r="F1263" t="inlineStr">
+        <is>
+          <t>Pashan Road</t>
+        </is>
+      </c>
+      <c r="G1263" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1263" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1263" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1263" t="inlineStr">
+        <is>
+          <t>411008</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" s="1" t="inlineStr">
+        <is>
+          <t>A52100007712</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Sharad Ganeshrao Chatte</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>A52100007712</t>
+        </is>
+      </c>
+      <c r="D1264" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LC2u%2bkNd5IZjqMQuEsAK%2bFgRsn8Rkxu28qN6T4qeKAmDFulVm4PMhRZQC30AUDp1VlRIVQ2Ml5CEYe4Opx4FpBra5hpSSxv%2bedmabntWcgPFlgXRq9kXfEZWjDYWq2sjwRCHzyrQBni81er4EvrjyOymieNddxwW7butYTX4Ki5di48O1fHhxA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1264" t="inlineStr">
+        <is>
+          <t>02065343437</t>
+        </is>
+      </c>
+      <c r="F1264" t="inlineStr">
+        <is>
+          <t>Ganesh Nagar, Dhayari</t>
+        </is>
+      </c>
+      <c r="G1264" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1264" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1264" t="inlineStr">
+        <is>
+          <t>Dhayari (Part)</t>
+        </is>
+      </c>
+      <c r="J1264" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" s="1" t="inlineStr">
+        <is>
+          <t>A52100007129</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Mantra Properties And Developers Private Limited</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>A52100007129</t>
+        </is>
+      </c>
+      <c r="D1265" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KIQCphPbF0N6hB2Q4aKSQ35c9PPbNWaoQy0nPnyRQ%2bEjFpKaC0kIO4aE%2fla5KxZc3eKrxF%2bYomluULzwbDWhNhNVc47ATl753EQJvt92xATSniZgGP0PQJEAuco87nuZwYYJ9GrWIAzmTcnkMdKiQABBGwIuGPcNokDV2AtWWPXkzzOEduD8fQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1265" t="inlineStr">
+        <is>
+          <t>02066081700</t>
+        </is>
+      </c>
+      <c r="F1265" t="inlineStr">
+        <is>
+          <t>Bundgarden</t>
+        </is>
+      </c>
+      <c r="G1265" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1265" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1265" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1265" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" s="1" t="inlineStr">
+        <is>
+          <t>A52100009059</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Vijay Harakchand Navalakha</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>A52100009059</t>
+        </is>
+      </c>
+      <c r="D1266" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=RrlqDAPtamPwtd7axo6Yv0v9gothCWIsBdkIHsb6X%2fHZE%2f3ZL4wl8d%2fckYB%2f6%2bYmNzDItA6mWW%2fhpbzgCbj0i4b77w9Mxhc3oSwcwlVXW4frmBYfdZWxHR1JrDlfGz3cZt%2fYWnJJS2evlEBhRbavHDzq%2baIfzK64F5kgpBIyvZJzoyrpC500Lg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1266" t="inlineStr">
+        <is>
+          <t>02024261620</t>
+        </is>
+      </c>
+      <c r="F1266" t="inlineStr">
+        <is>
+          <t>Market Yard</t>
+        </is>
+      </c>
+      <c r="G1266" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1266" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1266" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1266" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" s="1" t="inlineStr">
+        <is>
+          <t>A52100006131</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Prashanta Pratim Das</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>A52100006131</t>
+        </is>
+      </c>
+      <c r="D1267" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=B2nQaUTpnRgRj41hBsgjZ8DIAqCJ4X%2flxndL7LZ7xGSeKKsxBrzEHKljCwRIdJO4%2fMiahZWm1UMIBmoOGcAmBBAdBQyE0GJ%2f4xDLwk9XUpX%2b8%2fGRsdBeeJWLFcaw0%2ffgFodrQzLIZF4TiyO1DR%2fHPcW8jlW1rN9yMa3Hczj67cmsrH8x96LxMQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1267" t="inlineStr">
+        <is>
+          <t>02030684228</t>
+        </is>
+      </c>
+      <c r="F1267" t="inlineStr">
+        <is>
+          <t>Sakore Nagar, Viman Nagar</t>
+        </is>
+      </c>
+      <c r="G1267" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1267" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1267" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1267" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" s="1" t="inlineStr">
+        <is>
+          <t>A52100002379</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Shivraj Jayaram Hegde</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>A52100002379</t>
+        </is>
+      </c>
+      <c r="D1268" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=G6bu%2bQBbnG4g5Qgpoao8fdev29tArrLijyg8yXyDmVu%2bGx6OfkdsiiwO%2fp10N2UKKZJD4Y9RPYFgpfWVZ6Vqb5C6chpOHHLJxHUwXPp%2fFDx04OWJMRNcKkxsiBdToMjQMH6zmhGvsAxKNU%2fgYP1fZQV4Q9cBHhDZJBkOZ9i6w5DbAuqH6LMOZQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1268" t="inlineStr">
+        <is>
+          <t>09990931189</t>
+        </is>
+      </c>
+      <c r="F1268" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1268" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1268" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1268" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1268" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" s="1" t="inlineStr">
+        <is>
+          <t>A52100003648</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Sagar  Sharma</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>A52100003648</t>
+        </is>
+      </c>
+      <c r="D1269" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=GLefF19tJX6D%2fCQcECGD45mwHxK38rQ4axPUYN7S0a5s3P6ITkiPs9wzDo3e66uINe7vQR6GkWNLZ9w2Yd5Twc%2bx8Pkd3Lk%2faVk9VDlVogy%2bjF4kS%2f8s1Xk0e17%2bPtQll5oljpwiLkUwWQpaJJ5fqZ%2fe08CmhOnujJNyZj8yAozrBWxGnMFRbg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1269" t="inlineStr">
+        <is>
+          <t>09067330999</t>
+        </is>
+      </c>
+      <c r="F1269" t="inlineStr">
+        <is>
+          <t>Chandan Nagar Bypass</t>
+        </is>
+      </c>
+      <c r="G1269" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1269" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1269" t="inlineStr">
+        <is>
+          <t>Chandannagar</t>
+        </is>
+      </c>
+      <c r="J1269" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" s="1" t="inlineStr">
+        <is>
+          <t>A52100002623</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Josef George Anthuny</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>A52100002623</t>
+        </is>
+      </c>
+      <c r="D1270" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2fmbYQcYIS%2f0g%2fzZWLXftm7%2fBS53DufVb1PKJoxHHjLzue0%2bqVwEiLD6yMaxtSHmQxchMEB%2fY99E2kAF12xHW5BbxbWH4JtgXao1TCEES2CU9pwXrCG0PXoP%2bvK3klyU%2fyxOG7eAgSMwPq6moHi%2bLpgVKpgkTZfHB5Ap%2bQINc7Gk55U2x8B5Q4g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1270" t="inlineStr">
+        <is>
+          <t>07276372582</t>
+        </is>
+      </c>
+      <c r="F1270" t="inlineStr">
+        <is>
+          <t>Handewadi Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1270" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1270" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1270" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1270" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" s="1" t="inlineStr">
+        <is>
+          <t>A52100003486</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Loveena  Leonardo</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>A52100003486</t>
+        </is>
+      </c>
+      <c r="D1271" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=4GGAwDdbOyc5L7W2fuVVZQcLLx5nF1d99jCcdhW51ME0ZMUUw8UhuGoQVKywX9ofi6R9hlzCPy3N4xZA%2fe8Cb2ho92vwZ0AFAjK9Kp%2bkk7rtIqQY7QWqOvkZi6gSsHC3LNg5Bw0KYUNi06Wqah5xu6Nw3ARRWDM8UVJkp%2bad3H1zWtiHynkvlA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1271" t="inlineStr">
+        <is>
+          <t>02065342229</t>
+        </is>
+      </c>
+      <c r="F1271" t="inlineStr">
+        <is>
+          <t>Bund Garden</t>
+        </is>
+      </c>
+      <c r="G1271" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1271" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1271" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1271" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" s="1" t="inlineStr">
+        <is>
+          <t>A52100008207</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Shubhangi Sanjeev Sindgikar</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>A52100008207</t>
+        </is>
+      </c>
+      <c r="D1272" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2esLE2j6t%2bQwe3xhXnzdY%2b%2fLTMfP%2f39FtpW18bx%2bvNLkEAy%2bElr9ffHR8%2bFlOkHKUdUuTLGjo3YWUkYYj7mZoPUc1zzAO%2fhhAj1iyg2iLpqa5Y8yXkSmfKVg%2fxFhBOz1bvnJXPKh7taflwfY473AStmu48w6N%2fq0R%2frxqNj9d98%3d</t>
+        </is>
+      </c>
+      <c r="E1272" t="inlineStr">
+        <is>
+          <t>02025900160</t>
+        </is>
+      </c>
+      <c r="F1272" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1272" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1272" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1272" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1272" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" s="1" t="inlineStr">
+        <is>
+          <t>A52100002771</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Nitin Mohanlal Ghiya Khandelwal</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>A52100002771</t>
+        </is>
+      </c>
+      <c r="D1273" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=FUeP7tmi6C%2bfFUH7mk%2bQ%2bEsErOBHIrFrGY7PFNvM%2baPtbKePqVTmI9ipjGA9egF%2beJsiwUg3KFq1m5H90%2fgyhUnSgOek9m5q0e7fQsIrc1Lfwx4BRWPfR%2f%2fR35SFINIFnZPpB7F5QAKHjeDKyljDNgPMFZu9hIMNhVkyYidulDwLNBkgPTGCFg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1273" t="inlineStr">
+        <is>
+          <t>02026722082</t>
+        </is>
+      </c>
+      <c r="F1273" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1273" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1273" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1273" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1273" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" s="1" t="inlineStr">
+        <is>
+          <t>A52100006602</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Amol  Awale</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>A52100006602</t>
+        </is>
+      </c>
+      <c r="D1274" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=87cv6wT8Tap73JCXqyZRU8lJDGWzwJ59Mk7Cd3SH41I6TJsWnaerfPdVY7mRTkLExkWzEJWAS%2bKqZ0euZXSGzbVHYqCKnGP8yVVev3NZxkRevqzOQdT3wUF7J5L632lrxZ7MoyQblm1Lg1p9KpDoj5Pal9%2f0h3e2K5SoODCHngg%3d</t>
+        </is>
+      </c>
+      <c r="E1274" t="inlineStr">
+        <is>
+          <t>07219607388</t>
+        </is>
+      </c>
+      <c r="F1274" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="G1274" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1274" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1274" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1274" t="inlineStr">
+        <is>
+          <t>411043</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" s="1" t="inlineStr">
+        <is>
+          <t>A52100002577</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Awanish  Kumar</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>A52100002577</t>
+        </is>
+      </c>
+      <c r="D1275" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QPhDcAxhYsk0jaqmMjEHJDmROhg3q4pobTB1XOJBQgZ4MzfUmES2SO6BJ4vR3l5UrW1DuHEBVgolPJDxbap0jKI9T3NE2tKUsbfcnaAdxf3MHi4YhDQft19%2bB%2f9k0F5KR%2bGJ%2fSgwCWwTGJjLQf%2bxebIzDZPLZsV483yiIDipK2WEQ7RARAibBA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1275" t="inlineStr">
+        <is>
+          <t>07875333360</t>
+        </is>
+      </c>
+      <c r="F1275" t="inlineStr">
+        <is>
+          <t>Near H.P. Petrol Pump</t>
+        </is>
+      </c>
+      <c r="G1275" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1275" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1275" t="inlineStr">
+        <is>
+          <t>Marunji</t>
+        </is>
+      </c>
+      <c r="J1275" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" s="1" t="inlineStr">
+        <is>
+          <t>A52100009755</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Suvarna Tukaram Pansare</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>A52100009755</t>
+        </is>
+      </c>
+      <c r="D1276" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=oKOFWZhLFY7XHruyXnIEH6cwUHiGiwbki0nS7L4C7EvPaIJ7tdSAM27n3imcSgvAiQRjrCwNLDPlrFj8TQLM5e90SYG0xvQ2IoPxcAwwzoy%2bALolhPLApSH2mEJa%2bTudEizvAVe1avmvp5atfwMNNCcSJsqClZNuc6BNyZADLiuwulpyhE2T3Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1276" t="inlineStr">
+        <is>
+          <t>02067074100</t>
+        </is>
+      </c>
+      <c r="F1276" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="G1276" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1276" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1276" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J1276" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" s="1" t="inlineStr">
+        <is>
+          <t>A52100004450</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Mukesh Gridharilal Agrawal</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>A52100004450</t>
+        </is>
+      </c>
+      <c r="D1277" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KASb6gP60C6b7gkmUSz0fzl%2f%2fxMtzqC2NOIeCpWr4rNCdI%2fvkTJAbpizPgXiLh0xQQaw0yD5h8YDv3LVqv5%2fL03WAvM0Oj2lz95VZh00yu9G%2bsyYQl1aG9vPGi4POjc4oTr%2fYXLA8kmLn8B4mS4g314f5tr%2bN9RR2X3kZT9b8WAIo5aYmBQFYw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1277" t="inlineStr">
+        <is>
+          <t>02065271010</t>
+        </is>
+      </c>
+      <c r="F1277" t="inlineStr">
+        <is>
+          <t>Wadgaon Sheri</t>
+        </is>
+      </c>
+      <c r="G1277" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1277" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1277" t="inlineStr">
+        <is>
+          <t>Vadgaonsheri</t>
+        </is>
+      </c>
+      <c r="J1277" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" s="1" t="inlineStr">
+        <is>
+          <t>A52100002452</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Sayed Hussain Hussaini</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>A52100002452</t>
+        </is>
+      </c>
+      <c r="D1278" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=B6Tyt358U6msPHFxWoXh2l7%2fYn%2fJMJv6Wb0kRJANUaX8VKJs1b3jPP4WeArY%2f0G%2fqBtzpNyfs9D9qU3p10P%2bDzObDogJuulpoDtiWM61%2b3lSVxvxWzMpUFbQwViwkK2RqJX3qSwhfLfozdCJmRRG1u8qUpA%2fI7MXpOpwLH5xYC99FekkY0%2fAsQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1278" t="inlineStr">
+        <is>
+          <t>02041205277</t>
+        </is>
+      </c>
+      <c r="F1278" t="inlineStr">
+        <is>
+          <t>Wanawadi</t>
+        </is>
+      </c>
+      <c r="G1278" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1278" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1278" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1278" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" s="1" t="inlineStr">
+        <is>
+          <t>A52100002443</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Abhay Shrirang Dandekar</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>A52100002443</t>
+        </is>
+      </c>
+      <c r="D1279" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=kWgfyu5FEqO5ql2PhF5qcu8f0dt8B%2fNRhtqEK07XyIwo82gYRmPL4e%2fe26tpQ8hyxQ4ZRxPmHqHSPzWQrrZaTro5pS%2boTXYBFiR2Gn1kvkzPCOVngdcmpCbpku8sDPxBE4LKouosqe14kIpmhe9o3DqfZiPsa43CJu9Ze%2bWtQgmzcyKeVyofRw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1279" t="inlineStr">
+        <is>
+          <t>02027653727</t>
+        </is>
+      </c>
+      <c r="F1279" t="inlineStr">
+        <is>
+          <t>Nigdi Pradhikaran</t>
+        </is>
+      </c>
+      <c r="G1279" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1279" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1279" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1279" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" s="1" t="inlineStr">
+        <is>
+          <t>A52100004303</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Mahesh Sharad Shendge</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>A52100004303</t>
+        </is>
+      </c>
+      <c r="D1280" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=EWiXyIEHpaYlwr58JkP9XIQXu8JD4sqAsaqZbSU%2bYMk1PmxIGAP33%2fWG8hD3ZO2ZBpTzYuLK4VMt51mVJmr1V9Z138KwPFb6A%2bXtuM9%2bYDUMVD698HmhjOu%2fLZVs4E3tEsIz50fmlwpmMk3tx4sLI3pm6ci%2fq%2f49zEmiffWmo7P3WRVqohJmEg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1280" t="inlineStr">
+        <is>
+          <t>02060200400</t>
+        </is>
+      </c>
+      <c r="F1280" t="inlineStr">
+        <is>
+          <t>Swargate</t>
+        </is>
+      </c>
+      <c r="G1280" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1280" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1280" t="inlineStr">
+        <is>
+          <t>Swargate</t>
+        </is>
+      </c>
+      <c r="J1280" t="inlineStr">
+        <is>
+          <t>411009</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" s="1" t="inlineStr">
+        <is>
+          <t>A52100002071</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Deepali Shrikant Patil</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>A52100002071</t>
+        </is>
+      </c>
+      <c r="D1281" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=M03dGLBFuh8Pj4m914VEq4tlu9hKi4ExmH%2bxD%2bdGiD4I8TEMH72tLcMXBo2mT1Elois97cQL7%2bFXZRI9iD%2bFeXCLkWBwLV7ARxVdq%2bfIO2a9RDnO3akNrgi82nZXULPbKwAPUXsBy%2bgmWs7NE9ZUaKWWL7OmMQvECXQE1e6QO8M%2fVpMV9%2fDhVw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1281" t="inlineStr">
+        <is>
+          <t>09881440546</t>
+        </is>
+      </c>
+      <c r="F1281" t="inlineStr">
+        <is>
+          <t>Gokul Nagar Dhanori</t>
+        </is>
+      </c>
+      <c r="G1281" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1281" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1281" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1281" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" s="1" t="inlineStr">
+        <is>
+          <t>A52100002469</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Suresh J Jhuramalani</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>A52100002469</t>
+        </is>
+      </c>
+      <c r="D1282" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=rIpFrA9c%2fUBfWDMnEv30GbnTpQ7kldKKs4wkeF%2bRg2DGUvv5hhQq3OC%2bb9tqtvQXnMHMHFcJ%2bEKqg3fgh0Fl4JIzYCS2UBKxhmhb%2f6%2fS8bXcrv1Nh37HOjGKfKaJ5ySBP%2fBeDXn7haXRQTZyRo6VvBLV5JS45wqTuWBr9hzG3oFEYFgVo26z%2fg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1282" t="inlineStr">
+        <is>
+          <t>09730958000</t>
+        </is>
+      </c>
+      <c r="F1282" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1282" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1282" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1282" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1282" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" s="1" t="inlineStr">
+        <is>
+          <t>A52100002560</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>A2Z Online Services Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>A52100002560</t>
+        </is>
+      </c>
+      <c r="D1283" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=poHw%2frJAmcn2xX9prY7GxAGwjhV0lH1O596qcypxNVoHch9bX0xcA2JZbkA6Sa28x6m%2bF3X7Yqord1%2bM0w0se14pvqmWlU9o6CLMRaQLpiA35wZbSkRx0wmvFN6205yi9OEfHTFJVLwL7Ytw18aRuX0zF7209SJyqLJXDlfkp245KGDR5o4Suw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1283" t="inlineStr">
+        <is>
+          <t>02066473200</t>
+        </is>
+      </c>
+      <c r="F1283" t="inlineStr">
+        <is>
+          <t>Yerwada</t>
+        </is>
+      </c>
+      <c r="G1283" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1283" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1283" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1283" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" s="1" t="inlineStr">
+        <is>
+          <t>A52100000903</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Ravi Chaitanya Varma</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>A52100000903</t>
+        </is>
+      </c>
+      <c r="D1284" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ywy40ZI8dIq35CWm8gPLakc%2buZLn2VVwn%2f5MI%2f17n9pISdFjLcoEcOtPmY815e%2bjIN2k6qjjBu3ZXOuncODUuueCO49IMWr4yqx49BoCID3tlELX%2fsfasgUylfMcskewIUicVKomiAsokO6idiYHzEiVF%2fntiCpcniwGeJ1mvilDgKYBKLykEg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1284" t="inlineStr">
+        <is>
+          <t>02026138104</t>
+        </is>
+      </c>
+      <c r="F1284" t="inlineStr">
+        <is>
+          <t>Camp</t>
+        </is>
+      </c>
+      <c r="G1284" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1284" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1284" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1284" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" s="1" t="inlineStr">
+        <is>
+          <t>A52100002732</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>K G Ramesh Kumar Nair</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>A52100002732</t>
+        </is>
+      </c>
+      <c r="D1285" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=4fNCazRENoDnDmxiTyvh%2fD%2bgVuCiQnHhA%2bnxrpkwhMaIsbAE5BYL5amR3A3P5Gk5SMXl%2fEcWGyNCVl%2b%2beDZR35Qj9tC46WluXDmWdGyGr3VpEdiE%2b%2bbqzBd%2bK8jYX7%2fjeBX8Y4i4wdJs7AJVfSqokmw4O59o%2bPtqsK0AJwsWsgF2NYW%2fDPI89Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1285" t="inlineStr">
+        <is>
+          <t>02027001007</t>
+        </is>
+      </c>
+      <c r="F1285" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1285" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1285" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1285" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1285" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" s="1" t="inlineStr">
+        <is>
+          <t>A52100004647</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Vinayak Raghunath Medhi</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>A52100004647</t>
+        </is>
+      </c>
+      <c r="D1286" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3f3y0KSkEsg6PIdZOXCPDcgR2ePRH%2fpSafxQfF1Ky0z%2f9v9vno6HyRRPBj5uggUcnX86wzezNYEny%2bf2cmi3xjnL827T5EVxFKBEhz7fXOXaHDJBvJKbs97VaSq2sv0sQJ0vMmxHcc9VicaTXuUpfpRpRCQrEpmwErWEVGXOrW%2bKQAZR1aHfYA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1286" t="inlineStr">
+        <is>
+          <t>02024492149</t>
+        </is>
+      </c>
+      <c r="F1286" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1286" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1286" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1286" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1286" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" s="1" t="inlineStr">
+        <is>
+          <t>A52100004366</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Rafiq Ramzanali Premji</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>A52100004366</t>
+        </is>
+      </c>
+      <c r="D1287" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Jo3OIVpM%2bFcb8APBM%2b%2bvDwAn5F5iImDSeCoVyBiZR5j%2bvrUsj8hSUHFlYqxxgGzsT76uhnvgpWmljua8Hc6C%2b7M4Gh%2fOH1vf2Xhk3%2bzZHhTn%2fNVHIPuQAEVxwB2OTW6M13qsUgBDFeyGjXbhL%2fVStejZTkn7V32tVoMvZsbXAbD5UFqShCtbSA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1287" t="inlineStr">
+        <is>
+          <t>02026600456</t>
+        </is>
+      </c>
+      <c r="F1287" t="inlineStr">
+        <is>
+          <t>Kalyaninagar</t>
+        </is>
+      </c>
+      <c r="G1287" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1287" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1287" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1287" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" s="1" t="inlineStr">
+        <is>
+          <t>A52100019543</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Estatepedia Llp</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>A52100019543</t>
+        </is>
+      </c>
+      <c r="D1288" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=x5rzeXDm40%2bpyxnonZF0z8y9LZADjaFrs02JsdJSZ%2bKhCRZUPABu24R1bw2ulG9%2bTocR6%2bBBP%2bJ1%2bSsG6uA%2b35c4NwC7Y4sYpsH4UAli4tw0hfcEmKj7QOZPthi55m0eyKNngRlt0onvPmqPJkIcJRK%2bi74Yc0eGE11GvS%2fdb2AxenOTTdIzeQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1288" t="inlineStr">
+        <is>
+          <t>08007776246</t>
+        </is>
+      </c>
+      <c r="F1288" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1288" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1288" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1288" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1288" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" s="1" t="inlineStr">
+        <is>
+          <t>A52100019190</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Mudita Realty Services Llp</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>A52100019190</t>
+        </is>
+      </c>
+      <c r="D1289" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=IJcD8fymFbOWN21LTaqFETjFnxOiAn3PUc%2fpa7zacL8dk4N%2fkeTPmbrwb6xAviZsjBPVNnNA3izfXQaKjfKE%2bRY4Xe0v9w4hi77jV6zmzavxwanQ1G6CKMFXrDW8t772AC0Na1g5azxeyALaeH3kOpMXPWEt2nwoe6r6d3KyNaRcGCpL6eGnWg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1289" t="inlineStr">
+        <is>
+          <t>09890499111</t>
+        </is>
+      </c>
+      <c r="F1289" t="inlineStr">
+        <is>
+          <t>Telco Road Pimpri</t>
+        </is>
+      </c>
+      <c r="G1289" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1289" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1289" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1289" t="inlineStr">
+        <is>
+          <t>411018</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" s="1" t="inlineStr">
+        <is>
+          <t>A52100018846</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Ajay Prabhakar Patukale</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>A52100018846</t>
+        </is>
+      </c>
+      <c r="D1290" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ShPQgRKadgUE0NHqaJu4cDIaatQim8VBOB4s3keKMPSpSVN9%2fdFXxhDMSyC3yTybBnjqJ21pRifow3xIsu2mfHhPcpn%2fRIW%2fQzcL9H3jGPPQMJSg4PDZPbm3sC2hk5DuezWIUfmyNBtMlGcBMzDc9E0ioCgQ1UQrvTlQwgqN68wNF2wJf8AFmw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1290" t="inlineStr">
+        <is>
+          <t>09850085503</t>
+        </is>
+      </c>
+      <c r="F1290" t="inlineStr">
+        <is>
+          <t>Pimple Nilakh</t>
+        </is>
+      </c>
+      <c r="G1290" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1290" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1290" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1290" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" s="1" t="inlineStr">
+        <is>
+          <t>A52100018709</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Tasmiya Imran Shaikh</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>A52100018709</t>
+        </is>
+      </c>
+      <c r="D1291" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xruYwtL650htsL%2b1gJkr83aJ8Gt%2fnHF7zYa6Dkyl7IRqUsUgJl3Ye2bEXbD3ClH47a%2fAc%2f0c4yOXwGFXHGg89YDziEih9lWaPcvxQ9i9lg%2fDhubeeeiAwUi5TqnzXvevtx5oEVvFs32n7zzPB9ON34AlfHsIhQiE9kwzZ%2biv1m8qSJExO0b5YQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1291" t="inlineStr">
+        <is>
+          <t>02048604927</t>
+        </is>
+      </c>
+      <c r="F1291" t="inlineStr">
+        <is>
+          <t>Lohagaon</t>
+        </is>
+      </c>
+      <c r="G1291" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1291" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1291" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1291" t="inlineStr">
+        <is>
+          <t>411032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" s="1" t="inlineStr">
+        <is>
+          <t>A52100018905</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Ashok A Palke</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>A52100018905</t>
+        </is>
+      </c>
+      <c r="D1292" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=VqOgv%2bzfm%2bQ40QM%2fBYj8tHsy8scQagThnGE%2bU7P%2bmkLezQJp1g5Vs%2fmijt%2b%2b9cDR8juaGAJEubqrzy1%2fN9q2XHrw6XNcPwiCs94P59UN%2bRubGTF%2bBwh8NVaj0j9OynMtQzWTGKR7ZDOsmE%2b0yTQj2MqjiZ6To%2bKDz3Op9eczMajaoMtMs9RoeQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1292" t="inlineStr">
+        <is>
+          <t>09011347178</t>
+        </is>
+      </c>
+      <c r="F1292" t="inlineStr">
+        <is>
+          <t>Opp Vanaz Paud Road</t>
+        </is>
+      </c>
+      <c r="G1292" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1292" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1292" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1292" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" s="1" t="inlineStr">
+        <is>
+          <t>A52100018927</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Rahul Vishwanath Gowaikar</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>A52100018927</t>
+        </is>
+      </c>
+      <c r="D1293" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=F8En5mVo05%2fxEOptmo5FUZHBSqbfvJneFn%2fvgpS0B4OsNgQwFoFULhjzbtfI6bArEyOidp%2bpJtryf%2feKP9rKkNLLMK5USQN2Y7lUHgtPBLhi4HhHr5ExgsFYvOf92qof%2fpQkHZTKrVtV5cEWGTERUybkBKnPM80MjLn%2bdxTQ5d8fvORnFoqUWQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1293" t="inlineStr">
+        <is>
+          <t>02025430312</t>
+        </is>
+      </c>
+      <c r="F1293" t="inlineStr">
+        <is>
+          <t>Erandwane</t>
+        </is>
+      </c>
+      <c r="G1293" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1293" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1293" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1293" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" s="1" t="inlineStr">
+        <is>
+          <t>A52100020029</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Clear Space Realty</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>A52100020029</t>
+        </is>
+      </c>
+      <c r="D1294" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CbsNVA0Jb2nxlNtSX2TQcC3%2fhOLdMZTQqiSRsyjWtOht3JHP7X3sLMceAjvv7UgggVTxEr3UshMl6HBQKk1o4pePZDi%2f46bfGNF1GYfXeNKGUQl0ExQifhVazv7gaQDxCxEL6qxA8FTzyRp1rPCZ99l1mpEhUlvBUAgO05vnwu%2fU7Ov%2b0WDvjg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1294" t="inlineStr">
+        <is>
+          <t>09881290000</t>
+        </is>
+      </c>
+      <c r="F1294" t="inlineStr">
+        <is>
+          <t>Bavdhan</t>
+        </is>
+      </c>
+      <c r="G1294" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1294" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1294" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1294" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" s="1" t="inlineStr">
+        <is>
+          <t>A52100019454</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Rahul Yashwant Karandikar</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>A52100019454</t>
+        </is>
+      </c>
+      <c r="D1295" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Ath5E1ywDqO9zU7qzemP%2b1NRArArQzwUjhScACuHb6mMJi%2f4J4kP7Y6mp%2fqYPF54OTso%2f5MCMUgdAGOaw9CzNfHBpi6%2fD71Ue9pDzFa6LQS2crzJu2dFFy6CjiizlXjDYOAQkWZxuX8%2bTysNK6SZigVJbLZzaPTt1Z8e4t%2bDqRh2zaRh%2bDxKKg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1295" t="inlineStr">
+        <is>
+          <t>02026111111</t>
+        </is>
+      </c>
+      <c r="F1295" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="G1295" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1295" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1295" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J1295" t="inlineStr">
+        <is>
+          <t>411058</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" s="1" t="inlineStr">
+        <is>
+          <t>A52100018839</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Rahul Santosh Jain Proprietor Of Akshaysagar Properties</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>A52100018839</t>
+        </is>
+      </c>
+      <c r="D1296" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=cwGrY4Hqbnff6GI3KCfPtJ9NifJZp%2b0An8jUO8JpM0KRNeVnXIm0VlezlzLHUQf42X4TqptO57pafjriOBkAmMEmIWcn8K%2fCNsDYRbkBQbX5iPitMtpRU5I%2bnWfccXuS%2bBZJ7GY8Y7l2hI2Vv6pOqOR0HwGAMTe4QSarKIE%2bHiqJ7mGW4FKoCQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1296" t="inlineStr">
+        <is>
+          <t>09420531008</t>
+        </is>
+      </c>
+      <c r="F1296" t="inlineStr">
+        <is>
+          <t>Karvenagar</t>
+        </is>
+      </c>
+      <c r="G1296" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1296" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1296" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1296" t="inlineStr">
+        <is>
+          <t>411052</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" s="1" t="inlineStr">
+        <is>
+          <t>A52100018903</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Dipak Ramdas Sabale</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>A52100018903</t>
+        </is>
+      </c>
+      <c r="D1297" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ithvh34A72tgzVPnACKp8ikIoJEerFOXupTo7CIMKftBJwxcSP2rdGRFP3AC%2benaZK3ABqqOmTkOyWlsXUT2oCTsgwFhoBVlJzaVLm1DTEhzfmfLFvyHM8KbKaMvRBrkwcmxLAk6q5xIsoh0s4lL3m8b7bqMuVct341L%2fbsnhVyVVMmxNGaUvg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1297" t="inlineStr">
+        <is>
+          <t>07517670505</t>
+        </is>
+      </c>
+      <c r="F1297" t="inlineStr">
+        <is>
+          <t>Hinjewadi</t>
+        </is>
+      </c>
+      <c r="G1297" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1297" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1297" t="inlineStr">
+        <is>
+          <t>Hinjavadi (Ct)</t>
+        </is>
+      </c>
+      <c r="J1297" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" s="1" t="inlineStr">
+        <is>
+          <t>A52100019651</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Shailesh Siddheshwar Mamadapure</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>A52100019651</t>
+        </is>
+      </c>
+      <c r="D1298" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=igqz%2fLm8H%2fMToy6cS204SX%2b9rcJHE%2f5oHGgfXs%2fIz4cqn7ol8BYSRaGeTuGNYsTDS11HJiFTH8QlGd8XxIKP0HRNuhrdXh1MMshpIEnPCNRjsPAL%2br8pQANrmA8KOzPSbKRy1LS26X351D0H%2f2k9rJ8DB83IypEQVMx9LLrOHrxYkJA87NG8nQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1298" t="inlineStr">
+        <is>
+          <t>02000000000</t>
+        </is>
+      </c>
+      <c r="F1298" t="inlineStr">
+        <is>
+          <t>Ambegaon Budruk</t>
+        </is>
+      </c>
+      <c r="G1298" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1298" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1298" t="inlineStr">
+        <is>
+          <t>Wadgaon Bk</t>
+        </is>
+      </c>
+      <c r="J1298" t="inlineStr">
+        <is>
+          <t>412406</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" s="1" t="inlineStr">
+        <is>
+          <t>A52100018848</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Sangmesh Shevappa Dudagi</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>A52100018848</t>
+        </is>
+      </c>
+      <c r="D1299" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2f3jNGX3MJb5fdtH4V3bL36774JOyRITEbcV5a6dJyqNv46nK3jtFb2xY3mlN%2b8FodbcrTDNInMrrQYrkMMTCbNoiFr4UQhiJOJ7PROUeM574JUlT5tjhHv3qfZR7OjZEobRu0%2fm4aIdWRxa%2bjN6bgpw0icnZP7WJ2QwtqNy1frgacWBLAKu4Lw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1299" t="inlineStr">
+        <is>
+          <t>02024486060</t>
+        </is>
+      </c>
+      <c r="F1299" t="inlineStr">
+        <is>
+          <t>283, Shukrawar Peth</t>
+        </is>
+      </c>
+      <c r="G1299" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1299" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1299" t="inlineStr">
+        <is>
+          <t>Swargate</t>
+        </is>
+      </c>
+      <c r="J1299" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" s="1" t="inlineStr">
+        <is>
+          <t>A52100018777</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Md Mujtaba  Alam</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>A52100018777</t>
+        </is>
+      </c>
+      <c r="D1300" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=mYf35h2J4SXoKzWusg9C%2bCKJU%2b%2fLXyRvsBdXWra%2fakB2dXGJhi0p5BRlrl8DiQ4zKFCCkqSWww0OTzhajRyfGXk5oiNKXt%2bWpMvvCUnkTxPi6jd3IXwFj2KkYvlcXV1X2OpScewag4gLhJPZ2KETCT9K%2bPBxy%2boxr5zN%2b9DpJ1NHtNabpMUSsg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1300" t="inlineStr">
+        <is>
+          <t>09470711623</t>
+        </is>
+      </c>
+      <c r="F1300" t="inlineStr">
+        <is>
+          <t>Nibm</t>
+        </is>
+      </c>
+      <c r="G1300" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1300" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1300" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1300" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" s="1" t="inlineStr">
+        <is>
+          <t>A52100018845</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Satish S Bhandarkawathe</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>A52100018845</t>
+        </is>
+      </c>
+      <c r="D1301" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Jz7uThVfwjUJ0JSzfD0zoSJkNpa2B4cPEXPvEtfknnAkgtdNaw9NA6R6jpsjpWG8j8CrLkJA4CewAOITMdNeRmt5d%2beVab1ylHg6je7C7QQLgw1B4xUOiTVUVNvMqLvI%2fZ%2bxkiYXeBgQ112LyJam5oGZo6KF9gjEfaxep8zty%2fQHgyQ%2fTU%2bEqQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1301" t="inlineStr">
+        <is>
+          <t>02046910509</t>
+        </is>
+      </c>
+      <c r="F1301" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1301" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1301" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1301" t="inlineStr">
+        <is>
+          <t>Mulshi Kh.</t>
+        </is>
+      </c>
+      <c r="J1301" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1350]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1301"/>
+  <dimension ref="A1:J1351"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -67560,6 +67560,2606 @@
         </is>
       </c>
     </row>
+    <row r="1302">
+      <c r="A1302" s="1" t="inlineStr">
+        <is>
+          <t>A52100003876</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Anil Sadashiv Deshmukh</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>A52100003876</t>
+        </is>
+      </c>
+      <c r="D1302" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xq14E7mHsXZQIoII9XyDngec5TV0AKRGLHA3qqEMGuHiG0nD44I7O65aAJIM3%2by88mLAPmW%2bcmazfNOea54k5tV7T2hAlxfLE3lne8Vr8qPXexHntbIzQaYc7a36OjGGyLAKsQaX5AY0zz61GSO4szl5saBylnds4tn5L1md%2b1VSehuDMMCmGw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1302" t="inlineStr">
+        <is>
+          <t>02025465854</t>
+        </is>
+      </c>
+      <c r="F1302" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G1302" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1302" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1302" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1302" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" s="1" t="inlineStr">
+        <is>
+          <t>A52100018796</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Baliram Devidasrao Patil</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>A52100018796</t>
+        </is>
+      </c>
+      <c r="D1303" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=i2%2f7xg15NJ2susJEcP4gSnhHpxwoPu8QMfH0AGYk87sWQamP7ve9smF3jiuZ1XpPidtLSykMCirLf9Qwi6sbVSoguSR%2bT%2fEhwcOtoVThet1uNUVCeTkQWTLbXw1mQOgrNZm00%2bnwN%2b4J0GS7puagvj6w%2bGndTFfFeOna7sNtcetytJUc%2fWm6CQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1303" t="inlineStr">
+        <is>
+          <t>09766712222</t>
+        </is>
+      </c>
+      <c r="F1303" t="inlineStr">
+        <is>
+          <t>Vallabh Nagar</t>
+        </is>
+      </c>
+      <c r="G1303" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1303" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1303" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1303" t="inlineStr">
+        <is>
+          <t>411018</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" s="1" t="inlineStr">
+        <is>
+          <t>A52100019036</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Yogita Sanjay Wagh</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>A52100019036</t>
+        </is>
+      </c>
+      <c r="D1304" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=tRMCJNSdB97eI4ZufB3fVGTJ4KM84aCWTYqT8BBho5bJG7AoEKij2UNdaO%2f5fjQ3rg93U%2bBJFMU8p48NXvyMoCjY%2bF0N6oi3krtlxevOa3%2buZlI2KHpp%2f4hN4CN1KIlhNlKFcLrH42%2f%2fQLRyXp%2fCVpT5iPKRuBRdZ5MHjBuuTr9U1jhAmasYog%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1304" t="inlineStr">
+        <is>
+          <t>02065700700</t>
+        </is>
+      </c>
+      <c r="F1304" t="inlineStr">
+        <is>
+          <t>Mahatma Society</t>
+        </is>
+      </c>
+      <c r="G1304" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1304" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1304" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J1304" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" s="1" t="inlineStr">
+        <is>
+          <t>A52100018817</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Jashoda  Thapliyal</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>A52100018817</t>
+        </is>
+      </c>
+      <c r="D1305" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=nBGkDZk7JSOgP%2bNx%2bVsy2dfch0abqt9iz6J2DdsmuUCBqDHb7orQ60eyVToWhb2PsX2bY6JtHRkC8y4wJmEZ2FAaIl184mOJ9sPTY%2fuFN0p%2fzbLkTe4TwJKytPkHXo%2fJSvZ0MV5ax5Y0Du%2bWkShR8ztJ9%2bkI8y7eYdUU8XmA9HmEPkOtWS2%2fIg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1305" t="inlineStr">
+        <is>
+          <t>07507505339</t>
+        </is>
+      </c>
+      <c r="F1305" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="G1305" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1305" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1305" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1305" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" s="1" t="inlineStr">
+        <is>
+          <t>A52100018958</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Aakash Deepak Topre</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>A52100018958</t>
+        </is>
+      </c>
+      <c r="D1306" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=DTbjYnfTLtp5MUyyg0ygkCoBelp8FE4POlDaGSfwrf0x3XxC4FvHtvVRMzK3Yamfo1%2bUUFis4cvj5xKVWHwZh6TpvKn56OAw8tzdm8xsq3H%2frahIFJ4huNWPmdXXaUeXMWJm1D%2bbMyEEIAxcey3OBwMSEJH4vM9pgD%2f9pOP6BpNlS71KtVDqmw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1306" t="inlineStr">
+        <is>
+          <t>02066004928</t>
+        </is>
+      </c>
+      <c r="F1306" t="inlineStr">
+        <is>
+          <t>Wadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G1306" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1306" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1306" t="inlineStr">
+        <is>
+          <t>Vadgaonsheri</t>
+        </is>
+      </c>
+      <c r="J1306" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" s="1" t="inlineStr">
+        <is>
+          <t>A52100018837</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Rajesh Babulal Oswal</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>A52100018837</t>
+        </is>
+      </c>
+      <c r="D1307" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3oDSn19GGd9ZJ82l4MD143XchpodAlObL5FpMmR8y5BEbWRTko2QiRFyUpQiVqvl37Lxyu5%2fffr57HP8NIOXh0Sqzh2zoAus0DLBX7bOj%2fHm1eSUjSneDI9SvdgPvYiODS7pu4Mhb3PzwGt%2fe0uopqBpYlfdbELRkmLqnZNtf%2bAByX5Pke209g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1307" t="inlineStr">
+        <is>
+          <t>09595489678</t>
+        </is>
+      </c>
+      <c r="F1307" t="inlineStr">
+        <is>
+          <t>Kondhwa Road</t>
+        </is>
+      </c>
+      <c r="G1307" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1307" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1307" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1307" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" s="1" t="inlineStr">
+        <is>
+          <t>A52100018892</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Tariq  Khan</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>A52100018892</t>
+        </is>
+      </c>
+      <c r="D1308" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=UiLf8rrtMM7YdVeTIrrNGv6ISxENI9MRhPvzhPYfFx1AzlGI0EMFTXaBqeWIyyQCUEbTBnRiytQg2Dgly5hDnee1b7dsGvn485VdoF9gFrro9ueehL6ztQg72VLAwocD31AYyIP8ojWJDyJeLEB7wmONDwE2Eht2XFEuJj%2fcIoontbApX5s%2fWg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1308" t="inlineStr">
+        <is>
+          <t>02298209637</t>
+        </is>
+      </c>
+      <c r="F1308" t="inlineStr">
+        <is>
+          <t>Andheri West , Mumbai</t>
+        </is>
+      </c>
+      <c r="G1308" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1308" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1308" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1308" t="inlineStr">
+        <is>
+          <t>400053</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" s="1" t="inlineStr">
+        <is>
+          <t>A52100019058</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Santosh Dajirao Chavan</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>A52100019058</t>
+        </is>
+      </c>
+      <c r="D1309" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Ph%2ba8TpCHNAz6DSro2ziTOHR7Ep25hJsDJPgNboUpyxq7T2rrqFvjkYbDJvIuDm2zJgRLs46i9sGj1%2fiZhWoap9rqu%2fzglqJbuoc%2bCEI21ueGN%2bCnTp0QRmIeuIWF1KCBQAL58g4OyBhv3Z6xenx%2byhMKD6CUMCNkNLAFT9xoZqaOTfaR7fCiw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1309" t="inlineStr">
+        <is>
+          <t>98055165120</t>
+        </is>
+      </c>
+      <c r="F1309" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="G1309" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1309" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1309" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J1309" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" s="1" t="inlineStr">
+        <is>
+          <t>A52100018821</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Prafulla Vivek Vaidya</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>A52100018821</t>
+        </is>
+      </c>
+      <c r="D1310" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MZ7TI0tYcrXehf5SCdMmoR%2bRggt%2fJqhYzOTxcQuaorDZ%2fzXBUik%2b4i%2fEnzJJ2bTlDndIdYY7nbSmXnSFHwwC1xKaAIAkQRmjSazhONne2yd%2fYMwy6UuM50Ms%2fgbMln2SOxlOsTWQPI1jBSoq3cnhFwERqnfTdKzezzFOwedw2lBdoW9%2beGAVAw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1310" t="inlineStr">
+        <is>
+          <t>02027287400</t>
+        </is>
+      </c>
+      <c r="F1310" t="inlineStr">
+        <is>
+          <t>Lane No 5</t>
+        </is>
+      </c>
+      <c r="G1310" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1310" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1310" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1310" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" s="1" t="inlineStr">
+        <is>
+          <t>A52100019398</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Vijay Associates</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>A52100019398</t>
+        </is>
+      </c>
+      <c r="D1311" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bytnFIgaVW7vhNknjdZBm2sANlHGyNMFC2mudy1A%2fyNKFcEM9mTXpKH4xTF%2bNYv0b6A6u3chFSGemSsVyArN0C%2b4r2UT4hpEOYa%2fWZbtmbQxq99xI8fPgNNxik7TOpJnhRAPtxYnIXtMLmRnpi511XzJb0s88be094iR6jtDdyL2QZJGQck7nA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1311" t="inlineStr">
+        <is>
+          <t>02025384120</t>
+        </is>
+      </c>
+      <c r="F1311" t="inlineStr">
+        <is>
+          <t>Kalyani Nagar</t>
+        </is>
+      </c>
+      <c r="G1311" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1311" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1311" t="inlineStr">
+        <is>
+          <t>Kalyaninagar</t>
+        </is>
+      </c>
+      <c r="J1311" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" s="1" t="inlineStr">
+        <is>
+          <t>A52100018838</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Bharati Tilokchand Raisoni</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>A52100018838</t>
+        </is>
+      </c>
+      <c r="D1312" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3IVydsCv4obowc2PuqFp0k%2fXSmO6cUoB%2bM62Fv%2bFGK%2bpOxBaGoSIuByBT47731LaRhWUn%2fAjEjRHda3DjC%2b6F7fQSHknSiZpb%2bEZ9XeOpMurtya7vmuLKA%2b1SDgbK%2bcxCLsJc%2fA2R5SyyvJln0uL5ays7oRluoAm7JlsVO2%2faPXd0D%2f7ZRPNfA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1312" t="inlineStr">
+        <is>
+          <t>09822690400</t>
+        </is>
+      </c>
+      <c r="F1312" t="inlineStr">
+        <is>
+          <t>Marketyard</t>
+        </is>
+      </c>
+      <c r="G1312" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1312" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1312" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1312" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" s="1" t="inlineStr">
+        <is>
+          <t>A52100019166</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Buy India Homes Digital Private Limited</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>A52100019166</t>
+        </is>
+      </c>
+      <c r="D1313" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=51nZCNLLEbhrpEBQGVrq4rjcwb8S9K%2fJf0ovPsWgxdqPEiUnWYfPdugAmKpit2bmoVLpaY0o7LUr3%2bt5ymqCBHXwey%2b1O5ieVZXwsyTxQb2u%2fww0m9MZbiYwvgTsmSqGqGPgXFV1wUrbhh5KdLOS%2bkDlRshDyY0AMzzMFjw8bZ61sPFf16QlFQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1313" t="inlineStr">
+        <is>
+          <t>02026850086</t>
+        </is>
+      </c>
+      <c r="F1313" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G1313" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1313" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1313" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1313" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" s="1" t="inlineStr">
+        <is>
+          <t>A52100002628</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Panchshil Realty And Developers Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>A52100002628</t>
+        </is>
+      </c>
+      <c r="D1314" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wsvYq%2fSyHiIgwbcuX%2fJS3ct4ZxMTauodHGlK9JKppoWKRU00GDNTl3AQL%2fkj1Zb%2flw%2fmT6v2em34dTpaBk4Jhf8UXL7ebP1SxXOmI5h6ivdiyKuJJzzPQZgHN4sSDP2k%2bwKWT4UHc3HhkfmYDyfCnfpetZKOGWyqUDPoi28xOFGAuOjpxQ%2ffLA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1314" t="inlineStr">
+        <is>
+          <t>02066473200</t>
+        </is>
+      </c>
+      <c r="F1314" t="inlineStr">
+        <is>
+          <t>Yerwada</t>
+        </is>
+      </c>
+      <c r="G1314" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1314" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1314" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1314" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" s="1" t="inlineStr">
+        <is>
+          <t>A52100018913</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Santosh Kumar Dash</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>A52100018913</t>
+        </is>
+      </c>
+      <c r="D1315" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=FVek02MQohHE631WvujkGDS0e7RsXi0x%2fJ87Fgcbs86R%2bh%2fDYGWrYw40durVqmKqMLzAOx04sL9vm%2fvVGOFK30eQxU%2bMZpw3%2bxjTn3GEavNMZDC560mhKgAXYDssJUDod7%2bIclLYPz%2bt1P4a0%2bDTyyRf%2fumyttjcvQli2v4g2y5vVcIzJ5XPRg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1315" t="inlineStr">
+        <is>
+          <t>08880516111</t>
+        </is>
+      </c>
+      <c r="F1315" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1315" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1315" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1315" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J1315" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" s="1" t="inlineStr">
+        <is>
+          <t>A52100018860</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Tafazzul Hussain Saiyed</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>A52100018860</t>
+        </is>
+      </c>
+      <c r="D1316" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=VlJG%2fiK412e%2b54LJx0Q6Ku52d8Nw1BM7ZbyDeX4ixXZJNAby8hxnarjL8lZr%2bzl%2fkJGW5lbLJdbeSqu1Yw0%2bYIO%2bg5JjbWN5%2fpNwho4p6l3OgGHlMjoY4DnozUapPw62kFzeu1ObIb4%2b75FCJco7UToses4sZzg2Uot0S3su%2fjE4wt327boO4g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1316" t="inlineStr">
+        <is>
+          <t>09011383183</t>
+        </is>
+      </c>
+      <c r="F1316" t="inlineStr">
+        <is>
+          <t>Kondhwa Khurd</t>
+        </is>
+      </c>
+      <c r="G1316" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1316" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1316" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1316" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" s="1" t="inlineStr">
+        <is>
+          <t>A52100018960</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Devdatta Prabhakar Beke</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>A52100018960</t>
+        </is>
+      </c>
+      <c r="D1317" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2oFvhih727Ta%2faP1AL0TVWynmi19NHMzhVOw0ibNsOIK5gUjIYs9l2bIvKi5z64uJY23ju9c36qfzBOpW2sV%2bESFMbmoAnc9pZv%2bu1a3fNej15IOhssFhtqd0Ob7rr5uv6%2bwsQtB4N0hAgUuKWVRnEkSSqRLKKx6S2Hg7KgaIoltpZUl8HJGmg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1317" t="inlineStr">
+        <is>
+          <t>02025386776</t>
+        </is>
+      </c>
+      <c r="F1317" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G1317" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1317" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1317" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J1317" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" s="1" t="inlineStr">
+        <is>
+          <t>A52100018879</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Netaji Maruti Salunke</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>A52100018879</t>
+        </is>
+      </c>
+      <c r="D1318" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2h67qOZbnwv25KNQtuBdz15zHpVU3%2fOZ2TFT2RIwVovSwGDGB%2bYr0T0BkyFoDghZz%2b%2bllS%2f%2bGyWQtbJintvVqvG0wlCaR6WOyl%2bzIRiBnV9zKwpX5YUFL18dWS8v1xiCjnt%2fOlukWje%2f2b8hZPsm7o%2bkiDJjoBZViEnXAoXEiXp28wrPUcxCWQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1318" t="inlineStr">
+        <is>
+          <t>02086002767</t>
+        </is>
+      </c>
+      <c r="F1318" t="inlineStr">
+        <is>
+          <t>Kaspate Wasti</t>
+        </is>
+      </c>
+      <c r="G1318" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1318" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1318" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1318" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" s="1" t="inlineStr">
+        <is>
+          <t>A52100018849</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Rojarani Nareshkumar Nekkanti</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>A52100018849</t>
+        </is>
+      </c>
+      <c r="D1319" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=B8evqOazAoD2qtYGCZIGXYmtEwSz6JK5JSv0njXVHoeY5vclT0ckH7M1fEvqIPvP1IRVIaYcrF32VE0DRfLUCaTjRPE97wQxkM3WkCsd9efmylur%2bTveLSN1pH4IhMxQ5xw3q5wdZ%2bY02ktedOl8AnXaxHDZNvw89TX5FQUJ%2bTJ48AjpxkFoMA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1319" t="inlineStr">
+        <is>
+          <t>09545559949</t>
+        </is>
+      </c>
+      <c r="F1319" t="inlineStr">
+        <is>
+          <t>Bandal Estate</t>
+        </is>
+      </c>
+      <c r="G1319" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1319" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1319" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1319" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" s="1" t="inlineStr">
+        <is>
+          <t>A52100018963</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Mak Infra</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>A52100018963</t>
+        </is>
+      </c>
+      <c r="D1320" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=dhRgouSu6HJyFAMM6URzlaDu3K1ApsmdjUhO5rci%2fyFlp90XcU4W2dYhERW4wenIEDDL3GJ6lTbw7lY8XOaSGA1BZxbSTP%2bi7LGjh3qyAAffMy01wwZcduTuI0N5rXWAOVK%2bIXjNtAn8HvSb%2bsmlc7r4nwXWCNEOs6NiK9e3oxi8gV6Vr2l26A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1320" t="inlineStr">
+        <is>
+          <t>02046703070</t>
+        </is>
+      </c>
+      <c r="F1320" t="inlineStr">
+        <is>
+          <t>Nigdi</t>
+        </is>
+      </c>
+      <c r="G1320" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1320" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1320" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1320" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" s="1" t="inlineStr">
+        <is>
+          <t>A52100018972</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Rajiv  Gupta</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>A52100018972</t>
+        </is>
+      </c>
+      <c r="D1321" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=GfkLMi70ONQTHiC1pEAQYULeLtA54o6BD3Z4UoUQ4x5VRP6GYX1saybzEzPfhwYuKTSXidYEJADCRXw%2bzVpekC9CfNKlnw33u4KlgYrNMLwJzwSHOWauh6za1k%2bvkFRzzQTyrmN2D8xQLZ549fHk6fj12%2b13kV3%2bV7hEWsbTGicJDn2hTaFhTQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1321" t="inlineStr">
+        <is>
+          <t>02066010678</t>
+        </is>
+      </c>
+      <c r="F1321" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="G1321" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1321" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1321" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1321" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" s="1" t="inlineStr">
+        <is>
+          <t>A52100018999</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Manohar Namdev Jadhav</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>A52100018999</t>
+        </is>
+      </c>
+      <c r="D1322" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=j5MZxaIv8Bab0yVSalO0HMdMG2m%2fgglN1ZsUHsWbt9Y9Jo7h3ORQQwKmZhn2DA7yMRvkC%2bVF4wkiw4PydVz%2bkdovD6eVNs1f6ouFG1OqSnP4oFzOqifrofpQAKuJfX9h1xUBAjU%2fJBbPetAr6H1qZ9dhv1s2AcfwpIXeHEP5i1ATqHwSfqp3NA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1322" t="inlineStr">
+        <is>
+          <t>02024459938</t>
+        </is>
+      </c>
+      <c r="F1322" t="inlineStr">
+        <is>
+          <t>Shaniwar Peth</t>
+        </is>
+      </c>
+      <c r="G1322" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1322" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1322" t="inlineStr">
+        <is>
+          <t>Peth</t>
+        </is>
+      </c>
+      <c r="J1322" t="inlineStr">
+        <is>
+          <t>411030</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" s="1" t="inlineStr">
+        <is>
+          <t>A52100018882</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Pavan Prabhakar Merukar</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>A52100018882</t>
+        </is>
+      </c>
+      <c r="D1323" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=s9pPSSOtEcC10r%2fDpUYrocL6JN8vYtJN4WS0muP8Ay2o9yy2WZpg%2f%2bJBRFlK0lRGErvyVTNWdfM82oh2khm8QSUgelW1%2fAqYyQk4iob0n5UL3s9wQji4AwZakB74zl3fa%2flnCUb%2bBq2hsk1m0YqB5BPcs3UTeg62UU0mMVKfHxik%2bqYk8uA1Ag%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1323" t="inlineStr">
+        <is>
+          <t>02027287400</t>
+        </is>
+      </c>
+      <c r="F1323" t="inlineStr">
+        <is>
+          <t>Sector No 21 Yamunanagar</t>
+        </is>
+      </c>
+      <c r="G1323" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1323" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1323" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1323" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" s="1" t="inlineStr">
+        <is>
+          <t>A52100019089</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Sonia  Menghani</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>A52100019089</t>
+        </is>
+      </c>
+      <c r="D1324" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fWAQa8eSaydLc7Z%2ffgpmrZp0MRJRJc0Oo6FATdDJ33r8Lr5qcRiL5gINW6TQzZ2RVfodmfiLQ0%2bTNqbfouLt1QX7rSzIh9gbUEAyLpBJq6BVHTR7TU7Ie9el04%2f6E2mF20nrtEf3Lct7LRiHnJPBYd1bJRdOEk4i4EKktOFt7AK7ztgparJRWA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1324" t="inlineStr">
+        <is>
+          <t>02041226010</t>
+        </is>
+      </c>
+      <c r="F1324" t="inlineStr">
+        <is>
+          <t>Dhole Patil Road</t>
+        </is>
+      </c>
+      <c r="G1324" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1324" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1324" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1324" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" s="1" t="inlineStr">
+        <is>
+          <t>A52100018918</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Pankaj  Singh</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>A52100018918</t>
+        </is>
+      </c>
+      <c r="D1325" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=EQ3dyR%2fgt5KI7DKS59WG11I4hJBZo5y1VSUETGbRlxuQ%2fhZpKVVbD2520Kke6bloR5VBag6rv8qUOZ58gHfM%2beJ%2fmIMuwbZxYVV7FC1t25J00lTM2pY1G%2fbS89ynotEclvzP2V2DDalI8YMZapzMMb13MYhiiwx%2b3Wx0VFLRzeoNAeFoYa7Fww%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1325" t="inlineStr">
+        <is>
+          <t>07798865563</t>
+        </is>
+      </c>
+      <c r="F1325" t="inlineStr">
+        <is>
+          <t>Porwal Road</t>
+        </is>
+      </c>
+      <c r="G1325" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1325" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1325" t="inlineStr">
+        <is>
+          <t>Lohgaon</t>
+        </is>
+      </c>
+      <c r="J1325" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" s="1" t="inlineStr">
+        <is>
+          <t>A52100018886</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Harsh Ashok Bajoria</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>A52100018886</t>
+        </is>
+      </c>
+      <c r="D1326" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2tGmvn4dkh3FPSSawwTuiNcRi4muA37kxX8ViJWymL9dYQVpvbhYAuUofoMkT%2folYxrgbGCH3Or0Nva%2b90XK8UD5LCsC6VQn2MLY4YLm%2bStBk%2f0Fu%2fZxUMZ5Hf1w58NgwKSfXDyHDSy%2bLyEdTMLMXfUaLJsnoU4zs3yn9xd%2bGlexlQp7r1%2bc4A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1326" t="inlineStr">
+        <is>
+          <t>09665559432</t>
+        </is>
+      </c>
+      <c r="F1326" t="inlineStr">
+        <is>
+          <t>Manjari Budruk</t>
+        </is>
+      </c>
+      <c r="G1326" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1326" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1326" t="inlineStr">
+        <is>
+          <t>Keshavnagar-Mundwa</t>
+        </is>
+      </c>
+      <c r="J1326" t="inlineStr">
+        <is>
+          <t>412307</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" s="1" t="inlineStr">
+        <is>
+          <t>A52100019365</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Abhilasha  Shrivastava</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>A52100019365</t>
+        </is>
+      </c>
+      <c r="D1327" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=GVTfHbf1S0g55CHAPXu1b2DU4MFffGSV4QAWddp0hQy3pt61CTcK0CKtTzGlc4pM%2fLhb9uLkWryQAHKFit%2b7qY8nqA%2bWZlzT99BNllWdu5Ud9ZfaMvbgvwqc%2fJiIm4lV6XunZ4CnYs2oSaHmB2dGfldYXq5dJCPyGJSuKmL3%2fuFMw1D8GdJVXw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1327" t="inlineStr">
+        <is>
+          <t>02027028199</t>
+        </is>
+      </c>
+      <c r="F1327" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="G1327" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1327" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1327" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J1327" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" s="1" t="inlineStr">
+        <is>
+          <t>A52100018873</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Chandrakant Dnyaneshwar Jangam</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>A52100018873</t>
+        </is>
+      </c>
+      <c r="D1328" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=WqXgZRvsK35c3pHC1fjdf0rD2IPZPtnLItMjGBq5JjBH1oQB57J%2fdYkTgullUVvWg1vXE4LtGC15ZNflSUEqH4rDE3o8ufSJ6Qxhu7z5GQ1NlX89PlLp4ynizTEaxk0VhlZyi2l2W3bQDqYzrx%2fSC8ujSgDx7%2bm9215vQVvfFHr%2bnuTIe33xUw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1328" t="inlineStr">
+        <is>
+          <t>08793350569</t>
+        </is>
+      </c>
+      <c r="F1328" t="inlineStr">
+        <is>
+          <t>Nal Stop</t>
+        </is>
+      </c>
+      <c r="G1328" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1328" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1328" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="J1328" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" s="1" t="inlineStr">
+        <is>
+          <t>A52100019108</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Sangita Sanjay Desai</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>A52100019108</t>
+        </is>
+      </c>
+      <c r="D1329" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=TZYdZmgNm50zCJl8dat%2bv0kdULjgpR%2bHSbRVtuyJpxnVTiIieI7eYIi%2bpZ5rZXjA40AYtzrMq6XYzMdLfCPKG5T0VmcLT4XLqa%2b3LVbXqZHU%2f6ds%2bnbNfhfmJpLB0L4o5l1NHjyNmOMChLqWuL5vXy4C4GFKxbcE2bMjNGvI6RLSBS51Z5uaRw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1329" t="inlineStr">
+        <is>
+          <t>08788719256</t>
+        </is>
+      </c>
+      <c r="F1329" t="inlineStr">
+        <is>
+          <t>Ambegaon Bk</t>
+        </is>
+      </c>
+      <c r="G1329" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1329" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1329" t="inlineStr">
+        <is>
+          <t>Ambegaon Bk</t>
+        </is>
+      </c>
+      <c r="J1329" t="inlineStr">
+        <is>
+          <t>411046</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" s="1" t="inlineStr">
+        <is>
+          <t>A52100019056</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Rabneshwar Narayan Diwakar</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>A52100019056</t>
+        </is>
+      </c>
+      <c r="D1330" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=pJeGNHG028rVHxm%2fftx0KLDuTcuZnZ452bAItloShCpahynGSMwqkMUgzTtcWglLDkH2N9Ad%2bcWULWse3FKjUjeYSVLXdW7sVWRtEk%2frnHaNEN65ja36b5rmRB%2bHADZ2sS9LiH6acepzbYaIQ4jYJJkFcT4haW%2bPMqBTHoVmkR1%2fLwrqRLaRJw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1330" t="inlineStr">
+        <is>
+          <t>02041000000</t>
+        </is>
+      </c>
+      <c r="F1330" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1330" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1330" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1330" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1330" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" s="1" t="inlineStr">
+        <is>
+          <t>A52100019661</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Yash Gulabchand Karaniya</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>A52100019661</t>
+        </is>
+      </c>
+      <c r="D1331" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=I%2b2P9faaetq9RSn3d96o2Hu2rEQRswX6TkaQYhlWi2XKP0k7lGHhRqHk9ncK3Gj8O1vPwiNw21zYc2r81Po%2bMIS4XJYAg3BlZ%2bWxHrDJ76SO4%2bkbyjunUaBhSbSiynzdJA98bm4223m%2bkQ%2bVXfMfzDNQn72ZaqTKnJEc0%2bNhSQtbhhI%2bzXo34g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1331" t="inlineStr">
+        <is>
+          <t>02228984518</t>
+        </is>
+      </c>
+      <c r="F1331" t="inlineStr">
+        <is>
+          <t>Borivali</t>
+        </is>
+      </c>
+      <c r="G1331" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1331" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1331" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1331" t="inlineStr">
+        <is>
+          <t>400091</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" s="1" t="inlineStr">
+        <is>
+          <t>A52100019832</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Crowdshare House Exchange Private Limited</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>A52100019832</t>
+        </is>
+      </c>
+      <c r="D1332" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xl5Bq%2btu57PSTdl3Qp4N%2f6UpnwUYqlL%2b4gAArBVKCmAXtcJVK9DWgSQrMfhbb6VfDc0ibFDJl%2fgxprpmlc6IVppmA4OOf1SzLt8jsr2PO42EszS4ypqteHyfUwZ4csgA7tryKCDU0x6QtmO8HkBD6tXnvy%2bd7QBAEanjiRGUy%2fPvUOwj6FMdDA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1332" t="inlineStr">
+        <is>
+          <t>02039116305</t>
+        </is>
+      </c>
+      <c r="F1332" t="inlineStr">
+        <is>
+          <t>Lavale</t>
+        </is>
+      </c>
+      <c r="G1332" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1332" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1332" t="inlineStr">
+        <is>
+          <t>Lavale</t>
+        </is>
+      </c>
+      <c r="J1332" t="inlineStr">
+        <is>
+          <t>411215</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" s="1" t="inlineStr">
+        <is>
+          <t>A52100018938</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Shristi  Kumari</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>A52100018938</t>
+        </is>
+      </c>
+      <c r="D1333" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=I4eOd3xMm%2fcuPQ1poTygKOCtKbRmiCOmN2eOzIsj7e2WWyyHpmsEkA9DSu8egCH9rivq3kJG%2fJkG%2fzgy4%2fHtRXg3DXyhS8X7%2b93mamJu%2fFNgr904xHe6XE0YksJQaOZEQSumhVp1yJfJ21uF7lseLW9T4EE0bY8Mpr%2btLh%2fBXRLZTWqS7%2fHiPA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1333" t="inlineStr">
+        <is>
+          <t>09552413629</t>
+        </is>
+      </c>
+      <c r="F1333" t="inlineStr">
+        <is>
+          <t>Tathawade</t>
+        </is>
+      </c>
+      <c r="G1333" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1333" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1333" t="inlineStr">
+        <is>
+          <t>Tathwade</t>
+        </is>
+      </c>
+      <c r="J1333" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" s="1" t="inlineStr">
+        <is>
+          <t>A52100021240</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Sudev Enterprises</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>A52100021240</t>
+        </is>
+      </c>
+      <c r="D1334" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=WciX9RrXssCGQi1Ft7Xkkxl2konCFApWZVTFhovVKw7n1tkcZ9LXnIvmaPYPXq%2ffuAC48T2S4MU8CtEOR6pjeQnvl%2fHpbRh9pQB9dS%2fI3N8l6%2boQ9FQbZryGk1lzZ7L8VZ5OXnP0F5V0Acc57x4EwfTy%2bWIlYieWdJi5KEVgKaexSyiAwbjrhA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1334" t="inlineStr">
+        <is>
+          <t>02025468978</t>
+        </is>
+      </c>
+      <c r="F1334" t="inlineStr">
+        <is>
+          <t>Nera Maruti Mandir</t>
+        </is>
+      </c>
+      <c r="G1334" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1334" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1334" t="inlineStr">
+        <is>
+          <t>Karve Nagar</t>
+        </is>
+      </c>
+      <c r="J1334" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" s="1" t="inlineStr">
+        <is>
+          <t>A52100018944</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Rajesh  Mendiratta</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>A52100018944</t>
+        </is>
+      </c>
+      <c r="D1335" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=tNLKAxYNSclcpLeSrXcuBtKhfVLh8RCN6Zqf8VGtTF34g%2fWjCyttn6KsUG0h34Yk5wEWweQbc5dQZr%2fjVJl4DVs8ur1tfXh9bCLeX6qByDPXER1qnW2q1vK7jCvjsR6CPGxejft%2bNy9i3vhAxHlXnGKaSz4j7m9JKF4eCfaMr4fa0EpoqZeYWw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1335" t="inlineStr">
+        <is>
+          <t>02226056262</t>
+        </is>
+      </c>
+      <c r="F1335" t="inlineStr">
+        <is>
+          <t>Kotle Patil</t>
+        </is>
+      </c>
+      <c r="G1335" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1335" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1335" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1335" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" s="1" t="inlineStr">
+        <is>
+          <t>A52100018937</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Rizwan Rafique Ali Sayed</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>A52100018937</t>
+        </is>
+      </c>
+      <c r="D1336" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CNhiHIgiP9dyJuMx01fFRKpQghO6faU1O%2fu4grHiSbFhH30w%2bU4b%2fma4dzSxo11iellfvkc4S5x8NVljh1EzIZA7Hf0Dhidy8wKN%2bETeGkUmEmrtfv7LYCimY5iPBk9ceRRdDJtZEcOyrVjXVz%2bcLbgfy2lq4SMb1wdtv10PTQzRyjjcwtB1rg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1336" t="inlineStr">
+        <is>
+          <t>02226396242</t>
+        </is>
+      </c>
+      <c r="F1336" t="inlineStr">
+        <is>
+          <t>Andheri West,</t>
+        </is>
+      </c>
+      <c r="G1336" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1336" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1336" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1336" t="inlineStr">
+        <is>
+          <t>400053</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" s="1" t="inlineStr">
+        <is>
+          <t>A52100003421</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Suresh  Yadav</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>A52100003421</t>
+        </is>
+      </c>
+      <c r="D1337" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5UDyc3yihlZmUQ5De%2bEaBkpvrmp7nibeF%2fcM8kCQfGSrtg1mkDb0mOfCttmHsmZn3f1S3yA0AqQA2jV84%2bmmTv5Au6Wmk%2f9DNyH0694Hqxx8BJi74NKNLu%2f%2bOE6q3WRObwQA9k5elQyMyB31n4%2fRr7suqrDpUoYWyXcuxL%2fowUTfv8nJ0K%2f4Ew%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1337" t="inlineStr">
+        <is>
+          <t>02065206599</t>
+        </is>
+      </c>
+      <c r="F1337" t="inlineStr">
+        <is>
+          <t>Bavdhan</t>
+        </is>
+      </c>
+      <c r="G1337" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1337" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1337" t="inlineStr">
+        <is>
+          <t>Bavadhan Bk</t>
+        </is>
+      </c>
+      <c r="J1337" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" s="1" t="inlineStr">
+        <is>
+          <t>A52100018933</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Pravin Prakash Shrishrimal</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>A52100018933</t>
+        </is>
+      </c>
+      <c r="D1338" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QVuSURDcOdMLeDhIfX1iZpK3o%2fSOHnugdXLN4aRLtoh1xT81trgcGzvulVsNLH8akc7GlI%2bjwq8kFryZVMLMxsLXTz48VkeZrZLL9u%2fjRV4M%2btrHsMBGPO333Db%2bsKh%2fxXk5DTDz%2bn8Sdfz4JeAj%2bu3JFPjBa9t4%2bz0LBhL91a0Qn3XHEf1iuw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1338" t="inlineStr">
+        <is>
+          <t>09850607393</t>
+        </is>
+      </c>
+      <c r="F1338" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="G1338" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1338" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1338" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1338" t="inlineStr">
+        <is>
+          <t>411043</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" s="1" t="inlineStr">
+        <is>
+          <t>A52100002515</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Nitin Lakhmichand Chabria</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>A52100002515</t>
+        </is>
+      </c>
+      <c r="D1339" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=mKl0q4lJIigazNxh9db8ccsDAhWZYbR3MWKH8UJDdqVnGRqSv%2fv9UQSm2mO4cQM%2f1Z7cc7aNrOjQHVMbthYuJOvg6YHF7r5u%2ba7yK4mJ0vVWi0v%2fVMRJ0%2bawCOHW%2f7folS94dvkAhpx2M22cKflHBHh69Mye7DMmQJM3Iygiq%2fCRjxOMvSLVtg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1339" t="inlineStr">
+        <is>
+          <t>02025889489</t>
+        </is>
+      </c>
+      <c r="F1339" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1339" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1339" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1339" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1339" t="inlineStr">
+        <is>
+          <t>411067</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" s="1" t="inlineStr">
+        <is>
+          <t>A52100019259</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Prabhat  Vijay</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>A52100019259</t>
+        </is>
+      </c>
+      <c r="D1340" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=YAnR1m8RXtINiyhmj9HQHm3SSjRAl3YdfMB13XNborTGE01GRfv8%2fiZYIVUE%2folGqgtbMzAN3Kf3ykFg3O5kftjHf341MYYsWJ1PeUz9xkw0wDahJNjHiEhJ%2bVLwAbBkIKLZ0KOXZH%2f6JKcU15C4kFCwDeSzFX9lNn3j5EHYuT2luwV%2flE787Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1340" t="inlineStr">
+        <is>
+          <t>02046910509</t>
+        </is>
+      </c>
+      <c r="F1340" t="inlineStr">
+        <is>
+          <t>Hinjewadi</t>
+        </is>
+      </c>
+      <c r="G1340" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1340" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1340" t="inlineStr">
+        <is>
+          <t>Hinjavadi (Ct)</t>
+        </is>
+      </c>
+      <c r="J1340" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" s="1" t="inlineStr">
+        <is>
+          <t>A52100000044</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Property Chef Consulting Services</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>A52100000044</t>
+        </is>
+      </c>
+      <c r="D1341" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=EEVQPv2j9mrsWtRNSjcG0Lcz4IBQ3ljZuVmtpZ0fNNwHnBl922sh2gaSfgIg1REgdjKJfY1i7x7b68IhsGHSMOXcOCWLwqmWg2FWv4JTC9gPH3nJWqcTueiFiJgDjSK%2fCipQ942%2fgAUWHTAR7s9hfZczFnpSwv1SXZhydgBK9BnsPWkg69583g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1341" t="inlineStr">
+        <is>
+          <t>09923044020</t>
+        </is>
+      </c>
+      <c r="F1341" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1341" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1341" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1341" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1341" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" s="1" t="inlineStr">
+        <is>
+          <t>A52100019180</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Shadab Iqbal Shaikh</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>A52100019180</t>
+        </is>
+      </c>
+      <c r="D1342" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=k3%2feRQ1bf7VfGF9PIebNVEQE4Up38qS0KsnAq9dH%2boBOqSRQWA%2fQKp9xUe08rgoqLIS0YB2QTDUxQEFQdc2YHkNnFrFMxZlpHvE3zInSUhLo%2fMOwGjQpVgl73uc06NvNqIVvGcbgbC0Za1CNFtzA8DsRBTU08b%2bQSns%2fVI%2fKKnHJU%2bVW9Dd1pA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1342" t="inlineStr">
+        <is>
+          <t>02026050900</t>
+        </is>
+      </c>
+      <c r="F1342" t="inlineStr">
+        <is>
+          <t>Shashtri Nagar</t>
+        </is>
+      </c>
+      <c r="G1342" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1342" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1342" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1342" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" s="1" t="inlineStr">
+        <is>
+          <t>A52100003430</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Tukaram Kashinath Kalbhor</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>A52100003430</t>
+        </is>
+      </c>
+      <c r="D1343" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=i7E%2bBFusaFGa5QznVIqP23urTMJeqQmvfr7EI7oYEG4ADh0pIazFVnTXJHfn3MuLqxtND6gdHyyrw14XBT%2bqzc02kt%2freAHjNu9eDjoZX5y8W9tSsFANpY6UZPQdw3x%2ffkDBxgc%2fmWKCTgiNkGLtoAQdl5TQeiMd2z2p7aGxNqg1xQuQYc70QQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1343" t="inlineStr">
+        <is>
+          <t>09881135335</t>
+        </is>
+      </c>
+      <c r="F1343" t="inlineStr">
+        <is>
+          <t>Nigdi</t>
+        </is>
+      </c>
+      <c r="G1343" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1343" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1343" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1343" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" s="1" t="inlineStr">
+        <is>
+          <t>A52100019020</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Bhagyashri Nitin Landge</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>A52100019020</t>
+        </is>
+      </c>
+      <c r="D1344" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=nsTCC00QmZ%2b%2bL93P5f56fHwqrgEEJid9q7NW7bz78rkf5lXI8JwUuIHIg4tdEFoXBUQ4Q7lZVyYr7WgglhDOa92JicrjyC8MQgtUs6Tm4Wqk%2bqc%2fMntRtsj40wHgEouiisU1p0SfzZ0fgrmdqF7NgQK8tfSquEY2jQMgWpi0pRLEw77m0bsgiw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1344" t="inlineStr">
+        <is>
+          <t>02012345678</t>
+        </is>
+      </c>
+      <c r="F1344" t="inlineStr">
+        <is>
+          <t>Ambegaon Bk</t>
+        </is>
+      </c>
+      <c r="G1344" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1344" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1344" t="inlineStr">
+        <is>
+          <t>Ambegaon Bk</t>
+        </is>
+      </c>
+      <c r="J1344" t="inlineStr">
+        <is>
+          <t>411046</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" s="1" t="inlineStr">
+        <is>
+          <t>A52100018954</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Kishor Sheshrao Musale</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>A52100018954</t>
+        </is>
+      </c>
+      <c r="D1345" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=NTJXnrCOJOlq%2byyioxsLE9M9g6ayfq2WukD4pAYCUX3fCqNNcyHM9rvIRFRNC0V%2bhDJ8v4jvHuL%2b6G7sL1uV8rK6AHdWdWzSB6G3EwsPNmnAPok6KaMQ0DlAOMb6EM6H54v2OVOutpVyiMYs1mDy63GaHF5kt4Jd4doOPxs1Ar73A5k%2b7zwvGA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1345" t="inlineStr">
+        <is>
+          <t>08888606611</t>
+        </is>
+      </c>
+      <c r="F1345" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="G1345" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1345" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1345" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1345" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" s="1" t="inlineStr">
+        <is>
+          <t>A52100019282</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Neela  Soans</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>A52100019282</t>
+        </is>
+      </c>
+      <c r="D1346" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Y731%2bwXcaHFPrRZf95ZgIV%2bJcUqGwOGegez%2bBdnRaRI7Q1gGYr6jzXVvHpvyChlp7JFC4eT5JjjKECTMGRXkUWDkofaef8bKOy0%2fW%2bYCjuXTx18n8STFRF5ckhQoKpMdrVgk9QKXWuo5BrP1kTCfsEKqNvIbbtlNE0DYfH5vAMDMGkOre50Z3g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1346" t="inlineStr">
+        <is>
+          <t>02228129115</t>
+        </is>
+      </c>
+      <c r="F1346" t="inlineStr">
+        <is>
+          <t>Mira Road</t>
+        </is>
+      </c>
+      <c r="G1346" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1346" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1346" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1346" t="inlineStr">
+        <is>
+          <t>401107</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" s="1" t="inlineStr">
+        <is>
+          <t>A52100002956</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Harmeet Singh  Oberoi</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>A52100002956</t>
+        </is>
+      </c>
+      <c r="D1347" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=0t0yXmQdVOy2NiNiNC3Hk%2feG%2bGvw51h10KJ0NzMso09QO%2bVvSgD1s%2bz9%2fNFxhKywsIoPzr0rEyFHhA9zw0snm5drwcxEU9vNSmJ7wQnkfBPCrPiLuuoSUgaW3qJHoeCtnOwu%2fgyB0mlB%2bSXMek32v2hUOj8ak3NEmOjKBE7Ub%2fo6K1uf1eV0Lg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1347" t="inlineStr">
+        <is>
+          <t>09922340340</t>
+        </is>
+      </c>
+      <c r="F1347" t="inlineStr">
+        <is>
+          <t>Boat Club Road</t>
+        </is>
+      </c>
+      <c r="G1347" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1347" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1347" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1347" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" s="1" t="inlineStr">
+        <is>
+          <t>A52100019070</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>C J Jose</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>A52100019070</t>
+        </is>
+      </c>
+      <c r="D1348" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=zLkPeJJLSyZW8Zm1vdlRvc4L0yQbSvoC2%2fL%2fdlViIWlkTm%2bZtTKr0bd0NWAREsKni0zLWk2T2JE2WfPkvYd%2fnvOR9OXayC%2fTZ8484AChFxLI8NsPoqE9mBDzanAdBs%2bUkHzrfq65Y8QVL6TVc6%2fCZIO6OU28p6FFzSedfnu1UPcupjR9xRtC0Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1348" t="inlineStr">
+        <is>
+          <t>07755926978</t>
+        </is>
+      </c>
+      <c r="F1348" t="inlineStr">
+        <is>
+          <t>Tingre Nagar</t>
+        </is>
+      </c>
+      <c r="G1348" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1348" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1348" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1348" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" s="1" t="inlineStr">
+        <is>
+          <t>A52100018969</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Neelima Rishikant Shende</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>A52100018969</t>
+        </is>
+      </c>
+      <c r="D1349" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3gfkJb8TTASdFsfnkLvKJr%2bfxoI2bDAeGXXes6yqEtopKPssWm74KRPRUREt8Y9m75KgMFSvq6XlOCgWTtn1Oe292mv%2f9w7FNyUgvymAhZtkbva9GwtfUplpwQpXPcJKiXKFMmPYbY3RJ5DZf%2fqJe3D0%2fl3r4QjMHzT%2fU3n8%2f201Cy%2fbFZrGoQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1349" t="inlineStr">
+        <is>
+          <t>02024374296</t>
+        </is>
+      </c>
+      <c r="F1349" t="inlineStr">
+        <is>
+          <t>Dhanakawadi</t>
+        </is>
+      </c>
+      <c r="G1349" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1349" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1349" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1349" t="inlineStr">
+        <is>
+          <t>411043</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" s="1" t="inlineStr">
+        <is>
+          <t>A52100019100</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Amol Lalasaheb Deshmukh</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>A52100019100</t>
+        </is>
+      </c>
+      <c r="D1350" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=owH4zT111GJUbuTqnma%2f9e1CRgMjtBfYGVWRdK%2fXVB70I4RVONBKpd9djnk5vf%2bG9c0z7GXj3nPI2I4Y%2bBzTRi22oPpGVdx5vpLghormNx0NnQEa59oN%2fcuQ3bBWR4O4qlUVkBFP6snDeTD8OnHUnoT%2bn5VzkY2Vpi2arDiBo4D%2btBFxdKEECA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1350" t="inlineStr">
+        <is>
+          <t>02024373680</t>
+        </is>
+      </c>
+      <c r="F1350" t="inlineStr">
+        <is>
+          <t>Shani Nagar</t>
+        </is>
+      </c>
+      <c r="G1350" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1350" t="inlineStr">
+        <is>
+          <t>Ambegaon</t>
+        </is>
+      </c>
+      <c r="I1350" t="inlineStr">
+        <is>
+          <t>Ambegaon</t>
+        </is>
+      </c>
+      <c r="J1350" t="inlineStr">
+        <is>
+          <t>411046</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" s="1" t="inlineStr">
+        <is>
+          <t>A52100002520</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Lakhmichand Jethanand Chabria</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>A52100002520</t>
+        </is>
+      </c>
+      <c r="D1351" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=m4ZOA65BEOfL6oPH8jn17w2KQUJt7DhUFOjjujfkSmiHPmNZyu4VpvZI7gfGf14nuymvFi5S%2fHeEhB3yM7jq8is3vzAxNtNCW9wptfekUIaPmdE%2bI%2bryCU86o9zMOOUk5%2bROGCnVOl5s9MN3%2fMI%2fuNA7ysyMbGLaLqwEzYNPUDiJsl9mfBQpFw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1351" t="inlineStr">
+        <is>
+          <t>02025889489</t>
+        </is>
+      </c>
+      <c r="F1351" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1351" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1351" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1351" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1351" t="inlineStr">
+        <is>
+          <t>411067</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1400]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1351"/>
+  <dimension ref="A1:J1401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -70160,6 +70160,2606 @@
         </is>
       </c>
     </row>
+    <row r="1352">
+      <c r="A1352" s="1" t="inlineStr">
+        <is>
+          <t>A52100019047</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Sunil Kumar Singh</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>A52100019047</t>
+        </is>
+      </c>
+      <c r="D1352" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=G8jdQyLnhi1h%2bb3PggfpceyQO8J78Mgdym0UenCNYWZ4Pu%2b7z6G493CNLej9OypRL58BjF4CRcObkcchdKtW8oymJ5dLOBVvpejYkpEC%2b0zaTf3YMhzr2hQy8E1v7U%2byG%2bHupp%2b4hQtu1hEz20k2VA9TLImKYMSSz6bh%2fy2fyc9CuD7eC0NGKQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1352" t="inlineStr">
+        <is>
+          <t>07720868783</t>
+        </is>
+      </c>
+      <c r="F1352" t="inlineStr">
+        <is>
+          <t>Talegaon</t>
+        </is>
+      </c>
+      <c r="G1352" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1352" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I1352" t="inlineStr">
+        <is>
+          <t>Talegaon Dabhade (R)</t>
+        </is>
+      </c>
+      <c r="J1352" t="inlineStr">
+        <is>
+          <t>410507</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" s="1" t="inlineStr">
+        <is>
+          <t>A52100018991</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Amit Bajirao Kharat</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>A52100018991</t>
+        </is>
+      </c>
+      <c r="D1353" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=f21g3pAuvWeTT26jpgHJbMOPwDjubjZ42yNNrDMfoiL9nZoRxOBtMIre4K0oTzDeLI41ZGidhl3ziRDpGdkS0uerEi0PIm4tvHoG4otEojLzMbauKBjNkijsL9n7dKYpvrbANSg%2fyE8KtA3N9REHweNFoqRvpz%2biuFwYhXozkZpJIkY7BVd5kw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1353" t="inlineStr">
+        <is>
+          <t>02022445267</t>
+        </is>
+      </c>
+      <c r="F1353" t="inlineStr">
+        <is>
+          <t>Vadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G1353" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1353" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1353" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1353" t="inlineStr">
+        <is>
+          <t>411036</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" s="1" t="inlineStr">
+        <is>
+          <t>A52100019131</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Vikas Umesh Wagh</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>A52100019131</t>
+        </is>
+      </c>
+      <c r="D1354" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1SSgjHqSqZNR2JgRfb%2bIt%2fMHRGha4k%2bOogd0bZx2UvxWyOAQD%2f90iXghEbW7zGpvjvjwM%2bXxNXK8DS%2fwdJy9avcEUTZ%2bqx9jX2vnsr204tINlhyM4x0Nd4XldhX5sdK5Nfs3PY5yESO9d20DQOWQC4znTbmOJCYuH2t1BlhW%2fYRUjkEbJsiQjQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1354" t="inlineStr">
+        <is>
+          <t>07709300136</t>
+        </is>
+      </c>
+      <c r="F1354" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1354" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1354" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1354" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1354" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" s="1" t="inlineStr">
+        <is>
+          <t>A52100019026</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Kadir Shukur Shaikh</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>A52100019026</t>
+        </is>
+      </c>
+      <c r="D1355" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=sFYSHIXeighZiyIrXRrBg1JIiv9J59IjMurcWFzhmqDln%2f%2bES2x%2bUMxKFTwruZVhD2ZBStKrJpeEw9lE7E1801EP2IAbOwg8ms4pSy%2bvmMNdChg5iV623UmHVJqM8Qwf5obCiDHAZEv1Up%2bwSlnGkXGXzDLeyZCA%2byyHSL2aUN%2bS8hIzeqgUuQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1355" t="inlineStr">
+        <is>
+          <t>02048617230</t>
+        </is>
+      </c>
+      <c r="F1355" t="inlineStr">
+        <is>
+          <t>Nibm</t>
+        </is>
+      </c>
+      <c r="G1355" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1355" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1355" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1355" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" s="1" t="inlineStr">
+        <is>
+          <t>A52100002971</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Kamlesh Kirit Davavala</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>A52100002971</t>
+        </is>
+      </c>
+      <c r="D1356" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=OMkooqXx74M%2bwJs2HZoP2LgquM6vGY7ml%2fcjdq%2bjm9zJb%2bw0K5wWEjY5njhxuqm3QUwOZnv86RnCnFvgEEC2BdkTmqPfWvxZymb42ZzKe58Inx93DmUp7hHFl%2fZRVsqZtP0j%2bOyPGRCx8vE8Xcm3hqaA3qNsff%2fJLmCKmqNd3m%2bChJTmBaJ7Lg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1356" t="inlineStr">
+        <is>
+          <t>02041003302</t>
+        </is>
+      </c>
+      <c r="F1356" t="inlineStr">
+        <is>
+          <t>Kondhwa Budruk</t>
+        </is>
+      </c>
+      <c r="G1356" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1356" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1356" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1356" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" s="1" t="inlineStr">
+        <is>
+          <t>A52100019029</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Sanjay Dattatray Magar</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>A52100019029</t>
+        </is>
+      </c>
+      <c r="D1357" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1PYudFIQlKPMMwKRiv16xfbL91eaGNFwRJvblstwJoJie80Nh8EqtH3unOGGqMWfR2XGgWU%2fMUEt%2blNByC3bDrrFk9%2b3Y6hHLOTRERPgMMPBFNkHjzW2gzIxiaFXldZOiGa0LAaAHMBpqVo99z3ghnjYbWuybOl1UgPLWrGhU6%2bFLTdRtGnwlg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1357" t="inlineStr">
+        <is>
+          <t>09850435050</t>
+        </is>
+      </c>
+      <c r="F1357" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1357" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1357" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1357" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1357" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" s="1" t="inlineStr">
+        <is>
+          <t>A52100019065</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Rohan Sanjay Magar</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>A52100019065</t>
+        </is>
+      </c>
+      <c r="D1358" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=t0YtVsSGYwduluKkZ872%2fgm8R48XUa6cc8N4hPJ5DGsg9wKh16EFoRmVjDIX3f4cuH%2b25JcUILeUBPf6Qi1zYM71Pgz%2bwyf3cgqo67NR6UUIU%2f0gMI%2brwyTQUx1qRqCQNupHAXxOAkAdDMBwDSigUgPEz1SnGU9PurZxiwq%2br8eBlMqonpVLnw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1358" t="inlineStr">
+        <is>
+          <t>09657776565</t>
+        </is>
+      </c>
+      <c r="F1358" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1358" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1358" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1358" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1358" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" s="1" t="inlineStr">
+        <is>
+          <t>A52100019104</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Riddhi  Bansal</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>A52100019104</t>
+        </is>
+      </c>
+      <c r="D1359" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=yCWVch%2biiAkMOBaw0v4HQzR%2bTW0RmSgnk81rEE0SmuG9w5%2b3FEA8Mp%2fGB9fcCcBr%2flQE3M058Ps2nuoxqydZY6rbTo3on750TyzKgBYxw%2bO%2bRhNLJ219hI3TUdiPRMfPPDKQiaS6EVWIQ7EoAVmikMm66%2flejdP3msn%2f7vzkbH7HWbjVRHaunw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1359" t="inlineStr">
+        <is>
+          <t>02026690331</t>
+        </is>
+      </c>
+      <c r="F1359" t="inlineStr">
+        <is>
+          <t>Lohegaon</t>
+        </is>
+      </c>
+      <c r="G1359" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1359" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1359" t="inlineStr">
+        <is>
+          <t>Lohgaon</t>
+        </is>
+      </c>
+      <c r="J1359" t="inlineStr">
+        <is>
+          <t>411032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" s="1" t="inlineStr">
+        <is>
+          <t>A52100019078</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Mangal Sanjay Magar</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>A52100019078</t>
+        </is>
+      </c>
+      <c r="D1360" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5NQX%2bXCSwzGjKuLrJIQOSYBKmkf4Rc%2bYa89D2RcEq9uLPw6J0PS0YdwsZIX0qlRgrPzxF3CC2EOnJnWVBxepVDXElu%2bWTWsstn18VXZNmvzoMVD9KeWrOvCVgIijPVXF0f7eURUJ91VJyKaIJuly3QcJLFmQffGdtcB%2bP5dqDyPEwSGLKFKiQA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1360" t="inlineStr">
+        <is>
+          <t>09623154154</t>
+        </is>
+      </c>
+      <c r="F1360" t="inlineStr">
+        <is>
+          <t>Magarpatta City</t>
+        </is>
+      </c>
+      <c r="G1360" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1360" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1360" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1360" t="inlineStr">
+        <is>
+          <t>411013</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" s="1" t="inlineStr">
+        <is>
+          <t>A52100019050</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Murtaza Firoz Dahodwala</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>A52100019050</t>
+        </is>
+      </c>
+      <c r="D1361" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=cJ3NWTs2QRawVad%2byGpjZBAXzZq7vOGg1itX9MeK03TiHX4QHEhrN0ZllA2FU5vbr%2fWln9OW%2fIn0RVxkeBbg%2b2H3BiyIPPknvTLRwSv2L%2b8QlR9TI8I%2b3EW88K%2b2%2fsChmTbxxXiKxMR8yNW3l8BUhekzZ3BQuewK9LjqHxYUhX2X4JmQhkCHsg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1361" t="inlineStr">
+        <is>
+          <t>02026344610</t>
+        </is>
+      </c>
+      <c r="F1361" t="inlineStr">
+        <is>
+          <t>Wanawdi</t>
+        </is>
+      </c>
+      <c r="G1361" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1361" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1361" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="J1361" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" s="1" t="inlineStr">
+        <is>
+          <t>A52100019098</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Rajesh Sampat Tiwari</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>A52100019098</t>
+        </is>
+      </c>
+      <c r="D1362" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=RnMzqvtBKeIkH63Bx94l%2b8M%2fI3A5N8zMwa5v8oyBZBo%2fELva9bIfNK2GhfbxaFVowtgLm07ag7kn5kAp%2blnSZcV0WQyVe2ESbr4vOL%2bGmdsxZnuuRmgk9zw6kQDJb6R0DZA3%2fEL9Pm3vbhrlGA4F6am4OwavsB1kdSaliAiPigkvWl%2fuUqFrwA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1362" t="inlineStr">
+        <is>
+          <t>07272933444</t>
+        </is>
+      </c>
+      <c r="F1362" t="inlineStr">
+        <is>
+          <t>Bhugaon</t>
+        </is>
+      </c>
+      <c r="G1362" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1362" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1362" t="inlineStr">
+        <is>
+          <t>Bhugaon</t>
+        </is>
+      </c>
+      <c r="J1362" t="inlineStr">
+        <is>
+          <t>411023</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" s="1" t="inlineStr">
+        <is>
+          <t>A52100019038</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Shekhar Sunil Thite</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>A52100019038</t>
+        </is>
+      </c>
+      <c r="D1363" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fV%2fw5uKjHG7fVwnASI7CNmuyphVLVZ6WtwnIIjvjDO1KAPvmFD8PP9l9yyMtFp4pF%2fprwphdtfuo%2bo3wLTAgf4XyBfmUUNJmzR1AhVPYFPOIKr2o80STfvuMgH6vtDO2pr7UNxv8h6yYshoHPbTnyjGxAa4krSmnlATlypjkqTWXrhBR3pIC0g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1363" t="inlineStr">
+        <is>
+          <t>02027033513</t>
+        </is>
+      </c>
+      <c r="F1363" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1363" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1363" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1363" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1363" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" s="1" t="inlineStr">
+        <is>
+          <t>A52100019093</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Chahat Dheeraj Parwani</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>A52100019093</t>
+        </is>
+      </c>
+      <c r="D1364" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CbqgflLQtsWGEoXSf%2b3YIum%2bIinrxo5eGKiC0VrGI%2bX1YhQk8cK3qygNVOnAy29eLEaRqArp%2bvky8%2fKzhqY7qSsz6TbFgsceIj4VbkefpgwI4Ir3wzYyFifMKyHFzhjY9YgrNlpN%2brP8xIKiTj%2bHDnZyxG%2bBnhRo1wVnqruoknW2tTbYDoYg9A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1364" t="inlineStr">
+        <is>
+          <t>09923420492</t>
+        </is>
+      </c>
+      <c r="F1364" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="G1364" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1364" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1364" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="J1364" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" s="1" t="inlineStr">
+        <is>
+          <t>A52100003919</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Balram Shashikant Jha</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>A52100003919</t>
+        </is>
+      </c>
+      <c r="D1365" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KAr%2bhPHlXuYRzHd4iezvfRgVue9poMHEVSvdRLcgIVOcVDGQmSPGFA5mnQWW199LsSfXl3lQsTD9YpZ73Kq9%2bazdGXJxICZWX1ipZGnTzvHFKblmhoe%2f0HfjRZH8avl4ZDefPfjwLhwnCrt5y5psKVxZKryCvGdQIQrWgUbFjNvtS%2b6z3RckuA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1365" t="inlineStr">
+        <is>
+          <t>02228118623</t>
+        </is>
+      </c>
+      <c r="F1365" t="inlineStr">
+        <is>
+          <t>Mira Road East</t>
+        </is>
+      </c>
+      <c r="G1365" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1365" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1365" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1365" t="inlineStr">
+        <is>
+          <t>401107</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" s="1" t="inlineStr">
+        <is>
+          <t>A52100019489</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Susmita  Kumari</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>A52100019489</t>
+        </is>
+      </c>
+      <c r="D1366" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=TPPaDttBXwOZxGajeQDvGNSnUzEjGsX0ZDk733%2fJtho%2fCrzpbA8Pn5pPDs5nTs7RWx%2ba2YxU%2fA1cdamqRAlpM5Vdl4oTe4Tdhuk6sU92gDycgbAPK6eGcHboiIT1NqCziw8K9zVUtCxqPUH54RYV81QLQ04DALI8zLkd7QUtYVRkTgqgPbwWlA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1366" t="inlineStr">
+        <is>
+          <t>09923005932</t>
+        </is>
+      </c>
+      <c r="F1366" t="inlineStr">
+        <is>
+          <t>Dhanori Road</t>
+        </is>
+      </c>
+      <c r="G1366" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1366" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1366" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J1366" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" s="1" t="inlineStr">
+        <is>
+          <t>A52100019147</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Abhishek Nayan Shah</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>A52100019147</t>
+        </is>
+      </c>
+      <c r="D1367" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=oGkVnfLrfaTiAZjAIfNBOwQpZ%2bzHJX2VC84J%2ftBkh%2bbp7%2bKovAApwct168OMgicQg8JT%2bJQcDD%2f%2fgeXWDthCXJG%2ffuKuEk94iw7tEJVWFXcK1YfYWwtpAA%2beNtaYQ7iONhLkQfxO7dwIhFj6RXKLCJvnCa3a3hqjEOR7QgxupJ4PRnzK0ZEpMQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1367" t="inlineStr">
+        <is>
+          <t>09823685853</t>
+        </is>
+      </c>
+      <c r="F1367" t="inlineStr">
+        <is>
+          <t>Near To Mount Carmel</t>
+        </is>
+      </c>
+      <c r="G1367" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1367" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1367" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1367" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" s="1" t="inlineStr">
+        <is>
+          <t>A52100019110</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Sanjay Asharam Shukla</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>A52100019110</t>
+        </is>
+      </c>
+      <c r="D1368" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1a%2bXcmjwZEdz%2faZ1iSeaRtUvwjoJawCMlNo0T2nMrGu0qCL%2f%2fRlOtce7K8ouN6IfS1PQDz7mwAdgzhs5w3nU1FTkGPP2B3%2fwKJM1nCWJK4liaqxim3%2fV%2bQBE14wynFV%2blvbbVbFD9fEBVE3aew1sTD66Sm4TXwHqOKxabhRYE8VHNYXTky%2bJfg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1368" t="inlineStr">
+        <is>
+          <t>09867518722</t>
+        </is>
+      </c>
+      <c r="F1368" t="inlineStr">
+        <is>
+          <t>Near Dhobi Ghat</t>
+        </is>
+      </c>
+      <c r="G1368" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1368" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1368" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1368" t="inlineStr">
+        <is>
+          <t>400060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" s="1" t="inlineStr">
+        <is>
+          <t>A52100019165</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Joseph Thomas Francis</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>A52100019165</t>
+        </is>
+      </c>
+      <c r="D1369" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=I5AXyvrxxY6SJbMKVaUKJD2mSJwZZ2p%2bgi%2fsz9BL2C%2fGeg%2fi2HcLbuV7dAJtOlOHCH4iiwYYKcUCle3zckZt97rJqjVMVl2u0AofKFU%2bVdTPB9DCspS9OTkxQKJyG58Px8Kgmd76O69PMILRJaFJJSm6RaUVzGrAnyWHD4Odt3wm0kdjGo0%2fQA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1369" t="inlineStr">
+        <is>
+          <t>07774877168</t>
+        </is>
+      </c>
+      <c r="F1369" t="inlineStr">
+        <is>
+          <t>Sutarwadi</t>
+        </is>
+      </c>
+      <c r="G1369" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1369" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1369" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1369" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" s="1" t="inlineStr">
+        <is>
+          <t>A52100019343</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Rupeshkumar Satishkumar Zanzari</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>A52100019343</t>
+        </is>
+      </c>
+      <c r="D1370" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hyWbhkdsOk0f2JSR7H6I5kNUPE8vF5Qf3pCRfMT7QlqU6MR3gcEqbBrd5f%2fcI8MwcuCcVlBO7B%2bVu4sVXeZuIf%2fHSB%2bUH2%2fkSELnl1ghEdBJvGULtq%2bjX3mDA%2b66JPByOnbbZeYUwXP1ZXHdBZRq06CCV4f6GYHQdqzj0om%2fidW83%2bMkUKphdQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1370" t="inlineStr">
+        <is>
+          <t>07252232069</t>
+        </is>
+      </c>
+      <c r="F1370" t="inlineStr">
+        <is>
+          <t>Karvenagar</t>
+        </is>
+      </c>
+      <c r="G1370" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1370" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1370" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J1370" t="inlineStr">
+        <is>
+          <t>411052</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" s="1" t="inlineStr">
+        <is>
+          <t>A52100036306</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Mangesh Hawyya Mathpati</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>A52100036306</t>
+        </is>
+      </c>
+      <c r="D1371" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=kJTgJhB241T%2fnFfa5SPWXuD5RLGSzReWNQ7gGeLv1tBx52K%2fNDs5wkj%2bbexVM%2benwgQQAI4USTvluetxWDfGaqff9sCwQ%2f2qZLl5CswmtN%2bHKiTPuyKRveXbh1j6YL7gy92QDwIERGdwRLypg%2f2xoX%2btyrJvk2Xta7pauH1WRMFqHC7V9VDo0w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1371" t="inlineStr">
+        <is>
+          <t>09175275159</t>
+        </is>
+      </c>
+      <c r="F1371" t="inlineStr">
+        <is>
+          <t>Charoli Budruk</t>
+        </is>
+      </c>
+      <c r="G1371" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1371" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1371" t="inlineStr">
+        <is>
+          <t>Charholi</t>
+        </is>
+      </c>
+      <c r="J1371" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" s="1" t="inlineStr">
+        <is>
+          <t>A52100019163</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Manoj Bastimal Parmar</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>A52100019163</t>
+        </is>
+      </c>
+      <c r="D1372" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=8B0Myq52cjQ8r2%2ffI5wl8WWa%2fIm9n7VCW%2fyhhQiLFH6zkpVFcWNduhd4PoPR4pFuIFO26nnTR3H0hUwt4uji7%2fu0Uw4NodVHvKuHnBuHiM9jKd3mYhUsdnUlZG0BM3efOq4mdewY8crt%2fRKbQu2E%2bTuWWenbnRU9HOsrZ5nEstLrkWvLdrwilA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1372" t="inlineStr">
+        <is>
+          <t>02038141011</t>
+        </is>
+      </c>
+      <c r="F1372" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G1372" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1372" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1372" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1372" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" s="1" t="inlineStr">
+        <is>
+          <t>A52100019188</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Suchitra  Sawant</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>A52100019188</t>
+        </is>
+      </c>
+      <c r="D1373" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=YKi2wm8Nff80%2b%2bsLVXDK1oN4KYu6d7%2bK5I9MZOhj9cCBSPm7uqOQkEMQY9HGJm1U3xxUNHN25SfKk7IivzNirBfbtJER%2fUbLqq%2bfk2V73dqc2lzJTYP8rDX7amJEJJpwSUfhTSbKyiRPVksCKu%2buTPPDsaaqORTW6wgcI3SURlDoe8Jn7HtHUA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1373" t="inlineStr">
+        <is>
+          <t>09657002674</t>
+        </is>
+      </c>
+      <c r="F1373" t="inlineStr">
+        <is>
+          <t>Pimple Gurav</t>
+        </is>
+      </c>
+      <c r="G1373" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1373" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1373" t="inlineStr">
+        <is>
+          <t>Pimpale Gurav</t>
+        </is>
+      </c>
+      <c r="J1373" t="inlineStr">
+        <is>
+          <t>411061</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" s="1" t="inlineStr">
+        <is>
+          <t>A52100019233</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Ashok  Patidar</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>A52100019233</t>
+        </is>
+      </c>
+      <c r="D1374" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=HqbMOS6I6QrfQYypq5XoVCH%2b6%2boVk0gTjEB3MDPyKDt1MmmnZUGLGXSyPt8nWPMA%2beHkHISduMoTs8mMa3T9wCETkTb22uZ9Zg7DV5hSj6NA7ohAKgr3uiRRnpuN1275FbKwDUgWcmNHfPpCnuwQWDrCTfEC%2b1ED9mhiHrMHcKX2brXOG1dHtQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1374" t="inlineStr">
+        <is>
+          <t>02027504257</t>
+        </is>
+      </c>
+      <c r="F1374" t="inlineStr">
+        <is>
+          <t>Hinjewadi</t>
+        </is>
+      </c>
+      <c r="G1374" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1374" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1374" t="inlineStr">
+        <is>
+          <t>Marunji</t>
+        </is>
+      </c>
+      <c r="J1374" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" s="1" t="inlineStr">
+        <is>
+          <t>A52100019146</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Savita Shekhar Gundlapelli</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>A52100019146</t>
+        </is>
+      </c>
+      <c r="D1375" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QwU8A6r6Y7qKJK3VwdhuH9arZPZDONePa5nAX7k%2bUT7jbsc5MsFlQSbt4%2bCy10Z3Hclr0f3fYOmTWnQW4rVO2ZWX6zOJO7i6syWMI1o9A3Pw%2fQL30i6QAtkv7lPM2BRyl4iB5u5fmaUM2sJ6e%2beNdECbhGpr5SgpEo5DQLn6eHZ61IyB8QQRhQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1375" t="inlineStr">
+        <is>
+          <t>08446884462</t>
+        </is>
+      </c>
+      <c r="F1375" t="inlineStr">
+        <is>
+          <t>Vadgaon Budruk</t>
+        </is>
+      </c>
+      <c r="G1375" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1375" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1375" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1375" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" s="1" t="inlineStr">
+        <is>
+          <t>A52100003165</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Santosh Dnyandev Nanaware</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>A52100003165</t>
+        </is>
+      </c>
+      <c r="D1376" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QR%2b9NQD%2fetjacK4JynuJqgbbFO5SyXyuL16aHhD1OpqzXBVjYQRz3O4ZytPVvnbKSXWkGB9gtrzHLqgi2XaDLR6gNJXts8gCgBkawKj3YMTd7ny%2bNnz2CdMJMqhtm8yGpYqGJZPyXr0gd9XuETesPAGVf440CVWvqjArEFsz2Eh7DOeRpQE5kQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1376" t="inlineStr">
+        <is>
+          <t>08087548386</t>
+        </is>
+      </c>
+      <c r="F1376" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1376" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1376" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1376" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1376" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" s="1" t="inlineStr">
+        <is>
+          <t>A52100019151</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Priyanka Bhavesh Tagalpallewar</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>A52100019151</t>
+        </is>
+      </c>
+      <c r="D1377" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=DEWWCmi7zabEovMMuWUYlN8RzZkWkY3aVB6nLlURLgmZyQmfIK5sVX9eQBo0N9qoH4YDBACYYnx5s4RMD2QksDk9RT%2bBedVh0jyUEwURy2v8eGOf24BMitdA34dY5Daa%2faYGPBbY3SdIl4O2jNam4Ma7c7c1uJSw7qhR6zPAuEmBJnG1JLcWNg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1377" t="inlineStr">
+        <is>
+          <t>09921141661</t>
+        </is>
+      </c>
+      <c r="F1377" t="inlineStr">
+        <is>
+          <t>Survey Number 4/2B/1/1A</t>
+        </is>
+      </c>
+      <c r="G1377" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1377" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1377" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J1377" t="inlineStr">
+        <is>
+          <t>411058</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" s="1" t="inlineStr">
+        <is>
+          <t>A52100019150</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Rajesh Bholanath Vishwakarma</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>A52100019150</t>
+        </is>
+      </c>
+      <c r="D1378" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=YwtP%2fKbYYikTY5j5ydn4I7Dk6OMK71cPRBBqYT40HCxvePd6yFVYL6LVoTDxwAom641th%2fnjQBGQmHscudUKZ2Rn43DTJxLiKkl3ugf2sWCAwJRtH9IMZ%2bDbgrxiAHgNh7LWD3Q%2fgHd6HLPHq7g%2bdlSAED2bQ8bVO5yVGzhOPc%2fhJzPm%2fQ%2bqKg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1378" t="inlineStr">
+        <is>
+          <t>09146292100</t>
+        </is>
+      </c>
+      <c r="F1378" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="G1378" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1378" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1378" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1378" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" s="1" t="inlineStr">
+        <is>
+          <t>A52100019183</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Raj Dattatray Donhe</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>A52100019183</t>
+        </is>
+      </c>
+      <c r="D1379" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=P8I7jCuvEF8kWOLF3AXzoOUdfZSFgf%2bz5gvQK%2b34mwyFL1oiRjLq%2bMnexMrNXmK1h%2b6PpMNyxlFgqD8p1ED%2bF549GmYWvcOq%2bnhlLN06OYEeLRrJrA73EtrEa%2bxDoSBf1h3MI4%2b0CHga7wWjfc3EqrIWv3yATYbTVqMwNm5X5S5zslxe021eCQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1379" t="inlineStr">
+        <is>
+          <t>08421126437</t>
+        </is>
+      </c>
+      <c r="F1379" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G1379" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1379" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1379" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1379" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" s="1" t="inlineStr">
+        <is>
+          <t>A52100019161</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Sameet Nayan Shah</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>A52100019161</t>
+        </is>
+      </c>
+      <c r="D1380" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=szlSnSwiJW5LLIgDafHO0d82ug1QU2tam0HJI0qW1StyNxHiDHe4jmfG73QzfCRImhPUUdNrv83MGfCqCFz1YaXfYkCcUvjZsyNPFfYt5C77uH%2b1fiZXZLqyilRWwnlrIjxKQEa17xS6YIwQ%2fbg5vzh8v8VgCNk%2b0Cp%2fpxMRbRM5cLkQPGrp3w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1380" t="inlineStr">
+        <is>
+          <t>09890112567</t>
+        </is>
+      </c>
+      <c r="F1380" t="inlineStr">
+        <is>
+          <t>Nr Mount Carmel</t>
+        </is>
+      </c>
+      <c r="G1380" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1380" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1380" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1380" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" s="1" t="inlineStr">
+        <is>
+          <t>A52100019292</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Manisha Tapan Shah</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>A52100019292</t>
+        </is>
+      </c>
+      <c r="D1381" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=joBOH1PKiOmQqi8YRXa4gzYqnXgP%2fONDm4zxrBTZ3M65C7Fk%2flVOBfSRHaApbUJhMOD8k7D353I3c8eMAxefIfY2LMhJUc8PFQeTQnBNCOZzvfXk1lfWuqXpMM5Opz6wa%2fbIUrImZqqCI0DeVgovtPmIVs%2brqQvYDbOSoxXOWQxcTUjtzdJR9g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1381" t="inlineStr">
+        <is>
+          <t>08830107646</t>
+        </is>
+      </c>
+      <c r="F1381" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G1381" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1381" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1381" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1381" t="inlineStr">
+        <is>
+          <t>411039</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" s="1" t="inlineStr">
+        <is>
+          <t>A52100019160</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Rishikesh Kashinath Solanki</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>A52100019160</t>
+        </is>
+      </c>
+      <c r="D1382" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=YOYyyxI36hNsW7lp9k6HbkgmHnyaR4dhE%2bcizlDqAz40yHlhqS2coz14yAelz6Z7HY2RwPRqnc%2fUi3CaxbllmqXaWAH4pIwSOJL7X6pjP7oVZFbMb4DTzWSMppa0lah9YZ%2bKPr5nqFmFvkZClEkkQdnKanekRh9%2bByUtVBgDmOVcCtkfPi5ASQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1382" t="inlineStr">
+        <is>
+          <t>02071017101</t>
+        </is>
+      </c>
+      <c r="F1382" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="G1382" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1382" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1382" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1382" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" s="1" t="inlineStr">
+        <is>
+          <t>A52100019168</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Mahesh Ankush Babar</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>A52100019168</t>
+        </is>
+      </c>
+      <c r="D1383" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=aF0p3yB63ucQFw7ugtypeli8Lip1TLc%2fBaopXsEh9kH8ntO5v3v46M%2fCxSDO0RkgK9rb17IeWAH9vP9bGQL1qFhsYHJbqTJzTyfJG82JTLW%2b%2bjO9ClX1U6eDuNQZq08n1GNcK2KBEpqth7nRoF%2bBmthCfx4rJ%2fldyD1QxuuQmAZqWtsbkOVzfw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1383" t="inlineStr">
+        <is>
+          <t>02027662409</t>
+        </is>
+      </c>
+      <c r="F1383" t="inlineStr">
+        <is>
+          <t>Nigdi</t>
+        </is>
+      </c>
+      <c r="G1383" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1383" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1383" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1383" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" s="1" t="inlineStr">
+        <is>
+          <t>A52100019210</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Mukesh Madanlal Chhajed</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>A52100019210</t>
+        </is>
+      </c>
+      <c r="D1384" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=tzWWymlAn3nQoCutC45mwYP6xIjHkgKmTp%2bpP1MCDULFEcSVUXuhWQ%2bop1R%2bZq7bIKWKPtBjdL9CvxNrv7rnFEIajECpabdEeZHMi%2fBT3okyYO0w30S0xb4kbrkX5MtIbenfLG3DGuv6utKkGAyLeRMVYkgLYSCiifCDETx9P%2b67zJM8KaO%2bhA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1384" t="inlineStr">
+        <is>
+          <t>02041209837</t>
+        </is>
+      </c>
+      <c r="F1384" t="inlineStr">
+        <is>
+          <t>Mukund Nagar</t>
+        </is>
+      </c>
+      <c r="G1384" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1384" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1384" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1384" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" s="1" t="inlineStr">
+        <is>
+          <t>A52100019197</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Sharmila Mukesh Chhajed</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>A52100019197</t>
+        </is>
+      </c>
+      <c r="D1385" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xD0p3x6WVrNZbT20EHKcGtmt5KdYLJ2dTVV4Mf47Ug0U5mX%2fT5dh2wQkMp0bbQwzbdYt1gtwskzYVbpf0EsGkYxufq5XFOHEJIiA5wxCRzdmLsGWSxgXr%2fddWxJxapoN6d1pXGphzml815%2fg8pdbTVcb01iGXCs5MhPSFL0hI6at3W01qUIe3A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1385" t="inlineStr">
+        <is>
+          <t>02041209837</t>
+        </is>
+      </c>
+      <c r="F1385" t="inlineStr">
+        <is>
+          <t>Mukund Nagar</t>
+        </is>
+      </c>
+      <c r="G1385" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1385" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1385" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1385" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" s="1" t="inlineStr">
+        <is>
+          <t>A52100019175</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Siddhant Mukesh Chhajed</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>A52100019175</t>
+        </is>
+      </c>
+      <c r="D1386" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PN2moyjjAueHfdJebHvb94lAAegf29O4MQ6veddQT5lUk9cAonpEoUEsECYPXpOzLMAHDsRebWoS7fndYJNypLrKnr63zBq%2fiIEi4yqVbwSu22K4dA8ZWEmq1QC%2b3Xr1of16rJ4BtgEWAd3nhRGv%2btk3%2fF9FQFZjAcc4QqwiWIhWdXYuyAi4HA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1386" t="inlineStr">
+        <is>
+          <t>02041209837</t>
+        </is>
+      </c>
+      <c r="F1386" t="inlineStr">
+        <is>
+          <t>Mukund Nagar</t>
+        </is>
+      </c>
+      <c r="G1386" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1386" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1386" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1386" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" s="1" t="inlineStr">
+        <is>
+          <t>A52100019220</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Anisha Lifespaces Private Limited</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>A52100019220</t>
+        </is>
+      </c>
+      <c r="D1387" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=XnZCH8%2bxgskcEt%2fIFeBjGlMCQcOQwJlF0W4Da2e3Z2gbuE8Y6%2bovl57njQoaQNkHvW2K1WvacnUU7M6%2ftgX6oJNhyZUd4wIsaZEETFxJXJ0hzbOLfklVqhavY9onIBkj7lzzei7Ya6FPxLaeYq530rn7B06CMibM1f9yivfsyCIwsoXr4PDi2Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1387" t="inlineStr">
+        <is>
+          <t>02066226500</t>
+        </is>
+      </c>
+      <c r="F1387" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1387" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1387" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1387" t="inlineStr">
+        <is>
+          <t>Umaroli</t>
+        </is>
+      </c>
+      <c r="J1387" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" s="1" t="inlineStr">
+        <is>
+          <t>A52100019283</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Supriya Manoj Bokil</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>A52100019283</t>
+        </is>
+      </c>
+      <c r="D1388" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=9%2ficHUXLJfmyfJKVc1Rav4NP%2fwkQ%2fkARHaeQNzDAuk%2bxYZO2jW97Oabg%2fM5Dw1LCpWN8VtVc5CByfP45uJonB1QeGZ2TCsSfuXKVT5%2fqzeQ4cNX%2bPRUxu%2fwf9BfPuKeUVjbR%2frwauIHPIs0MaELore9vfNjAKcz0EoYnbuA%2f4drOtrOaqOYrLA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1388" t="inlineStr">
+        <is>
+          <t>02024379252</t>
+        </is>
+      </c>
+      <c r="F1388" t="inlineStr">
+        <is>
+          <t>Dhayari</t>
+        </is>
+      </c>
+      <c r="G1388" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1388" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1388" t="inlineStr">
+        <is>
+          <t>Umaroli</t>
+        </is>
+      </c>
+      <c r="J1388" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" s="1" t="inlineStr">
+        <is>
+          <t>A52100019321</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Laxman Tulsiram Tambe</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>A52100019321</t>
+        </is>
+      </c>
+      <c r="D1389" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=vhLhoxbHqTf4FyhCevcgF%2f1imIsJXRaFk4A%2f4gJ%2bjtKudfKnKiunl8RlydY%2bEuViEaeWoLG6dB%2fggRbpypJ11cVqnRDjtxBqkfqt8vh%2bCoS3Otvu2eP46juxEhFwFkNTcdPMKqlWArnr1rAY79%2bNe0Dh6Tb%2bwYmt4eW3a%2ffsvkmUZjkIXLPtbA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1389" t="inlineStr">
+        <is>
+          <t>02025655000</t>
+        </is>
+      </c>
+      <c r="F1389" t="inlineStr">
+        <is>
+          <t>Vishrantwadi Pune</t>
+        </is>
+      </c>
+      <c r="G1389" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1389" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1389" t="inlineStr">
+        <is>
+          <t>Vishrantwadi</t>
+        </is>
+      </c>
+      <c r="J1389" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" s="1" t="inlineStr">
+        <is>
+          <t>A52100019198</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Danaram Kaluram Sutar</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>A52100019198</t>
+        </is>
+      </c>
+      <c r="D1390" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=irAmEXTwGkIc8vOJpcRl8NuA6QPYKqJzTwF1460%2b23ICCZNtxd%2fheZQAWqKgtDtoFGbzE2%2fUCp0eu5oDHRPa%2fgvxLxaHbpXTP7IinvHIHuiTrHwc1nERfpETpQSaSdP%2bctSqOPmjRF0r1TusMaIxdq%2bsJmBhfb%2fD16URp%2b1YTtN%2b9L7xGBaROg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1390" t="inlineStr">
+        <is>
+          <t>02228684535</t>
+        </is>
+      </c>
+      <c r="F1390" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="G1390" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1390" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1390" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J1390" t="inlineStr">
+        <is>
+          <t>411058</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" s="1" t="inlineStr">
+        <is>
+          <t>A52100019185</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Alpa Rajendra Jain</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>A52100019185</t>
+        </is>
+      </c>
+      <c r="D1391" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KjpTjT1xiZs065xfXks0HYqp1qvVha3%2bjYX1AqIOyTuQkf%2f9mPeFT5k5yY%2fAwzGXLG7Eak6xs%2fuzktbArkt4n%2fDg8FT%2faxkWCmm4UyfCK1TODabygrGtxGsZwJN%2f8NFl9JuiX9R3N6Rydzk5WusafwBWkcGF87qpm0wGA0jGxBTlsqlV%2fft8Yw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1391" t="inlineStr">
+        <is>
+          <t>02223674702</t>
+        </is>
+      </c>
+      <c r="F1391" t="inlineStr">
+        <is>
+          <t>Marine Drive</t>
+        </is>
+      </c>
+      <c r="G1391" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1391" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1391" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1391" t="inlineStr">
+        <is>
+          <t>400020</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" s="1" t="inlineStr">
+        <is>
+          <t>A52100019262</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Arti Shailesh Jain</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>A52100019262</t>
+        </is>
+      </c>
+      <c r="D1392" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=T%2f2a4IrtqqQlJr90FSl%2ffnI0xLXSoxjwasuKVJrfiO1moR6IsS3q4bLtYkwbb1JB7ppvvv4Usz9sh3bdltg3Qctd8i4f5USL87NLF0GEaRhugDIfgQJoo1ywnooSBb6Q6nEf4cI63bx02hzyA1VWrNDtj3pZxjeI5SiQcZaCWOsz4td7mUdB1g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1392" t="inlineStr">
+        <is>
+          <t>02223674702</t>
+        </is>
+      </c>
+      <c r="F1392" t="inlineStr">
+        <is>
+          <t>Grant Road</t>
+        </is>
+      </c>
+      <c r="G1392" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1392" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1392" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1392" t="inlineStr">
+        <is>
+          <t>400007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" s="1" t="inlineStr">
+        <is>
+          <t>A52100019192</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Tanvi Hitesh Jain</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>A52100019192</t>
+        </is>
+      </c>
+      <c r="D1393" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=o273pQTq1JCONQx2mD5g%2bj4knqpUDZpI%2f1ZSqQBdkbwdqw%2fG6U25%2bUmr%2bTNULRA1AJ%2b5vg4J67h2VGwsdr9Oqgv5rf1JvSHlHuHqD2z%2f6qwzQvjMPoHDmMlAqR%2fUmsH%2fTp5ZlYU2yJ6ZCEc4rGD896P9Jkhu1ZVQE2lpx%2fcrebh87crVeG1l1A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1393" t="inlineStr">
+        <is>
+          <t>02223674702</t>
+        </is>
+      </c>
+      <c r="F1393" t="inlineStr">
+        <is>
+          <t>Prabhadevi</t>
+        </is>
+      </c>
+      <c r="G1393" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1393" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1393" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1393" t="inlineStr">
+        <is>
+          <t>400025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" s="1" t="inlineStr">
+        <is>
+          <t>A52100019209</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Nishant  Kumar</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>A52100019209</t>
+        </is>
+      </c>
+      <c r="D1394" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fkli90dmLVHn5HO1G25aKB8nxZQ64PEz51uEMtvKuJqwz%2fDqi0wNtZK9liNqGO%2bETlxa2epu3xJZq%2bXbdHqiPMd6w6fyQgE631nszbc%2bZbJfG6a7T1VGDT1ahWZhAcCQ%2fVL4O%2fxf5JjCyZjLPzHoF6Kgw%2fm5bnul49OguyRfYNLtBgpIGi%2bcbA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1394" t="inlineStr">
+        <is>
+          <t>09960925726</t>
+        </is>
+      </c>
+      <c r="F1394" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1394" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1394" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1394" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1394" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" s="1" t="inlineStr">
+        <is>
+          <t>A52100019387</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Shama  Khan Proprietor Of F S Realty</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>A52100019387</t>
+        </is>
+      </c>
+      <c r="D1395" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=q6e2zfDOmUzxKep5BbY96fT0YpMS5Z%2fzT0p9C3Z33pBeVQk4g4evupoUH%2fmGNjPqUiC8D0B%2fu5G4XE03AXpuL73GSQM26hZTlSLYBKQMbOPeX9kEVACg6HikA9GSfc6qRYvQ0Xw43LqrTlLq%2fkLqXpsnCwai8ACtGcGnS4vnaQB1%2fS0LRvoKbw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1395" t="inlineStr">
+        <is>
+          <t>07875104474</t>
+        </is>
+      </c>
+      <c r="F1395" t="inlineStr">
+        <is>
+          <t>Bhosari</t>
+        </is>
+      </c>
+      <c r="G1395" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1395" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1395" t="inlineStr">
+        <is>
+          <t>Bhosari</t>
+        </is>
+      </c>
+      <c r="J1395" t="inlineStr">
+        <is>
+          <t>411039</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" s="1" t="inlineStr">
+        <is>
+          <t>A52100019277</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Sandeep Babulal Mahatma</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>A52100019277</t>
+        </is>
+      </c>
+      <c r="D1396" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=VK4wdXbJmSS%2b1Sb2VHJfGVHG5BiEjXl46usQLq3AFEPOnRD2vEYRCj8Xw8HlE%2fe%2fx3OYi0G4RQAEqxI3q7UULLftIjXFhZB8Km2F%2fFCvD%2fmFWftBmenBi012dr12ac7aH0m38RP%2fpBUgcV38o%2bR7%2bpdxTyhhdXLKjIUbWbi4%2fYmfkvyqYKlMiA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1396" t="inlineStr">
+        <is>
+          <t>02067278596</t>
+        </is>
+      </c>
+      <c r="F1396" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1396" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1396" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1396" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1396" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" s="1" t="inlineStr">
+        <is>
+          <t>A52100019468</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Ashutosh Purushottam Joshi</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>A52100019468</t>
+        </is>
+      </c>
+      <c r="D1397" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=L16SJugEk7KLOqpGTZIzb5K4BDkLegdNNkmYhq1vBvxwA91umBD0e2HFES5n3tjSs9wQvpbQn0JJ0YtHMZEDUuiQuPRskA1xhF362%2bqNMfLm2WWYzZwDVwWfgFTUq2m8Ya4lCAgxy8%2bSFleNiIanO5x8yBm3XK0CNyqRmpiFutlfZ2QIBuq5kw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1397" t="inlineStr">
+        <is>
+          <t>02026349793</t>
+        </is>
+      </c>
+      <c r="F1397" t="inlineStr">
+        <is>
+          <t>Camp</t>
+        </is>
+      </c>
+      <c r="G1397" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1397" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1397" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1397" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" s="1" t="inlineStr">
+        <is>
+          <t>A52100019326</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Kapil Basantilal Chopda</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>A52100019326</t>
+        </is>
+      </c>
+      <c r="D1398" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=6oSY95qfbShwKnB%2fdxSter6zHvVfcVmMntx7m6kBwdPsS%2fjhdfylJDbQhy5BK6kN2rXnMM1Bewi64xgD6LX4aiMHnfTiVQW5kO0NnDqChD5N0WGzq5Cn%2fwchlaMds1LVwgHhxXS%2bjEWkECG4s4ha9Phehm5zbbfzNntQ9PYLT7sV3xTV%2brlSfQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1398" t="inlineStr">
+        <is>
+          <t>02027430051</t>
+        </is>
+      </c>
+      <c r="F1398" t="inlineStr">
+        <is>
+          <t>Pradhikaran</t>
+        </is>
+      </c>
+      <c r="G1398" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1398" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1398" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1398" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" s="1" t="inlineStr">
+        <is>
+          <t>A52100002492</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Randhir Narayan Kumar</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>A52100002492</t>
+        </is>
+      </c>
+      <c r="D1399" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=sc%2fhoTFsz%2fxuKroNrdqdFqSjLkwgQRmMP%2fQYnNEYlUk48NWk7tksxvwgpZafUBBygnjv1SrIcA8Urd1hA1GozmNqEwdsRlXDJbV%2fgtI2VnqXwZAdwTdANNDCS3zDIZb9Mq6xYY9peEVhl1N2HRN0bfWl%2fS1I19bLGRzPg3GfNDr3m1CfFzYh%2fg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1399" t="inlineStr">
+        <is>
+          <t>08888894065</t>
+        </is>
+      </c>
+      <c r="F1399" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1399" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1399" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1399" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1399" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" s="1" t="inlineStr">
+        <is>
+          <t>A52100002897</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Abhishek  Nair</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>A52100002897</t>
+        </is>
+      </c>
+      <c r="D1400" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2fxHqdvUHZOo8yLaIMIv8nzSQgDjxxNL2wBxoNnGDxFqIITW4RIDbrXweW1W7%2bHIRZn9fomQ%2byDPD7I9a6UC2qDEa%2bGv2uanUfaOmCIjhMKBUm%2ftaZyLps3ZZA61EilxXxty8hBGFcMm%2byLikW7uQIhq%2bGlwxIwOtCRF9gQgTxRXPsHFX04P8g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1400" t="inlineStr">
+        <is>
+          <t>02049306209</t>
+        </is>
+      </c>
+      <c r="F1400" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1400" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1400" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1400" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1400" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" s="1" t="inlineStr">
+        <is>
+          <t>A52100002694</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Yogesh Shankar Ramsagar Tripathi</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>A52100002694</t>
+        </is>
+      </c>
+      <c r="D1401" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=aroHcEaYJIV0j8ophPBLl6rO3cMPvXpptBLfsbOcqD%2bQWuikbzyO7WepteQCWOlfccETCutPJmgo7pkh3i1Mp3ADGTh%2b2OBasHjoQo%2f%2bvkpvLzuXaz4%2f80e7hnLQfnm5QOhN2K%2bKnc0f8ot3xuklXG4B5CRMzGNA5lPcXdhb7OxvucSmMbxczg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1401" t="inlineStr">
+        <is>
+          <t>09890655466</t>
+        </is>
+      </c>
+      <c r="F1401" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1401" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1401" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1401" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1401" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1450]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1401"/>
+  <dimension ref="A1:J1451"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -72760,6 +72760,2606 @@
         </is>
       </c>
     </row>
+    <row r="1402">
+      <c r="A1402" s="1" t="inlineStr">
+        <is>
+          <t>A52100019615</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Abhishek  Priyadarshi</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>A52100019615</t>
+        </is>
+      </c>
+      <c r="D1402" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=15CcSXFyg%2bP%2b%2byYU6GZncgM7BglK%2fRxlKh1TXXWjYSmjob9lk9ngWzoyDsjpHryngYVVUU40zEIjTP9Nfk3P4MFvHG7Gb52pNFmWLZ3OVGj3jl5lqaW8E2A2CZJ6NG46CzO0TpQMHdhiEp9D1F8CPaJqzvhOzmpD7S0l4avvxQXW9GpTWszn4g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1402" t="inlineStr">
+        <is>
+          <t>02048600423</t>
+        </is>
+      </c>
+      <c r="F1402" t="inlineStr">
+        <is>
+          <t>Ghorpade</t>
+        </is>
+      </c>
+      <c r="G1402" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1402" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1402" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1402" t="inlineStr">
+        <is>
+          <t>411036</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" s="1" t="inlineStr">
+        <is>
+          <t>A52100019532</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Anil Vitthal Jadhav</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>A52100019532</t>
+        </is>
+      </c>
+      <c r="D1403" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=oT60fhIXrADPp%2bRzQIzEd8anGcOCwsvlpGVO4I1apSqU94fWLxW2%2fghI2inLw0cHX4jbjeHmcMSbwlFzTlMK9kVqRID3AFV8i2uR0MIRByjuT7rPtcQ0jI8IbEGRbfx5ufbGszz3gMYKDjcGtDsH4TvdKFzl9EjIgunLPIIX8E9%2fXtgnHTeP9A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1403" t="inlineStr">
+        <is>
+          <t>02024348642</t>
+        </is>
+      </c>
+      <c r="F1403" t="inlineStr">
+        <is>
+          <t>Nanded City</t>
+        </is>
+      </c>
+      <c r="G1403" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1403" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1403" t="inlineStr">
+        <is>
+          <t>Nanded</t>
+        </is>
+      </c>
+      <c r="J1403" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" s="1" t="inlineStr">
+        <is>
+          <t>A52100003085</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Ankit Anil Abrol</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>A52100003085</t>
+        </is>
+      </c>
+      <c r="D1404" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=LcVkOjzbG5yT7SfNYr5eC4ihq9ewS22FOT2634g5HKCg22bNgQGkcO%2bvOzEF9F6DknnbbB9LQOScLYSxh6uNo85h0sqje6m8lYGQHnevR9Yhnm7P4pLJqF7AZAxceJUojWUgV5rgkCdxpg5lWJ4J3pUNNUI5dwX9w%2fjnUQQWNUAP27SUpa7CZQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1404" t="inlineStr">
+        <is>
+          <t>08783745444</t>
+        </is>
+      </c>
+      <c r="F1404" t="inlineStr">
+        <is>
+          <t>Vishrantwadi</t>
+        </is>
+      </c>
+      <c r="G1404" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1404" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1404" t="inlineStr">
+        <is>
+          <t>Vishrantwadi</t>
+        </is>
+      </c>
+      <c r="J1404" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" s="1" t="inlineStr">
+        <is>
+          <t>A52100019417</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Karam Chand  Garg</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>A52100019417</t>
+        </is>
+      </c>
+      <c r="D1405" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1ckPmBugtQC370L0cvro2Wr2L2ptc9zFWTrnxD2S2jSk7JJSh3SaOMuSoHYaT4S8RjNDBLpdYrOqiwwn64PpOSLXMnfgGRpj6UV%2bAGIs8737kFGAx%2fbanjw1sk4NyG53xXnWAPWF35fbMXh1SMkrJnCScS4%2fVevttMA%2fz8klScUWMETU%2bXw2RA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1405" t="inlineStr">
+        <is>
+          <t>02046740537</t>
+        </is>
+      </c>
+      <c r="F1405" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1405" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1405" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1405" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1405" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" s="1" t="inlineStr">
+        <is>
+          <t>A52100019479</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Nitin  Doshi</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>A52100019479</t>
+        </is>
+      </c>
+      <c r="D1406" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=DADpLn%2fIiJn4gHpAgILVxWvxb5FGAvK8cUGuO7ci6D7c2yi8dFAes3QDJ0nYBmoV8CpFR4%2bUOaXy4isVw7JtD4cCJBvLgM5rHdYVUadbXHpuXUzp0DdOShEDt8yqaKNmWohm0Z3aJfSfIXY4ZHoCaxMhRVaWNZsyL%2fRVza%2fW9FRaLanOLz39Dw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1406" t="inlineStr">
+        <is>
+          <t>02026401163</t>
+        </is>
+      </c>
+      <c r="F1406" t="inlineStr">
+        <is>
+          <t>Senapati Bapat Road</t>
+        </is>
+      </c>
+      <c r="G1406" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1406" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1406" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1406" t="inlineStr">
+        <is>
+          <t>411016</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" s="1" t="inlineStr">
+        <is>
+          <t>A52100019452</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>3M Estate</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>A52100019452</t>
+        </is>
+      </c>
+      <c r="D1407" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xbjSuGgCmGIpUNGNy1eMjq2n2B6jRAYpq6XdSv2GqOKqrC0wn8dcseBXill%2boXB9quXJOiWvsbt%2fcrgcFDyM5mqfXO31VHDeWGCyejEPKnDoPrC%2bnqXcrY1JP4cfLxKfX87vU6LGrHfTIZVqaByObO8PrWCO9G1gZF%2bDUgfuXOsAlcVrz7%2fk7w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1407" t="inlineStr">
+        <is>
+          <t>04040131202</t>
+        </is>
+      </c>
+      <c r="F1407" t="inlineStr">
+        <is>
+          <t>Kalyaninagar</t>
+        </is>
+      </c>
+      <c r="G1407" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1407" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1407" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1407" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" s="1" t="inlineStr">
+        <is>
+          <t>A52100019419</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Amol Suresh Mavle</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>A52100019419</t>
+        </is>
+      </c>
+      <c r="D1408" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1au7QQl9pRbDiOVpXkq1bhwivpHLHJ0Pv47x0nKRmDly9jKN%2fXC4ZxDbtaxP5r%2fn7RyUee%2bBm0z9uAAtsWh61Lfn%2bXC0dXnx3g1Vt7lmWIxbPs3b4m%2bukkl98A38geMTHJX%2fTj04SEWYDOx89RpPuwavAopuav2bDfh40rYT5ucwgD0qaG%2b%2ftw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1408" t="inlineStr">
+        <is>
+          <t>09158556655</t>
+        </is>
+      </c>
+      <c r="F1408" t="inlineStr">
+        <is>
+          <t>Swargate</t>
+        </is>
+      </c>
+      <c r="G1408" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1408" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1408" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1408" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" s="1" t="inlineStr">
+        <is>
+          <t>A52100019324</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Amit Madanlal Dhadiwal</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>A52100019324</t>
+        </is>
+      </c>
+      <c r="D1409" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=DpcFqZw%2bjBfF6ecY0qXEVJtUfFStPwteAwK7BB6wf2KifhfCNLjca5Q68TQpHyR6thaQtNQjtTd9sa9B3%2ft%2fnjNTM2wnbxC5GFCguuS2DvvFzu9kyXXYi%2ffUeXhDntnYWDg5MJO4FeSOfQWJRFfvmEcxTih%2bPrFwl2IRLost5sC3anV9c%2f4rwg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1409" t="inlineStr">
+        <is>
+          <t>02025670030</t>
+        </is>
+      </c>
+      <c r="F1409" t="inlineStr">
+        <is>
+          <t>Shivaji Nagar</t>
+        </is>
+      </c>
+      <c r="G1409" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1409" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1409" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1409" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" s="1" t="inlineStr">
+        <is>
+          <t>A52100019330</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Ramsharan Madho Mandal</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>A52100019330</t>
+        </is>
+      </c>
+      <c r="D1410" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Nhl8XefS1dv%2bCdv9kN4KT19lIMH61StrGsLUqRw2cNhPu%2bqysqLwhYYJYIBWWzZltpx8LB7FenxA8gmeU79WnFf5rq08JtZaSRmgvvCnSPmr%2fv2X5xxiBMnjkhQs0R%2f3%2bR60z1zYnVC%2fSZrDplqVpf7DY%2bNkFf1X9WfxlVpFAH%2byvTRRMU1KLQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1410" t="inlineStr">
+        <is>
+          <t>02027032242</t>
+        </is>
+      </c>
+      <c r="F1410" t="inlineStr">
+        <is>
+          <t>Wadgoansheri</t>
+        </is>
+      </c>
+      <c r="G1410" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1410" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1410" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1410" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" s="1" t="inlineStr">
+        <is>
+          <t>A52100002436</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Amit  Bhutani</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>A52100002436</t>
+        </is>
+      </c>
+      <c r="D1411" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2UBZDwCjv30VaALd5G3cAMovyaPV3a132iN5yI9W02fE79cXKpkNR%2bxaXBEnfUI3tDw93IrHxHOFWbvoLDhxH2y4xWJceeM0aoXjJ3zgkgb39552UOVMnoBa7RtbhJiRfGYesmrmud51isY79HPiWShtu%2b9FoyE5Zumr6oMUNqYh0iaibYkpXg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1411" t="inlineStr">
+        <is>
+          <t>02026684634</t>
+        </is>
+      </c>
+      <c r="F1411" t="inlineStr">
+        <is>
+          <t>Koregaon Park</t>
+        </is>
+      </c>
+      <c r="G1411" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1411" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1411" t="inlineStr">
+        <is>
+          <t>Keshavnagar-Mundwa</t>
+        </is>
+      </c>
+      <c r="J1411" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" s="1" t="inlineStr">
+        <is>
+          <t>A52100019444</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Chetana Dilip Dhobale</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>A52100019444</t>
+        </is>
+      </c>
+      <c r="D1412" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=p3Bk8mJfaQazR4oFsBeqJC56ODzXjE4VAm707KsvdnNXQTxiGQ9HMLEtD%2buqyyh9BNauXsm0YvFR6Q1VBPxGDKJTp0Bw16CBgkmqPskO3LALdFVBpwNeY%2fPKMPvFOJPgVcc%2bGS8uorqTe04KL2eGEmWU8nOvZK5pSY8o%2fkAoC6uDQn%2fizv7kbg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1412" t="inlineStr">
+        <is>
+          <t>02025460993</t>
+        </is>
+      </c>
+      <c r="F1412" t="inlineStr">
+        <is>
+          <t>Karve Nagar</t>
+        </is>
+      </c>
+      <c r="G1412" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1412" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1412" t="inlineStr">
+        <is>
+          <t>Karve Nagar</t>
+        </is>
+      </c>
+      <c r="J1412" t="inlineStr">
+        <is>
+          <t>411052</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" s="1" t="inlineStr">
+        <is>
+          <t>A52100004139</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Jn Realtors And Property Managers</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>A52100004139</t>
+        </is>
+      </c>
+      <c r="D1413" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=GHCLIxGHCe1HA39omWm65Ce3qSvfa1AU9%2bwUCFgBu4KFjLEwlxQtZPAOpd8hIxn%2fIiiL6aT0Av2Xok954jP96CHgDmj0yKKxcsclju%2bz%2fw233JOfnJbbIPxYQWCsbboGRF5Ug2%2fujR4ktttDx8qEw6jwcVMSNhVJqxf3%2bjyMvIM%3d</t>
+        </is>
+      </c>
+      <c r="E1413" t="inlineStr">
+        <is>
+          <t>20919049001</t>
+        </is>
+      </c>
+      <c r="F1413" t="inlineStr">
+        <is>
+          <t>Kalyani Nagar</t>
+        </is>
+      </c>
+      <c r="G1413" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1413" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1413" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1413" t="inlineStr">
+        <is>
+          <t>411006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" s="1" t="inlineStr">
+        <is>
+          <t>A52100019406</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Anita Vijaykumar Agarwal</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>A52100019406</t>
+        </is>
+      </c>
+      <c r="D1414" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wcqy5uYtYJiJOH3SDRDPX27QCx87DkUKexHADf8DRe2hvLJaiXbVQRvQ3F1VqwE8BhNsFlw9dJHuAhsk3n2pWzxXg16pUwMHVVvdNQqVeRknHsxIde%2bLCMcBWxyREK2%2bxEC44%2beg8tT5Kd%2bmQad1be9uXq8ZDhIvWgERTva2lmJZAJbPvShGJg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1414" t="inlineStr">
+        <is>
+          <t>09823410411</t>
+        </is>
+      </c>
+      <c r="F1414" t="inlineStr">
+        <is>
+          <t>Nigdi Pradhkaran</t>
+        </is>
+      </c>
+      <c r="G1414" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1414" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1414" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1414" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" s="1" t="inlineStr">
+        <is>
+          <t>A52100019361</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Coconut Estates Llp</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>A52100019361</t>
+        </is>
+      </c>
+      <c r="D1415" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ptTLHXUdnWYEp5vtNId10UekAoS1XwHg%2fGwIrVP7Cp0bdsfgE4SpkQQTwx4Apr249JYXCnaM4biQw7kJd5gnMDvcVjYK2gYUDQSzx1pQNwNsIM1IhB%2fbfPLfHNuOrXV0LOOM%2bEryVAj5BM6fJaHESucA%2bmVvB4DQNeVzcEsuc18E1tnhlzqtIg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1415" t="inlineStr">
+        <is>
+          <t>06262620606</t>
+        </is>
+      </c>
+      <c r="F1415" t="inlineStr">
+        <is>
+          <t>Kothrud</t>
+        </is>
+      </c>
+      <c r="G1415" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1415" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1415" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1415" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" s="1" t="inlineStr">
+        <is>
+          <t>A52100019388</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Lalit Dudaram Choudhary</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>A52100019388</t>
+        </is>
+      </c>
+      <c r="D1416" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2faThpv%2fidQX5KqihEjWHEnSGlRi3DB4uD1kiV32XgM4ASoyLrg7gIgExxBSXdekVSM1GHkx5a5RYf4KpB85f9TIiiXlcw2MNGgeKcGT0PNv%2bS4gTYqMTLHMLUGIIDo7UFcJNBrk2CJGdL26P1xvyf9XJzz2dLNwV9X8HNeWSk2M%2fq1HcRNefVg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1416" t="inlineStr">
+        <is>
+          <t>08149948608</t>
+        </is>
+      </c>
+      <c r="F1416" t="inlineStr">
+        <is>
+          <t>Bavdhan</t>
+        </is>
+      </c>
+      <c r="G1416" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1416" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1416" t="inlineStr">
+        <is>
+          <t>Bavadhan Bk</t>
+        </is>
+      </c>
+      <c r="J1416" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" s="1" t="inlineStr">
+        <is>
+          <t>A52100019442</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Dharmendra  Kumar</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>A52100019442</t>
+        </is>
+      </c>
+      <c r="D1417" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=EU8t8lVbIcSf9yb%2fpROhAZi1O1VHEZpL15GQTSZdMhU%2bOiHNOLFyUG7frLaTZQG286rsSUMtHpkIAv0RSpsbRcLRvg6Y9DjwnPd8f%2fAs2b2wodrCed5x99OZsg9astiTsLQP%2fbK4dkXvdWpf7d4283m%2fDeWdpAhv2CEezTvopy335SZKjK%2fUzA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1417" t="inlineStr">
+        <is>
+          <t>02067588085</t>
+        </is>
+      </c>
+      <c r="F1417" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="G1417" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1417" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1417" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J1417" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" s="1" t="inlineStr">
+        <is>
+          <t>A52100019356</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Akash Vijaykumar Agarwal</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>A52100019356</t>
+        </is>
+      </c>
+      <c r="D1418" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=f2Yqg6d3Ylvz1mzszIF1s%2bl%2b3Rx3%2bBWw5Sm%2bbKSaviznkFfIMCzBMotQzsm1juOdT9lf9TzqZg9xIkxIMg0Z6vt0cnqHxxPA6pVGQ4edrhQcVy38FOiXxyz%2b9YgzLyz5F61GI4qLN93MQJH11s0Vn663VguQm1ZWW68Yao7LLuegjIGgs%2brFeQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1418" t="inlineStr">
+        <is>
+          <t>09823410411</t>
+        </is>
+      </c>
+      <c r="F1418" t="inlineStr">
+        <is>
+          <t>Nigdi Pradhikaran</t>
+        </is>
+      </c>
+      <c r="G1418" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1418" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1418" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1418" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" s="1" t="inlineStr">
+        <is>
+          <t>A52100019385</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Sundeep Prem Sahijwani</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>A52100019385</t>
+        </is>
+      </c>
+      <c r="D1419" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=z8%2f9WVOTXH6wRl%2f5TuGOVtpXjJ5pPAH5TQn0gKDMlKLYrPtKqHGquD3B5nldqIBWfkIqHZgHG%2flDauRvmGvD0z%2fnV%2fOSSjUxm%2bqsjeu46TUb23KmfdkC0utDTpOppEriq5C8DqYLVc9uQPg3%2fI%2fq4DMqt%2bKRmLlPv9jV2dv1DLfkTYezyMmvPA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1419" t="inlineStr">
+        <is>
+          <t>02041229929</t>
+        </is>
+      </c>
+      <c r="F1419" t="inlineStr">
+        <is>
+          <t>Wanorie</t>
+        </is>
+      </c>
+      <c r="G1419" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1419" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1419" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1419" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" s="1" t="inlineStr">
+        <is>
+          <t>A52100019438</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Suman  Chandra</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>A52100019438</t>
+        </is>
+      </c>
+      <c r="D1420" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=14cydnJC%2fCfBvmAH3eblQdRQUo6eFzWFnnCPb0mF1Xm75omibv8kpLaaqRm%2bYAPQDnhSDvCBwGE8kM6YZEVj5WctLZDAkU14AupdZY9tmgKLoTt8EJV0TWejMC2IMQI%2f6QDq0FifZsfm9vsVqDHgyuRMjGpckKpwfr0bYv%2bAFNuKYIlLFJb3ag%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1420" t="inlineStr">
+        <is>
+          <t>02065106570</t>
+        </is>
+      </c>
+      <c r="F1420" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G1420" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1420" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1420" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1420" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" s="1" t="inlineStr">
+        <is>
+          <t>A52100019580</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Vaibhav Narayan Phadtare</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>A52100019580</t>
+        </is>
+      </c>
+      <c r="D1421" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=FnAE1HaBJANu9Gkn0bY6wtalRITSdqvFJuSeW2WLFVHehg9wscxWcg%2bwOv7uMKIbtvsi2q5LO5fRgqSyXU%2bk86KjlKcPbBZFCj%2fvreDVrZGWL87qhmWcQ7e%2fttyXXQJtOxPF3AU%2fQNZY1Wx5xEANr5p0xSvdS0wY6awysjgaDRq5gVH8AIzUaQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1421" t="inlineStr">
+        <is>
+          <t>02373272293</t>
+        </is>
+      </c>
+      <c r="F1421" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="G1421" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1421" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1421" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="J1421" t="inlineStr">
+        <is>
+          <t>411018</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" s="1" t="inlineStr">
+        <is>
+          <t>A52100019428</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>K Surendra Alias Sunny Nayar</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>A52100019428</t>
+        </is>
+      </c>
+      <c r="D1422" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=RmKcF87A7tT63I8vba8%2bQysjsjBMDwggEGc%2fQWRc8Xg5cHiZZbS5RhQeDx4wHVGVWIdKsOMuYV4AfYg9wcBj9E%2fQVCP5QOtKsE6waza2tQcEUFZRnOIaBBwJSwd1vqwyaeFRkJjpw6Ny4Z6OCqq%2b944W9BVRQnA2ogBu4jr%2fLleKzRVSWThR6w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1422" t="inlineStr">
+        <is>
+          <t>02240035105</t>
+        </is>
+      </c>
+      <c r="F1422" t="inlineStr">
+        <is>
+          <t>Hadapsar Pune</t>
+        </is>
+      </c>
+      <c r="G1422" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1422" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1422" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1422" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" s="1" t="inlineStr">
+        <is>
+          <t>A52100019461</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Vicky Rameshlal Advani</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>A52100019461</t>
+        </is>
+      </c>
+      <c r="D1423" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=VZKBK%2bsN%2b0hCQEzkh9GyjpSKACK2t0FIaHcCz%2fxMYKn2sjnYJ%2fA1%2fKCVeCFc6xmzJ9nUwPFlgVyv9qa%2bGaZ0So58nqiyiX70Bc1GVZQvQ4aoNZ7EQjFwd3majjL%2faxKAoi73r5z9MnespB%2fLoCfxWVcHxuKLxhjQAQzmv0nteGxb%2bCb50hc0%2fg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1423" t="inlineStr">
+        <is>
+          <t>07744909443</t>
+        </is>
+      </c>
+      <c r="F1423" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G1423" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1423" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1423" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1423" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" s="1" t="inlineStr">
+        <is>
+          <t>A52100019378</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Rajendra Prabhakar Kothawade</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>A52100019378</t>
+        </is>
+      </c>
+      <c r="D1424" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=G3m2l9%2fpRsezQ8qh5AQmvlRyHRZg0IinioAJMoJFPbQ%2bKr4BKXGA9vmiCZHnf4HtczhrJTjXGfbvrX6cEq0rUs9eivpi%2fS6HOpD1X1vh1A4%2bwP47OzJEHtdCixl5Dbeyc4Z6%2b3f6%2fpDljdHz%2fwryJBSCv55WR4opgfKecJ1ugI69nHB%2bjNyaSg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1424" t="inlineStr">
+        <is>
+          <t>09175559555</t>
+        </is>
+      </c>
+      <c r="F1424" t="inlineStr">
+        <is>
+          <t>Vardayani Society</t>
+        </is>
+      </c>
+      <c r="G1424" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1424" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1424" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1424" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" s="1" t="inlineStr">
+        <is>
+          <t>A52100019425</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Sachin Nandkishor Parakhi</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>A52100019425</t>
+        </is>
+      </c>
+      <c r="D1425" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Dpw2sMWM5u8Fyl9WgB3JZC7LVmG6IstoeMgSen%2fd6VyS%2bO%2bVpImImBFAl0luQ%2fraLm%2f2%2bZRakJwI6xFLA9Jq17YEn9u8W8B4iFRuhP4IeCVwMM%2bzdjWxLmYOkdrkOzLOfzKgoGf7tWcP9qYYub9VC6Ub1d6CpEU%2bAwq7HaRlbofTisog7e3lJg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1425" t="inlineStr">
+        <is>
+          <t>91895679991</t>
+        </is>
+      </c>
+      <c r="F1425" t="inlineStr">
+        <is>
+          <t>Sus</t>
+        </is>
+      </c>
+      <c r="G1425" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1425" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1425" t="inlineStr">
+        <is>
+          <t>Sus</t>
+        </is>
+      </c>
+      <c r="J1425" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" s="1" t="inlineStr">
+        <is>
+          <t>A52100019649</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Kaustubh  Sarda</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>A52100019649</t>
+        </is>
+      </c>
+      <c r="D1426" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=sHFLeAdF%2fNaPh81NRtu%2b2XNv%2f6WuYIp7aCZzTs2S3b6KDmPoimkr7s3YzLAzlzjRWZEJWvZqy8H05uzDsN3sxT40EUhbQxk%2biaSv9g53JF1n%2f3l2IU%2bSxavaIeVhhUFaA1Ww8Zf74Kc0G60tlfttV2ehoZWcnjUu%2fHi1Z2wevdWzIoF2DxjmHw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1426" t="inlineStr">
+        <is>
+          <t>07798311188</t>
+        </is>
+      </c>
+      <c r="F1426" t="inlineStr">
+        <is>
+          <t>Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="G1426" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1426" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1426" t="inlineStr">
+        <is>
+          <t>Pimpale Saudagar</t>
+        </is>
+      </c>
+      <c r="J1426" t="inlineStr">
+        <is>
+          <t>411027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" s="1" t="inlineStr">
+        <is>
+          <t>A52100019499</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Abir  Kaushik</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>A52100019499</t>
+        </is>
+      </c>
+      <c r="D1427" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=xJZx8GFPIBWqd9%2f64usN3XSvVigu58LYi0BJmJsLgYWu8AkiDBwYtNwkrhsVwDbeGHsy8puzhrpa3LXadkAmYS3eYZvltzIeskMsiHVl4CJ9Cx5GyATZF9iCQaJs0vgrTbTQBpdCgfAgB4GQLIdwQWVdddAM6qtRg2YaxW5NTJFnyBApj6F5Wg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1427" t="inlineStr">
+        <is>
+          <t>09892678292</t>
+        </is>
+      </c>
+      <c r="F1427" t="inlineStr">
+        <is>
+          <t>Wadgaon Sheri</t>
+        </is>
+      </c>
+      <c r="G1427" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1427" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1427" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1427" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" s="1" t="inlineStr">
+        <is>
+          <t>A52100020363</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Sayyad Abdul Rehman Bahoddin Quadri</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>A52100020363</t>
+        </is>
+      </c>
+      <c r="D1428" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=x3jo0%2fqK6isvSQ4QFmM%2f0mIpZMCpmdrGlxTdKVBQvMi1rcSGuI1mutB%2f7lA8E%2f5BRsM2rSgVXS2dT18WCEL8y2AjOJQQL5taH%2b7iC1S63%2b23viTCz9cfRg8HarlDaSOTwAKDJ2xGnYRMUr68FGJ5JkIPPGnqJzMZopikU8D8%2b9ld3mDdDKG9EQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1428" t="inlineStr">
+        <is>
+          <t>09921981591</t>
+        </is>
+      </c>
+      <c r="F1428" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1428" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1428" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1428" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1428" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" s="1" t="inlineStr">
+        <is>
+          <t>A52100019462</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Vikrant Suresh Shinde</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>A52100019462</t>
+        </is>
+      </c>
+      <c r="D1429" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=yvQ5NfPFQ15ahU3TrbqzmL3MIKHprHCCJXkrxhnqgyI%2bgcFxGkVRNk28qXXissMGQAs2T3npsBDuuNAMpjn1xIklAR6pM9hNW2uzW7rD98aqqQN1T53izrSDQAU4pxILjWrveku1Iwoc7mT20fpuLbdCinwQOh%2b78vsttLLbFoMJrhnspvOZjA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1429" t="inlineStr">
+        <is>
+          <t>02027393151</t>
+        </is>
+      </c>
+      <c r="F1429" t="inlineStr">
+        <is>
+          <t>Baner Annex,Mhalunge</t>
+        </is>
+      </c>
+      <c r="G1429" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1429" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1429" t="inlineStr">
+        <is>
+          <t>Mahalunge</t>
+        </is>
+      </c>
+      <c r="J1429" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" s="1" t="inlineStr">
+        <is>
+          <t>A52100019640</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Mubashshir Kabir Syed</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>A52100019640</t>
+        </is>
+      </c>
+      <c r="D1430" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Pn5Ucd%2bla5BKdu3FQApBZ9AK0YmmsYK55D%2f%2fX9ZvD3d4eHZXaSFfETU%2bOjL1IsRbdc2xED3yD2Bdd%2b4JHtQKVKcdJ%2bVARVQncDUGU63pBSBx68lQm%2bUZq7MgcSwIQEPfWN1QwpYs7Lw0l%2fbXAwyRbM26v3j%2f2XLDzYYBqHbZ9X%2f1rbCDiw%2b5xw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1430" t="inlineStr">
+        <is>
+          <t>02064642229</t>
+        </is>
+      </c>
+      <c r="F1430" t="inlineStr">
+        <is>
+          <t>Kondwa Khrud</t>
+        </is>
+      </c>
+      <c r="G1430" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1430" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1430" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1430" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" s="1" t="inlineStr">
+        <is>
+          <t>A52100019478</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Hitendra Rashmikant Sheth</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>A52100019478</t>
+        </is>
+      </c>
+      <c r="D1431" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=7VIPzmQVzwjDOxY3THhSalShPdtWg%2bWRvdYI93%2f4ra6sLNwPGuWBVavSL5TcO2232udTShodwko7s7dEGyl6T1u2CxdLZxgukdFvBDiECH561X2%2bIx4i3bVlMug5InU%2bLpzZ80ClBxtc4pwX4AUywdjGcJw8DyR5aBL%2bWEOa74wqhjpSHp%2f0Hg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1431" t="inlineStr">
+        <is>
+          <t>02024328521</t>
+        </is>
+      </c>
+      <c r="F1431" t="inlineStr">
+        <is>
+          <t>Sr. No. 253</t>
+        </is>
+      </c>
+      <c r="G1431" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1431" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1431" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1431" t="inlineStr">
+        <is>
+          <t>411032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" s="1" t="inlineStr">
+        <is>
+          <t>A52100019495</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Sunil Jatiram Gogaliya</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>A52100019495</t>
+        </is>
+      </c>
+      <c r="D1432" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=nueWNbivSahnoKty%2fc2Qi1YIMFsRuHjhyZ3oJwb822x5lbQr2uEu459tLoTICr%2boJSL7pqjUSS8%2bZZMmnxqKfmDXk9%2fcAsxdQ%2bGAxZvkWjE6XsMzEHl7HsagRD%2fDkWA2I1FWNssb8ehk%2bp%2bqCQlp63fJ7T6bLFnxkplm151yzmuiJmfJt3vowg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1432" t="inlineStr">
+        <is>
+          <t>20202448576</t>
+        </is>
+      </c>
+      <c r="F1432" t="inlineStr">
+        <is>
+          <t>Pisoli</t>
+        </is>
+      </c>
+      <c r="G1432" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1432" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1432" t="inlineStr">
+        <is>
+          <t>Pisoli</t>
+        </is>
+      </c>
+      <c r="J1432" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" s="1" t="inlineStr">
+        <is>
+          <t>A52100019597</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Sonia  Sadhotra</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>A52100019597</t>
+        </is>
+      </c>
+      <c r="D1433" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=a5jkLWsESSpLv6gTmh8j%2fq8yHEO0PQT4rj5cwGzfTySpYmHqgkvXlrt6m0wY6BHYddDmgHhWuOT0GiolKrSzH69Au5Tw1ssc9f%2f%2fQdWcRXBeT%2blinh0GPqEUmonXIVfZVrR00%2fwxSOWQknq%2fMGMc%2frbWbrd76HD%2bokwNvsiK5HgyBIY7bvXF0g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1433" t="inlineStr">
+        <is>
+          <t>02026804592</t>
+        </is>
+      </c>
+      <c r="F1433" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="G1433" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1433" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1433" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="J1433" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" s="1" t="inlineStr">
+        <is>
+          <t>A52100019524</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Estansa Realty Consulting Private Limited</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>A52100019524</t>
+        </is>
+      </c>
+      <c r="D1434" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=oJvUX8RS4wc6GNDjcdkgbfkT%2b2dxmNtYCmBMsipnFoP3P6sVcRRwsqmaOgff6B3%2foUXDJn17ypwKP09a6pB1tnlpAQfbGYgDEWnBC3mWcnI%2bT3%2b%2bcbHPmGgPNdpzLvoJsM58%2bc1LzIQRwsqjRxj3pxf12Ez3PZy0ZRhcokR5iSSMz6zux7j%2fEg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1434" t="inlineStr">
+        <is>
+          <t>02026050500</t>
+        </is>
+      </c>
+      <c r="F1434" t="inlineStr">
+        <is>
+          <t>Mangalwar Peth</t>
+        </is>
+      </c>
+      <c r="G1434" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1434" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1434" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1434" t="inlineStr">
+        <is>
+          <t>411011</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" s="1" t="inlineStr">
+        <is>
+          <t>A52100019541</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Nikhil Dnyaneshvar Vavle</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>A52100019541</t>
+        </is>
+      </c>
+      <c r="D1435" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Smp6NW7tYKZdsSlMhEbu2%2fzD93gBrM4AtdFlcLAgYVU0RK9wkIDCS7WJDviGEuLHckbRnhWRSom%2fnWPBjsLHQvmnP4wXapgYXeASeMfhsTxMY%2bwswXiaD%2fWaBEOqMN%2fPRG3MTMwuc8f4XqFuabpyaC%2fOYRndfG4K9uKkoh2Ck8RERqGfJkEm2Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1435" t="inlineStr">
+        <is>
+          <t>02025870145</t>
+        </is>
+      </c>
+      <c r="F1435" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G1435" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1435" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1435" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1435" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" s="1" t="inlineStr">
+        <is>
+          <t>A52100019533</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Ashish  Mestry</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>A52100019533</t>
+        </is>
+      </c>
+      <c r="D1436" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=U9FdBK3LbSWSj7sqJiJiSUy3r2BLBCTpqAD%2fJpoWY%2fT8Re9kKZD7qGf44ZRbsYifD7ZwU%2bWkIDqlR56rZc%2bfb%2bO29TLCChYNBMdOPGYbnR%2bIfLs7qFEciOS562k9k0MydMb7nHL2gDLwFhncK8N0%2bjbuS%2b4bP5jpJGvfStjl1YAQfiWFFL5OIw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1436" t="inlineStr">
+        <is>
+          <t>02046302146</t>
+        </is>
+      </c>
+      <c r="F1436" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="G1436" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1436" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1436" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1436" t="inlineStr">
+        <is>
+          <t>411018</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" s="1" t="inlineStr">
+        <is>
+          <t>A52100019606</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Moreshwar Tatyaba Andhale</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>A52100019606</t>
+        </is>
+      </c>
+      <c r="D1437" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3lB7QnMWdSzD2hxAtCjCPg9Ytx2b7o8TZABenbyVgjZt40ljrv5aAWunC6xbnxA05o94qp1Ozk0Z%2fOhhO7KcSZSW9Ewscb5GKeeVKkWVhyKEnRptG%2ffLFQ8I7oTcXLzF4ARH7iDjppQE%2bDo36lJFYQ4hytEkMLgvsgCG84rGP3JR0nO9TFXusg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1437" t="inlineStr">
+        <is>
+          <t>09923746310</t>
+        </is>
+      </c>
+      <c r="F1437" t="inlineStr">
+        <is>
+          <t>Pisoli</t>
+        </is>
+      </c>
+      <c r="G1437" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1437" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1437" t="inlineStr">
+        <is>
+          <t>Pisoli</t>
+        </is>
+      </c>
+      <c r="J1437" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" s="1" t="inlineStr">
+        <is>
+          <t>A52100019563</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Sagar Anand Kulkarni</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>A52100019563</t>
+        </is>
+      </c>
+      <c r="D1438" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=i2N9L%2fsuAVHy2crfKq4JYJHjujAn8gsqiwq1MzlljNjjS5agc0AoW8PTjKaEu5rbiyHBAS3orNPlCwJoI%2bofqmgF48kdOAgr1wd4AI9Ka%2bIxrYigdqEFVADg%2fOECHyvJa5q0BmdogrsoGtRvD8rojYk66zpGCfNMSEDvNxGQLjBngKMiW7k3cg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1438" t="inlineStr">
+        <is>
+          <t>08087710419</t>
+        </is>
+      </c>
+      <c r="F1438" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="G1438" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1438" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1438" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="J1438" t="inlineStr">
+        <is>
+          <t>411043</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" s="1" t="inlineStr">
+        <is>
+          <t>A52100019559</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Rahul Shantilal Mutha</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>A52100019559</t>
+        </is>
+      </c>
+      <c r="D1439" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=g9EnvqHV3wnDqMRzGwFGX9ozvIBtQatYyUpbApSOtOdxG%2fnNkmYnHls1UtEV%2bI7v709Z4LqwhxWzm0oJflJCRkCr1SHLqV7HKBZfPXPEr32Uc%2fhRoJ28EsAgHzOlIIY5eV2fOeqEPPGJNEiKw%2byPaY%2f0aLSH6EvHOEYW92Lgrm%2bircf7TfTxSg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1439" t="inlineStr">
+        <is>
+          <t>02024222451</t>
+        </is>
+      </c>
+      <c r="F1439" t="inlineStr">
+        <is>
+          <t>Parvati</t>
+        </is>
+      </c>
+      <c r="G1439" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1439" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1439" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1439" t="inlineStr">
+        <is>
+          <t>411009</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" s="1" t="inlineStr">
+        <is>
+          <t>A52100019566</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Shweta Vishal Shah</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>A52100019566</t>
+        </is>
+      </c>
+      <c r="D1440" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KskH4gZJT61iLzZNWBdiJBzpJoAXGG%2f4QLgPicfhTL%2b2zXI6%2b4f2fsU5AvXDw4wZ5uW0rqRGfuAD4ujVcyGeKg79F6R9vB7JACQVwgwR4IUzlgS4ePYpS6jfkTLpc1vDr61Chtc5nJlmYmzFnlyf9WGcrt044gWOw1%2fGzM9MHFx9aVql54fkVw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1440" t="inlineStr">
+        <is>
+          <t>02041206680</t>
+        </is>
+      </c>
+      <c r="F1440" t="inlineStr">
+        <is>
+          <t>Rambaug Colony</t>
+        </is>
+      </c>
+      <c r="G1440" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1440" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1440" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1440" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" s="1" t="inlineStr">
+        <is>
+          <t>A52100019748</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Gm&amp;J Consultants</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>A52100019748</t>
+        </is>
+      </c>
+      <c r="D1441" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Qa5zzKVKOiN4jQk%2frvy7Tt2f9Bh45l%2f8UXIhdPfeIuU4RnURF9XC%2f5llUMXi2g7p6CRS%2bSESORDdfbQhww93XiT%2bclOmEAU4UFgU2L5vgV57qsyiuhwFYJimTS1cNo9Pn904Fho%2bIG2bErQ0IOp93yrSQ8lAfwZfGZ86IxOk78Xnuhra4I9uiQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1441" t="inlineStr">
+        <is>
+          <t>91976307844</t>
+        </is>
+      </c>
+      <c r="F1441" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1441" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1441" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1441" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1441" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" s="1" t="inlineStr">
+        <is>
+          <t>A52100019642</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Sharad Baban Khalse</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>A52100019642</t>
+        </is>
+      </c>
+      <c r="D1442" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=n8DLZ4NQG9Ee7kF8o4x2EiRint2V9fCjr%2bCaviJQIU5QyK1ZnmRGHbnisHNFUNfcrOBP4Sfcm%2fwqr5ACaV%2bwN%2f7xYexFRiuBxg5VmKeTBiKku4aa3bQqG3imyUObgGntJ1dlTe7cyuy11jAfCTDVCf7LSI6YucUO4S%2bSd%2fvUV9%2fQ7TlngUuJfg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1442" t="inlineStr">
+        <is>
+          <t>08149444359</t>
+        </is>
+      </c>
+      <c r="F1442" t="inlineStr">
+        <is>
+          <t>Dhanorigaon</t>
+        </is>
+      </c>
+      <c r="G1442" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1442" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1442" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J1442" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" s="1" t="inlineStr">
+        <is>
+          <t>A52100019638</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Bhagwandas Laxmandas Gujarathi</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>A52100019638</t>
+        </is>
+      </c>
+      <c r="D1443" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=37r3JldLH1vOzpSMBf4G%2f67nrLeGu%2bj6R%2f%2b7g7uuUiy%2bIXqReITppznFb7hVGpaWfrlMv3h0WQ%2b0WeGwHy8Pj7eHJUPX7U6zbVhEOguNC1UPJy%2bNqm6Wjl1b41377ukHSYtrazdShIOgKVjnRWpjX3HF%2bcgK0o6Id21rLYBFGdfkKip0wueboA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1443" t="inlineStr">
+        <is>
+          <t>09422083479</t>
+        </is>
+      </c>
+      <c r="F1443" t="inlineStr">
+        <is>
+          <t>Bibwewadi</t>
+        </is>
+      </c>
+      <c r="G1443" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1443" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1443" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1443" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" s="1" t="inlineStr">
+        <is>
+          <t>A52100019747</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Pooja Vijay Marwadi</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>A52100019747</t>
+        </is>
+      </c>
+      <c r="D1444" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=XPpNwhqS0pHceMOXw5oWHUWyaY5EQ89HOgg5RcrTezeXnuWq4DdRtrDRYW2Ee8LlQ%2b0Xa01EJyohUd2ODQYP9XscEltD%2bky7Xcv%2fyfZuUvL1jxEsMBJ%2fIHrfpxzxSgQTch2WRPH6ZnIfeXkmLN1HU5UsNCUB4vo%2beGpO08%2fVeICkiQIWJjs%2fKw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1444" t="inlineStr">
+        <is>
+          <t>02095115881</t>
+        </is>
+      </c>
+      <c r="F1444" t="inlineStr">
+        <is>
+          <t>Gokhalenagar</t>
+        </is>
+      </c>
+      <c r="G1444" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1444" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1444" t="inlineStr">
+        <is>
+          <t>Ramoshiwadi</t>
+        </is>
+      </c>
+      <c r="J1444" t="inlineStr">
+        <is>
+          <t>411016</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" s="1" t="inlineStr">
+        <is>
+          <t>A52100020149</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Madhura Anand Kulkarni</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>A52100020149</t>
+        </is>
+      </c>
+      <c r="D1445" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=0X1pABLh%2fA6yx8AWsqWUlNYdjxBECXPTWb4FlWGeGVYFQ%2fWHXv968GG8x6BFrgSilr%2bNkBXwz8r62R3LSYT%2bTaIUOY0VMOW%2b5G%2b2WdeZ741X3tD3f9MzKpDWzNLYkQW2KvWm43LMSsLA0iX4ZfgrAKdcANuctVmKPeBcbzneHPJ%2bnm7VNPDUgQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1445" t="inlineStr">
+        <is>
+          <t>09920390480</t>
+        </is>
+      </c>
+      <c r="F1445" t="inlineStr">
+        <is>
+          <t>Ravet</t>
+        </is>
+      </c>
+      <c r="G1445" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1445" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I1445" t="inlineStr">
+        <is>
+          <t>Kivale</t>
+        </is>
+      </c>
+      <c r="J1445" t="inlineStr">
+        <is>
+          <t>412101</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" s="1" t="inlineStr">
+        <is>
+          <t>A52100019612</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Debabrata  Behera</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>A52100019612</t>
+        </is>
+      </c>
+      <c r="D1446" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=E8VgHDDRkTjj5lKrGKLGhCI48LjjQI5DfxxSELSP7PfKTp8xt5NVb73AlB0AzksGeWbORw3VU4i7EQlJsXvgBU8ZByFNkKb%2fi1EXpyMJ5wgJXC4hYu7K6u36gV034m2fDs9zsUt%2bn6XMvrdVz0oot91MKuqRikR488kk6fNVI57NL%2bU%2fAWTnnQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1446" t="inlineStr">
+        <is>
+          <t>09096208880</t>
+        </is>
+      </c>
+      <c r="F1446" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1446" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1446" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1446" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1446" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" s="1" t="inlineStr">
+        <is>
+          <t>A52100020047</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Sanket Sanjay Kisar</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>A52100020047</t>
+        </is>
+      </c>
+      <c r="D1447" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=pTjjIVgkfnkpN5aVUxSbyvYRkgErXPXQILZEiypMlr%2fdgFD1%2b22EwqwpSaG85xRC%2fvBX%2fioWZDLi4DTRnX3rhJNN9RcahlVBA3hc3IHYH7rth9GXZvSsc2wGPYhTxJBfHVFVofAzmVZUSm8QyS0tUX8LRIFpDCgPNtY048da08Gzc%2fcmyhh6sA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1447" t="inlineStr">
+        <is>
+          <t>09552230586</t>
+        </is>
+      </c>
+      <c r="F1447" t="inlineStr">
+        <is>
+          <t>Kaspate Wasti, Wakad</t>
+        </is>
+      </c>
+      <c r="G1447" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1447" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1447" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1447" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" s="1" t="inlineStr">
+        <is>
+          <t>A52100019579</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Kunda Anil Tamboli Proprietor Of Eagle Homes Realty</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>A52100019579</t>
+        </is>
+      </c>
+      <c r="D1448" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=fkiXeDAjEOX5v%2bMX8jiPoMhePCzs9DQj87icMgX0yNkysUxXd28hQOxsvv94E4kXl4mhM01KtXrm1lYQfSjMcBhOhh%2fBKASMp4iuaUUd2Zh2ZLrzq0aeQ7NyG%2f4gWngMi7VMWlDeKZQeePI1sgO620XSx3ZyCC%2f3hNiMLBNLViv2oLY4pz7zfA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1448" t="inlineStr">
+        <is>
+          <t>09960420259</t>
+        </is>
+      </c>
+      <c r="F1448" t="inlineStr">
+        <is>
+          <t>Shirur</t>
+        </is>
+      </c>
+      <c r="G1448" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1448" t="inlineStr">
+        <is>
+          <t>Shirur</t>
+        </is>
+      </c>
+      <c r="I1448" t="inlineStr">
+        <is>
+          <t>Shirur</t>
+        </is>
+      </c>
+      <c r="J1448" t="inlineStr">
+        <is>
+          <t>412210</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" s="1" t="inlineStr">
+        <is>
+          <t>A52100019575</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Pradeep Rabhaji Jadhav</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>A52100019575</t>
+        </is>
+      </c>
+      <c r="D1449" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2%2fSxcP3Ck9b83nsoo%2fPQ%2faOYFr%2fZu0A%2fvPHJsd6bYmcC57E%2boNQNQouU6j0z4PPk5MsnyptIqTp%2bBs2gG%2bkMUBbGoi4KprpRQ62zYcI5DZ0OyLgQBCeoagJ4oCE5v%2fNW2fJngzqat%2fTFswoFAyoZu8LIF%2fL8s2oIez8pNtAGAx6d7v1mvFtP0w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1449" t="inlineStr">
+        <is>
+          <t>09049988999</t>
+        </is>
+      </c>
+      <c r="F1449" t="inlineStr">
+        <is>
+          <t>Marunji</t>
+        </is>
+      </c>
+      <c r="G1449" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1449" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1449" t="inlineStr">
+        <is>
+          <t>Marunji</t>
+        </is>
+      </c>
+      <c r="J1449" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" s="1" t="inlineStr">
+        <is>
+          <t>A52100019621</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Priyesh Prakash Nahar</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>A52100019621</t>
+        </is>
+      </c>
+      <c r="D1450" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=VqZrqtykI6fNsz%2bnVkeb7XIiN56JmltXlnkpfxBBgoe4YJGFhP%2f05prxDPBIMeEFqybNEnYXQCkM4iOu%2fXjIljJgS%2bXKA9lI%2f%2fIOtLn5KaeNoF%2bn0H1mNVwnjEqUe%2bQ7sh9spAWvM42sZoQgOtMsPSke%2fUmzFg014ROTxC%2f1TkcO%2frdGnH%2b0tg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1450" t="inlineStr">
+        <is>
+          <t>02000000000</t>
+        </is>
+      </c>
+      <c r="F1450" t="inlineStr">
+        <is>
+          <t>Rasta Peth</t>
+        </is>
+      </c>
+      <c r="G1450" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1450" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1450" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1450" t="inlineStr">
+        <is>
+          <t>411011</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" s="1" t="inlineStr">
+        <is>
+          <t>A52100019574</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>Priyanka Santosh Lakhera</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>A52100019574</t>
+        </is>
+      </c>
+      <c r="D1451" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5fF%2bsykGD4pzu4YHL81ygaULjzaN%2f0p7CIj50nEwEYKeekHebL4fbu1Ve5nPX4HNngiUUt6SSD0tYXBgvD1vKBpeHEMQ2kXpz66h3RkisfZ6SQH9nDyBq1OB4WfDN%2brwevHNqH4lD9yN1lZOYr9a4mNPnyrvqeS4C9U9zumB8YNaB0d%2bjaeMvg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1451" t="inlineStr">
+        <is>
+          <t>02027515575</t>
+        </is>
+      </c>
+      <c r="F1451" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="G1451" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1451" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1451" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1451" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1500]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1451"/>
+  <dimension ref="A1:J1501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -75360,6 +75360,2606 @@
         </is>
       </c>
     </row>
+    <row r="1452">
+      <c r="A1452" s="1" t="inlineStr">
+        <is>
+          <t>A52100021762</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Dhanesh Somnath Salian</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>A52100021762</t>
+        </is>
+      </c>
+      <c r="D1452" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=4clNwGdgv9tjpFgFttPZtHeh6QEGYRx7TNOJtvC9ZiLSCpXwdY2Q%2bLHyttlf1AI3fGsdwi13aNBmIGYgRhPhqj%2bJmpmg7oF5BJu3Wj3l%2fQ1AW2Vbj7duu3d8paovUHhlWtG6xjooISmQ94LmfWsIbAUnYuFE0ppKAAMcIYiwldyHRjvtoEqugg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1452" t="inlineStr">
+        <is>
+          <t>09860078678</t>
+        </is>
+      </c>
+      <c r="F1452" t="inlineStr">
+        <is>
+          <t>Yamunanagar</t>
+        </is>
+      </c>
+      <c r="G1452" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1452" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1452" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1452" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" s="1" t="inlineStr">
+        <is>
+          <t>A52100003079</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Priyesh Prakash Jain</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>A52100003079</t>
+        </is>
+      </c>
+      <c r="D1453" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Y3fpJedkj5Uv2yjzaUHvbsA20Zzg%2bJyjUF4tO4mxOM%2fsgfHqU5bWIwG8nvDsS8loiJretxKIRAf9TmGkvxv65r3jujQmKN0V6bNfvLClZRW%2bXJh0WeDM2ExLwICQdhZo24IR9enSK3xV4XrALaFO%2fYs3xYRLxGRsyNpQMlSnyar16RFH8uu%2f3A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1453" t="inlineStr">
+        <is>
+          <t>02025293441</t>
+        </is>
+      </c>
+      <c r="F1453" t="inlineStr">
+        <is>
+          <t>Warje Malwadi</t>
+        </is>
+      </c>
+      <c r="G1453" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1453" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1453" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J1453" t="inlineStr">
+        <is>
+          <t>411038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" s="1" t="inlineStr">
+        <is>
+          <t>A52100019655</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Aniruddha Avinash Dukane</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>A52100019655</t>
+        </is>
+      </c>
+      <c r="D1454" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=v1Gn2WYlzY9eQDeHXPYmsFRVTOQUzuHdpYI55S0kg7XjlCleFnNprmmaw4nB8xYx7KID3H1MNhfWt66NYnhq3ta33eWz7Uq%2bCdxbO5pFqNrMdmDSKLnWHwu75ZldXMV9xsbfJohG5dBDP7m%2bjQT4rFuOnMBBZFBLSZRAkZM8zJWNW1TBYKP4Bg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1454" t="inlineStr">
+        <is>
+          <t>09604639050</t>
+        </is>
+      </c>
+      <c r="F1454" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="G1454" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1454" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1454" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="J1454" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" s="1" t="inlineStr">
+        <is>
+          <t>A52100019707</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Rohan Harish Patil</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>A52100019707</t>
+        </is>
+      </c>
+      <c r="D1455" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=9MxeuyT6AIbUfxVXg2lrYLY1FzwxJvQsJVJ7akXVTzpTkAfkj2Orc3GG5rclSv6Nvz06FoteCjP2lYAc17bD7kkOgbKuWGuCg8EMu%2fk4Mc6IlIr%2fDFDcgcIu0Wb7bg84AVmw5SFRIqaP8sLZ03gyAayI5q7qzSW08KWq6023Ngq7KcQf0ooGcg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1455" t="inlineStr">
+        <is>
+          <t>02024260432</t>
+        </is>
+      </c>
+      <c r="F1455" t="inlineStr">
+        <is>
+          <t>Market Yard</t>
+        </is>
+      </c>
+      <c r="G1455" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1455" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1455" t="inlineStr">
+        <is>
+          <t>Parvati</t>
+        </is>
+      </c>
+      <c r="J1455" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" s="1" t="inlineStr">
+        <is>
+          <t>A52100019582</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Jayant Govind Umbrajkar</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>A52100019582</t>
+        </is>
+      </c>
+      <c r="D1456" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=rhezrtnz9IHGBDJI6FLUk1X4wjB5u5nCsuzxKXuL3gNiSPb1sXBaWfMyMtI1YXZWQWxUGWclDouPUTifwgLFtEL582A0e5USS%2bYeQGLZaPPWLFXRzTCEb9FerrSrKJrzgMYPpJnYqUv9ZZRj4p4WBrgaD337NRdRu1sGepZ0ZToA4qW2GADdFA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1456" t="inlineStr">
+        <is>
+          <t>02025650090</t>
+        </is>
+      </c>
+      <c r="F1456" t="inlineStr">
+        <is>
+          <t>Lane No 10</t>
+        </is>
+      </c>
+      <c r="G1456" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1456" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1456" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1456" t="inlineStr">
+        <is>
+          <t>411004</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" s="1" t="inlineStr">
+        <is>
+          <t>A52100019705</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Raju Pukhraj Porwal</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>A52100019705</t>
+        </is>
+      </c>
+      <c r="D1457" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=OMjFQD%2bA%2bx3XHArM2%2fOkR35rHVcvVx%2b8VRZJM2xQrvfHIT7EtgKnhP9Iqk0Pf7jSMvqT19xP5VA7bLM07%2fyHu7S%2f1ptcXO%2b%2fm6apfERqdSjYubRVaLHIw8plLOFIUjZghpp9nTUF6t7K09Aqh4UynStgCAKzJlJv5CUtedjAwQIp5maJwvsRYA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1457" t="inlineStr">
+        <is>
+          <t>02224979944</t>
+        </is>
+      </c>
+      <c r="F1457" t="inlineStr">
+        <is>
+          <t>Ghatkopar East Mumbai</t>
+        </is>
+      </c>
+      <c r="G1457" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1457" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1457" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1457" t="inlineStr">
+        <is>
+          <t>400075</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" s="1" t="inlineStr">
+        <is>
+          <t>A52100004005</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Propfinder India Private Limited</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>A52100004005</t>
+        </is>
+      </c>
+      <c r="D1458" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=aRIbBrf5OmkiRVu77Lm7htKaK9Q5nd8DAiJpvWz%2f1FF36Wwuq9zb7X7223556zVHAajcZBT9%2fsbyUyT7IcAdU5Q36ZzLVGd8WtWTUExP5ttLis7xPNaY%2bUQhaZQdAJ9wEsf5NqaKObrpDa14%2fDCJNIF9ku1KrKWV5p3ii1UT0bya90AYzfEqow%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1458" t="inlineStr">
+        <is>
+          <t>02069105107</t>
+        </is>
+      </c>
+      <c r="F1458" t="inlineStr">
+        <is>
+          <t>Shivajinagar</t>
+        </is>
+      </c>
+      <c r="G1458" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1458" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1458" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1458" t="inlineStr">
+        <is>
+          <t>411005</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" s="1" t="inlineStr">
+        <is>
+          <t>A52100019670</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Sanjay Jaybhagwan Agarwal</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>A52100019670</t>
+        </is>
+      </c>
+      <c r="D1459" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=aWlg5Ho53R8IhtaDO751Xf%2fIsU4YS2xEy3zy3xuEyq1NN3cMwZ0gMXj6Ce5jp2xXz2K%2flSDNdOyJkS9%2bK0rTy8iz6Blx%2bzYdCvwO%2bA%2fBJlkf%2bIDmEtFoaFMq4JI4J7n9lmUPScZ0WicxZltZtGUfY5NOgTc3irsNddHGj805sEuUmBzlVgVE4g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1459" t="inlineStr">
+        <is>
+          <t>09665551020</t>
+        </is>
+      </c>
+      <c r="F1459" t="inlineStr">
+        <is>
+          <t>B.T Kawade Rd</t>
+        </is>
+      </c>
+      <c r="G1459" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1459" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1459" t="inlineStr">
+        <is>
+          <t>Gorhe Bk.</t>
+        </is>
+      </c>
+      <c r="J1459" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" s="1" t="inlineStr">
+        <is>
+          <t>A52100019607</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Ganesh Bhagwan Supankar Proprietor Of Quick Brick Properties</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>A52100019607</t>
+        </is>
+      </c>
+      <c r="D1460" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PfBtC03hNA1Ei1RnvCxB7ILLy8WxblfA6qPrnUmffMNF%2bHlwewqmZEFgUlS9JEe964oXjY06bc77LBGnbKb%2bpk6vx4Kb57srsg3%2bOM9A%2bGV0KqNMipoahvQNSijqV%2fYBaVqqltAufAR65r7L5uP6NLoifNFgQ9gpsboTJhVlDt%2bnksQOa42Y4A%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1460" t="inlineStr">
+        <is>
+          <t>09923572896</t>
+        </is>
+      </c>
+      <c r="F1460" t="inlineStr">
+        <is>
+          <t>Kondhawale</t>
+        </is>
+      </c>
+      <c r="G1460" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1460" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1460" t="inlineStr">
+        <is>
+          <t>Kondhawale</t>
+        </is>
+      </c>
+      <c r="J1460" t="inlineStr">
+        <is>
+          <t>412108</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" s="1" t="inlineStr">
+        <is>
+          <t>A52100019593</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Harshal Madhav Gaikwad</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>A52100019593</t>
+        </is>
+      </c>
+      <c r="D1461" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5OvAWyL%2fJGWrvJO%2bUAbir8MgqDTQKhUGN7fpQAzFHcv5f1q40etHMwvSUJKdP3LyHjhAcpjlu6x09D%2fruxmvUpSdvUS1FtGHwBXbl18KZKHUolUp4wisgTzOQTVgAAlAW7UJnAlUW7H7yKgFY9RMnGqhu9ri7vitncrL8lluNmG96tQcwKfPnA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1461" t="inlineStr">
+        <is>
+          <t>08087122082</t>
+        </is>
+      </c>
+      <c r="F1461" t="inlineStr">
+        <is>
+          <t>Kalewadi</t>
+        </is>
+      </c>
+      <c r="G1461" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1461" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1461" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1461" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" s="1" t="inlineStr">
+        <is>
+          <t>A52100019675</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Atul Ramchandra Shinde</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>A52100019675</t>
+        </is>
+      </c>
+      <c r="D1462" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=9ABLiwC7sABoXiUGyoKWRxlgg8fbk0IO53kcVvapBdopUOhi1G1SlLNfMiVwjbmVfVAzUCcTlRgnQ5KSYUaw6wqtxisELi3X9yD0zVuxP23u%2b6n40IbHcED%2fuxunQwprePW%2bBsIBoZggoowSoIKqEzahKyQV5bwRT1ELcsf5l9MzOQLPsbGV2Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1462" t="inlineStr">
+        <is>
+          <t>07058000262</t>
+        </is>
+      </c>
+      <c r="F1462" t="inlineStr">
+        <is>
+          <t>Near Balaji Tredars</t>
+        </is>
+      </c>
+      <c r="G1462" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1462" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1462" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1462" t="inlineStr">
+        <is>
+          <t>411032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" s="1" t="inlineStr">
+        <is>
+          <t>A52100019672</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Property Hint Consulting Services</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>A52100019672</t>
+        </is>
+      </c>
+      <c r="D1463" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=7ZB3fHGipnCyY3omdc%2f7RWuR%2f%2brK94Cxo23Se4nGbqJMyCWKmHbfmqWH%2bIqk4ziaH2Skvx4TTH82hu6vl%2fhEi0nEcpehuPL6WSHVleQwabNJH7wR6XEgdH0gFHi7H3ytNdWyIWQpkdnXj96Q7jrLCQEa%2fMh8TRYEKb5tpAYGrTWV%2bHQQ8qMyOg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1463" t="inlineStr">
+        <is>
+          <t>08308141800</t>
+        </is>
+      </c>
+      <c r="F1463" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="G1463" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1463" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1463" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1463" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" s="1" t="inlineStr">
+        <is>
+          <t>A52100019590</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Swapnil Satyawan Dethe</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>A52100019590</t>
+        </is>
+      </c>
+      <c r="D1464" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Ed7DpAmmlnp29ey5mrcr1y8Bv9MpkTBFaeJfyzu0QlGSUWphetQrnWyHZEyY5jO496KNVYQSqJl%2f5yxo%2fVABibk6raGSjZ7R6DQpruAcaysGpUh%2bdtZvYw2xzW96ZCpMfQXt1mOJw9VlNOCLqGvfHiE11fHH2HaoH5a7YMqoBcBHrNNxXY4CfQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1464" t="inlineStr">
+        <is>
+          <t>09767147460</t>
+        </is>
+      </c>
+      <c r="F1464" t="inlineStr">
+        <is>
+          <t>Kaspate Wasti,Wakad</t>
+        </is>
+      </c>
+      <c r="G1464" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1464" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1464" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1464" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" s="1" t="inlineStr">
+        <is>
+          <t>A52100002476</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Anwar Akhtar Hashmi</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>A52100002476</t>
+        </is>
+      </c>
+      <c r="D1465" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=HH3qsJEGhf9rkZZ59tcqNICxk4IrqKoKd0x8G5OVGa34y3BUjlvML59r6LW9%2bJp741ldYuvhqgtzMcdpm2Ppu5bQxOdzYeDzFT5rih%2fQ5yt7c%2fliyKbgftue4eM%2bG6e%2fIbal6rbkjJ0zZtTlJg6SGIKQnXV86Uly9wzvG67OqciJ7DztCaXdsA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1465" t="inlineStr">
+        <is>
+          <t>02027000003</t>
+        </is>
+      </c>
+      <c r="F1465" t="inlineStr">
+        <is>
+          <t>Vadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G1465" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1465" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1465" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1465" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" s="1" t="inlineStr">
+        <is>
+          <t>A52100003292</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Chandrakant Shripatrao Biradar</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>A52100003292</t>
+        </is>
+      </c>
+      <c r="D1466" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CO7NkDynjReDYGZTMksMzzfdYdOwk6uPhlr9r3LEtv1ibvLuUEgSvdFWbE1o8AEobQtD5uGTqnLOiAefrOKmsQ8P4SMX1T1Z7KXzrwWLAiV2%2bwuuJwTVFXnY5FHAfeNME3eajXtYQHohIBHOaFLpks5Vzkw9cd1NUIeHMTI0shJhjTQ6IIpvZA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1466" t="inlineStr">
+        <is>
+          <t>02027477373</t>
+        </is>
+      </c>
+      <c r="F1466" t="inlineStr">
+        <is>
+          <t>Dange Chowk Thergaon</t>
+        </is>
+      </c>
+      <c r="G1466" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1466" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1466" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="J1466" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" s="1" t="inlineStr">
+        <is>
+          <t>A52100019719</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Harish Raoji Patil</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>A52100019719</t>
+        </is>
+      </c>
+      <c r="D1467" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ODelm6k2rtn%2f0l89Csb8hem1nDeUM4NAB9IwUcNtq1avgeDobPRtHgfJRrTSEso%2fMvYc0NfqWvldOJVh7yXBjCguV9f3pG%2fH8eF6K4PAuzytHWo3rnkmCtm5tOZ7V9JqBGytrmPT2S31XNmVGzWNXFfy0sgZWA9965jWJYaMv5SgPcHb4OZBHQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1467" t="inlineStr">
+        <is>
+          <t>02024260432</t>
+        </is>
+      </c>
+      <c r="F1467" t="inlineStr">
+        <is>
+          <t>Marketyard</t>
+        </is>
+      </c>
+      <c r="G1467" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1467" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1467" t="inlineStr">
+        <is>
+          <t>Dhankawadi</t>
+        </is>
+      </c>
+      <c r="J1467" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" s="1" t="inlineStr">
+        <is>
+          <t>A52100019716</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>Saroj  Naik</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>A52100019716</t>
+        </is>
+      </c>
+      <c r="D1468" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=EdGdeRazXpzuO%2bJ0NQhyntCP4ICrDfUFeVQD9VncFbwV6ZS7MfhysOAsLGEqjDYJFD0nICjavT4un%2f7dKMr2LNX%2bcmnQhCjXivAqOnzT6wb16axpWFABBHBznWMuLxipmfw9FytZeMud4qdNS%2bW6R7%2faK9Y6N7ZJgij3qVcn7SwM3Ju8ltkqLg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1468" t="inlineStr">
+        <is>
+          <t>02027662263</t>
+        </is>
+      </c>
+      <c r="F1468" t="inlineStr">
+        <is>
+          <t>Keshav Nagar</t>
+        </is>
+      </c>
+      <c r="G1468" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1468" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1468" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1468" t="inlineStr">
+        <is>
+          <t>411036</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" s="1" t="inlineStr">
+        <is>
+          <t>A52100019720</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Rahul Gunvant Deshmukh</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>A52100019720</t>
+        </is>
+      </c>
+      <c r="D1469" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=sm6Gb4pj3yCCMilVaTsm9WmDKkz4gQefbhdQlakktaAS0IzStwZsA%2blF7kFc7vz7M9hoU%2b2M%2fnPwD%2frx2hID%2bUjo1vQjY%2bCbUVWQI47j2uEAKi6khBmNOHC9HTShCOo3Y6sUgolbp5zAOJLULjL75lKmliMaV6GMsA8eD0HCYJwKE8sm4UfQ8w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1469" t="inlineStr">
+        <is>
+          <t>09850628630</t>
+        </is>
+      </c>
+      <c r="F1469" t="inlineStr">
+        <is>
+          <t>Bhairavnagar</t>
+        </is>
+      </c>
+      <c r="G1469" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1469" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1469" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J1469" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" s="1" t="inlineStr">
+        <is>
+          <t>A52100019736</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Gautamchand  Dudhediya</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>A52100019736</t>
+        </is>
+      </c>
+      <c r="D1470" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=C67%2b25UMoxRtWSnKRYUvruSq5JcO0Mt3ata9n6ubnrqZUaTDd3QAdrWKjPOnCbAVahE8am6OiySSpb6rwLjoJzzOfjzmLNed2ipi5Aq7Rx8nGM5K7fgHR%2be4zXTcaIYgpEBH5zMQz7u6BLPczpfy5zEzRze90Objs0zpG9k%2fbW%2bUX7ke3BibMA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1470" t="inlineStr">
+        <is>
+          <t>02026860027</t>
+        </is>
+      </c>
+      <c r="F1470" t="inlineStr">
+        <is>
+          <t>Salunke Vihar</t>
+        </is>
+      </c>
+      <c r="G1470" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1470" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1470" t="inlineStr">
+        <is>
+          <t>Wanwadi</t>
+        </is>
+      </c>
+      <c r="J1470" t="inlineStr">
+        <is>
+          <t>411040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" s="1" t="inlineStr">
+        <is>
+          <t>A52100019664</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Samir Jaysing Auti Proprietor Of Spy Realty</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>A52100019664</t>
+        </is>
+      </c>
+      <c r="D1471" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=WaQDPFhkyXF45Nf5NHL7h%2fTx7542Uean%2b1sQckhcTsDJ%2bTrGIoqbkUV3J5Peid%2fn2XzIB39PUY8qZ8K2OFOTCOZKBcSPcKVUumYC7nVCy3gBAXUH2VkGQCUI4xKEwYBWRhzlFcwn4S7mClTnn51Gt7ELaHT0VYHRH1QGdLjXCH3io0Xw%2bngvrw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1471" t="inlineStr">
+        <is>
+          <t>08668704112</t>
+        </is>
+      </c>
+      <c r="F1471" t="inlineStr">
+        <is>
+          <t>Kondhwa Budruk</t>
+        </is>
+      </c>
+      <c r="G1471" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1471" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1471" t="inlineStr">
+        <is>
+          <t>Kondhwa Bk</t>
+        </is>
+      </c>
+      <c r="J1471" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" s="1" t="inlineStr">
+        <is>
+          <t>A52100019737</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Yogesh Kailash Malpani</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>A52100019737</t>
+        </is>
+      </c>
+      <c r="D1472" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=v7paJ112G9%2f2rXC00UrYMlC0BXJxBg9LftQ7hjYWHZZJrIX5ymeEYTX9ae0PhDlws55TRVJTXln0kg7s%2f27rO3HITog%2bD6i4uGC2MMK%2fGomFDaD8A5T9X1SAn2tsZGl7wrn2dC5URPDRl%2bPGKLeiayFIhMmsFVDlifvFPtBhgmEKlnAxUEKJPA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1472" t="inlineStr">
+        <is>
+          <t>09421961412</t>
+        </is>
+      </c>
+      <c r="F1472" t="inlineStr">
+        <is>
+          <t>Kaspate Vasti</t>
+        </is>
+      </c>
+      <c r="G1472" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1472" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1472" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1472" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" s="1" t="inlineStr">
+        <is>
+          <t>A52100019660</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Archana Manoj Otari</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>A52100019660</t>
+        </is>
+      </c>
+      <c r="D1473" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=zbZ8dmsKo%2bzNEvFiyWaRXNFaZhxktA%2bptHef%2bXPqpnryB9GOlfG3e6Lf0q8sOXHT7dFpqw6e%2bfHRUW7pNe9UHw3gpE0PWNA4vw%2fxkEt%2frYCmiuyPUyGZROgAHJrqXEFQNST%2fSS9q4teuo9eGTlhFhQjauk2uEVLD3tiQQvNaoXI8RznPgHfTew%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1473" t="inlineStr">
+        <is>
+          <t>02024481379</t>
+        </is>
+      </c>
+      <c r="F1473" t="inlineStr">
+        <is>
+          <t>1333 Shukrawar Peth</t>
+        </is>
+      </c>
+      <c r="G1473" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1473" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1473" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1473" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" s="1" t="inlineStr">
+        <is>
+          <t>A52100019851</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>Abhishek  Saini</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>A52100019851</t>
+        </is>
+      </c>
+      <c r="D1474" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=lz6Hem9xRxjcSBUZPEJ8%2bIEgkYIX8etuI25rkYP4Nu4bYkJM579TdWUGvb%2bHCbBx83kAVdkybtF92DsBxfN%2fj6gT%2b2ebIx4he9IMomnodORTLaFyzwjpp3oHfhRk65q9MuxAm8fj49sQy6EfkPGgdKpIreLUp8ojt%2bSL6zMtrKzXeUxXjVqL%2fw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1474" t="inlineStr">
+        <is>
+          <t>02022442277</t>
+        </is>
+      </c>
+      <c r="F1474" t="inlineStr">
+        <is>
+          <t>Pisoli</t>
+        </is>
+      </c>
+      <c r="G1474" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1474" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1474" t="inlineStr">
+        <is>
+          <t>Pisoli</t>
+        </is>
+      </c>
+      <c r="J1474" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" s="1" t="inlineStr">
+        <is>
+          <t>A52100019677</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Govind Rajaram Mundada</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>A52100019677</t>
+        </is>
+      </c>
+      <c r="D1475" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=k4bk4R7gqleeKtGyagG2Tk8IAc99OrzXYCN1TQzjRCOPGK7adB14YSesofGgIk6jxtPwNqZQR2KiMGs%2fnIJXru1%2b2P0uPe4f1gLi8qiPWxYQDg70pmahZdoqfONbSnS3tl1HjnrxJAl%2bO%2b4U2DUsoUSs8yM1i%2bExILQUrN%2bwPocQ39U62p2L%2fQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1475" t="inlineStr">
+        <is>
+          <t>09822199911</t>
+        </is>
+      </c>
+      <c r="F1475" t="inlineStr">
+        <is>
+          <t>Kapad Gunj</t>
+        </is>
+      </c>
+      <c r="G1475" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1475" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1475" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1475" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" s="1" t="inlineStr">
+        <is>
+          <t>A52100019790</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Vikas Dhondiba Pawar</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>A52100019790</t>
+        </is>
+      </c>
+      <c r="D1476" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=FHronxu%2bmZ7ELyqC2N4cvYgqlNZeLaxu5kU3ypPZFVWQXtigfuJxLiFQle9LJHG%2b2pgGSeN80BMhhY27L9xTa8w%2f2iyjzvF03x5oj%2bGQJ3e0OIGKiOF88GSWiQl32PM03n3ttwFavhAdsS04AahWqCIVraLGmd2snYUXmIl8qwv1pHfHgbaPYA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1476" t="inlineStr">
+        <is>
+          <t>09545858224</t>
+        </is>
+      </c>
+      <c r="F1476" t="inlineStr">
+        <is>
+          <t>Vishrantwadi</t>
+        </is>
+      </c>
+      <c r="G1476" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1476" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1476" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1476" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" s="1" t="inlineStr">
+        <is>
+          <t>A52100002543</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Tahseen Anwar Hashmi</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>A52100002543</t>
+        </is>
+      </c>
+      <c r="D1477" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Ef4lBnNXPMccXkB3awlwLT2Mq6T4COlqJy82d77foPlqrX99kHAL71x2bC%2bJSpXFG3R%2bJGnBCUV35rezr0DIF4Oo5%2fkkaOxiKhcRsxMtzlWOrzWLMsQStGrefc21c2OaPS3w3GB2o0TdKoTMqFIxdeZxdJPREegAJpp476XkyRdhkKBCQ5AJYQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1477" t="inlineStr">
+        <is>
+          <t>02027000003</t>
+        </is>
+      </c>
+      <c r="F1477" t="inlineStr">
+        <is>
+          <t>Vadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G1477" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1477" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1477" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1477" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" s="1" t="inlineStr">
+        <is>
+          <t>A52100019780</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Kiran Nandkishor Nagpure</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>A52100019780</t>
+        </is>
+      </c>
+      <c r="D1478" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=y68GrgXQdTPUd1rcboJwleHG76VVXKa%2bRtW9QQN%2bpl7rFPdxPii%2bEQ0yP7NcgR7KcZOzzm1OYKJgsaSA4RGXEWfR7mpiuMp3c2ow%2bolChdfIfWQHDWe%2bLoC%2frHrAJ%2fOAUh8vUDcFtXhZnWxUhiE8ONd9gYz1iCP7r%2fiZoJk%2faV5f2l3b35uNQQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1478" t="inlineStr">
+        <is>
+          <t>02025881123</t>
+        </is>
+      </c>
+      <c r="F1478" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G1478" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1478" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1478" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1478" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" s="1" t="inlineStr">
+        <is>
+          <t>A52100019752</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Rajesh Ramsajivan Pandey</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>A52100019752</t>
+        </is>
+      </c>
+      <c r="D1479" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2b8SuF7858FR4WN%2bZ%2fHKn4zbIwze9AbttvI3wcEzBxUs8LWSdH3ctXkuMtViN5t1kmuqvA2%2fuCx5Rva3dnDDr1iKoXhs3BKY0ooygQF%2fnjP7a6i5U8TcdiD7RA2RCnshypQPZ%2fPKgVY3JpT6YsbcZG5agGMj67UdleG5AUHo50SBieamobLVMFQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1479" t="inlineStr">
+        <is>
+          <t>09769139982</t>
+        </is>
+      </c>
+      <c r="F1479" t="inlineStr">
+        <is>
+          <t>Ghorpadi</t>
+        </is>
+      </c>
+      <c r="G1479" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1479" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1479" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1479" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" s="1" t="inlineStr">
+        <is>
+          <t>A52100019682</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Shweta  Kadam</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>A52100019682</t>
+        </is>
+      </c>
+      <c r="D1480" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=3rhQoMZWPQW89OMALIXRBUAgs0XAEI5TCoPCbJo9LIdoid8Ih57v8ROgZcLYYIHWJBBFs%2fn7S0FpiKWcTWiDJp7yazmfSmpOyKNggv2VGChCXEF4aG3G6NwwJuhEl07k6Kzlc6nEwC8ak1Lrw%2f8iSMxAgMm69aOH20I7sIvwxrQozeuZQhoGJQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1480" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
+      <c r="F1480" t="inlineStr">
+        <is>
+          <t>Nanded City</t>
+        </is>
+      </c>
+      <c r="G1480" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1480" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1480" t="inlineStr">
+        <is>
+          <t>Nanded</t>
+        </is>
+      </c>
+      <c r="J1480" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" s="1" t="inlineStr">
+        <is>
+          <t>A52100019807</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Ahilya Devi  Singh</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>A52100019807</t>
+        </is>
+      </c>
+      <c r="D1481" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=kq%2fBIqOBiQLZdq0HeRQXjC9zEtCQ7O8AbBS9AbJ7YSUzdYtbtIjMiE24yvfGR%2baZXp9vyeksdAITOWj5wiAkEfx%2bjmu0euglioJxNQoliKboy4gFabC6rC55hZgxIAayuzGMhT%2bP3OSURvJ%2bVz%2fS6cteWT4Ucbzz1J5lwvgsWvCMy5OB8IGhTA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1481" t="inlineStr">
+        <is>
+          <t>07274977667</t>
+        </is>
+      </c>
+      <c r="F1481" t="inlineStr">
+        <is>
+          <t>Lohegaon</t>
+        </is>
+      </c>
+      <c r="G1481" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1481" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1481" t="inlineStr">
+        <is>
+          <t>Lohgaon</t>
+        </is>
+      </c>
+      <c r="J1481" t="inlineStr">
+        <is>
+          <t>411047</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" s="1" t="inlineStr">
+        <is>
+          <t>A52100021203</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Kirit C Shanghvi</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>A52100021203</t>
+        </is>
+      </c>
+      <c r="D1482" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2bAarXrqJeDj9GSX%2fZfsrVNqXOOcjUxibEHENHakEGv4CWmOdyuR7vc1CNlK8JatppOTXemJCwPx%2fupt9Sjq47v%2fMrWAunmWVN1x1Avf4vMvWiIkaCExLHV8HJI8yHDoq1I0tY5OKXfLaLdXoXJvTWdFMKEVeWG6zycF7TObLAZBwNtJ6OT0r%2fA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1482" t="inlineStr">
+        <is>
+          <t>02226711549</t>
+        </is>
+      </c>
+      <c r="F1482" t="inlineStr">
+        <is>
+          <t>Khadakale</t>
+        </is>
+      </c>
+      <c r="G1482" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1482" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I1482" t="inlineStr">
+        <is>
+          <t>Khadakale (Ct)</t>
+        </is>
+      </c>
+      <c r="J1482" t="inlineStr">
+        <is>
+          <t>410405</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" s="1" t="inlineStr">
+        <is>
+          <t>A52100019810</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Pradeep Tukaram Sangave</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>A52100019810</t>
+        </is>
+      </c>
+      <c r="D1483" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hQCpEu9LggbTChWKxuQFcQYMA4AhTc9MDC271rlacBGSrk2Djanu9MNsHhNZBm3J3zzBtiCzkFGn56VWYOpfNt2cIuAIrmvRI0HRNgEdB5v2CmHJNC90ah9hHF%2btbrt5QRRpvbCIuSTbsctRBsExkhF3y5iqG0kfCufG275o4kylA9CiRv920g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1483" t="inlineStr">
+        <is>
+          <t>02027308002</t>
+        </is>
+      </c>
+      <c r="F1483" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="G1483" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1483" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1483" t="inlineStr">
+        <is>
+          <t>Thergaon</t>
+        </is>
+      </c>
+      <c r="J1483" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" s="1" t="inlineStr">
+        <is>
+          <t>A52100019726</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Statland Realty Private Limited</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>A52100019726</t>
+        </is>
+      </c>
+      <c r="D1484" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2f7dc8sqKu0eFfk%2bRHd3q45KOmQi9vIqJcD1r4TIz1I72thke%2bkEV9mmRYPULkVuun3r1TAqKF%2f9S7EuJs3Slzjulk5QUw8Ibuniyymf5Ld%2bXjVsdU1%2b0cjydqHdMfF%2byolLvBnFZNOuk0iVPIFAkcssU0KXCOpdWji4O92rPd2jieN%2bY8ml%2bKg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1484" t="inlineStr">
+        <is>
+          <t>02027292425</t>
+        </is>
+      </c>
+      <c r="F1484" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1484" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1484" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1484" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1484" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" s="1" t="inlineStr">
+        <is>
+          <t>A52100019744</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>Kamlesh Prakash Advani Proprietor Of Kimaya Real Estate</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>A52100019744</t>
+        </is>
+      </c>
+      <c r="D1485" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=WXyOsvgXxhjlePbt9%2fsD%2bGniG2P9lBUveb6p5lpNrwX7qjZKVLtGqMwapZO8mtyaYVzrt2oVjVfhebZc3gsyqFD9YNop2wsGIOIerrqjA2LTxFHxB%2fpDwGYfmDp9supNipsRzoe1o7ByTb6SK9Uv6Aqeke34xYl0ZiN2K6pRPivwlFbHdecrng%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1485" t="inlineStr">
+        <is>
+          <t>09028895959</t>
+        </is>
+      </c>
+      <c r="F1485" t="inlineStr">
+        <is>
+          <t>N I B M Kondhwa</t>
+        </is>
+      </c>
+      <c r="G1485" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1485" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1485" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1485" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" s="1" t="inlineStr">
+        <is>
+          <t>A52100019738</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Vijay Shankar Advani</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>A52100019738</t>
+        </is>
+      </c>
+      <c r="D1486" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bpuCAbBST8hojWhPRYvbkUw1cSapPIlTT2lEwTsiJ89yazt9PlXgqCAfPLRzmaVn6ed9b7gfwCfnobUDLq32SDC4bz7%2bWCrutO97my6KtU4O1Tsx%2fcHgPDqZ8thA1QKSwid5xaHma9Rym1P6Arwf%2bpvAaKqyCV%2bfwDOfTRbsHH6be5C1dFEXtQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1486" t="inlineStr">
+        <is>
+          <t>02025384120</t>
+        </is>
+      </c>
+      <c r="F1486" t="inlineStr">
+        <is>
+          <t>Kalyani Nagar</t>
+        </is>
+      </c>
+      <c r="G1486" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1486" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1486" t="inlineStr">
+        <is>
+          <t>Kalyaninagar</t>
+        </is>
+      </c>
+      <c r="J1486" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" s="1" t="inlineStr">
+        <is>
+          <t>A52100019696</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Sunil Ram Peswani</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>A52100019696</t>
+        </is>
+      </c>
+      <c r="D1487" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=cQABK2hrkAZJSJ2hOE3oybwGuU6MS0IY0ksH2fNWj8IsZbawJkBzSAvfQSqybOTUsGQK6NGznvUCehEQAwBU4Jg4nIgDz7zla4tfihf5vkXSpXts6KR4cs%2b60fbIjhBEQt14D7qONSjrjUtRibSzIC7E6abnV1k10ULyLAhLsfQficSKz7p9HQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1487" t="inlineStr">
+        <is>
+          <t>02027659858</t>
+        </is>
+      </c>
+      <c r="F1487" t="inlineStr">
+        <is>
+          <t>Nigdi</t>
+        </is>
+      </c>
+      <c r="G1487" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1487" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1487" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1487" t="inlineStr">
+        <is>
+          <t>411044</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" s="1" t="inlineStr">
+        <is>
+          <t>A52100020626</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Hannah  Joythi</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>A52100020626</t>
+        </is>
+      </c>
+      <c r="D1488" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=yK31pyKLc7%2fOBSjw9jOulM0f4fQRwa3ADZK3JwCbVGZGpqRUAR6rY%2bYCnbf9j7OJVJLskofZZi3T9YW%2bRR570dnhOAYPzu6TjEq0V%2fbKLUpD%2fv%2fdlI5bWShl9frAxnUdychdn0DDZ6ja49P%2ft0ym21duTx9nWzCOuvT29BGDfy8lmU2vSz7ymw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1488" t="inlineStr">
+        <is>
+          <t>02026737051</t>
+        </is>
+      </c>
+      <c r="F1488" t="inlineStr">
+        <is>
+          <t>Phursungi</t>
+        </is>
+      </c>
+      <c r="G1488" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1488" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1488" t="inlineStr">
+        <is>
+          <t>Pune (Cb)</t>
+        </is>
+      </c>
+      <c r="J1488" t="inlineStr">
+        <is>
+          <t>412308</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" s="1" t="inlineStr">
+        <is>
+          <t>A52100019826</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>Bipin Kumar  Sharma</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>A52100019826</t>
+        </is>
+      </c>
+      <c r="D1489" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=2csE%2fDMBvCzr7h%2fpXo6Nfe2TeQ1%2bEYAgw4fBwYfDh%2b2JzFa7v4HTvF0%2bXfgHLbVKyiMLccxhJK%2bh326fsGY4lBnOxO0itjUvwTWJxzfout8Bh4kl5DyqcpfT3fmE%2fFx9Ky3GSj9ndaz3kqGT7ikF1sy1w0RVjXxj7H6Fke80nb1cUofdbn0U4g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1489" t="inlineStr">
+        <is>
+          <t>08888939505</t>
+        </is>
+      </c>
+      <c r="F1489" t="inlineStr">
+        <is>
+          <t>Sunita Nagar</t>
+        </is>
+      </c>
+      <c r="G1489" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1489" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1489" t="inlineStr">
+        <is>
+          <t>Chandannagar</t>
+        </is>
+      </c>
+      <c r="J1489" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" s="1" t="inlineStr">
+        <is>
+          <t>A52100020246</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Abhishek  Singh</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>A52100020246</t>
+        </is>
+      </c>
+      <c r="D1490" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=OwAFFj%2fYcTDgWXa1modNRWdKJCXsvOyCiTX6kgnJJ00GhfJkgZbHwZhZ%2bAQ%2fJRtenel5OsDRu62NVx9%2bCjRONtaVDOAUulWFZ0kKmH7R0WUyZOsnoMUZ0V4VKnmHp1DBUl2DDApcR2CthkvzlPzSkJyatUOvdqcwtgFau5cmLsXiUwbGh3iLyg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1490" t="inlineStr">
+        <is>
+          <t>02071110973</t>
+        </is>
+      </c>
+      <c r="F1490" t="inlineStr">
+        <is>
+          <t>Vardayani Society</t>
+        </is>
+      </c>
+      <c r="G1490" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1490" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1490" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1490" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" s="1" t="inlineStr">
+        <is>
+          <t>A52100019734</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Rajiv Hiralal Surana</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>A52100019734</t>
+        </is>
+      </c>
+      <c r="D1491" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QMPuGWShNqPQOPFxBwaca7dg5nU5ckHms8%2brjmPUo3kqIGMjouNd%2fDj%2brCcLVvPHQ2vsCUk8yx8fcCKTHtnRphDv%2fCqIyAu32LZi5cW%2bOvu26I5aE5SGPNN9vLQB1hVCpBK4kppdNqP4QoiLNinAlmuKXz4W5CgFhtIGAFV9M81Gwnp7NqyZ5w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1491" t="inlineStr">
+        <is>
+          <t>02026120220</t>
+        </is>
+      </c>
+      <c r="F1491" t="inlineStr">
+        <is>
+          <t>Chinchechi Talim</t>
+        </is>
+      </c>
+      <c r="G1491" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1491" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1491" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1491" t="inlineStr">
+        <is>
+          <t>411002</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" s="1" t="inlineStr">
+        <is>
+          <t>A52100019802</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>Vijay Shantaram Taru</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>A52100019802</t>
+        </is>
+      </c>
+      <c r="D1492" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=sIpbBFP4W8EWXEuMN2j2u4vYuQX3zSfMtBNVqKsz1wq6HEqaaCQNJhepixhYYJGz0%2bU5GVtq239Cpy6Ivu6O4UMDBVVqo1H0YsiHCAULRiprlrGWyQ%2bEs9gF%2f3tL9YL8VSszXLr5Sxy%2bxbvvzOSiP3sZVm0l15P4GHU0YmKSrN0o48oE%2fobcPw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1492" t="inlineStr">
+        <is>
+          <t>09860143825</t>
+        </is>
+      </c>
+      <c r="F1492" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1492" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1492" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1492" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1492" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" s="1" t="inlineStr">
+        <is>
+          <t>A52100009725</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Prop Magica Property Consultants Llp</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>A52100009725</t>
+        </is>
+      </c>
+      <c r="D1493" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=iBbynkeeXNXCV8%2buVnmVusj8EL8rd8KAXkNJcOXrXyYoeT8mk%2bHY8lxKocewRXD%2fgPqJEPuY1DpoISZBDR6vTQlQKn91lVS1Dqjg68Ik4btIxbClU0Sc8BEXvqKwAiVGyVH9XR4OryjOhJ7szmgkBfvIsIc7pU4rfHxbYftvxmGgsSUYX2rnoA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1493" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
+      <c r="F1493" t="inlineStr">
+        <is>
+          <t>Kalyani Nagar</t>
+        </is>
+      </c>
+      <c r="G1493" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1493" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1493" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1493" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" s="1" t="inlineStr">
+        <is>
+          <t>A52100020044</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>Gopal  Krishna</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>A52100020044</t>
+        </is>
+      </c>
+      <c r="D1494" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MsO09LY4kFboVOFE0Uh01TyfLZ3ceTC%2fJqph66N3%2biXY8iRclSHQkvblrSCw3hdJFjy67UQaB2XbaMU8w51hk1GId1KWIDRIMF1s2CxD820TBjRjHn4uENY398t%2b9PHIP3eCLiV%2fqtuKXMmaRer%2fTvXJLNs4yQd%2baGQKE4k5QAekb7IYgoH0OA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1494" t="inlineStr">
+        <is>
+          <t>02024686090</t>
+        </is>
+      </c>
+      <c r="F1494" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1494" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1494" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1494" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1494" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" s="1" t="inlineStr">
+        <is>
+          <t>A52100019823</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>Prakash Chandrakant Shinde Proprietor Of Sahil Associate</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>A52100019823</t>
+        </is>
+      </c>
+      <c r="D1495" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Ry9M5ypt5%2fF3ee%2bSIlWbm0x6%2blF3lSZlvP3dFUVa4b6If%2bQPIlDAPydB%2fyhHKRmhisO%2bau6YI4G9jp8J%2biZbx%2bFNr3BkgKKZ26Mx5jIvNmnAWN%2fYTb89F3Xj3mVJUnlB9roPzflMUJ3RYyfK6pXOOHmFC1eVatsyWjNAKN%2f%2fIB2gyKQaYDq%2bmQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1495" t="inlineStr">
+        <is>
+          <t>09607071122</t>
+        </is>
+      </c>
+      <c r="F1495" t="inlineStr">
+        <is>
+          <t>Pimpri</t>
+        </is>
+      </c>
+      <c r="G1495" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1495" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1495" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1495" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" s="1" t="inlineStr">
+        <is>
+          <t>A52100020621</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Murli Manohar Vohra</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>A52100020621</t>
+        </is>
+      </c>
+      <c r="D1496" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=4CwqnTK9GfQmE%2bO2qYfTulM%2ftRwavCqNYcYvxCvuhZ00foiDdyc1b6QRwHW5x6mGaYPvgOmqy29p2vuYYwgB1x6qo3ZzDFrcTDAr0ZYk4OokoqTQLCE%2bTafc8xBJiFJbunRI3YznSXcgfKRRq%2fKbOAdu0sgCu4Eo9BVccPKyNAdli5Abi062Bg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1496" t="inlineStr">
+        <is>
+          <t>01204309392</t>
+        </is>
+      </c>
+      <c r="F1496" t="inlineStr">
+        <is>
+          <t>Fursungi, Hadapsar</t>
+        </is>
+      </c>
+      <c r="G1496" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1496" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1496" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1496" t="inlineStr">
+        <is>
+          <t>412308</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" s="1" t="inlineStr">
+        <is>
+          <t>A52100019742</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>Satyam Atul Surana</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>A52100019742</t>
+        </is>
+      </c>
+      <c r="D1497" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=TeI7F78Lg9R45mDJJlVIMcJbe9kyKPZjMLg5ie%2fZNCoMmFywd9C3Qb6N5ZpC4MidGklQ00y2yFbwSldVj3jYmJx2PtqQRsuIq7WRVt0YSGR%2fpuOk5idtehOCU4aJHOg8RcibvwQqgFmQGJ231tBbZRrEN7aVWWx74mCHhE0Llza65wRyYpE4sw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1497" t="inlineStr">
+        <is>
+          <t>02024441566</t>
+        </is>
+      </c>
+      <c r="F1497" t="inlineStr">
+        <is>
+          <t>Nr. Marketyard</t>
+        </is>
+      </c>
+      <c r="G1497" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1497" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1497" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1497" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" s="1" t="inlineStr">
+        <is>
+          <t>A52100020656</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Anil Balkrishna Phalke</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>A52100020656</t>
+        </is>
+      </c>
+      <c r="D1498" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=QkiQ6DxNy2sQg0IZm%2bbyGwal9AZuNsPXtA7p3hT5923iIO%2fHIZ7G6f8Xd%2bqb38LhCYA16UsRaw9%2fV1wXBLDS3PC3Ydp996yOREwTKlOIDWKydEAcZgZrBr%2bFrqdd92QFZ584GPaW9PTYUwpzdm5ufuso9Mmf5xg0qGoDMg5pgvFV4vp9UjFbhw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1498" t="inlineStr">
+        <is>
+          <t>09689509340</t>
+        </is>
+      </c>
+      <c r="F1498" t="inlineStr">
+        <is>
+          <t>Kiwale</t>
+        </is>
+      </c>
+      <c r="G1498" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1498" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1498" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1498" t="inlineStr">
+        <is>
+          <t>412101</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" s="1" t="inlineStr">
+        <is>
+          <t>A52100019750</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Amar Munnalal Kanojiya</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>A52100019750</t>
+        </is>
+      </c>
+      <c r="D1499" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=i0%2fI2p8Ma6CyCIRm7eJHZ8Q8QEY7EiI54CbDJjFNyFl5XJwqR%2bplFb0a8OciwKjZ0VwBHrZHmSo1p1sgJACCJWE7Gx0c9rbb%2fE%2fDAG71dzcEAb4iL4NpXRtba7c1JdHtVlykdkm4lbo5tsU6H%2fM2MR8qF7l7Bjv23b5CtXCqW4Rg5gafP1aKcw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1499" t="inlineStr">
+        <is>
+          <t>09765137443</t>
+        </is>
+      </c>
+      <c r="F1499" t="inlineStr">
+        <is>
+          <t>Shivne</t>
+        </is>
+      </c>
+      <c r="G1499" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1499" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1499" t="inlineStr">
+        <is>
+          <t>Shivne (Part)</t>
+        </is>
+      </c>
+      <c r="J1499" t="inlineStr">
+        <is>
+          <t>411023</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" s="1" t="inlineStr">
+        <is>
+          <t>A52100019911</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>Ravindra Gajendra Sarvale</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>A52100019911</t>
+        </is>
+      </c>
+      <c r="D1500" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=FYLsVBfbTIa%2bkYJpA1nDEBaxgpXtP%2bnzrhDHXAiXm6DzrrwRs0vN%2fPonMNeDBlPx2bmvk0TxkI2oEnNniAQX3zsFC6SG5gVMPri1dguoxOm1WXiq0e8ESRX4PaAtKSy792eqqu1cMLKdqvI4DA9Wg6O27dQ1pBopB1aI9cKoQ5wdAxS0%2bhI3AA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1500" t="inlineStr">
+        <is>
+          <t>02065330037</t>
+        </is>
+      </c>
+      <c r="F1500" t="inlineStr">
+        <is>
+          <t>Kad Nagar</t>
+        </is>
+      </c>
+      <c r="G1500" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1500" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1500" t="inlineStr">
+        <is>
+          <t>Undri</t>
+        </is>
+      </c>
+      <c r="J1500" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" s="1" t="inlineStr">
+        <is>
+          <t>A52100008616</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>Asmita Suresh Pawar</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>A52100008616</t>
+        </is>
+      </c>
+      <c r="D1501" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=412PQctnhOK9Es10ndmCBThz6vbtSHYFiAGmaicJLqikoiWX8fBIJPm8rwjt5%2bXNvFMJ2H1im8L%2fQ81L9TRfIpjvlMcstzT1CCaivYvnZjLenR1dkn%2bKmXRO1JNgJ5UTobKnmZjKxaBAcq0Ey70NE85GD4KDrBDlMeozYZsRNaw%2feeZyy90m7w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1501" t="inlineStr">
+        <is>
+          <t>09096006854</t>
+        </is>
+      </c>
+      <c r="F1501" t="inlineStr">
+        <is>
+          <t>Achal Nagar</t>
+        </is>
+      </c>
+      <c r="G1501" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1501" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1501" t="inlineStr">
+        <is>
+          <t>Kondhwa Bk</t>
+        </is>
+      </c>
+      <c r="J1501" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new peroperty agents [Total:1550]
</commit_message>
<xml_diff>
--- a/rera_agent_details.xlsx
+++ b/rera_agent_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1501"/>
+  <dimension ref="A1:J1551"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -77960,6 +77960,2594 @@
         </is>
       </c>
     </row>
+    <row r="1502">
+      <c r="A1502" s="1" t="inlineStr">
+        <is>
+          <t>A52100019822</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>Tajinder  Singh</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>A52100019822</t>
+        </is>
+      </c>
+      <c r="D1502" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=loNhiSexDkb%2bh7LeaMP6VLT3qh7jxsORW%2fAh57o6ZMFd51JRpPTpaj9XJMUwQ9Zf%2fd6%2fp1oCeiJTaLjhglE6TaTayUliHRfKO6k2%2fZkbAbzqhhOSkq1UFOo7owkdrafL2dEXfgMuZ%2b7ENwiqkwP0fetz3mceOx%2fgBGnuRqnJZ21F95aAkBaHAQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1502" t="inlineStr">
+        <is>
+          <t>02041241818</t>
+        </is>
+      </c>
+      <c r="F1502" t="inlineStr">
+        <is>
+          <t>Undry</t>
+        </is>
+      </c>
+      <c r="G1502" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1502" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1502" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1502" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" s="1" t="inlineStr">
+        <is>
+          <t>A52100019816</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Sudarshan Arjun Deshmane</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>A52100019816</t>
+        </is>
+      </c>
+      <c r="D1503" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=vCYpxnUxLLvv72JA%2fpydfjs76G8oe9XnhedRKBlYFoEQLaLtHtP2RSJQpwWihAl94%2fXHDImaJa9%2fivEZ7SGQ84x25oGOvoDTjWJIpgzT4iDoOob8tTMt%2fDptaeCBLV3YpUVd5biXEw1F6UwFaSKa56uyG709U6VBHRIBtmn7S2UHlAMRnblSfA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1503" t="inlineStr">
+        <is>
+          <t>02024392907</t>
+        </is>
+      </c>
+      <c r="F1503" t="inlineStr">
+        <is>
+          <t>Dhayari</t>
+        </is>
+      </c>
+      <c r="G1503" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1503" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1503" t="inlineStr">
+        <is>
+          <t>Dhayari (Part)</t>
+        </is>
+      </c>
+      <c r="J1503" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" s="1" t="inlineStr">
+        <is>
+          <t>A52100019814</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>Ashok Dilip Patil Proprietor Of Ask Realty</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>A52100019814</t>
+        </is>
+      </c>
+      <c r="D1504" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Elpuoek3Qt%2fGZj68G7TcOzeHorpSD6OCG835Jus2GZzNE%2bJ9I0U4jY3or0oKUQJdKq41y%2bqzNTdkDLfAOmZui0x5Uycz6P12AYQW1btTcw8o6UFX8QOUBIjGf2CKd38HpvCzjBeCfGVvgSm%2bejvcyXEXL2v5AHBlk8dKHmtezc%2fZBKKkTOx%2fkg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1504" t="inlineStr">
+        <is>
+          <t>09637992286</t>
+        </is>
+      </c>
+      <c r="F1504" t="inlineStr">
+        <is>
+          <t>Dighi</t>
+        </is>
+      </c>
+      <c r="G1504" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1504" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1504" t="inlineStr">
+        <is>
+          <t>Dighi</t>
+        </is>
+      </c>
+      <c r="J1504" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" s="1" t="inlineStr">
+        <is>
+          <t>A52100019942</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>Mannu Udaybhan Singh</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>A52100019942</t>
+        </is>
+      </c>
+      <c r="D1505" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2f3jH2TFp1fL2Og8SdkCBuvodLbAb%2foYFAqXfWZzUmA1RUTn8J97y21FvyXeGt%2fh2lSpydbum%2f9ef4cFzn10CJQ1pzh2UVLb9ByNxYlwdDTIYSyooF8M1ovP%2fCA23TcWYsqx99ki4WvSTnrlGnLqZGqSb1iVZRendL3dN%2f9S6Tw5xS7%2fTJg6q2w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1505" t="inlineStr">
+        <is>
+          <t>02022222222</t>
+        </is>
+      </c>
+      <c r="F1505" t="inlineStr">
+        <is>
+          <t>Hapadsar</t>
+        </is>
+      </c>
+      <c r="G1505" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1505" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1505" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1505" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" s="1" t="inlineStr">
+        <is>
+          <t>A52100019858</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>Pruthviraj Mahendra Shinde</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>A52100019858</t>
+        </is>
+      </c>
+      <c r="D1506" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=%2fJLc5ivzc%2byZ%2bVgPsD%2bh%2f9r1TDaBY5urV2bbNmitTEvDrIQswQCNlNtNX3mC7cLMp7l9PUCgDKwIv8hhHsUmbbxFHiowbQYUKCex8i5s%2b3pQ7Qs%2byWnNNUw1SBm%2f5PcN4Fi9LHwI8%2bg7JVAfT5%2b7GXzzYYHTq3xPWcjqoKNF%2bWmjLR0R7mbmWw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1506" t="inlineStr">
+        <is>
+          <t>08446262020</t>
+        </is>
+      </c>
+      <c r="F1506" t="inlineStr">
+        <is>
+          <t>Wadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G1506" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1506" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1506" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1506" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" s="1" t="inlineStr">
+        <is>
+          <t>A52100020480</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>Mayur Nimba Rane</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>A52100020480</t>
+        </is>
+      </c>
+      <c r="D1507" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=PGPWxth4qqKZOlu1AmUUd7D0cJrIChOT690b0FduKZ77PB%2ffV2gDQVdirT5OXP5P4lZtb2FJTkIrKvigQ%2b%2btVz5IcwzjmjKqutnr9Tl%2bsfM2p8L%2fX39snn9smxotLz%2b8ZIW86OC7b8Zbenkphy9uyY9tJgZEzGzqvqyI7e2B0CXEkSBE5zP0CA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1507" t="inlineStr">
+        <is>
+          <t>09028176475</t>
+        </is>
+      </c>
+      <c r="F1507" t="inlineStr">
+        <is>
+          <t>Dudhane Nagar</t>
+        </is>
+      </c>
+      <c r="G1507" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1507" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1507" t="inlineStr">
+        <is>
+          <t>Karve Nagar</t>
+        </is>
+      </c>
+      <c r="J1507" t="inlineStr">
+        <is>
+          <t>411052</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" s="1" t="inlineStr">
+        <is>
+          <t>A52100020230</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>Sharmila Sudip Chitale</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>A52100020230</t>
+        </is>
+      </c>
+      <c r="D1508" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=tdSXR3A4F%2b1Z6IAggoicczwaFzu3PY4Ev2LtuATjpksQA5%2bl2Kkg2mNeug%2bRK8PVDD29TId9sA9d1S%2bFCdHQO%2b1%2fnoysQAvsHu4lxcBvCUzFo8tbEOTY8cSVXLky8agSyFKuAhh7sL5B7aSvNTYvp9XolIc%2fRjV1DeVSBo9unLWrTqSGhzesKw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1508" t="inlineStr">
+        <is>
+          <t>02025668118</t>
+        </is>
+      </c>
+      <c r="F1508" t="inlineStr">
+        <is>
+          <t>Aundh</t>
+        </is>
+      </c>
+      <c r="G1508" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1508" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1508" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1508" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" s="1" t="inlineStr">
+        <is>
+          <t>A52100021608</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>Vikram Hiralal Koul</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>A52100021608</t>
+        </is>
+      </c>
+      <c r="D1509" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=CCtoPxoKPJr8FBoAOu1vVvGNx%2b1JFyvVG%2beAESHbzoKUFynGwUIWhEUu59mHDNrxLHP009QuuqMui3wcyCIxpkbkij2f1KyjKx5304jHRFTZyNPiFNUlx%2bY0Oo1O60Rx48eWEH%2fO6jLHdSHaTFb1pCPkTeLH9yj4t7OLKqHdrBYcd1nti1s%2fng%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1509" t="inlineStr">
+        <is>
+          <t>09881565678</t>
+        </is>
+      </c>
+      <c r="F1509" t="inlineStr">
+        <is>
+          <t>Ravet</t>
+        </is>
+      </c>
+      <c r="G1509" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1509" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1509" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1509" t="inlineStr">
+        <is>
+          <t>412101</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" s="1" t="inlineStr">
+        <is>
+          <t>A52100020050</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>Vineet  Kumar</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>A52100020050</t>
+        </is>
+      </c>
+      <c r="D1510" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=n7tc0zRnn3VH8mHrMNeiMx%2bZn63S%2ffqRThyaqVlyvhnp2IWCJzmna%2fwik0PelhbS27%2bYcjXBuEGkW8h7ktOyoknq4CmlxnR6iAXiVsVExnDFM2HPabTbLVw611dv3gEul%2buecCrJJ%2f8m93uPMG3%2fo%2b5TBgGKXgn%2f0Tw8xxgLzSMYKS6D1c%2fGWg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1510" t="inlineStr">
+        <is>
+          <t>99953278332</t>
+        </is>
+      </c>
+      <c r="F1510" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="G1510" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1510" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1510" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J1510" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" s="1" t="inlineStr">
+        <is>
+          <t>A52100019913</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>Sarang Raghunath Kelkar</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>A52100019913</t>
+        </is>
+      </c>
+      <c r="D1511" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=X5%2b8cBxDv6jUdDlJuZruO0Euph2SrfJpBRKoo6ZCst1G0R7lHPTIaX5gAbf3oAbYSttHinkjo0kJnwd2iPlInTDKw75xeyDzK9uzlp9thOj3B%2fazf2BbGqfEYRyYgsN%2foQ3IY7whsLUTghUCBe8KnGtEjf%2f%2bXRjWEvhTYUgblh%2b9monHOkLLrA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1511" t="inlineStr">
+        <is>
+          <t>02024336301</t>
+        </is>
+      </c>
+      <c r="F1511" t="inlineStr">
+        <is>
+          <t>Manik Baug Amruta Nagar</t>
+        </is>
+      </c>
+      <c r="G1511" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1511" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1511" t="inlineStr">
+        <is>
+          <t>Wadgaon Bk</t>
+        </is>
+      </c>
+      <c r="J1511" t="inlineStr">
+        <is>
+          <t>411051</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" s="1" t="inlineStr">
+        <is>
+          <t>A52100019863</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>Manjula  Naidu Proprietor Of Shri Properties</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>A52100019863</t>
+        </is>
+      </c>
+      <c r="D1512" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=K%2f3LwO6kheVmanaZNKTBdAT8oe9SaxGO3dJ5eERO3YnMlaIHoiQPbZOzbUJAG0SfkeC6iKVUyZNBMsIG%2fRc6%2bDkVVe0X2zNpdDbqiQtQ%2fUbH3a4%2fO978SwtigUoyJVHBKEtgu5YY7jgMwvgseM9BGlxyOFfWDdsiw3ww%2bv7rjft9csPIAjtDrw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1512" t="inlineStr">
+        <is>
+          <t>07350684016</t>
+        </is>
+      </c>
+      <c r="F1512" t="inlineStr">
+        <is>
+          <t>Keshav Nagar, Mundhwa</t>
+        </is>
+      </c>
+      <c r="G1512" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1512" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1512" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1512" t="inlineStr">
+        <is>
+          <t>411036</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" s="1" t="inlineStr">
+        <is>
+          <t>A52100020192</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>Skyvest Solutions</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>A52100020192</t>
+        </is>
+      </c>
+      <c r="D1513" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ECdDtk8oUVlSLUXuXV%2fy9CFprjHT0H2QjHZn7dwCafnI4OwjQ1P63GqqMNrKI8yw3pF9adOLPudUipGQqACXYTEILubSsOgsPUVpM7acM7rSILz30lgkBbGZMQyCnH0muDVKpPXGBnvwKVktsJcUEGUFunpodVt6wPolxzkjBjzZM4CTDfib2Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1513" t="inlineStr">
+        <is>
+          <t>02048632529</t>
+        </is>
+      </c>
+      <c r="F1513" t="inlineStr">
+        <is>
+          <t>Kondhwa</t>
+        </is>
+      </c>
+      <c r="G1513" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1513" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1513" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1513" t="inlineStr">
+        <is>
+          <t>411048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" s="1" t="inlineStr">
+        <is>
+          <t>A52100020182</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>Sonam  Agrawal</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>A52100020182</t>
+        </is>
+      </c>
+      <c r="D1514" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=uifVaU0T4jH9ugCIYPGsspyGuntz9lMWEgdOJAgUn9eEDg8dnEth4VvSLr26wO2ARvfwcB2WdsKl6nbVhUyAyj4pVFtL5FeCIbfmwnAkLUcfdk2vQ5VWJImi5CCYRjZ68JGQs96H%2fKih8HDP1tPGOixFb%2f4XtB4uNwulW3FHoaftU3FPxJHA5g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1514" t="inlineStr">
+        <is>
+          <t>02048604073</t>
+        </is>
+      </c>
+      <c r="F1514" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1514" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1514" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1514" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1514" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" s="1" t="inlineStr">
+        <is>
+          <t>A52100019995</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>Basavraj Suryakant Achalere</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>A52100019995</t>
+        </is>
+      </c>
+      <c r="D1515" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=I4q%2fCh8ZpS3OFRhWNKOJSWyESTv7swvwiHf9%2bIvo1KZwnEiAkDxeYNGuw9xemZdW73czmDfoRaivzltZN2Y63yJbr4f0v3UhhcjEGE2cPEEEdYez0Z0AQjbDuxgP8LvIgYCBr6mndrORefjfPyYEZ0uxDT0IOCUNJRuMZiKeVbQCg6PJ57Ct6g%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1515" t="inlineStr">
+        <is>
+          <t>02077689606</t>
+        </is>
+      </c>
+      <c r="F1515" t="inlineStr">
+        <is>
+          <t>Sahog Nagar</t>
+        </is>
+      </c>
+      <c r="G1515" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1515" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1515" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1515" t="inlineStr">
+        <is>
+          <t>412114</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" s="1" t="inlineStr">
+        <is>
+          <t>A52100019915</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>Bharat Shankar Tawar Proprietor Of Sai Real Estate Solution</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>A52100019915</t>
+        </is>
+      </c>
+      <c r="D1516" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KywK23A8mpZ02Jtr371ZubQCY2Qn0onHwk3y61hUeKiCe4Ia4OHutwtnQyE6viLPyWcz1PZYeBI8A2P0XmpTleUB8QScTCyD2tXFdvgSUa1xh2I%2bOuhucqsq8E3IHLCO8DZKZSqeoxFwZjyv9NtGSfzpJVabHP%2bKj1PQ0WjLat%2bgJtDDz0r0ng%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1516" t="inlineStr">
+        <is>
+          <t>09145579191</t>
+        </is>
+      </c>
+      <c r="F1516" t="inlineStr">
+        <is>
+          <t>Tukaramnagar</t>
+        </is>
+      </c>
+      <c r="G1516" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1516" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1516" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1516" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" s="1" t="inlineStr">
+        <is>
+          <t>A52100019937</t>
+        </is>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>Meghraj P Dendage Proprietor Of Sunrise Realties</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>A52100019937</t>
+        </is>
+      </c>
+      <c r="D1517" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hWBR5HEc1ktwhOHv%2faVuE9r0F%2fYzM%2fFZiaGkJpeJBSFs3xz4pw%2f1%2bMwJvlC6524WXpWSrYi486mowx5%2fOUG6HdwlP0ry5ppW2siv8IqlrG0mpENV9NYJsLXhJOO5mhxqi9cay2hgv6ke6eLrS41HKMxa2c1pgE6hfKQwIrdtFfTzg7FKuzjUGw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1517" t="inlineStr">
+        <is>
+          <t>08806054305</t>
+        </is>
+      </c>
+      <c r="F1517" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="G1517" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1517" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1517" t="inlineStr">
+        <is>
+          <t>Pashan</t>
+        </is>
+      </c>
+      <c r="J1517" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" s="1" t="inlineStr">
+        <is>
+          <t>A52100019895</t>
+        </is>
+      </c>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>Mukund  Chandak</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>A52100019895</t>
+        </is>
+      </c>
+      <c r="D1518" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=TY0bDSGVObffPyfaG%2b%2bNQutA0YMm8fIhNSmdCIzybDI%2fGXiwutQiuqMUC8Yke0m136MoJVICzPMfVAHqyrG2hrQPXjJP4d1ybKWm3KE0JhZ2Lj%2bfcUQmu2J0acpwEIOKfSChW2x2cjTxIxp7euuX5CQ7I1O1t32GycHJPYP6k1MRnSZys8Omyw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1518" t="inlineStr">
+        <is>
+          <t>02044667788</t>
+        </is>
+      </c>
+      <c r="F1518" t="inlineStr">
+        <is>
+          <t>Tingre Nagar</t>
+        </is>
+      </c>
+      <c r="G1518" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1518" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1518" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1518" t="inlineStr">
+        <is>
+          <t>411032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" s="1" t="inlineStr">
+        <is>
+          <t>A52100019902</t>
+        </is>
+      </c>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>Deepali Bharat Chavan</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>A52100019902</t>
+        </is>
+      </c>
+      <c r="D1519" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=hJ8FDY2QALqcfBRzYGexkG1R4b5WL0oAVu1UIzyd2NAcC2aGYHzKaA9Jv6NySibxaMWGNRG%2bcE4kVrGPNMtmfljyAoxQ%2fzbepfXt9qwMyvVVxftEafRHotuvOe7JadeCwF2UmBtnNEaAZeA1WUZdU68Ws%2bm23JZaigbbmRxhjt9%2bB%2fxDSaV2fw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1519" t="inlineStr">
+        <is>
+          <t>07020488018</t>
+        </is>
+      </c>
+      <c r="F1519" t="inlineStr">
+        <is>
+          <t>Sasane Nagar</t>
+        </is>
+      </c>
+      <c r="G1519" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1519" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1519" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1519" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" s="1" t="inlineStr">
+        <is>
+          <t>A52100019868</t>
+        </is>
+      </c>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Kunal  Kishore</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>A52100019868</t>
+        </is>
+      </c>
+      <c r="D1520" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Pg4RXPiw89x4rRXkUskHs6x%2bVf8fUsn6pLHxhEuzlGRK2BCoPX7XLrqWREYaWtef4ktvhs2kRJAgWntpVBQSL5ut8dhscyhLApgShaqaeHcIFG537CNT6%2fq%2f2gkjl0jFYVg%2bhTFMD9sakIuGLkx5ZmqKW98EZjwrSHO0JZYEklPX4cOFrlnYzg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1520" t="inlineStr">
+        <is>
+          <t>02026942135</t>
+        </is>
+      </c>
+      <c r="F1520" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="G1520" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1520" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1520" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1520" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" s="1" t="inlineStr">
+        <is>
+          <t>A52100020086</t>
+        </is>
+      </c>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>Yogesh Balu Kadam</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>A52100020086</t>
+        </is>
+      </c>
+      <c r="D1521" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=sRJbpmdAfOhgURMaOCwVcpq0ZS2GlS9HkTiCAJ4Y5AKOEOoOxam09kmLM2S6Mea9FZUBS0TUiMgR5R9zu2gxM1XBNMhCFGBj3ts%2fc%2fV1loqNlleL4zQ6mAtDr3DVlnh2B2urN5rRYUPz%2fIVsAGe2HwEW4CMUYpbZUElvr8y8j5LKkQAJr3oxAw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1521" t="inlineStr">
+        <is>
+          <t>07620074436</t>
+        </is>
+      </c>
+      <c r="F1521" t="inlineStr">
+        <is>
+          <t>Pisodi Gaon</t>
+        </is>
+      </c>
+      <c r="G1521" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1521" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1521" t="inlineStr">
+        <is>
+          <t>Pisoli</t>
+        </is>
+      </c>
+      <c r="J1521" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" s="1" t="inlineStr">
+        <is>
+          <t>A52100021423</t>
+        </is>
+      </c>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>Shweta Ajay Pasari</t>
+        </is>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>A52100021423</t>
+        </is>
+      </c>
+      <c r="D1522" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ijTRs7ZneiEdEKf1msx3SNHYKK6ds8RJpfPtHq%2fkON1w0g4TvTEoS%2bmdpU%2frk1pBMqZyw%2fhSfnLMOcAQmlIbJCdznIWQcS5h%2fE31OUyNUyiSWYIdicPKsXy0%2futE%2baRlKKHVmbU30CnZaG8gInCkmB%2fwdB56ev5fESr0eZyGo%2bMW7GwSGQ3enA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1522" t="inlineStr">
+        <is>
+          <t>09881427879</t>
+        </is>
+      </c>
+      <c r="F1522" t="inlineStr">
+        <is>
+          <t>Nagar Road</t>
+        </is>
+      </c>
+      <c r="G1522" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1522" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1522" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J1522" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" s="1" t="inlineStr">
+        <is>
+          <t>A52100019889</t>
+        </is>
+      </c>
+      <c r="B1523" t="inlineStr">
+        <is>
+          <t>Parvej Saipan Mulla</t>
+        </is>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>A52100019889</t>
+        </is>
+      </c>
+      <c r="D1523" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=NpIMpPgmw%2bzODwJdOvOe49jvau0iE5SDDNlj11N2%2bcnDVk%2b4f2aA5xl4IxMVu%2f8jAOai8tOHHWLDZMcrBPgRAoE1idyOybMyvq3xEMq0pPiFq0kQ%2bEF2gpFUAj28C82AKlHyH4huwoJVQR4ExBvbYat5lgNuiqmhwTogqq%2bIoGfpVZGiluvaFA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1523" t="inlineStr">
+        <is>
+          <t>02024456789</t>
+        </is>
+      </c>
+      <c r="F1523" t="inlineStr">
+        <is>
+          <t>Bibwewadi</t>
+        </is>
+      </c>
+      <c r="G1523" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1523" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1523" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1523" t="inlineStr">
+        <is>
+          <t>411037</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" s="1" t="inlineStr">
+        <is>
+          <t>A52100019980</t>
+        </is>
+      </c>
+      <c r="B1524" t="inlineStr">
+        <is>
+          <t>Gajendra Roopsingh Rajpurohit</t>
+        </is>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>A52100019980</t>
+        </is>
+      </c>
+      <c r="D1524" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=gxvggIHPDesIZ1OTCIZewsqsgIfDAUcb27ecTUww6gjNKYAO2WM0dbC4c72CjPs81yRo9TQm0b2bwbTMrHb0cYGPA556VYLANdqYQVC7COvMZsG1jsK1k2y538qMzmMfCl5Ohj1F9U4LWUjbEGxc%2bH7mgtqbO6eJoySWOLsd6NTuweZSpmCytg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1524" t="inlineStr">
+        <is>
+          <t>07030394488</t>
+        </is>
+      </c>
+      <c r="F1524" t="inlineStr">
+        <is>
+          <t>Koregaon Park</t>
+        </is>
+      </c>
+      <c r="G1524" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1524" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1524" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1524" t="inlineStr">
+        <is>
+          <t>411001</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" s="1" t="inlineStr">
+        <is>
+          <t>A52100019945</t>
+        </is>
+      </c>
+      <c r="B1525" t="inlineStr">
+        <is>
+          <t>Yogesh Panduraang Rajguruu</t>
+        </is>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>A52100019945</t>
+        </is>
+      </c>
+      <c r="D1525" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MVPT1zhnU5sz0%2b%2bR75eBTzsQe9mfOIdVF1hTDVTm1mKzPsjzeEYQJEag9or71Jk%2bg8nlSGA8eV0yYLuK05JlhK8JrV7nJZYQItkiRmkImnljKxNNM5pEoCqivQ7sXlNR3ajNu%2fJZC%2fzACraW0ENQyrKLaq4TaV6o0xdKwr2z8lz8MI7COCj7yQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1525" t="inlineStr">
+        <is>
+          <t>09823024974</t>
+        </is>
+      </c>
+      <c r="F1525" t="inlineStr">
+        <is>
+          <t>Vishrantwadi</t>
+        </is>
+      </c>
+      <c r="G1525" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1525" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1525" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1525" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" s="1" t="inlineStr">
+        <is>
+          <t>A52100020006</t>
+        </is>
+      </c>
+      <c r="B1526" t="inlineStr">
+        <is>
+          <t>Harshal Madhukar Bajad</t>
+        </is>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>A52100020006</t>
+        </is>
+      </c>
+      <c r="D1526" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wpMPmQTWJNdQ9aY8clV7Af5IljEb2KjCd3R5q%2fOst8eM1KSBsPBIAu%2boNrCKAvhj5sAC9HaXfJEqm5rIvF4otjrtrcWWIGIt%2f6Myg0SYdNC8WJYXubb6q%2fePuW7fKeLzDYExr2BnGsXi1EAB6BCFhUHxM6VXoL1qNkIQgAaHF4EPhTAmx9IrmQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1526" t="inlineStr">
+        <is>
+          <t>08446123555</t>
+        </is>
+      </c>
+      <c r="F1526" t="inlineStr">
+        <is>
+          <t>Ganraj Chowk</t>
+        </is>
+      </c>
+      <c r="G1526" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1526" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1526" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1526" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" s="1" t="inlineStr">
+        <is>
+          <t>A52100019922</t>
+        </is>
+      </c>
+      <c r="B1527" t="inlineStr">
+        <is>
+          <t>Sukhdev Haribhau Shendkar</t>
+        </is>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>A52100019922</t>
+        </is>
+      </c>
+      <c r="D1527" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=itjoqG3FXLxE5RnTP8JTGOT30xRBtxzogHeTdXtSfH5J%2bxzAH4e8ZRQBhyT1djE9fJqy4JvOXU0MfSq5v%2fM8%2bxHOrzXP9%2bMoezo7Pcksh3%2fmwOiKig7FIN4CqOWHbKt0IMbOwrQN8V3%2btyD1k%2byoWzyVUIvtVjwdNG0bKkR9FkGFPh5w6XcMIA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1527" t="inlineStr">
+        <is>
+          <t>02227710778</t>
+        </is>
+      </c>
+      <c r="F1527" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="G1527" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1527" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1527" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1527" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" s="1" t="inlineStr">
+        <is>
+          <t>A52100019975</t>
+        </is>
+      </c>
+      <c r="B1528" t="inlineStr">
+        <is>
+          <t>Aparna Ashok Giri</t>
+        </is>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>A52100019975</t>
+        </is>
+      </c>
+      <c r="D1528" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=ZZM%2bxUsG%2bmHIQAH98iKc4trL587t2p1kY2uYYaZDm0Z7TGBtp2b%2bWDouhJ5tw5%2b2%2bkRdgNoKkbBfbWSKPfcvQwUSTC4f4zf50FNS0EhsPrJw044wcUEK362YFmqzXckfYpB3VqBoM7A9UoTVv4BrfrAEzpvyjPi54Y%2b74fR9gMD8qAqxq223wg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1528" t="inlineStr">
+        <is>
+          <t>02024220578</t>
+        </is>
+      </c>
+      <c r="F1528" t="inlineStr">
+        <is>
+          <t>Satara Road</t>
+        </is>
+      </c>
+      <c r="G1528" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1528" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1528" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1528" t="inlineStr">
+        <is>
+          <t>411009</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" s="1" t="inlineStr">
+        <is>
+          <t>A52100029078</t>
+        </is>
+      </c>
+      <c r="B1529" t="inlineStr">
+        <is>
+          <t>Supriya Mahendra Kasar</t>
+        </is>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>A52100029078</t>
+        </is>
+      </c>
+      <c r="D1529" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=vxR2AetmWrg62rO0EDVpPIT2%2fwpqmaw5TIwS128ETe5WohSUh3Yx6yQJc3CKBVaWLWxecK58M2S9rnuO0yauSFq1aK2BDHU6Al9%2fFxODcmqnBtuFb71F3aZKev1VzURa181pAW2xL%2b4ilwpTWDbLJdqmAbKzMzLO7cKPO3W5rNOwuV4NVl%2bCFw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1529" t="inlineStr">
+        <is>
+          <t>07030920699</t>
+        </is>
+      </c>
+      <c r="F1529" t="inlineStr">
+        <is>
+          <t>Dighi</t>
+        </is>
+      </c>
+      <c r="G1529" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1529" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1529" t="inlineStr">
+        <is>
+          <t>Dighi</t>
+        </is>
+      </c>
+      <c r="J1529" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" s="1" t="inlineStr">
+        <is>
+          <t>A52100019909</t>
+        </is>
+      </c>
+      <c r="B1530" t="inlineStr">
+        <is>
+          <t>Meghana  Vyas</t>
+        </is>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>A52100019909</t>
+        </is>
+      </c>
+      <c r="D1530" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=MjMR5eH0Gh1oJ471zSRXuYLw9JZuw%2f20SqqjREYTHLucWRxzfogJgh3dvyaepPvDRzKF%2fbDSEGUVSUfduzVFt%2b%2bCV5wNmobm5Tfw9rMGt3UXikb84%2bS3wOGzsZ06xKIaV7FBE7dbbOUcc1nY8d474%2boTaNon0qArgNVHIfqx9uF9eZORboo7tw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1530" t="inlineStr">
+        <is>
+          <t>02025687746</t>
+        </is>
+      </c>
+      <c r="F1530" t="inlineStr">
+        <is>
+          <t>Rajiv Gandhi Infotech Park Hinjewadi</t>
+        </is>
+      </c>
+      <c r="G1530" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1530" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1530" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="J1530" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" s="1" t="inlineStr">
+        <is>
+          <t>A52100019933</t>
+        </is>
+      </c>
+      <c r="B1531" t="inlineStr">
+        <is>
+          <t>Mahesh B Gogawale Proprietor Of Reyaansh Real Estate Services</t>
+        </is>
+      </c>
+      <c r="C1531" t="inlineStr">
+        <is>
+          <t>A52100019933</t>
+        </is>
+      </c>
+      <c r="D1531" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=TUw3%2bo7VsjoNkuk2A0nQaFvxNap5NqfyIoJRCXo7CCNB91E%2fQphI6vGAD3rFiQls6RNtOu1gV3K3BrUtjVAEvTgjswBgHRW8sJJIFnmBO5gSvxGMGIiQZerRjQeguiXGLuYyAX0m90GX7PCEumtqy6GN05DW4Byly%2f%2bz07W%2fO9vKHGWk9y8Y7w%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1531" t="inlineStr">
+        <is>
+          <t>07709190808</t>
+        </is>
+      </c>
+      <c r="F1531" t="inlineStr">
+        <is>
+          <t>Warje Malwadi</t>
+        </is>
+      </c>
+      <c r="G1531" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1531" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1531" t="inlineStr">
+        <is>
+          <t>Warje</t>
+        </is>
+      </c>
+      <c r="J1531" t="inlineStr">
+        <is>
+          <t>411058</t>
+        </is>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" s="1" t="inlineStr">
+        <is>
+          <t>A52100019954</t>
+        </is>
+      </c>
+      <c r="B1532" t="inlineStr">
+        <is>
+          <t>Dharmdas Manikmal Kundnani</t>
+        </is>
+      </c>
+      <c r="C1532" t="inlineStr">
+        <is>
+          <t>A52100019954</t>
+        </is>
+      </c>
+      <c r="D1532" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=W0zkaIVEhhdgXBy3H7trPTsRyf%2fk%2b5JiIFkkSvZXPE7dAdM3kSyCkwxUmCjIC4Z4YVsYzQ%2fHJawIeeibPCsOGFkjkmppIGCNWh5TLN%2b5W68m8hlLpUasA%2fQVJsOHB0bWT8aJb1LU5QfVm7Fy4eGm12hZIpsCBl8Jw1n1pyhvpviL8aCdXWUUqA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1532" t="inlineStr">
+        <is>
+          <t>02027410226</t>
+        </is>
+      </c>
+      <c r="F1532" t="inlineStr">
+        <is>
+          <t>Pimprigaon</t>
+        </is>
+      </c>
+      <c r="G1532" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1532" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1532" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1532" t="inlineStr">
+        <is>
+          <t>411017</t>
+        </is>
+      </c>
+    </row>
+    <row r="1533">
+      <c r="A1533" s="1" t="inlineStr">
+        <is>
+          <t>A52100020304</t>
+        </is>
+      </c>
+      <c r="B1533" t="inlineStr">
+        <is>
+          <t>Manisha Prashant Abnave</t>
+        </is>
+      </c>
+      <c r="C1533" t="inlineStr">
+        <is>
+          <t>A52100020304</t>
+        </is>
+      </c>
+      <c r="D1533" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5snJw%2fb%2fC2VA7MMxfKn8ug75VlAjxo6H5uVffzzG%2boI09ChSgkrZBwdMSvWFl5tV70jUdMfPbZT6Xst728h8CSrMG2YHrXEJHGmim4ezjCZfpTOlZQ6qEGHxTFd9QcjfyTY%2f0lA5Fh%2fSMOHrFdXJWW86pEDS86pW8tf3Tnb2veKlIAPt3KTGQQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1533" t="inlineStr">
+        <is>
+          <t>00000000000</t>
+        </is>
+      </c>
+      <c r="F1533" t="inlineStr">
+        <is>
+          <t>Sasane Nagar</t>
+        </is>
+      </c>
+      <c r="G1533" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1533" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1533" t="inlineStr">
+        <is>
+          <t>Hadapsar</t>
+        </is>
+      </c>
+      <c r="J1533" t="inlineStr">
+        <is>
+          <t>411028</t>
+        </is>
+      </c>
+    </row>
+    <row r="1534">
+      <c r="A1534" s="1" t="inlineStr">
+        <is>
+          <t>A52100020043</t>
+        </is>
+      </c>
+      <c r="B1534" t="inlineStr">
+        <is>
+          <t>Sudha  Chaurasiya</t>
+        </is>
+      </c>
+      <c r="C1534" t="inlineStr">
+        <is>
+          <t>A52100020043</t>
+        </is>
+      </c>
+      <c r="D1534" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=1nFGM9N76PMy9GQTKia%2f%2bjcYFhb4T8o9Rt4xw0%2bvPMPm4YuVvvHhUd3Rf%2fHhKBDp5tMkTYtTcbOYrvosBTzMi7sgn75dM8M6iw1DnZSjoohwIcKLphnp1oAX7FCKDJUgIrVaehEOLtInK3qoQBLcufCs5cLyefkS8FYnKAyo14YpGy%2f60stqWw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1534" t="inlineStr">
+        <is>
+          <t>09096192507</t>
+        </is>
+      </c>
+      <c r="F1534" t="inlineStr">
+        <is>
+          <t>Kaspatewasti</t>
+        </is>
+      </c>
+      <c r="G1534" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1534" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1534" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1534" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" s="1" t="inlineStr">
+        <is>
+          <t>A52100020081</t>
+        </is>
+      </c>
+      <c r="B1535" t="inlineStr">
+        <is>
+          <t>Abhijeet Eknath Aajgaonkar</t>
+        </is>
+      </c>
+      <c r="C1535" t="inlineStr">
+        <is>
+          <t>A52100020081</t>
+        </is>
+      </c>
+      <c r="D1535" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=SzuJzZFCd6EMK%2fihJqSrNnhtNVaQa6KS9Uho7whEeS5WZuQ4GfD9CtrsooXZy9r6KFJGdV1AXK55IFXaz3A2Up%2bbuJLEumzSWGldSAnOLjZGE%2bvqUOcK20nV1TLPhHSQDpt%2fc66K%2fXOe9VhH3WFs3DxiJ1CN61urZ3v1ys0AlQeN5rEU7yYbBQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1535" t="inlineStr">
+        <is>
+          <t>02225973174</t>
+        </is>
+      </c>
+      <c r="F1535" t="inlineStr">
+        <is>
+          <t>Thane</t>
+        </is>
+      </c>
+      <c r="G1535" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1535" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1535" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1535" t="inlineStr">
+        <is>
+          <t>400607</t>
+        </is>
+      </c>
+    </row>
+    <row r="1536">
+      <c r="A1536" s="1" t="inlineStr">
+        <is>
+          <t>A52100019988</t>
+        </is>
+      </c>
+      <c r="B1536" t="inlineStr">
+        <is>
+          <t>Aatif Eqbal  Khan</t>
+        </is>
+      </c>
+      <c r="C1536" t="inlineStr">
+        <is>
+          <t>A52100019988</t>
+        </is>
+      </c>
+      <c r="D1536" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=wwQ4lVQQnwkvUzezBDcW3%2bHRBjSRKmpmxRpxXjgo06bJb%2bTOszXLNYD2gjieLUr4Yu3Kz6vDDF1IvjEF%2fzXA5qm3Qg%2fpSKsYqMhjIsjHOj%2fQnbkhapVXQsOx4mrSUpfGnDPQtek9kEVG%2bha5NE7L%2bKCOg9QBdataCu%2fZgTaBp7%2f7w9nrGC0gFw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1536" t="inlineStr">
+        <is>
+          <t>02027420910</t>
+        </is>
+      </c>
+      <c r="F1536" t="inlineStr">
+        <is>
+          <t>Srno; 7/8/9</t>
+        </is>
+      </c>
+      <c r="G1536" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1536" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1536" t="inlineStr">
+        <is>
+          <t>Bavdhan Kh.</t>
+        </is>
+      </c>
+      <c r="J1536" t="inlineStr">
+        <is>
+          <t>411021</t>
+        </is>
+      </c>
+    </row>
+    <row r="1537">
+      <c r="A1537" s="1" t="inlineStr">
+        <is>
+          <t>A52100019953</t>
+        </is>
+      </c>
+      <c r="B1537" t="inlineStr">
+        <is>
+          <t>Afsar Ayub Khan</t>
+        </is>
+      </c>
+      <c r="C1537" t="inlineStr">
+        <is>
+          <t>A52100019953</t>
+        </is>
+      </c>
+      <c r="D1537" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=yZrzC8AvmfHpsoah9%2bJZJi%2bxlTteFzbsbn1ADDeIzW9%2fdCXP%2btpkTlACZPTpIsB9tVB1Wb1msBJL6tS3o4Zn6MkDdvd5%2f639%2f2qovgLgDASX70wRQJsyCSJWaUBtUjnCrzsAj8kcoHAzn9zJBDHBKhioyQkQglAgcK224vkXX07WqfrZMZTb5Q%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1537" t="inlineStr">
+        <is>
+          <t>07798571755</t>
+        </is>
+      </c>
+      <c r="F1537" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="G1537" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1537" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1537" t="inlineStr">
+        <is>
+          <t>Mohammadwadi</t>
+        </is>
+      </c>
+      <c r="J1537" t="inlineStr">
+        <is>
+          <t>411060</t>
+        </is>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" s="1" t="inlineStr">
+        <is>
+          <t>A52100002853</t>
+        </is>
+      </c>
+      <c r="B1538" t="inlineStr">
+        <is>
+          <t>Dhananjay Subhash Deshmukh</t>
+        </is>
+      </c>
+      <c r="C1538" t="inlineStr">
+        <is>
+          <t>A52100002853</t>
+        </is>
+      </c>
+      <c r="D1538" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=Xb0zesJZsg9HEZbyEfxh%2boh%2fF%2fT99AydUsuWReTUX1YJmZ2jl6BA%2b1FF41jRpuoboGYlJLwASl3kZV1%2be8RDfZ1CW17bCY%2bO4mt4NgifCLb34pXEjI91lJFK4E1axIjnQew%2fH5c64rWcQhRBBaIGuBj3BzTEYDY%2fOOnPpqpmut6hN%2bmtZNM1qA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1538" t="inlineStr">
+        <is>
+          <t>09595825300</t>
+        </is>
+      </c>
+      <c r="F1538" t="inlineStr">
+        <is>
+          <t>Borade Vasti</t>
+        </is>
+      </c>
+      <c r="G1538" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1538" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1538" t="inlineStr">
+        <is>
+          <t>Aalandi</t>
+        </is>
+      </c>
+      <c r="J1538" t="inlineStr">
+        <is>
+          <t>412105</t>
+        </is>
+      </c>
+    </row>
+    <row r="1539">
+      <c r="A1539" s="1" t="inlineStr">
+        <is>
+          <t>A52100020037</t>
+        </is>
+      </c>
+      <c r="B1539" t="inlineStr">
+        <is>
+          <t>Avinash  Srivastava Proprietor Of Right House Property</t>
+        </is>
+      </c>
+      <c r="C1539" t="inlineStr">
+        <is>
+          <t>A52100020037</t>
+        </is>
+      </c>
+      <c r="D1539" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=8nOKXp7tyZ0AJ%2bgTrSU6S%2bw8r3bLf8ArFs5rQ9V%2bIcUzYz2AFUW5MSmHvVjOpyzQZzaYY1csGbkhAT7XknRoM0Hx98xyHQfX3i%2fW1ospL9plVz6nU9xJxBjApN6TUG40qFfYNeYfmbf4U1DFIvLGY2Q%2fPilhml0Fpfg4zYQH8zFPjOQL7wXVQg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1539" t="inlineStr">
+        <is>
+          <t>09604268830</t>
+        </is>
+      </c>
+      <c r="F1539" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="G1539" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1539" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1539" t="inlineStr">
+        <is>
+          <t>Dhanori</t>
+        </is>
+      </c>
+      <c r="J1539" t="inlineStr">
+        <is>
+          <t>411015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1540">
+      <c r="A1540" s="1" t="inlineStr">
+        <is>
+          <t>A52100020011</t>
+        </is>
+      </c>
+      <c r="B1540" t="inlineStr">
+        <is>
+          <t>Umesh  Kumar</t>
+        </is>
+      </c>
+      <c r="C1540" t="inlineStr">
+        <is>
+          <t>A52100020011</t>
+        </is>
+      </c>
+      <c r="D1540" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=5pO1WstuxmpcA7LwHKzac5xS4l8gUqbZI3npe63tKgeCGMta2VV4ZaTGM2gbjKsbd6MyfP05Y7TIJ9wSGR4IGQPNQkSBOUV59PGCKLpxu8UdgS84DK7itDVzC8RZa4JpDrV4mQDt6so1PFkKrbUX05NajagaVlpdaZrqumWB7WGEhXCRNOOQjQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1540" t="inlineStr">
+        <is>
+          <t>09028533829</t>
+        </is>
+      </c>
+      <c r="F1540" t="inlineStr">
+        <is>
+          <t>Nahre</t>
+        </is>
+      </c>
+      <c r="G1540" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1540" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1540" t="inlineStr">
+        <is>
+          <t>Narhe</t>
+        </is>
+      </c>
+      <c r="J1540" t="inlineStr">
+        <is>
+          <t>411041</t>
+        </is>
+      </c>
+    </row>
+    <row r="1541">
+      <c r="A1541" s="1" t="inlineStr">
+        <is>
+          <t>A52100020033</t>
+        </is>
+      </c>
+      <c r="B1541" t="inlineStr">
+        <is>
+          <t>Rajendra Balasaheb Patait</t>
+        </is>
+      </c>
+      <c r="C1541" t="inlineStr">
+        <is>
+          <t>A52100020033</t>
+        </is>
+      </c>
+      <c r="D1541" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=v5bx7WxieMazC3%2bYbHBzZqF2BSuMcVPRZpRs4jBJ%2btN8aBWk%2fyDTX4Af2%2bud2zBOl63FvQGfaiIV5OZx%2boBg0TQXeg6M6OPpWu9ZdMzit%2blqPu0AjC6w4dcKKX4yA1YvfxhYQOMs62LdjMViiazLick186DURhZ11uHQ6csIdT6gNWoir%2f7Cbw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1541" t="inlineStr">
+        <is>
+          <t>09657191000</t>
+        </is>
+      </c>
+      <c r="F1541" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="G1541" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1541" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1541" t="inlineStr">
+        <is>
+          <t>Wagholi</t>
+        </is>
+      </c>
+      <c r="J1541" t="inlineStr">
+        <is>
+          <t>412207</t>
+        </is>
+      </c>
+    </row>
+    <row r="1542">
+      <c r="A1542" s="1" t="inlineStr">
+        <is>
+          <t>A52100020156</t>
+        </is>
+      </c>
+      <c r="B1542" t="inlineStr">
+        <is>
+          <t>Lijihas Ussain Kakkarambath</t>
+        </is>
+      </c>
+      <c r="C1542" t="inlineStr">
+        <is>
+          <t>A52100020156</t>
+        </is>
+      </c>
+      <c r="D1542" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=qHu0Vsm1Jxop0K0cvxCmQTRKa7DTW0UnHiIcaV63H%2b24fz62ABOW6wgpMIbhWlekC1iQ3jEfk4jeVbvc%2bZi%2bqw3irFN9%2bSXK9YgPGksp3oBaIbKjEgBsRiQLqh3ybgP3vdO9U6PJCwIO9IcD%2bNWEg%2fJvkCRKBhFdeE78ojGlEsY%2fMbqCpfUtYw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1542" t="inlineStr">
+        <is>
+          <t>02225105211</t>
+        </is>
+      </c>
+      <c r="F1542" t="inlineStr">
+        <is>
+          <t>Kharadi Pune</t>
+        </is>
+      </c>
+      <c r="G1542" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1542" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1542" t="inlineStr">
+        <is>
+          <t>Kharadi</t>
+        </is>
+      </c>
+      <c r="J1542" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1543">
+      <c r="A1543" s="1" t="inlineStr">
+        <is>
+          <t>A52100019972</t>
+        </is>
+      </c>
+      <c r="B1543" t="inlineStr">
+        <is>
+          <t>Achala Sachin Pradhan</t>
+        </is>
+      </c>
+      <c r="C1543" t="inlineStr">
+        <is>
+          <t>A52100019972</t>
+        </is>
+      </c>
+      <c r="D1543" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=d5Q17UtWq2t5TSoiv91R2%2fkgc4VGh6jsmMlFYmApZYL%2bX9HuBnsAnwqHhfWGnSQSe%2bALKS9%2bz2TSMAK5JunrAGDTHxy%2fPL40oNEyuaBjA6o8qoymeQX%2bkfUHtrwtgtdHujAEmm5f3u%2b9Qvn7srP5wE0gV6M7PL%2bNM74PWAG7yq2c9iHhrJtaUA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1543" t="inlineStr">
+        <is>
+          <t>02025885301</t>
+        </is>
+      </c>
+      <c r="F1543" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+      <c r="G1543" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1543" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1543" t="inlineStr"/>
+      <c r="J1543" t="inlineStr">
+        <is>
+          <t>411007</t>
+        </is>
+      </c>
+    </row>
+    <row r="1544">
+      <c r="A1544" s="1" t="inlineStr">
+        <is>
+          <t>A52100020128</t>
+        </is>
+      </c>
+      <c r="B1544" t="inlineStr">
+        <is>
+          <t>Jinalayaspaces</t>
+        </is>
+      </c>
+      <c r="C1544" t="inlineStr">
+        <is>
+          <t>A52100020128</t>
+        </is>
+      </c>
+      <c r="D1544" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=L40gowWis9dTFheuZNIGw4r63s1SH4F%2flT8TsZVhIatOMSFy9xs1tC%2f%2bVaNlMKPd7RA55p8iUjwZvSi4Gs37W4P%2bnb9t%2blsGRby5Uwhj0uCptu3tSCN%2byRy4arY0j5%2bshMWT2MSxR%2bQ1dna6Oo%2fJ9D%2fsmXHR1bj7XDVJwAg%2f8xfX6jdSB1geJQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1544" t="inlineStr">
+        <is>
+          <t>02041230728</t>
+        </is>
+      </c>
+      <c r="F1544" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="G1544" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1544" t="inlineStr">
+        <is>
+          <t>Mawal</t>
+        </is>
+      </c>
+      <c r="I1544" t="inlineStr"/>
+      <c r="J1544" t="inlineStr">
+        <is>
+          <t>411019</t>
+        </is>
+      </c>
+    </row>
+    <row r="1545">
+      <c r="A1545" s="1" t="inlineStr">
+        <is>
+          <t>A52100002919</t>
+        </is>
+      </c>
+      <c r="B1545" t="inlineStr">
+        <is>
+          <t>Ganesh Dashrath Jainak</t>
+        </is>
+      </c>
+      <c r="C1545" t="inlineStr">
+        <is>
+          <t>A52100002919</t>
+        </is>
+      </c>
+      <c r="D1545" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=bnb3uzZLoTeyAulSo8Og5QSk%2fkz%2fwXt0VuFC5i%2bEeRQzqBlmUfa7JM11wPT6Q4jNKSyWQwns9jxwc%2b%2bH6PZgf8xpG4e6A96pRikyNUD%2fOt0ZARDf%2bl%2bOZuIOfXHBOcht29Lj92MFg3Qm%2bLuNeGjoAubz5q533KUhKDzOhm5xsWtz2f0I%2fKynAQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1545" t="inlineStr">
+        <is>
+          <t>02024332071</t>
+        </is>
+      </c>
+      <c r="F1545" t="inlineStr">
+        <is>
+          <t>Sadashiv Peth</t>
+        </is>
+      </c>
+      <c r="G1545" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1545" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1545" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1545" t="inlineStr">
+        <is>
+          <t>411030</t>
+        </is>
+      </c>
+    </row>
+    <row r="1546">
+      <c r="A1546" s="1" t="inlineStr">
+        <is>
+          <t>A52100020067</t>
+        </is>
+      </c>
+      <c r="B1546" t="inlineStr">
+        <is>
+          <t>Laju  Menon</t>
+        </is>
+      </c>
+      <c r="C1546" t="inlineStr">
+        <is>
+          <t>A52100020067</t>
+        </is>
+      </c>
+      <c r="D1546" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=cac0uxkIWLm61sDwcFUxbG67as1BOgl6U4oOHSP0bmvCxd0OKa0BbPK%2bFh396mUBn5ygcdNEJSOz9neWnJTb3ZETzmt%2bZzLH1CAQWwRX53zLwHJgopedPqd2bwsZn6B%2fJELP4c9WawhCNRna8LrR45QajMjVaGurwHtQUR2RxZKxK5oHvV6Vvw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1546" t="inlineStr">
+        <is>
+          <t>09518391868</t>
+        </is>
+      </c>
+      <c r="F1546" t="inlineStr">
+        <is>
+          <t>Chinchwad</t>
+        </is>
+      </c>
+      <c r="G1546" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1546" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1546" t="inlineStr">
+        <is>
+          <t>Pimpri Chinchawad (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1546" t="inlineStr">
+        <is>
+          <t>411033</t>
+        </is>
+      </c>
+    </row>
+    <row r="1547">
+      <c r="A1547" s="1" t="inlineStr">
+        <is>
+          <t>A52100002800</t>
+        </is>
+      </c>
+      <c r="B1547" t="inlineStr">
+        <is>
+          <t>Kapil Dilip Laghate</t>
+        </is>
+      </c>
+      <c r="C1547" t="inlineStr">
+        <is>
+          <t>A52100002800</t>
+        </is>
+      </c>
+      <c r="D1547" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=tIPPCHVTMe7pprO%2bVlUXZvglk7XAnlYutIOaaEvZ4tX6xvVKbSWcLA9xd8QncY566rzhgLExVYoKhWFQjK7NPo716dkh%2bEMAZzwQTR%2b1pQXKk%2fT5KtamJSXLIeiSJiz%2bXWaDvEYRMaOxh8%2fATTLO5Kl3r4ZrVvugS%2bEvwr3paY6IbYFw82xnzw%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1547" t="inlineStr">
+        <is>
+          <t>91962343000</t>
+        </is>
+      </c>
+      <c r="F1547" t="inlineStr">
+        <is>
+          <t>Karvenagar</t>
+        </is>
+      </c>
+      <c r="G1547" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1547" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1547" t="inlineStr">
+        <is>
+          <t>Karve Nagar</t>
+        </is>
+      </c>
+      <c r="J1547" t="inlineStr">
+        <is>
+          <t>411052</t>
+        </is>
+      </c>
+    </row>
+    <row r="1548">
+      <c r="A1548" s="1" t="inlineStr">
+        <is>
+          <t>A52100020349</t>
+        </is>
+      </c>
+      <c r="B1548" t="inlineStr">
+        <is>
+          <t>Smita Satish Giri</t>
+        </is>
+      </c>
+      <c r="C1548" t="inlineStr">
+        <is>
+          <t>A52100020349</t>
+        </is>
+      </c>
+      <c r="D1548" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=JSdXU7Jj1vP0QdiVREPjgyJ%2fSK2Eo90h%2fr9DtqC0jdyhnci3MPeM9s6sjnnKr1Xo6VvSBEYnTU2ebNxKm1Ej9ezYhRd5dOrRAwIx%2fc6Vbflnx4NxzZUAagOjapASbcicW%2feL5%2fCkoNw42%2bOAdGv%2fB4JTuJvHWnil1WVWs2IAg9o0lZpFRQ1agg%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1548" t="inlineStr">
+        <is>
+          <t>02065266526</t>
+        </is>
+      </c>
+      <c r="F1548" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="G1548" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1548" t="inlineStr">
+        <is>
+          <t>Haveli</t>
+        </is>
+      </c>
+      <c r="I1548" t="inlineStr">
+        <is>
+          <t>Baner</t>
+        </is>
+      </c>
+      <c r="J1548" t="inlineStr">
+        <is>
+          <t>411045</t>
+        </is>
+      </c>
+    </row>
+    <row r="1549">
+      <c r="A1549" s="1" t="inlineStr">
+        <is>
+          <t>A52100020001</t>
+        </is>
+      </c>
+      <c r="B1549" t="inlineStr">
+        <is>
+          <t>Divya Vijay Gwalani</t>
+        </is>
+      </c>
+      <c r="C1549" t="inlineStr">
+        <is>
+          <t>A52100020001</t>
+        </is>
+      </c>
+      <c r="D1549" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=baYhnrgBbCydplzAVSgpnCKFnvOcbPJTFsAjxc1bx%2flTAwW5mtZYmoyXu3PcJe9r%2fEtALKDpVzkwiWCZXNoeq8sLQFUnuMfRN4J7Q30%2fBdGYZnrpxWyQt5uZ6CBXgcBoqPr3PqvbcwsjASzutPYoE24fM0h7CnspOL%2fs59Ww6n2NpygP7Wo%2bPA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1549" t="inlineStr">
+        <is>
+          <t>09820235761</t>
+        </is>
+      </c>
+      <c r="F1549" t="inlineStr">
+        <is>
+          <t>Kalyani Nagar</t>
+        </is>
+      </c>
+      <c r="G1549" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1549" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1549" t="inlineStr"/>
+      <c r="J1549" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1550">
+      <c r="A1550" s="1" t="inlineStr">
+        <is>
+          <t>A52100019990</t>
+        </is>
+      </c>
+      <c r="B1550" t="inlineStr">
+        <is>
+          <t>Nilesh Shantaram Deshmukh</t>
+        </is>
+      </c>
+      <c r="C1550" t="inlineStr">
+        <is>
+          <t>A52100019990</t>
+        </is>
+      </c>
+      <c r="D1550" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=H8YgtpvclgdleYfV43ct9ujMmQG%2bp99Nb9fqFAqc%2b8Y3D1vQMIycH6wQ%2b6jIM%2bpWqWjrQ8LZQsQfRUrZC4DGuk6lCXFzzdzfeVynO8rykExg8olcp5BjEQ0ZTFZ49W5ynuyFIzUj%2f22PNOyEuz%2bTcR3SB6rSc8vYJOWl8XE9Dlu74RE05Eg4pQ%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1550" t="inlineStr">
+        <is>
+          <t>09764233600</t>
+        </is>
+      </c>
+      <c r="F1550" t="inlineStr">
+        <is>
+          <t>Wadgaonsheri</t>
+        </is>
+      </c>
+      <c r="G1550" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1550" t="inlineStr">
+        <is>
+          <t>Pune City</t>
+        </is>
+      </c>
+      <c r="I1550" t="inlineStr">
+        <is>
+          <t>Pune (M Corp.)</t>
+        </is>
+      </c>
+      <c r="J1550" t="inlineStr">
+        <is>
+          <t>411014</t>
+        </is>
+      </c>
+    </row>
+    <row r="1551">
+      <c r="A1551" s="1" t="inlineStr">
+        <is>
+          <t>A52100020002</t>
+        </is>
+      </c>
+      <c r="B1551" t="inlineStr">
+        <is>
+          <t>Ashwani  Fotedar</t>
+        </is>
+      </c>
+      <c r="C1551" t="inlineStr">
+        <is>
+          <t>A52100020002</t>
+        </is>
+      </c>
+      <c r="D1551" t="inlineStr">
+        <is>
+          <t>https://maharerait.mahaonline.gov.in/PrintPreview/PrintPreview?q=KOIoFjM4YWgk%2bHBzj6ggJxOgmXUBdIWs%2fVhoWYX%2fPn1kFCuGVHZYDzcIOWGkliBRGIoyXpQmf6F1RsQl138VvUO59UySFCRi6v6WUxtbdKMjESWIiugIM7NuELcCBPNzgEcVL0tTlCv2kjYKThGahHHdajGEISBecPyG2eDmuJ7R9VFOCARlsA%3d%3d</t>
+        </is>
+      </c>
+      <c r="E1551" t="inlineStr">
+        <is>
+          <t>08446477774</t>
+        </is>
+      </c>
+      <c r="F1551" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="G1551" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="H1551" t="inlineStr">
+        <is>
+          <t>Mulshi</t>
+        </is>
+      </c>
+      <c r="I1551" t="inlineStr">
+        <is>
+          <t>Wakad</t>
+        </is>
+      </c>
+      <c r="J1551" t="inlineStr">
+        <is>
+          <t>411057</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>